<commit_message>
Model now requires a list of all parameters
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -4319,7 +4319,7 @@
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,9 +4616,6 @@
       <c r="U4" s="112">
         <v>0</v>
       </c>
-      <c r="Y4" s="112">
-        <v>1</v>
-      </c>
       <c r="Z4" s="112">
         <v>0.5</v>
       </c>

</xml_diff>

<commit_message>
Added scenario functionality through spreadsheet
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10230" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="5" r:id="rId2"/>
     <sheet name="base" sheetId="15" r:id="rId3"/>
-    <sheet name="timepars" sheetId="20" r:id="rId4"/>
-    <sheet name="PrEPX" sheetId="21" r:id="rId5"/>
+    <sheet name="PrEPX" sheetId="21" r:id="rId4"/>
+    <sheet name="timepars" sheetId="20" r:id="rId5"/>
+    <sheet name="scen_1" sheetId="23" r:id="rId6"/>
+    <sheet name="scen_2" sheetId="22" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1020,7 +1022,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="158">
   <si>
     <t>Waiting list</t>
   </si>
@@ -1488,6 +1490,12 @@
   </si>
   <si>
     <t>test_wait</t>
+  </si>
+  <si>
+    <t>relative_foi</t>
+  </si>
+  <si>
+    <t>num_prep</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2302,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4315,11 +4323,348 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" style="89" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="89" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="89" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" style="89" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" style="89" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="89"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="89">
+        <v>6925</v>
+      </c>
+      <c r="C3" s="89">
+        <v>5115</v>
+      </c>
+      <c r="D3" s="89">
+        <v>431</v>
+      </c>
+      <c r="E3" s="89">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="89">
+        <v>100</v>
+      </c>
+      <c r="C4" s="89">
+        <v>91.21</v>
+      </c>
+      <c r="D4" s="89">
+        <v>7.69</v>
+      </c>
+      <c r="E4" s="89">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="89">
+        <v>1.59</v>
+      </c>
+      <c r="C5" s="89">
+        <v>1.48</v>
+      </c>
+      <c r="D5" s="89">
+        <v>2.42</v>
+      </c>
+      <c r="E5" s="89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="89">
+        <v>3.21</v>
+      </c>
+      <c r="C6" s="89">
+        <v>0</v>
+      </c>
+      <c r="D6" s="89">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="E6" s="89">
+        <v>25.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="89">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C7" s="89">
+        <v>0</v>
+      </c>
+      <c r="D7" s="89">
+        <v>47.38</v>
+      </c>
+      <c r="E7" s="89">
+        <v>100.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="89" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="89">
+        <v>2074</v>
+      </c>
+      <c r="C12" s="89">
+        <v>1330</v>
+      </c>
+      <c r="D12" s="89">
+        <v>476</v>
+      </c>
+      <c r="E12" s="89">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="89">
+        <v>100</v>
+      </c>
+      <c r="C13" s="89">
+        <v>64.13</v>
+      </c>
+      <c r="D13" s="89">
+        <v>22.95</v>
+      </c>
+      <c r="E13" s="89">
+        <v>12.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="89">
+        <v>4.55</v>
+      </c>
+      <c r="C14" s="89">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="D14" s="89">
+        <v>4.71</v>
+      </c>
+      <c r="E14" s="89">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="89">
+        <v>8.61</v>
+      </c>
+      <c r="C15" s="89">
+        <v>0</v>
+      </c>
+      <c r="D15" s="89">
+        <v>13.18</v>
+      </c>
+      <c r="E15" s="89">
+        <v>27.21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="89">
+        <v>41.3</v>
+      </c>
+      <c r="C16" s="89">
+        <v>0</v>
+      </c>
+      <c r="D16" s="89">
+        <v>61.17</v>
+      </c>
+      <c r="E16" s="89">
+        <v>154.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="89">
+        <v>1356</v>
+      </c>
+      <c r="C21" s="89">
+        <v>1154</v>
+      </c>
+      <c r="D21" s="89">
+        <v>156</v>
+      </c>
+      <c r="E21" s="89">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="89">
+        <v>100</v>
+      </c>
+      <c r="C22" s="89">
+        <v>85.1</v>
+      </c>
+      <c r="D22" s="89">
+        <v>11.5</v>
+      </c>
+      <c r="E22" s="89">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="89">
+        <v>2</v>
+      </c>
+      <c r="C23" s="89">
+        <v>1.83</v>
+      </c>
+      <c r="D23" s="89">
+        <v>2.68</v>
+      </c>
+      <c r="E23" s="89">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="89">
+        <v>4.67</v>
+      </c>
+      <c r="C24" s="89">
+        <v>0</v>
+      </c>
+      <c r="D24" s="89">
+        <v>15.68</v>
+      </c>
+      <c r="E24" s="89">
+        <v>27.21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="89">
+        <v>9.33</v>
+      </c>
+      <c r="C25" s="89">
+        <v>0</v>
+      </c>
+      <c r="D25" s="89">
+        <v>43.56</v>
+      </c>
+      <c r="E25" s="89">
+        <v>98.07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,9 +4694,14 @@
     <col min="25" max="25" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -4433,8 +4783,23 @@
       <c r="AA1" s="89" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -4492,8 +4857,17 @@
       <c r="U2" s="89" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC2" s="89" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD2" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE2" s="89" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -4549,7 +4923,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -4616,44 +4990,62 @@
       <c r="U4" s="112">
         <v>0</v>
       </c>
+      <c r="Y4" s="112">
+        <v>1</v>
+      </c>
       <c r="Z4" s="112">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="112">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.04</v>
+      </c>
+      <c r="AB4" s="112">
+        <v>0.7</v>
+      </c>
+      <c r="AC4" s="112">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="112">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="112">
+        <v>0.05</v>
+      </c>
+      <c r="AF4" s="112">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89">
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89">
         <v>2003</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="89">
         <v>2004</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89">
         <v>2005</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89">
         <v>2006</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="89">
         <v>2007</v>
       </c>
@@ -4667,17 +5059,17 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89">
         <v>2008</v>
       </c>
     </row>
-    <row r="13" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89">
         <v>2009</v>
       </c>
     </row>
-    <row r="14" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89">
         <v>2010</v>
       </c>
@@ -4691,12 +5083,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89">
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="112" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" s="112" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89">
         <v>2012</v>
       </c>
@@ -4792,336 +5184,482 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="89" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="89"/>
+    <col min="1" max="1" width="9" style="89" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="89"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="89" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="89" t="s">
+        <v>147</v>
+      </c>
       <c r="B2" s="89" t="s">
-        <v>97</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="89">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="112">
+        <v>0.05</v>
+      </c>
+      <c r="C4" s="112">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="89">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="89">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="89">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="89">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="89">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="89">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="89">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="89">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="89">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89">
+        <v>2014</v>
+      </c>
+      <c r="B18" s="112">
+        <v>0.05</v>
+      </c>
+      <c r="C18" s="112">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89">
+        <v>2015</v>
+      </c>
+      <c r="B19" s="112">
+        <v>1</v>
+      </c>
+      <c r="C19" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="89">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="89">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="89">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="89" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="89" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="89"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="89" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="89" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>131</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="E2" s="89" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="F2" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="89" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="89" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="89" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="89">
-        <v>6925</v>
-      </c>
-      <c r="C3" s="89">
-        <v>5115</v>
-      </c>
-      <c r="D3" s="89">
-        <v>431</v>
-      </c>
-      <c r="E3" s="89">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="89">
-        <v>100</v>
-      </c>
-      <c r="C4" s="89">
-        <v>91.21</v>
-      </c>
-      <c r="D4" s="89">
-        <v>7.69</v>
-      </c>
-      <c r="E4" s="89">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="89">
-        <v>1.59</v>
-      </c>
-      <c r="C5" s="89">
-        <v>1.48</v>
-      </c>
-      <c r="D5" s="89">
-        <v>2.42</v>
-      </c>
-      <c r="E5" s="89">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="89">
-        <v>3.21</v>
-      </c>
-      <c r="C6" s="89">
-        <v>0</v>
-      </c>
-      <c r="D6" s="89">
-        <v>19.559999999999999</v>
-      </c>
-      <c r="E6" s="89">
-        <v>25.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="89" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="89">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C7" s="89">
-        <v>0</v>
-      </c>
-      <c r="D7" s="89">
-        <v>47.38</v>
-      </c>
-      <c r="E7" s="89">
-        <v>100.82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="89" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="89" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="89" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="89" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="89">
-        <v>2074</v>
-      </c>
-      <c r="C12" s="89">
-        <v>1330</v>
-      </c>
-      <c r="D12" s="89">
-        <v>476</v>
-      </c>
-      <c r="E12" s="89">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="89" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="89">
-        <v>100</v>
-      </c>
-      <c r="C13" s="89">
-        <v>64.13</v>
-      </c>
-      <c r="D13" s="89">
-        <v>22.95</v>
-      </c>
-      <c r="E13" s="89">
-        <v>12.92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="89">
-        <v>4.55</v>
-      </c>
-      <c r="C14" s="89">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="D14" s="89">
-        <v>4.71</v>
-      </c>
-      <c r="E14" s="89">
-        <v>5.53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="89">
-        <v>8.61</v>
-      </c>
-      <c r="C15" s="89">
-        <v>0</v>
-      </c>
-      <c r="D15" s="89">
-        <v>13.18</v>
-      </c>
-      <c r="E15" s="89">
-        <v>27.21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="89">
-        <v>41.3</v>
-      </c>
-      <c r="C16" s="89">
-        <v>0</v>
-      </c>
-      <c r="D16" s="89">
-        <v>61.17</v>
-      </c>
-      <c r="E16" s="89">
-        <v>154.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="89" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="89" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="89" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="89" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="89">
-        <v>1356</v>
-      </c>
-      <c r="C21" s="89">
-        <v>1154</v>
-      </c>
-      <c r="D21" s="89">
-        <v>156</v>
-      </c>
-      <c r="E21" s="89">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="89" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="89">
-        <v>100</v>
-      </c>
-      <c r="C22" s="89">
-        <v>85.1</v>
-      </c>
-      <c r="D22" s="89">
-        <v>11.5</v>
-      </c>
-      <c r="E22" s="89">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="89">
+        <v>148</v>
+      </c>
+      <c r="B3" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="89" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="89">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="112">
+        <v>1</v>
+      </c>
+      <c r="C4" s="112">
+        <v>3</v>
+      </c>
+      <c r="D4" s="112">
+        <v>10</v>
+      </c>
+      <c r="E4" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="112">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="112">
+        <v>5</v>
+      </c>
+      <c r="H4" s="112">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="112">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="112">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="89">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="89">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="89">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="89">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="89">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="89">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="89">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="89">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="89">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89">
+        <v>2014</v>
+      </c>
+      <c r="B18" s="112">
+        <v>1</v>
+      </c>
+      <c r="C18" s="112">
+        <v>3</v>
+      </c>
+      <c r="D18" s="112">
+        <v>10</v>
+      </c>
+      <c r="E18" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="112">
+        <v>1.5</v>
+      </c>
+      <c r="G18" s="112">
+        <v>5</v>
+      </c>
+      <c r="H18" s="112">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="I18" s="112">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="J18" s="112">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89">
+        <v>2015</v>
+      </c>
+      <c r="B19" s="112">
         <v>2</v>
       </c>
-      <c r="C23" s="89">
-        <v>1.83</v>
-      </c>
-      <c r="D23" s="89">
-        <v>2.68</v>
-      </c>
-      <c r="E23" s="89">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="89" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" s="89">
-        <v>4.67</v>
-      </c>
-      <c r="C24" s="89">
-        <v>0</v>
-      </c>
-      <c r="D24" s="89">
-        <v>15.68</v>
-      </c>
-      <c r="E24" s="89">
-        <v>27.21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="89" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="89">
-        <v>9.33</v>
-      </c>
-      <c r="C25" s="89">
-        <v>0</v>
-      </c>
-      <c r="D25" s="89">
-        <v>43.56</v>
-      </c>
-      <c r="E25" s="89">
-        <v>98.07</v>
+      <c r="C19" s="112">
+        <v>6</v>
+      </c>
+      <c r="D19" s="112">
+        <v>20</v>
+      </c>
+      <c r="E19" s="112">
+        <v>1</v>
+      </c>
+      <c r="F19" s="112">
+        <v>3</v>
+      </c>
+      <c r="G19" s="112">
+        <v>10</v>
+      </c>
+      <c r="H19" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="112">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="89">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="89">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="89">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearranged and condensed scripts
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -1701,9 +1701,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2172,9 +2172,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2184,7 +2184,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2210,11 +2210,11 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2599,7 +2599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2679,11 +2679,11 @@
         <v>4.0741237836483535E-3</v>
       </c>
       <c r="D3" s="23">
-        <f>C3-$I$2*C3</f>
+        <f t="shared" ref="D3:D8" si="0">C3-$I$2*C3</f>
         <v>3.8704175944659358E-3</v>
       </c>
       <c r="E3" s="23">
-        <f>C3+$I$2*C3</f>
+        <f t="shared" ref="E3:E8" si="1">C3+$I$2*C3</f>
         <v>4.2778299728307712E-3</v>
       </c>
       <c r="G3" s="52" t="s">
@@ -2706,11 +2706,11 @@
         <v>1E-3</v>
       </c>
       <c r="D4" s="24">
-        <f>C4-$I$2*C4</f>
+        <f t="shared" si="0"/>
         <v>9.5E-4</v>
       </c>
       <c r="E4" s="21">
-        <f>C4+$I$2*C4</f>
+        <f t="shared" si="1"/>
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="L4" s="57"/>
@@ -2730,11 +2730,11 @@
         <v>1E-3</v>
       </c>
       <c r="D5" s="21">
-        <f>C5-$I$2*C5</f>
+        <f t="shared" si="0"/>
         <v>9.5E-4</v>
       </c>
       <c r="E5" s="21">
-        <f>C5+$I$2*C5</f>
+        <f t="shared" si="1"/>
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="L5" s="27"/>
@@ -2754,11 +2754,11 @@
         <v>1E-3</v>
       </c>
       <c r="D6" s="21">
-        <f>C6-$I$2*C6</f>
+        <f t="shared" si="0"/>
         <v>9.5E-4</v>
       </c>
       <c r="E6" s="21">
-        <f>C6+$I$2*C6</f>
+        <f t="shared" si="1"/>
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="G6" s="52" t="s">
@@ -2784,11 +2784,11 @@
         <v>7.5</v>
       </c>
       <c r="D7" s="25">
-        <f>C7-$I$2*C7</f>
+        <f t="shared" si="0"/>
         <v>7.125</v>
       </c>
       <c r="E7" s="25">
-        <f>C7+$I$2*C7</f>
+        <f t="shared" si="1"/>
         <v>7.875</v>
       </c>
       <c r="G7" s="52" t="s">
@@ -2814,11 +2814,11 @@
         <v>0.13</v>
       </c>
       <c r="D8" s="23">
-        <f>C8-$I$2*C8</f>
+        <f t="shared" si="0"/>
         <v>0.1235</v>
       </c>
       <c r="E8" s="23">
-        <f>C8+$I$2*C8</f>
+        <f t="shared" si="1"/>
         <v>0.13650000000000001</v>
       </c>
     </row>
@@ -2833,11 +2833,11 @@
         <v>0.4</v>
       </c>
       <c r="D9" s="25">
-        <f t="shared" ref="D9:D10" si="0">C9-$I$2*C9</f>
+        <f t="shared" ref="D9:D10" si="2">C9-$I$2*C9</f>
         <v>0.38</v>
       </c>
       <c r="E9" s="25">
-        <f t="shared" ref="E9:E10" si="1">C9+$I$2*C9</f>
+        <f t="shared" ref="E9:E10" si="3">C9+$I$2*C9</f>
         <v>0.42000000000000004</v>
       </c>
     </row>
@@ -2852,11 +2852,11 @@
         <v>0.4</v>
       </c>
       <c r="D10" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.38</v>
       </c>
       <c r="E10" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.42000000000000004</v>
       </c>
     </row>
@@ -2888,11 +2888,11 @@
         <v>6.2</v>
       </c>
       <c r="D12" s="25">
-        <f t="shared" ref="D12:D20" si="2">C12-$I$2*C12</f>
+        <f t="shared" ref="D12:D20" si="4">C12-$I$2*C12</f>
         <v>5.8900000000000006</v>
       </c>
       <c r="E12" s="25">
-        <f t="shared" ref="E12:E20" si="3">C12+$I$2*C12</f>
+        <f t="shared" ref="E12:E20" si="5">C12+$I$2*C12</f>
         <v>6.51</v>
       </c>
       <c r="G12" s="52" t="s">
@@ -2910,11 +2910,11 @@
         <v>7</v>
       </c>
       <c r="D13" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.65</v>
       </c>
       <c r="E13" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.35</v>
       </c>
     </row>
@@ -2929,11 +2929,11 @@
         <v>0.1</v>
       </c>
       <c r="D14" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E14" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10500000000000001</v>
       </c>
     </row>
@@ -2948,11 +2948,11 @@
         <v>0.17</v>
       </c>
       <c r="D15" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1615</v>
       </c>
       <c r="E15" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.17850000000000002</v>
       </c>
     </row>
@@ -2967,11 +2967,11 @@
         <v>0.38800000000000001</v>
       </c>
       <c r="D16" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.36860000000000004</v>
       </c>
       <c r="E16" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.40739999999999998</v>
       </c>
     </row>
@@ -2986,11 +2986,11 @@
         <v>0.45</v>
       </c>
       <c r="D17" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.42749999999999999</v>
       </c>
       <c r="E17" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.47250000000000003</v>
       </c>
     </row>
@@ -3005,11 +3005,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.95</v>
       </c>
       <c r="E18" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.05</v>
       </c>
     </row>
@@ -3025,11 +3025,11 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D19" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.52250000000000008</v>
       </c>
       <c r="E19" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57750000000000001</v>
       </c>
     </row>
@@ -3044,11 +3044,11 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.47499999999999998</v>
       </c>
       <c r="E20" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.52500000000000002</v>
       </c>
     </row>
@@ -3090,7 +3090,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,7 +3996,7 @@
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5346,7 +5346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added cascade PLHIV plot
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -3996,7 +3996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -5409,8 +5409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5736,31 +5736,31 @@
         <v>2015</v>
       </c>
       <c r="B19" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="85">
         <v>2</v>
       </c>
-      <c r="C19" s="85">
-        <v>8</v>
-      </c>
       <c r="D19" s="85">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E19" s="85">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="F19" s="85">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G19" s="85">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H19" s="85">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="I19" s="85">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="J19" s="86">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed risk dimension to Medicare eligibility
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -971,7 +971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -995,7 +995,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0">
+    <comment ref="AC1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1375,7 +1375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="104">
   <si>
     <t>Waiting list</t>
   </si>
@@ -1398,18 +1398,9 @@
     <t>5 in a year may be normal</t>
   </si>
   <si>
-    <t>Dialysis costs ($)</t>
-  </si>
-  <si>
-    <t>mean of 55; range 4-70</t>
-  </si>
-  <si>
     <t>5% probability per year converted to rate</t>
   </si>
   <si>
-    <t>160 days</t>
-  </si>
-  <si>
     <t>dt</t>
   </si>
   <si>
@@ -1693,6 +1684,9 @@
   </si>
   <si>
     <t>prop_high_risk</t>
+  </si>
+  <si>
+    <t>medimix</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1873,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2095,6 +2089,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2115,7 +2118,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2277,6 +2280,10 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -2597,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,18 +2648,18 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="32">
         <f>1/12</f>
@@ -2665,15 +2672,15 @@
       </c>
       <c r="L2" s="59"/>
       <c r="M2" s="52" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="49">
         <v>4.0741237836483535E-3</v>
@@ -2686,20 +2693,17 @@
         <f t="shared" ref="E3:E8" si="1">C3+$I$2*C3</f>
         <v>4.2778299728307712E-3</v>
       </c>
-      <c r="G3" s="52" t="s">
-        <v>8</v>
-      </c>
       <c r="L3" s="61"/>
       <c r="M3" s="52" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="56">
         <f>0.001*12*C2</f>
@@ -2715,15 +2719,15 @@
       </c>
       <c r="L4" s="57"/>
       <c r="M4" s="52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="54">
         <f>0.001*12*C2</f>
@@ -2739,15 +2743,15 @@
       </c>
       <c r="L5" s="27"/>
       <c r="M5" s="52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="55">
         <f>0.001*12*C2</f>
@@ -2762,7 +2766,7 @@
         <v>1.0499999999999999E-3</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J6" s="52">
         <f>(1+C3)^(12*(2040-2007))</f>
@@ -2770,15 +2774,15 @@
       </c>
       <c r="L6" s="67"/>
       <c r="M6" s="52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="28">
         <v>7.5</v>
@@ -2805,10 +2809,10 @@
     </row>
     <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="28">
         <v>0.13</v>
@@ -2824,10 +2828,10 @@
     </row>
     <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="C9" s="28">
         <v>0.4</v>
@@ -2843,10 +2847,10 @@
     </row>
     <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="28">
         <v>0.4</v>
@@ -2862,26 +2866,23 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="66">
         <v>0</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
-      <c r="G11" s="52" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="62">
         <f>6.2</f>
@@ -2895,16 +2896,13 @@
         <f t="shared" ref="E12:E20" si="5">C12+$I$2*C12</f>
         <v>6.51</v>
       </c>
-      <c r="G12" s="52" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" s="28">
         <v>7</v>
@@ -2920,10 +2918,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="54">
         <v>0.1</v>
@@ -2939,10 +2937,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="54">
         <v>0.17</v>
@@ -2958,10 +2956,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="63">
         <v>0.38800000000000001</v>
@@ -2977,10 +2975,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="64">
         <v>0.45</v>
@@ -2996,10 +2994,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" s="31">
         <v>1</v>
@@ -3015,10 +3013,10 @@
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="60">
         <f>1-C17</f>
@@ -3035,10 +3033,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C20" s="58">
         <v>0.5</v>
@@ -3054,10 +3052,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C21" s="53">
         <v>2007</v>
@@ -3065,17 +3063,17 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C22" s="53">
         <v>42714</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="65"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3121,67 +3119,67 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="N1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="R1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="U1" s="50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V1" s="15"/>
     </row>
@@ -3994,10 +3992,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4022,168 +4020,172 @@
     <col min="23" max="23" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.85546875" style="69" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="28" style="69" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15" style="69" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15" style="69" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" style="69" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28" style="69" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" style="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C1" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="X1" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="76" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="U1" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="W1" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="X1" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y1" s="77" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA1" s="92" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB1" s="90" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC1" s="91" t="s">
-        <v>86</v>
+      <c r="AA1" s="90" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB1" s="92" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC1" s="90" t="s">
+        <v>83</v>
       </c>
       <c r="AD1" s="91" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AE1" s="91" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AF1" s="91" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG1" s="92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="AG1" s="91" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH1" s="92" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E2" s="80" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J2" s="80" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K2" s="78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L2" s="79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M2" s="79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q2" s="79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R2" s="79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="S2" s="80" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="T2" s="78"/>
       <c r="U2" s="79"/>
@@ -4191,30 +4193,30 @@
       <c r="W2" s="78"/>
       <c r="X2" s="79"/>
       <c r="Y2" s="80"/>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="95"/>
-      <c r="AB2" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC2" s="94" t="s">
-        <v>80</v>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="93" t="s">
+        <v>76</v>
       </c>
       <c r="AD2" s="94" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="AE2" s="94" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AF2" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG2" s="95" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="AG2" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH2" s="95" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="78"/>
@@ -4226,64 +4228,64 @@
       <c r="I3" s="79"/>
       <c r="J3" s="80"/>
       <c r="K3" s="78" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L3" s="79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M3" s="79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N3" s="79" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O3" s="79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P3" s="79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="79" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="R3" s="79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="S3" s="80" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="T3" s="78" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="U3" s="79" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V3" s="80" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="W3" s="78" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="X3" s="79" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Y3" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z3" s="93" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA3" s="95" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB3" s="93"/>
-      <c r="AC3" s="94"/>
+        <v>88</v>
+      </c>
+      <c r="AA3" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB3" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC3" s="93"/>
       <c r="AD3" s="94"/>
       <c r="AE3" s="94"/>
       <c r="AF3" s="94"/>
-      <c r="AG3" s="95"/>
-    </row>
-    <row r="4" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG3" s="94"/>
+      <c r="AH3" s="95"/>
+    </row>
+    <row r="4" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>2000</v>
       </c>
@@ -4354,16 +4356,16 @@
       <c r="Y4" s="83">
         <v>0.04</v>
       </c>
-      <c r="Z4" s="96">
+      <c r="Z4" s="106">
         <v>1</v>
       </c>
-      <c r="AA4" s="98">
+      <c r="AA4" s="96">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="98">
         <v>2</v>
       </c>
-      <c r="AB4" s="96">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="97">
+      <c r="AC4" s="96">
         <v>0</v>
       </c>
       <c r="AD4" s="97">
@@ -4375,11 +4377,14 @@
       <c r="AF4" s="97">
         <v>0</v>
       </c>
-      <c r="AG4" s="98">
+      <c r="AG4" s="97">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH4" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>2001</v>
       </c>
@@ -4407,16 +4412,17 @@
       <c r="W5" s="84"/>
       <c r="X5" s="85"/>
       <c r="Y5" s="86"/>
-      <c r="Z5" s="99"/>
-      <c r="AA5" s="101"/>
-      <c r="AB5" s="99"/>
-      <c r="AC5" s="100"/>
+      <c r="Z5" s="107"/>
+      <c r="AA5" s="99"/>
+      <c r="AB5" s="101"/>
+      <c r="AC5" s="99"/>
       <c r="AD5" s="100"/>
       <c r="AE5" s="100"/>
       <c r="AF5" s="100"/>
-      <c r="AG5" s="101"/>
-    </row>
-    <row r="6" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG5" s="100"/>
+      <c r="AH5" s="101"/>
+    </row>
+    <row r="6" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>2002</v>
       </c>
@@ -4444,16 +4450,17 @@
       <c r="W6" s="84"/>
       <c r="X6" s="85"/>
       <c r="Y6" s="86"/>
-      <c r="Z6" s="99"/>
-      <c r="AA6" s="101"/>
-      <c r="AB6" s="99"/>
-      <c r="AC6" s="100"/>
+      <c r="Z6" s="107"/>
+      <c r="AA6" s="99"/>
+      <c r="AB6" s="101"/>
+      <c r="AC6" s="99"/>
       <c r="AD6" s="100"/>
       <c r="AE6" s="100"/>
       <c r="AF6" s="100"/>
-      <c r="AG6" s="101"/>
-    </row>
-    <row r="7" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG6" s="100"/>
+      <c r="AH6" s="101"/>
+    </row>
+    <row r="7" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>2003</v>
       </c>
@@ -4481,16 +4488,17 @@
       <c r="W7" s="84"/>
       <c r="X7" s="85"/>
       <c r="Y7" s="86"/>
-      <c r="Z7" s="99"/>
-      <c r="AA7" s="101"/>
-      <c r="AB7" s="99"/>
-      <c r="AC7" s="100"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="99"/>
+      <c r="AB7" s="101"/>
+      <c r="AC7" s="99"/>
       <c r="AD7" s="100"/>
       <c r="AE7" s="100"/>
       <c r="AF7" s="100"/>
-      <c r="AG7" s="101"/>
-    </row>
-    <row r="8" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG7" s="100"/>
+      <c r="AH7" s="101"/>
+    </row>
+    <row r="8" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>2004</v>
       </c>
@@ -4518,16 +4526,17 @@
       <c r="W8" s="84"/>
       <c r="X8" s="85"/>
       <c r="Y8" s="86"/>
-      <c r="Z8" s="99"/>
-      <c r="AA8" s="101"/>
-      <c r="AB8" s="99"/>
-      <c r="AC8" s="100"/>
+      <c r="Z8" s="107"/>
+      <c r="AA8" s="99"/>
+      <c r="AB8" s="101"/>
+      <c r="AC8" s="99"/>
       <c r="AD8" s="100"/>
       <c r="AE8" s="100"/>
       <c r="AF8" s="100"/>
-      <c r="AG8" s="101"/>
-    </row>
-    <row r="9" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG8" s="100"/>
+      <c r="AH8" s="101"/>
+    </row>
+    <row r="9" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>2005</v>
       </c>
@@ -4555,16 +4564,17 @@
       <c r="W9" s="84"/>
       <c r="X9" s="85"/>
       <c r="Y9" s="86"/>
-      <c r="Z9" s="99"/>
-      <c r="AA9" s="101"/>
-      <c r="AB9" s="99"/>
-      <c r="AC9" s="100"/>
+      <c r="Z9" s="107"/>
+      <c r="AA9" s="99"/>
+      <c r="AB9" s="101"/>
+      <c r="AC9" s="99"/>
       <c r="AD9" s="100"/>
       <c r="AE9" s="100"/>
       <c r="AF9" s="100"/>
-      <c r="AG9" s="101"/>
-    </row>
-    <row r="10" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG9" s="100"/>
+      <c r="AH9" s="101"/>
+    </row>
+    <row r="10" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>2006</v>
       </c>
@@ -4592,16 +4602,17 @@
       <c r="W10" s="84"/>
       <c r="X10" s="85"/>
       <c r="Y10" s="86"/>
-      <c r="Z10" s="99"/>
-      <c r="AA10" s="101"/>
-      <c r="AB10" s="99"/>
-      <c r="AC10" s="100"/>
+      <c r="Z10" s="107"/>
+      <c r="AA10" s="99"/>
+      <c r="AB10" s="101"/>
+      <c r="AC10" s="99"/>
       <c r="AD10" s="100"/>
       <c r="AE10" s="100"/>
       <c r="AF10" s="100"/>
-      <c r="AG10" s="101"/>
-    </row>
-    <row r="11" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG10" s="100"/>
+      <c r="AH10" s="101"/>
+    </row>
+    <row r="11" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>2007</v>
       </c>
@@ -4635,16 +4646,17 @@
       <c r="W11" s="84"/>
       <c r="X11" s="85"/>
       <c r="Y11" s="86"/>
-      <c r="Z11" s="99"/>
-      <c r="AA11" s="101"/>
-      <c r="AB11" s="99"/>
-      <c r="AC11" s="100"/>
+      <c r="Z11" s="107"/>
+      <c r="AA11" s="99"/>
+      <c r="AB11" s="101"/>
+      <c r="AC11" s="99"/>
       <c r="AD11" s="100"/>
       <c r="AE11" s="100"/>
       <c r="AF11" s="100"/>
-      <c r="AG11" s="101"/>
-    </row>
-    <row r="12" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG11" s="100"/>
+      <c r="AH11" s="101"/>
+    </row>
+    <row r="12" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>2008</v>
       </c>
@@ -4672,16 +4684,17 @@
       <c r="W12" s="84"/>
       <c r="X12" s="85"/>
       <c r="Y12" s="86"/>
-      <c r="Z12" s="99"/>
-      <c r="AA12" s="101"/>
-      <c r="AB12" s="99"/>
-      <c r="AC12" s="100"/>
+      <c r="Z12" s="107"/>
+      <c r="AA12" s="99"/>
+      <c r="AB12" s="101"/>
+      <c r="AC12" s="99"/>
       <c r="AD12" s="100"/>
       <c r="AE12" s="100"/>
       <c r="AF12" s="100"/>
-      <c r="AG12" s="101"/>
-    </row>
-    <row r="13" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG12" s="100"/>
+      <c r="AH12" s="101"/>
+    </row>
+    <row r="13" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>2009</v>
       </c>
@@ -4711,16 +4724,17 @@
       <c r="W13" s="84"/>
       <c r="X13" s="85"/>
       <c r="Y13" s="86"/>
-      <c r="Z13" s="99"/>
-      <c r="AA13" s="101"/>
-      <c r="AB13" s="99"/>
-      <c r="AC13" s="100"/>
+      <c r="Z13" s="107"/>
+      <c r="AA13" s="99"/>
+      <c r="AB13" s="101"/>
+      <c r="AC13" s="99"/>
       <c r="AD13" s="100"/>
       <c r="AE13" s="100"/>
       <c r="AF13" s="100"/>
-      <c r="AG13" s="101"/>
-    </row>
-    <row r="14" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG13" s="100"/>
+      <c r="AH13" s="101"/>
+    </row>
+    <row r="14" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>2010</v>
       </c>
@@ -4756,16 +4770,17 @@
       <c r="W14" s="84"/>
       <c r="X14" s="85"/>
       <c r="Y14" s="86"/>
-      <c r="Z14" s="99"/>
-      <c r="AA14" s="101"/>
-      <c r="AB14" s="99"/>
-      <c r="AC14" s="100"/>
+      <c r="Z14" s="107"/>
+      <c r="AA14" s="99"/>
+      <c r="AB14" s="101"/>
+      <c r="AC14" s="99"/>
       <c r="AD14" s="100"/>
       <c r="AE14" s="100"/>
       <c r="AF14" s="100"/>
-      <c r="AG14" s="101"/>
-    </row>
-    <row r="15" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG14" s="100"/>
+      <c r="AH14" s="101"/>
+    </row>
+    <row r="15" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>2011</v>
       </c>
@@ -4793,16 +4808,17 @@
       <c r="W15" s="84"/>
       <c r="X15" s="85"/>
       <c r="Y15" s="86"/>
-      <c r="Z15" s="99"/>
-      <c r="AA15" s="101"/>
-      <c r="AB15" s="99"/>
-      <c r="AC15" s="100"/>
+      <c r="Z15" s="107"/>
+      <c r="AA15" s="99"/>
+      <c r="AB15" s="101"/>
+      <c r="AC15" s="99"/>
       <c r="AD15" s="100"/>
       <c r="AE15" s="100"/>
       <c r="AF15" s="100"/>
-      <c r="AG15" s="101"/>
-    </row>
-    <row r="16" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG15" s="100"/>
+      <c r="AH15" s="101"/>
+    </row>
+    <row r="16" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>2012</v>
       </c>
@@ -4836,16 +4852,17 @@
       <c r="W16" s="84"/>
       <c r="X16" s="85"/>
       <c r="Y16" s="86"/>
-      <c r="Z16" s="99"/>
-      <c r="AA16" s="101"/>
-      <c r="AB16" s="99"/>
-      <c r="AC16" s="100"/>
+      <c r="Z16" s="107"/>
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="101"/>
+      <c r="AC16" s="99"/>
       <c r="AD16" s="100"/>
       <c r="AE16" s="100"/>
       <c r="AF16" s="100"/>
-      <c r="AG16" s="101"/>
-    </row>
-    <row r="17" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG16" s="100"/>
+      <c r="AH16" s="101"/>
+    </row>
+    <row r="17" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>2013</v>
       </c>
@@ -4879,16 +4896,17 @@
       <c r="W17" s="84"/>
       <c r="X17" s="85"/>
       <c r="Y17" s="86"/>
-      <c r="Z17" s="99"/>
-      <c r="AA17" s="101"/>
-      <c r="AB17" s="99"/>
-      <c r="AC17" s="100"/>
+      <c r="Z17" s="107"/>
+      <c r="AA17" s="99"/>
+      <c r="AB17" s="101"/>
+      <c r="AC17" s="99"/>
       <c r="AD17" s="100"/>
       <c r="AE17" s="100"/>
       <c r="AF17" s="100"/>
-      <c r="AG17" s="101"/>
-    </row>
-    <row r="18" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG17" s="100"/>
+      <c r="AH17" s="101"/>
+    </row>
+    <row r="18" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
         <v>2014</v>
       </c>
@@ -4922,16 +4940,17 @@
       <c r="W18" s="84"/>
       <c r="X18" s="85"/>
       <c r="Y18" s="86"/>
-      <c r="Z18" s="99"/>
-      <c r="AA18" s="101"/>
-      <c r="AB18" s="99"/>
-      <c r="AC18" s="100"/>
+      <c r="Z18" s="107"/>
+      <c r="AA18" s="99"/>
+      <c r="AB18" s="101"/>
+      <c r="AC18" s="99"/>
       <c r="AD18" s="100"/>
       <c r="AE18" s="100"/>
       <c r="AF18" s="100"/>
-      <c r="AG18" s="101"/>
-    </row>
-    <row r="19" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG18" s="100"/>
+      <c r="AH18" s="101"/>
+    </row>
+    <row r="19" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
         <v>2015</v>
       </c>
@@ -4965,16 +4984,17 @@
       <c r="W19" s="84"/>
       <c r="X19" s="85"/>
       <c r="Y19" s="86"/>
-      <c r="Z19" s="99"/>
-      <c r="AA19" s="101"/>
-      <c r="AB19" s="99"/>
-      <c r="AC19" s="100"/>
+      <c r="Z19" s="107"/>
+      <c r="AA19" s="99"/>
+      <c r="AB19" s="101"/>
+      <c r="AC19" s="99"/>
       <c r="AD19" s="100"/>
       <c r="AE19" s="100"/>
       <c r="AF19" s="100"/>
-      <c r="AG19" s="101"/>
-    </row>
-    <row r="20" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG19" s="100"/>
+      <c r="AH19" s="101"/>
+    </row>
+    <row r="20" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>2016</v>
       </c>
@@ -5010,16 +5030,17 @@
       <c r="W20" s="84"/>
       <c r="X20" s="85"/>
       <c r="Y20" s="86"/>
-      <c r="Z20" s="99"/>
-      <c r="AA20" s="101"/>
-      <c r="AB20" s="99"/>
-      <c r="AC20" s="100"/>
+      <c r="Z20" s="107"/>
+      <c r="AA20" s="99"/>
+      <c r="AB20" s="101"/>
+      <c r="AC20" s="99"/>
       <c r="AD20" s="100"/>
       <c r="AE20" s="100"/>
       <c r="AF20" s="100"/>
-      <c r="AG20" s="101"/>
-    </row>
-    <row r="21" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG20" s="100"/>
+      <c r="AH20" s="101"/>
+    </row>
+    <row r="21" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
         <v>2017</v>
       </c>
@@ -5047,16 +5068,17 @@
       <c r="W21" s="84"/>
       <c r="X21" s="85"/>
       <c r="Y21" s="86"/>
-      <c r="Z21" s="99"/>
-      <c r="AA21" s="101"/>
-      <c r="AB21" s="99"/>
-      <c r="AC21" s="100"/>
+      <c r="Z21" s="107"/>
+      <c r="AA21" s="99"/>
+      <c r="AB21" s="101"/>
+      <c r="AC21" s="99"/>
       <c r="AD21" s="100"/>
       <c r="AE21" s="100"/>
       <c r="AF21" s="100"/>
-      <c r="AG21" s="101"/>
-    </row>
-    <row r="22" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG21" s="100"/>
+      <c r="AH21" s="101"/>
+    </row>
+    <row r="22" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>2018</v>
       </c>
@@ -5084,16 +5106,17 @@
       <c r="W22" s="84"/>
       <c r="X22" s="85"/>
       <c r="Y22" s="86"/>
-      <c r="Z22" s="99"/>
-      <c r="AA22" s="101"/>
-      <c r="AB22" s="99"/>
-      <c r="AC22" s="100"/>
+      <c r="Z22" s="107"/>
+      <c r="AA22" s="99"/>
+      <c r="AB22" s="101"/>
+      <c r="AC22" s="99"/>
       <c r="AD22" s="100"/>
       <c r="AE22" s="100"/>
       <c r="AF22" s="100"/>
-      <c r="AG22" s="101"/>
-    </row>
-    <row r="23" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG22" s="100"/>
+      <c r="AH22" s="101"/>
+    </row>
+    <row r="23" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>2019</v>
       </c>
@@ -5121,16 +5144,17 @@
       <c r="W23" s="84"/>
       <c r="X23" s="85"/>
       <c r="Y23" s="86"/>
-      <c r="Z23" s="99"/>
-      <c r="AA23" s="101"/>
-      <c r="AB23" s="99"/>
-      <c r="AC23" s="100"/>
+      <c r="Z23" s="107"/>
+      <c r="AA23" s="99"/>
+      <c r="AB23" s="101"/>
+      <c r="AC23" s="99"/>
       <c r="AD23" s="100"/>
       <c r="AE23" s="100"/>
       <c r="AF23" s="100"/>
-      <c r="AG23" s="101"/>
-    </row>
-    <row r="24" spans="1:33" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG23" s="100"/>
+      <c r="AH23" s="101"/>
+    </row>
+    <row r="24" spans="1:34" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="72">
         <v>2020</v>
       </c>
@@ -5158,36 +5182,37 @@
       <c r="W24" s="87"/>
       <c r="X24" s="88"/>
       <c r="Y24" s="89"/>
-      <c r="Z24" s="102"/>
-      <c r="AA24" s="104"/>
-      <c r="AB24" s="102"/>
-      <c r="AC24" s="103"/>
+      <c r="Z24" s="108"/>
+      <c r="AA24" s="102"/>
+      <c r="AB24" s="104"/>
+      <c r="AC24" s="102"/>
       <c r="AD24" s="103"/>
       <c r="AE24" s="103"/>
       <c r="AF24" s="103"/>
-      <c r="AG24" s="104"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG24" s="103"/>
+      <c r="AH24" s="104"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>2021</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>2022</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>2023</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
         <v>2024</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="72">
         <v>2025</v>
       </c>
@@ -5198,17 +5223,17 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
         <v>2026</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
         <v>2027</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
         <v>2028</v>
       </c>
@@ -5253,21 +5278,21 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="38"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -5409,7 +5434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
@@ -5427,98 +5452,98 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I1" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J1" s="77" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D2" s="79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G2" s="79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H2" s="79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I2" s="79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J2" s="80" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="78" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E3" s="79" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F3" s="79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H3" s="79" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I3" s="79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J3" s="80" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Further implemented medicare eligibility
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -847,11 +847,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Number of people on PrEP. Seemed to make more sense than proportion of people on PrEP</t>
+Relative force of infection multiplier for each risk group </t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Number of people on PrEP. Seemed to make more sense than proportion of people on PrEP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -872,30 +896,6 @@
           </rPr>
           <t xml:space="preserve">
 Effectiveness of condoms. This number doesn't actually matter because it gets absorbed into the force of infection. But its needed for a gel condom analysis</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Condom usage between risk groups. Might be set this to zero then absorb any relative risk into the relative_foi parameter</t>
         </r>
       </text>
     </comment>
@@ -919,11 +919,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time between HIV tests (in years)</t>
+Condom usage between risk groups. Might be set this to zero then absorb any relative risk into the relative_foi parameter</t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -943,7 +943,31 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Care cascade data</t>
+Condom usage between risk groups. Might be set this to zero then absorb any relative risk into the relative_foi parameter</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Time between HIV tests (in years)</t>
         </r>
       </text>
     </comment>
@@ -967,11 +991,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Effectiveness of each care stage in reducing infectiousness. The number of people in each infected compartment are multiplied by these values to get an overall relative proportion positive</t>
+Care cascade data</t>
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Effectiveness of each care stage in reducing infectiousness. The number of people in each infected compartment are multiplied by these values to get an overall relative proportion positive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -995,7 +1043,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0">
+    <comment ref="AF1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1019,7 +1067,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1043,7 +1091,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1063,35 +1111,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time between tests for people infected 1-3 years ago</t>
+Time between tests for people infected over 3 years ago</t>
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people infected over 3 years ago</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="W3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1116,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0">
+    <comment ref="X3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
+    <comment ref="Y3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1212,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="T16" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e. PrEP is 97% effective</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1212,7 +1260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T17" authorId="0" shapeId="0">
+    <comment ref="W17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1236,7 +1284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T20" authorId="1" shapeId="0">
+    <comment ref="W20" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1342,30 +1390,6 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time between tests for people infected 1-3 years ago</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
 Time between tests for people infected over 3 years ago</t>
         </r>
       </text>
@@ -1375,7 +1399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
   <si>
     <t>Waiting list</t>
   </si>
@@ -1620,9 +1644,6 @@
     <t>old_infection</t>
   </si>
   <si>
-    <t>mid_infection</t>
-  </si>
-  <si>
     <t>condom_usage</t>
   </si>
   <si>
@@ -1671,9 +1692,6 @@
     <t>new_to_mid</t>
   </si>
   <si>
-    <t>mid_to_old</t>
-  </si>
-  <si>
     <t>test_wait</t>
   </si>
   <si>
@@ -1690,6 +1708,12 @@
   </si>
   <si>
     <t>prop_medi</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -1876,7 +1900,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -2101,6 +2125,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2121,7 +2207,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2287,6 +2373,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -3055,10 +3151,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="53">
         <v>2007</v>
@@ -3066,10 +3162,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="53">
         <v>42714</v>
@@ -3089,9 +3185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+      <selection pane="topRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3215,11 +3311,11 @@
         <v>3.4931506849315071E-2</v>
       </c>
       <c r="J2" s="35">
-        <f t="shared" ref="J2:J12" si="0">G2-K2</f>
+        <f>G2-K2</f>
         <v>39638.591999999997</v>
       </c>
       <c r="K2" s="35">
-        <f t="shared" ref="K2:K12" si="1">C2</f>
+        <f>C2</f>
         <v>3075.4079999999999</v>
       </c>
       <c r="L2" s="40">
@@ -3227,7 +3323,7 @@
         <v>923</v>
       </c>
       <c r="M2" s="40">
-        <f t="shared" ref="M2" si="2">ROUND(I2*K2,0)</f>
+        <f t="shared" ref="M2" si="0">ROUND(I2*K2,0)</f>
         <v>107</v>
       </c>
       <c r="N2" s="12">
@@ -3263,7 +3359,7 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="35">
-        <f t="shared" ref="C3:C12" si="3">G3*7.2/100</f>
+        <f t="shared" ref="C3:C12" si="1">G3*7.2/100</f>
         <v>3229.1784000000002</v>
       </c>
       <c r="D3" s="11"/>
@@ -3276,11 +3372,11 @@
       <c r="H3" s="48"/>
       <c r="I3" s="48"/>
       <c r="J3" s="35">
-        <f t="shared" si="0"/>
+        <f>G3-K3</f>
         <v>41620.521600000007</v>
       </c>
       <c r="K3" s="35">
-        <f t="shared" si="1"/>
+        <f>C3</f>
         <v>3229.1784000000002</v>
       </c>
       <c r="L3" s="14"/>
@@ -3295,18 +3391,18 @@
         <v>0.82</v>
       </c>
       <c r="Q3" s="45">
-        <f t="shared" ref="Q3:Q12" si="4">N3*O3*P3</f>
+        <f t="shared" ref="Q3:Q12" si="2">N3*O3*P3</f>
         <v>612.39239999999995</v>
       </c>
       <c r="R3" s="41">
         <v>0.17</v>
       </c>
       <c r="S3" s="43">
-        <f t="shared" ref="S3:S12" si="5">Q3-T3</f>
+        <f t="shared" ref="S3:S12" si="3">Q3-T3</f>
         <v>508.28569199999993</v>
       </c>
       <c r="T3" s="43">
-        <f t="shared" ref="T3:T12" si="6">Q3*R3</f>
+        <f t="shared" ref="T3:T12" si="4">Q3*R3</f>
         <v>104.106708</v>
       </c>
       <c r="U3" s="16"/>
@@ -3318,24 +3414,24 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3390.6373200000003</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="35">
-        <f t="shared" ref="G4:G11" si="7">1.05*G3</f>
+        <f t="shared" ref="G4:G11" si="5">1.05*G3</f>
         <v>47092.185000000005</v>
       </c>
       <c r="H4" s="48"/>
       <c r="I4" s="48"/>
       <c r="J4" s="35">
-        <f t="shared" si="0"/>
+        <f>G4-K4</f>
         <v>43701.547680000003</v>
       </c>
       <c r="K4" s="35">
-        <f t="shared" si="1"/>
+        <f>C4</f>
         <v>3390.6373200000003</v>
       </c>
       <c r="L4" s="14"/>
@@ -3350,18 +3446,18 @@
         <v>0.82</v>
       </c>
       <c r="Q4" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>983.01600000000008</v>
       </c>
       <c r="R4" s="41">
         <v>0.17</v>
       </c>
       <c r="S4" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>815.90328</v>
       </c>
       <c r="T4" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>167.11272000000002</v>
       </c>
       <c r="U4" s="17"/>
@@ -3375,7 +3471,7 @@
         <v>178</v>
       </c>
       <c r="C5" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3560.1691860000005</v>
       </c>
       <c r="D5" s="12"/>
@@ -3386,7 +3482,7 @@
         <v>0.8</v>
       </c>
       <c r="G5" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>49446.794250000006</v>
       </c>
       <c r="H5" s="48">
@@ -3396,19 +3492,19 @@
         <v>4.3150684931506846E-2</v>
       </c>
       <c r="J5" s="35">
-        <f t="shared" si="0"/>
+        <f>G5-K5</f>
         <v>45886.625064000007</v>
       </c>
       <c r="K5" s="35">
-        <f t="shared" si="1"/>
+        <f>C5</f>
         <v>3560.1691860000005</v>
       </c>
       <c r="L5" s="39">
-        <f t="shared" ref="L5:L11" si="8">ROUND(H5*J5,0)</f>
+        <f t="shared" ref="L5:L11" si="6">ROUND(H5*J5,0)</f>
         <v>1848</v>
       </c>
       <c r="M5" s="39">
-        <f t="shared" ref="M5:M12" si="9">ROUND(I5*K5,0)</f>
+        <f t="shared" ref="M5:M12" si="7">ROUND(I5*K5,0)</f>
         <v>154</v>
       </c>
       <c r="N5" s="12">
@@ -3421,18 +3517,18 @@
         <v>0.82</v>
       </c>
       <c r="Q5" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1167.6635999999999</v>
       </c>
       <c r="R5" s="41">
         <v>0.17</v>
       </c>
       <c r="S5" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>969.16078799999991</v>
       </c>
       <c r="T5" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>198.50281199999998</v>
       </c>
       <c r="U5" s="17"/>
@@ -3446,14 +3542,14 @@
         <v>218</v>
       </c>
       <c r="C6" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3738.1776453000011</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>51919.133962500011</v>
       </c>
       <c r="H6" s="48">
@@ -3463,19 +3559,19 @@
         <v>4.726027397260274E-2</v>
       </c>
       <c r="J6" s="35">
-        <f t="shared" si="0"/>
+        <f>G6-K6</f>
         <v>48180.956317200013</v>
       </c>
       <c r="K6" s="35">
-        <f t="shared" si="1"/>
+        <f>C6</f>
         <v>3738.1776453000011</v>
       </c>
       <c r="L6" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1808</v>
       </c>
       <c r="M6" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>177</v>
       </c>
       <c r="N6" s="12">
@@ -3488,18 +3584,18 @@
         <v>0.82</v>
       </c>
       <c r="Q6" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1237.4046000000001</v>
       </c>
       <c r="R6" s="41">
         <v>0.17</v>
       </c>
       <c r="S6" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1027.0458180000001</v>
       </c>
       <c r="T6" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>210.35878200000002</v>
       </c>
       <c r="U6" s="17"/>
@@ -3513,7 +3609,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3925.0865275650012</v>
       </c>
       <c r="D7" s="12">
@@ -3526,7 +3622,7 @@
         <v>0.88</v>
       </c>
       <c r="G7" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>54515.090660625014</v>
       </c>
       <c r="H7" s="48">
@@ -3536,19 +3632,19 @@
         <v>5.3835616438356167E-2</v>
       </c>
       <c r="J7" s="35">
-        <f t="shared" si="0"/>
+        <f>G7-K7</f>
         <v>50590.004133060014</v>
       </c>
       <c r="K7" s="35">
-        <f t="shared" si="1"/>
+        <f>C7</f>
         <v>3925.0865275650012</v>
       </c>
       <c r="L7" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2467</v>
       </c>
       <c r="M7" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>211</v>
       </c>
       <c r="N7" s="12">
@@ -3561,18 +3657,18 @@
         <v>0.82</v>
       </c>
       <c r="Q7" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1617.9911999999999</v>
       </c>
       <c r="R7" s="41">
         <v>0.17</v>
       </c>
       <c r="S7" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1342.9326959999999</v>
       </c>
       <c r="T7" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>275.05850400000003</v>
       </c>
       <c r="U7" s="17"/>
@@ -3586,7 +3682,7 @@
         <v>218</v>
       </c>
       <c r="C8" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4121.3408539432512</v>
       </c>
       <c r="D8" s="12"/>
@@ -3597,7 +3693,7 @@
         <v>0.9</v>
       </c>
       <c r="G8" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>57240.845193656263</v>
       </c>
       <c r="H8" s="48">
@@ -3607,19 +3703,19 @@
         <v>6.2671232876712321E-2</v>
       </c>
       <c r="J8" s="35">
-        <f t="shared" si="0"/>
+        <f>G8-K8</f>
         <v>53119.504339713014</v>
       </c>
       <c r="K8" s="35">
-        <f t="shared" si="1"/>
+        <f>C8</f>
         <v>4121.3408539432512</v>
       </c>
       <c r="L8" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2809</v>
       </c>
       <c r="M8" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>258</v>
       </c>
       <c r="N8" s="12">
@@ -3632,18 +3728,18 @@
         <v>0.82</v>
       </c>
       <c r="Q8" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1977.9876000000002</v>
       </c>
       <c r="R8" s="41">
         <v>0.17</v>
       </c>
       <c r="S8" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1641.7297080000001</v>
       </c>
       <c r="T8" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>336.25789200000003</v>
       </c>
       <c r="U8" s="17"/>
@@ -3657,7 +3753,7 @@
         <v>219</v>
       </c>
       <c r="C9" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4327.407896640414</v>
       </c>
       <c r="D9" s="12">
@@ -3670,7 +3766,7 @@
         <v>0.9</v>
       </c>
       <c r="G9" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>60102.887453339077</v>
       </c>
       <c r="H9" s="48">
@@ -3680,19 +3776,19 @@
         <v>5.321917808219178E-2</v>
       </c>
       <c r="J9" s="35">
-        <f t="shared" si="0"/>
+        <f>G9-K9</f>
         <v>55775.479556698665</v>
       </c>
       <c r="K9" s="35">
-        <f t="shared" si="1"/>
+        <f>C9</f>
         <v>4327.407896640414</v>
       </c>
       <c r="L9" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2873</v>
       </c>
       <c r="M9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>230</v>
       </c>
       <c r="N9" s="12">
@@ -3705,18 +3801,18 @@
         <v>0.82</v>
       </c>
       <c r="Q9" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2171.2698</v>
       </c>
       <c r="R9" s="41">
         <v>0.17</v>
       </c>
       <c r="S9" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1802.1539339999999</v>
       </c>
       <c r="T9" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>369.11586600000004</v>
       </c>
       <c r="U9" s="17"/>
@@ -3730,7 +3826,7 @@
         <v>206</v>
       </c>
       <c r="C10" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4543.7782914724339</v>
       </c>
       <c r="D10" s="12">
@@ -3743,7 +3839,7 @@
         <v>0.92</v>
       </c>
       <c r="G10" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>63108.03182600603</v>
       </c>
       <c r="H10" s="48">
@@ -3753,19 +3849,19 @@
         <v>6.7191780821917804E-2</v>
       </c>
       <c r="J10" s="35">
-        <f t="shared" si="0"/>
+        <f>G10-K10</f>
         <v>58564.253534533593</v>
       </c>
       <c r="K10" s="35">
-        <f t="shared" si="1"/>
+        <f>C10</f>
         <v>4543.7782914724339</v>
       </c>
       <c r="L10" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3899</v>
       </c>
       <c r="M10" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="N10" s="12">
@@ -3778,18 +3874,18 @@
         <v>0.82</v>
       </c>
       <c r="Q10" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3231.3330000000001</v>
       </c>
       <c r="R10" s="42">
         <v>0.17</v>
       </c>
       <c r="S10" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2682.00639</v>
       </c>
       <c r="T10" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>549.32661000000007</v>
       </c>
       <c r="U10" s="17"/>
@@ -3803,7 +3899,7 @@
         <v>233</v>
       </c>
       <c r="C11" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4770.9672060460571</v>
       </c>
       <c r="D11" s="12">
@@ -3816,7 +3912,7 @@
         <v>0.94</v>
       </c>
       <c r="G11" s="35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>66263.43341730634</v>
       </c>
       <c r="H11" s="48">
@@ -3826,19 +3922,19 @@
         <v>6.9246575342465755E-2</v>
       </c>
       <c r="J11" s="35">
-        <f t="shared" si="0"/>
+        <f>G11-K11</f>
         <v>61492.466211260282</v>
       </c>
       <c r="K11" s="35">
-        <f t="shared" si="1"/>
+        <f>C11</f>
         <v>4770.9672060460571</v>
       </c>
       <c r="L11" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>3892</v>
       </c>
       <c r="M11" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>330</v>
       </c>
       <c r="N11" s="12">
@@ -3851,18 +3947,18 @@
         <v>0.82</v>
       </c>
       <c r="Q11" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4161.2130000000006</v>
       </c>
       <c r="R11" s="42">
         <v>0.13</v>
       </c>
       <c r="S11" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3620.2553100000005</v>
       </c>
       <c r="T11" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>540.95769000000007</v>
       </c>
       <c r="U11" s="51">
@@ -3877,7 +3973,7 @@
         <v>194</v>
       </c>
       <c r="C12" s="35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5009.5155663483602</v>
       </c>
       <c r="D12" s="11">
@@ -3897,16 +3993,16 @@
         <v>4.6699999999999998E-2</v>
       </c>
       <c r="J12" s="35">
-        <f t="shared" si="0"/>
+        <f>G12-K12</f>
         <v>64567.089521823305</v>
       </c>
       <c r="K12" s="35">
-        <f t="shared" si="1"/>
+        <f>C12</f>
         <v>5009.5155663483602</v>
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>234</v>
       </c>
       <c r="N12" s="12">
@@ -3919,18 +4015,18 @@
         <v>0.7</v>
       </c>
       <c r="Q12" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4132.8630000000003</v>
       </c>
       <c r="R12" s="41">
         <v>0.1</v>
       </c>
       <c r="S12" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3719.5767000000001</v>
       </c>
       <c r="T12" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>413.28630000000004</v>
       </c>
     </row>
@@ -3995,10 +4091,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4008,142 +4104,149 @@
     <col min="3" max="3" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="69" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16" style="69" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="69" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="16" style="69" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" style="69" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28" style="69" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" style="69" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.85546875" style="69" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="28" style="69" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="28" style="69" customWidth="1"/>
-    <col min="28" max="28" width="13.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15" style="69" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="69" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11" style="69" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28" style="69" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="28" style="69" customWidth="1"/>
+    <col min="31" max="31" width="13.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" style="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>82</v>
-      </c>
       <c r="K1" s="75" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="L1" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="76" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+      <c r="M1" s="109" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="114" t="s">
+        <v>81</v>
       </c>
       <c r="O1" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="75" t="s">
         <v>75</v>
       </c>
       <c r="R1" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="S1" s="77" t="s">
+      <c r="S1" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="75" t="s">
-        <v>85</v>
+      <c r="T1" s="76" t="s">
+        <v>75</v>
       </c>
       <c r="U1" s="76" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="V1" s="77" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="W1" s="75" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="X1" s="76" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="Y1" s="77" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="105" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA1" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB1" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC1" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z1" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB1" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC1" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD1" s="105" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE1" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF1" s="90" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG1" s="91" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" s="91" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI1" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="AE1" s="91" t="s">
+      <c r="AJ1" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="AF1" s="91" t="s">
+      <c r="AK1" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH1" s="91" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI1" s="92" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="78" t="s">
@@ -4155,143 +4258,169 @@
       <c r="E2" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="78" t="s">
+      <c r="F2" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="G2" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="80" t="s">
+      <c r="H2" s="80" t="s">
         <v>78</v>
       </c>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="78" t="s">
         <v>76</v>
       </c>
       <c r="L2" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="110" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="115" t="s">
         <v>76</v>
-      </c>
-      <c r="M2" s="79" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="79" t="s">
-        <v>77</v>
       </c>
       <c r="O2" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="P2" s="79" t="s">
+      <c r="P2" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" s="79" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="Q2" s="79" t="s">
+      <c r="T2" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="R2" s="79" t="s">
+      <c r="V2" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="T2" s="78"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="80"/>
       <c r="W2" s="78"/>
       <c r="X2" s="79"/>
       <c r="Y2" s="80"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="95"/>
-      <c r="AD2" s="93" t="s">
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="80"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="AE2" s="94" t="s">
+      <c r="AG2" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="AF2" s="94" t="s">
+      <c r="AH2" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="AG2" s="94" t="s">
+      <c r="AI2" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" s="94" t="s">
+      <c r="AJ2" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="AI2" s="95" t="s">
+      <c r="AK2" s="95" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="53"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80"/>
+      <c r="C3" s="78" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="78" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="110" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="115" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q3" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="M3" s="79" t="s">
+      <c r="R3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="79" t="s">
+      <c r="S3" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" s="79" t="s">
+      <c r="T3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="79" t="s">
+      <c r="U3" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="S3" s="80" t="s">
+      <c r="V3" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="78" t="s">
+      <c r="W3" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="X3" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="U3" s="79" t="s">
+      <c r="Y3" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="V3" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="W3" s="78" t="s">
+      <c r="Z3" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA3" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="X3" s="79" t="s">
+      <c r="AB3" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="Y3" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB3" s="93" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC3" s="95" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD3" s="93"/>
-      <c r="AE3" s="94"/>
-      <c r="AF3" s="94"/>
+      <c r="AE3" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF3" s="93"/>
       <c r="AG3" s="94"/>
       <c r="AH3" s="94"/>
-      <c r="AI3" s="95"/>
-    </row>
-    <row r="4" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI3" s="94"/>
+      <c r="AJ3" s="94"/>
+      <c r="AK3" s="95"/>
+    </row>
+    <row r="4" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>2000</v>
       </c>
@@ -4302,85 +4431,84 @@
         <v>1</v>
       </c>
       <c r="D4" s="82">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E4" s="83">
         <v>0.03</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74">
+      <c r="F4" s="81">
+        <v>1</v>
+      </c>
+      <c r="G4" s="82">
+        <v>1</v>
+      </c>
+      <c r="H4" s="83">
+        <v>0.03</v>
+      </c>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74">
         <v>0.7</v>
-      </c>
-      <c r="H4" s="81">
-        <v>0.42</v>
-      </c>
-      <c r="I4" s="82">
-        <v>0.35</v>
-      </c>
-      <c r="J4" s="83">
-        <v>0.1</v>
       </c>
       <c r="K4" s="81">
         <v>1</v>
       </c>
       <c r="L4" s="82">
+        <v>0</v>
+      </c>
+      <c r="M4" s="111">
+        <v>0</v>
+      </c>
+      <c r="N4" s="116">
+        <v>1</v>
+      </c>
+      <c r="O4" s="82">
+        <v>0</v>
+      </c>
+      <c r="P4" s="83">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="81">
+        <v>1</v>
+      </c>
+      <c r="R4" s="82">
+        <v>10</v>
+      </c>
+      <c r="S4" s="82">
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="82">
         <v>4</v>
       </c>
-      <c r="M4" s="82">
-        <v>10</v>
-      </c>
-      <c r="N4" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="O4" s="82">
-        <v>4</v>
-      </c>
-      <c r="P4" s="82">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="82">
+      <c r="U4" s="82">
         <f>3/12</f>
         <v>0.25</v>
       </c>
-      <c r="R4" s="82">
+      <c r="V4" s="83">
         <f>3/12</f>
         <v>0.25</v>
       </c>
-      <c r="S4" s="83">
-        <f>3/12</f>
-        <v>0.25</v>
-      </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="81">
+      <c r="W4" s="81"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="81">
         <v>1</v>
       </c>
-      <c r="X4" s="82">
+      <c r="AA4" s="82">
         <v>1</v>
       </c>
-      <c r="Y4" s="83">
+      <c r="AB4" s="83">
         <v>0.04</v>
       </c>
-      <c r="Z4" s="106">
+      <c r="AC4" s="106">
         <v>1</v>
       </c>
-      <c r="AA4" s="106">
+      <c r="AD4" s="106">
         <v>1</v>
       </c>
-      <c r="AB4" s="96">
+      <c r="AE4" s="96">
         <v>1</v>
       </c>
-      <c r="AC4" s="98">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="96">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="97">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="97">
+      <c r="AF4" s="96">
         <v>0</v>
       </c>
       <c r="AG4" s="97">
@@ -4389,11 +4517,17 @@
       <c r="AH4" s="97">
         <v>0</v>
       </c>
-      <c r="AI4" s="98">
+      <c r="AI4" s="97">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>2001</v>
       </c>
@@ -4401,38 +4535,40 @@
       <c r="C5" s="84"/>
       <c r="D5" s="85"/>
       <c r="E5" s="86"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
       <c r="K5" s="84"/>
       <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="117"/>
       <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="84"/>
       <c r="R5" s="85"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="84"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
       <c r="U5" s="85"/>
       <c r="V5" s="86"/>
       <c r="W5" s="84"/>
       <c r="X5" s="85"/>
       <c r="Y5" s="86"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="99"/>
-      <c r="AC5" s="101"/>
-      <c r="AD5" s="99"/>
-      <c r="AE5" s="100"/>
-      <c r="AF5" s="100"/>
+      <c r="Z5" s="84"/>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="107"/>
+      <c r="AD5" s="107"/>
+      <c r="AE5" s="99"/>
+      <c r="AF5" s="99"/>
       <c r="AG5" s="100"/>
       <c r="AH5" s="100"/>
-      <c r="AI5" s="101"/>
-    </row>
-    <row r="6" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI5" s="100"/>
+      <c r="AJ5" s="100"/>
+      <c r="AK5" s="101"/>
+    </row>
+    <row r="6" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>2002</v>
       </c>
@@ -4440,38 +4576,40 @@
       <c r="C6" s="84"/>
       <c r="D6" s="85"/>
       <c r="E6" s="86"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
       <c r="K6" s="84"/>
       <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="117"/>
       <c r="O6" s="85"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="85"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="84"/>
       <c r="R6" s="85"/>
-      <c r="S6" s="86"/>
-      <c r="T6" s="84"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
       <c r="U6" s="85"/>
       <c r="V6" s="86"/>
       <c r="W6" s="84"/>
       <c r="X6" s="85"/>
       <c r="Y6" s="86"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="99"/>
-      <c r="AC6" s="101"/>
-      <c r="AD6" s="99"/>
-      <c r="AE6" s="100"/>
-      <c r="AF6" s="100"/>
+      <c r="Z6" s="84"/>
+      <c r="AA6" s="85"/>
+      <c r="AB6" s="86"/>
+      <c r="AC6" s="107"/>
+      <c r="AD6" s="107"/>
+      <c r="AE6" s="99"/>
+      <c r="AF6" s="99"/>
       <c r="AG6" s="100"/>
       <c r="AH6" s="100"/>
-      <c r="AI6" s="101"/>
-    </row>
-    <row r="7" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI6" s="100"/>
+      <c r="AJ6" s="100"/>
+      <c r="AK6" s="101"/>
+    </row>
+    <row r="7" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>2003</v>
       </c>
@@ -4479,38 +4617,40 @@
       <c r="C7" s="84"/>
       <c r="D7" s="85"/>
       <c r="E7" s="86"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="86"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
       <c r="K7" s="84"/>
       <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="117"/>
       <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="84"/>
       <c r="R7" s="85"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="84"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="85"/>
       <c r="U7" s="85"/>
       <c r="V7" s="86"/>
       <c r="W7" s="84"/>
       <c r="X7" s="85"/>
       <c r="Y7" s="86"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="99"/>
-      <c r="AC7" s="101"/>
-      <c r="AD7" s="99"/>
-      <c r="AE7" s="100"/>
-      <c r="AF7" s="100"/>
+      <c r="Z7" s="84"/>
+      <c r="AA7" s="85"/>
+      <c r="AB7" s="86"/>
+      <c r="AC7" s="107"/>
+      <c r="AD7" s="107"/>
+      <c r="AE7" s="99"/>
+      <c r="AF7" s="99"/>
       <c r="AG7" s="100"/>
       <c r="AH7" s="100"/>
-      <c r="AI7" s="101"/>
-    </row>
-    <row r="8" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI7" s="100"/>
+      <c r="AJ7" s="100"/>
+      <c r="AK7" s="101"/>
+    </row>
+    <row r="8" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>2004</v>
       </c>
@@ -4518,38 +4658,40 @@
       <c r="C8" s="84"/>
       <c r="D8" s="85"/>
       <c r="E8" s="86"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="86"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
       <c r="K8" s="84"/>
       <c r="L8" s="85"/>
-      <c r="M8" s="85"/>
-      <c r="N8" s="85"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="117"/>
       <c r="O8" s="85"/>
-      <c r="P8" s="85"/>
-      <c r="Q8" s="85"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="84"/>
       <c r="R8" s="85"/>
-      <c r="S8" s="86"/>
-      <c r="T8" s="84"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="85"/>
       <c r="U8" s="85"/>
       <c r="V8" s="86"/>
       <c r="W8" s="84"/>
       <c r="X8" s="85"/>
       <c r="Y8" s="86"/>
-      <c r="Z8" s="107"/>
-      <c r="AA8" s="107"/>
-      <c r="AB8" s="99"/>
-      <c r="AC8" s="101"/>
-      <c r="AD8" s="99"/>
-      <c r="AE8" s="100"/>
-      <c r="AF8" s="100"/>
+      <c r="Z8" s="84"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="86"/>
+      <c r="AC8" s="107"/>
+      <c r="AD8" s="107"/>
+      <c r="AE8" s="99"/>
+      <c r="AF8" s="99"/>
       <c r="AG8" s="100"/>
       <c r="AH8" s="100"/>
-      <c r="AI8" s="101"/>
-    </row>
-    <row r="9" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI8" s="100"/>
+      <c r="AJ8" s="100"/>
+      <c r="AK8" s="101"/>
+    </row>
+    <row r="9" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>2005</v>
       </c>
@@ -4557,38 +4699,40 @@
       <c r="C9" s="84"/>
       <c r="D9" s="85"/>
       <c r="E9" s="86"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="86"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
       <c r="K9" s="84"/>
       <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="117"/>
       <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="84"/>
       <c r="R9" s="85"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="84"/>
+      <c r="S9" s="85"/>
+      <c r="T9" s="85"/>
       <c r="U9" s="85"/>
       <c r="V9" s="86"/>
       <c r="W9" s="84"/>
       <c r="X9" s="85"/>
       <c r="Y9" s="86"/>
-      <c r="Z9" s="107"/>
-      <c r="AA9" s="107"/>
-      <c r="AB9" s="99"/>
-      <c r="AC9" s="101"/>
-      <c r="AD9" s="99"/>
-      <c r="AE9" s="100"/>
-      <c r="AF9" s="100"/>
+      <c r="Z9" s="84"/>
+      <c r="AA9" s="85"/>
+      <c r="AB9" s="86"/>
+      <c r="AC9" s="107"/>
+      <c r="AD9" s="107"/>
+      <c r="AE9" s="99"/>
+      <c r="AF9" s="99"/>
       <c r="AG9" s="100"/>
       <c r="AH9" s="100"/>
-      <c r="AI9" s="101"/>
-    </row>
-    <row r="10" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI9" s="100"/>
+      <c r="AJ9" s="100"/>
+      <c r="AK9" s="101"/>
+    </row>
+    <row r="10" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>2006</v>
       </c>
@@ -4596,38 +4740,40 @@
       <c r="C10" s="84"/>
       <c r="D10" s="85"/>
       <c r="E10" s="86"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="86"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
       <c r="K10" s="84"/>
       <c r="L10" s="85"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="85"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="117"/>
       <c r="O10" s="85"/>
-      <c r="P10" s="85"/>
-      <c r="Q10" s="85"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="84"/>
       <c r="R10" s="85"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="84"/>
+      <c r="S10" s="85"/>
+      <c r="T10" s="85"/>
       <c r="U10" s="85"/>
       <c r="V10" s="86"/>
       <c r="W10" s="84"/>
       <c r="X10" s="85"/>
       <c r="Y10" s="86"/>
-      <c r="Z10" s="107"/>
-      <c r="AA10" s="107"/>
-      <c r="AB10" s="99"/>
-      <c r="AC10" s="101"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="100"/>
-      <c r="AF10" s="100"/>
+      <c r="Z10" s="84"/>
+      <c r="AA10" s="85"/>
+      <c r="AB10" s="86"/>
+      <c r="AC10" s="107"/>
+      <c r="AD10" s="107"/>
+      <c r="AE10" s="99"/>
+      <c r="AF10" s="99"/>
       <c r="AG10" s="100"/>
       <c r="AH10" s="100"/>
-      <c r="AI10" s="101"/>
-    </row>
-    <row r="11" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI10" s="100"/>
+      <c r="AJ10" s="100"/>
+      <c r="AK10" s="101"/>
+    </row>
+    <row r="11" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>2007</v>
       </c>
@@ -4635,44 +4781,46 @@
       <c r="C11" s="84"/>
       <c r="D11" s="85"/>
       <c r="E11" s="86"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="86"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
       <c r="K11" s="84"/>
       <c r="L11" s="85"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
+      <c r="M11" s="112"/>
+      <c r="N11" s="117"/>
       <c r="O11" s="85"/>
-      <c r="P11" s="85"/>
-      <c r="Q11" s="85"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="84"/>
       <c r="R11" s="85"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="84">
+      <c r="S11" s="85"/>
+      <c r="T11" s="85"/>
+      <c r="U11" s="85"/>
+      <c r="V11" s="86"/>
+      <c r="W11" s="84">
         <v>0.7</v>
       </c>
-      <c r="U11" s="85">
+      <c r="X11" s="85">
         <v>0.75</v>
       </c>
-      <c r="V11" s="86">
+      <c r="Y11" s="86">
         <v>0.8</v>
       </c>
-      <c r="W11" s="84"/>
-      <c r="X11" s="85"/>
-      <c r="Y11" s="86"/>
-      <c r="Z11" s="107"/>
-      <c r="AA11" s="107"/>
-      <c r="AB11" s="99"/>
-      <c r="AC11" s="101"/>
-      <c r="AD11" s="99"/>
-      <c r="AE11" s="100"/>
-      <c r="AF11" s="100"/>
+      <c r="Z11" s="84"/>
+      <c r="AA11" s="85"/>
+      <c r="AB11" s="86"/>
+      <c r="AC11" s="107"/>
+      <c r="AD11" s="107"/>
+      <c r="AE11" s="99"/>
+      <c r="AF11" s="99"/>
       <c r="AG11" s="100"/>
       <c r="AH11" s="100"/>
-      <c r="AI11" s="101"/>
-    </row>
-    <row r="12" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI11" s="100"/>
+      <c r="AJ11" s="100"/>
+      <c r="AK11" s="101"/>
+    </row>
+    <row r="12" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>2008</v>
       </c>
@@ -4680,38 +4828,40 @@
       <c r="C12" s="84"/>
       <c r="D12" s="85"/>
       <c r="E12" s="86"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="86"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
       <c r="K12" s="84"/>
       <c r="L12" s="85"/>
-      <c r="M12" s="85"/>
-      <c r="N12" s="85"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="117"/>
       <c r="O12" s="85"/>
-      <c r="P12" s="85"/>
-      <c r="Q12" s="85"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="84"/>
       <c r="R12" s="85"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="84"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="85"/>
       <c r="U12" s="85"/>
       <c r="V12" s="86"/>
       <c r="W12" s="84"/>
       <c r="X12" s="85"/>
       <c r="Y12" s="86"/>
-      <c r="Z12" s="107"/>
-      <c r="AA12" s="107"/>
-      <c r="AB12" s="99"/>
-      <c r="AC12" s="101"/>
-      <c r="AD12" s="99"/>
-      <c r="AE12" s="100"/>
-      <c r="AF12" s="100"/>
+      <c r="Z12" s="84"/>
+      <c r="AA12" s="85"/>
+      <c r="AB12" s="86"/>
+      <c r="AC12" s="107"/>
+      <c r="AD12" s="107"/>
+      <c r="AE12" s="99"/>
+      <c r="AF12" s="99"/>
       <c r="AG12" s="100"/>
       <c r="AH12" s="100"/>
-      <c r="AI12" s="101"/>
-    </row>
-    <row r="13" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI12" s="100"/>
+      <c r="AJ12" s="100"/>
+      <c r="AK12" s="101"/>
+    </row>
+    <row r="13" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>2009</v>
       </c>
@@ -4719,40 +4869,42 @@
       <c r="C13" s="84"/>
       <c r="D13" s="85"/>
       <c r="E13" s="86"/>
-      <c r="F13" s="71">
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="71">
         <v>0</v>
       </c>
-      <c r="G13" s="71"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="86"/>
+      <c r="J13" s="71"/>
       <c r="K13" s="84"/>
       <c r="L13" s="85"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="117"/>
       <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="84"/>
       <c r="R13" s="85"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="84"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
       <c r="U13" s="85"/>
       <c r="V13" s="86"/>
       <c r="W13" s="84"/>
       <c r="X13" s="85"/>
       <c r="Y13" s="86"/>
-      <c r="Z13" s="107"/>
-      <c r="AA13" s="107"/>
-      <c r="AB13" s="99"/>
-      <c r="AC13" s="101"/>
-      <c r="AD13" s="99"/>
-      <c r="AE13" s="100"/>
-      <c r="AF13" s="100"/>
+      <c r="Z13" s="84"/>
+      <c r="AA13" s="85"/>
+      <c r="AB13" s="86"/>
+      <c r="AC13" s="107"/>
+      <c r="AD13" s="107"/>
+      <c r="AE13" s="99"/>
+      <c r="AF13" s="99"/>
       <c r="AG13" s="100"/>
       <c r="AH13" s="100"/>
-      <c r="AI13" s="101"/>
-    </row>
-    <row r="14" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI13" s="100"/>
+      <c r="AJ13" s="100"/>
+      <c r="AK13" s="101"/>
+    </row>
+    <row r="14" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>2010</v>
       </c>
@@ -4760,46 +4912,48 @@
       <c r="C14" s="84"/>
       <c r="D14" s="85"/>
       <c r="E14" s="86"/>
-      <c r="F14" s="71">
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="71">
         <v>1500</v>
       </c>
-      <c r="G14" s="71"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="86"/>
+      <c r="J14" s="71"/>
       <c r="K14" s="84"/>
       <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="117"/>
       <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="84"/>
       <c r="R14" s="85"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="84">
+      <c r="S14" s="85"/>
+      <c r="T14" s="85"/>
+      <c r="U14" s="85"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="84">
         <v>0.7</v>
       </c>
-      <c r="U14" s="85">
+      <c r="X14" s="85">
         <v>0.75</v>
       </c>
-      <c r="V14" s="86">
+      <c r="Y14" s="86">
         <v>0.8</v>
       </c>
-      <c r="W14" s="84"/>
-      <c r="X14" s="85"/>
-      <c r="Y14" s="86"/>
-      <c r="Z14" s="107"/>
-      <c r="AA14" s="107"/>
-      <c r="AB14" s="99"/>
-      <c r="AC14" s="101"/>
-      <c r="AD14" s="99"/>
-      <c r="AE14" s="100"/>
-      <c r="AF14" s="100"/>
+      <c r="Z14" s="84"/>
+      <c r="AA14" s="85"/>
+      <c r="AB14" s="86"/>
+      <c r="AC14" s="107"/>
+      <c r="AD14" s="107"/>
+      <c r="AE14" s="99"/>
+      <c r="AF14" s="99"/>
       <c r="AG14" s="100"/>
       <c r="AH14" s="100"/>
-      <c r="AI14" s="101"/>
-    </row>
-    <row r="15" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI14" s="100"/>
+      <c r="AJ14" s="100"/>
+      <c r="AK14" s="101"/>
+    </row>
+    <row r="15" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>2011</v>
       </c>
@@ -4807,38 +4961,40 @@
       <c r="C15" s="84"/>
       <c r="D15" s="85"/>
       <c r="E15" s="86"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="86"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
       <c r="K15" s="84"/>
       <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="85"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="117"/>
       <c r="O15" s="85"/>
-      <c r="P15" s="85"/>
-      <c r="Q15" s="85"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="84"/>
       <c r="R15" s="85"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="84"/>
+      <c r="S15" s="85"/>
+      <c r="T15" s="85"/>
       <c r="U15" s="85"/>
       <c r="V15" s="86"/>
       <c r="W15" s="84"/>
       <c r="X15" s="85"/>
       <c r="Y15" s="86"/>
-      <c r="Z15" s="107"/>
-      <c r="AA15" s="107"/>
-      <c r="AB15" s="99"/>
-      <c r="AC15" s="101"/>
-      <c r="AD15" s="99"/>
-      <c r="AE15" s="100"/>
-      <c r="AF15" s="100"/>
+      <c r="Z15" s="84"/>
+      <c r="AA15" s="85"/>
+      <c r="AB15" s="86"/>
+      <c r="AC15" s="107"/>
+      <c r="AD15" s="107"/>
+      <c r="AE15" s="99"/>
+      <c r="AF15" s="99"/>
       <c r="AG15" s="100"/>
       <c r="AH15" s="100"/>
-      <c r="AI15" s="101"/>
-    </row>
-    <row r="16" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI15" s="100"/>
+      <c r="AJ15" s="100"/>
+      <c r="AK15" s="101"/>
+    </row>
+    <row r="16" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>2012</v>
       </c>
@@ -4846,44 +5002,46 @@
       <c r="C16" s="84"/>
       <c r="D16" s="85"/>
       <c r="E16" s="86"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="86"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
       <c r="K16" s="84"/>
       <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="117"/>
       <c r="O16" s="85"/>
-      <c r="P16" s="85"/>
-      <c r="Q16" s="85"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="84"/>
       <c r="R16" s="85"/>
-      <c r="S16" s="86"/>
-      <c r="T16" s="84">
+      <c r="S16" s="85"/>
+      <c r="T16" s="85"/>
+      <c r="U16" s="85"/>
+      <c r="V16" s="86"/>
+      <c r="W16" s="84">
         <v>0.91200000000000003</v>
       </c>
-      <c r="U16" s="85">
+      <c r="X16" s="85">
         <v>0.82</v>
       </c>
-      <c r="V16" s="86">
+      <c r="Y16" s="86">
         <v>0.88</v>
       </c>
-      <c r="W16" s="84"/>
-      <c r="X16" s="85"/>
-      <c r="Y16" s="86"/>
-      <c r="Z16" s="107"/>
-      <c r="AA16" s="107"/>
-      <c r="AB16" s="99"/>
-      <c r="AC16" s="101"/>
-      <c r="AD16" s="99"/>
-      <c r="AE16" s="100"/>
-      <c r="AF16" s="100"/>
+      <c r="Z16" s="84"/>
+      <c r="AA16" s="85"/>
+      <c r="AB16" s="86"/>
+      <c r="AC16" s="107"/>
+      <c r="AD16" s="107"/>
+      <c r="AE16" s="99"/>
+      <c r="AF16" s="99"/>
       <c r="AG16" s="100"/>
       <c r="AH16" s="100"/>
-      <c r="AI16" s="101"/>
-    </row>
-    <row r="17" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI16" s="100"/>
+      <c r="AJ16" s="100"/>
+      <c r="AK16" s="101"/>
+    </row>
+    <row r="17" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>2013</v>
       </c>
@@ -4891,44 +5049,46 @@
       <c r="C17" s="84"/>
       <c r="D17" s="85"/>
       <c r="E17" s="86"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="86"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
       <c r="K17" s="84"/>
       <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
+      <c r="M17" s="112"/>
+      <c r="N17" s="117"/>
       <c r="O17" s="85"/>
-      <c r="P17" s="85"/>
-      <c r="Q17" s="85"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="84"/>
       <c r="R17" s="85"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="84">
+      <c r="S17" s="85"/>
+      <c r="T17" s="85"/>
+      <c r="U17" s="85"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="84">
         <v>0.91200000000000003</v>
       </c>
-      <c r="U17" s="85">
+      <c r="X17" s="85">
         <v>0.86</v>
       </c>
-      <c r="V17" s="86">
+      <c r="Y17" s="86">
         <v>0.9</v>
       </c>
-      <c r="W17" s="84"/>
-      <c r="X17" s="85"/>
-      <c r="Y17" s="86"/>
-      <c r="Z17" s="107"/>
-      <c r="AA17" s="107"/>
-      <c r="AB17" s="99"/>
-      <c r="AC17" s="101"/>
-      <c r="AD17" s="99"/>
-      <c r="AE17" s="100"/>
-      <c r="AF17" s="100"/>
+      <c r="Z17" s="84"/>
+      <c r="AA17" s="85"/>
+      <c r="AB17" s="86"/>
+      <c r="AC17" s="107"/>
+      <c r="AD17" s="107"/>
+      <c r="AE17" s="99"/>
+      <c r="AF17" s="99"/>
       <c r="AG17" s="100"/>
       <c r="AH17" s="100"/>
-      <c r="AI17" s="101"/>
-    </row>
-    <row r="18" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI17" s="100"/>
+      <c r="AJ17" s="100"/>
+      <c r="AK17" s="101"/>
+    </row>
+    <row r="18" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
         <v>2014</v>
       </c>
@@ -4936,44 +5096,46 @@
       <c r="C18" s="84"/>
       <c r="D18" s="85"/>
       <c r="E18" s="86"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="86"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
       <c r="K18" s="84"/>
       <c r="L18" s="85"/>
-      <c r="M18" s="85"/>
-      <c r="N18" s="85"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="117"/>
       <c r="O18" s="85"/>
-      <c r="P18" s="85"/>
-      <c r="Q18" s="85"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="84"/>
       <c r="R18" s="85"/>
-      <c r="S18" s="86"/>
-      <c r="T18" s="84">
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="85"/>
+      <c r="V18" s="86"/>
+      <c r="W18" s="84">
         <v>0.91200000000000003</v>
       </c>
-      <c r="U18" s="85">
+      <c r="X18" s="85">
         <v>0.89</v>
       </c>
-      <c r="V18" s="86">
+      <c r="Y18" s="86">
         <v>0.9</v>
       </c>
-      <c r="W18" s="84"/>
-      <c r="X18" s="85"/>
-      <c r="Y18" s="86"/>
-      <c r="Z18" s="107"/>
-      <c r="AA18" s="107"/>
-      <c r="AB18" s="99"/>
-      <c r="AC18" s="101"/>
-      <c r="AD18" s="99"/>
-      <c r="AE18" s="100"/>
-      <c r="AF18" s="100"/>
+      <c r="Z18" s="84"/>
+      <c r="AA18" s="85"/>
+      <c r="AB18" s="86"/>
+      <c r="AC18" s="107"/>
+      <c r="AD18" s="107"/>
+      <c r="AE18" s="99"/>
+      <c r="AF18" s="99"/>
       <c r="AG18" s="100"/>
       <c r="AH18" s="100"/>
-      <c r="AI18" s="101"/>
-    </row>
-    <row r="19" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI18" s="100"/>
+      <c r="AJ18" s="100"/>
+      <c r="AK18" s="101"/>
+    </row>
+    <row r="19" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
         <v>2015</v>
       </c>
@@ -4981,44 +5143,46 @@
       <c r="C19" s="84"/>
       <c r="D19" s="85"/>
       <c r="E19" s="86"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="86"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="84"/>
       <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
+      <c r="M19" s="112"/>
+      <c r="N19" s="117"/>
       <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
+      <c r="P19" s="86"/>
+      <c r="Q19" s="84"/>
       <c r="R19" s="85"/>
-      <c r="S19" s="86"/>
-      <c r="T19" s="84">
+      <c r="S19" s="85"/>
+      <c r="T19" s="85"/>
+      <c r="U19" s="85"/>
+      <c r="V19" s="86"/>
+      <c r="W19" s="84">
         <v>0.91200000000000003</v>
       </c>
-      <c r="U19" s="85">
+      <c r="X19" s="85">
         <v>0.92</v>
       </c>
-      <c r="V19" s="86">
+      <c r="Y19" s="86">
         <v>0.92</v>
       </c>
-      <c r="W19" s="84"/>
-      <c r="X19" s="85"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="107"/>
-      <c r="AA19" s="107"/>
-      <c r="AB19" s="99"/>
-      <c r="AC19" s="101"/>
-      <c r="AD19" s="99"/>
-      <c r="AE19" s="100"/>
-      <c r="AF19" s="100"/>
+      <c r="Z19" s="84"/>
+      <c r="AA19" s="85"/>
+      <c r="AB19" s="86"/>
+      <c r="AC19" s="107"/>
+      <c r="AD19" s="107"/>
+      <c r="AE19" s="99"/>
+      <c r="AF19" s="99"/>
       <c r="AG19" s="100"/>
       <c r="AH19" s="100"/>
-      <c r="AI19" s="101"/>
-    </row>
-    <row r="20" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI19" s="100"/>
+      <c r="AJ19" s="100"/>
+      <c r="AK19" s="101"/>
+    </row>
+    <row r="20" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>2016</v>
       </c>
@@ -5026,46 +5190,48 @@
       <c r="C20" s="84"/>
       <c r="D20" s="85"/>
       <c r="E20" s="86"/>
-      <c r="F20" s="71">
+      <c r="F20" s="84"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="71">
         <v>4000</v>
       </c>
-      <c r="G20" s="71"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="86"/>
+      <c r="J20" s="71"/>
       <c r="K20" s="84"/>
       <c r="L20" s="85"/>
-      <c r="M20" s="85"/>
-      <c r="N20" s="85"/>
+      <c r="M20" s="112"/>
+      <c r="N20" s="117"/>
       <c r="O20" s="85"/>
-      <c r="P20" s="85"/>
-      <c r="Q20" s="85"/>
+      <c r="P20" s="86"/>
+      <c r="Q20" s="84"/>
       <c r="R20" s="85"/>
-      <c r="S20" s="86"/>
-      <c r="T20" s="84">
+      <c r="S20" s="85"/>
+      <c r="T20" s="85"/>
+      <c r="U20" s="85"/>
+      <c r="V20" s="86"/>
+      <c r="W20" s="84">
         <v>0.91200000000000003</v>
       </c>
-      <c r="U20" s="85">
+      <c r="X20" s="85">
         <v>0.95</v>
       </c>
-      <c r="V20" s="86">
+      <c r="Y20" s="86">
         <v>0.94</v>
       </c>
-      <c r="W20" s="84"/>
-      <c r="X20" s="85"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="107"/>
-      <c r="AA20" s="107"/>
-      <c r="AB20" s="99"/>
-      <c r="AC20" s="101"/>
-      <c r="AD20" s="99"/>
-      <c r="AE20" s="100"/>
-      <c r="AF20" s="100"/>
+      <c r="Z20" s="84"/>
+      <c r="AA20" s="85"/>
+      <c r="AB20" s="86"/>
+      <c r="AC20" s="107"/>
+      <c r="AD20" s="107"/>
+      <c r="AE20" s="99"/>
+      <c r="AF20" s="99"/>
       <c r="AG20" s="100"/>
       <c r="AH20" s="100"/>
-      <c r="AI20" s="101"/>
-    </row>
-    <row r="21" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI20" s="100"/>
+      <c r="AJ20" s="100"/>
+      <c r="AK20" s="101"/>
+    </row>
+    <row r="21" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
         <v>2017</v>
       </c>
@@ -5073,38 +5239,40 @@
       <c r="C21" s="84"/>
       <c r="D21" s="85"/>
       <c r="E21" s="86"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="86"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
       <c r="K21" s="84"/>
       <c r="L21" s="85"/>
-      <c r="M21" s="85"/>
-      <c r="N21" s="85"/>
+      <c r="M21" s="112"/>
+      <c r="N21" s="117"/>
       <c r="O21" s="85"/>
-      <c r="P21" s="85"/>
-      <c r="Q21" s="85"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="84"/>
       <c r="R21" s="85"/>
-      <c r="S21" s="86"/>
-      <c r="T21" s="84"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="85"/>
       <c r="U21" s="85"/>
       <c r="V21" s="86"/>
       <c r="W21" s="84"/>
       <c r="X21" s="85"/>
       <c r="Y21" s="86"/>
-      <c r="Z21" s="107"/>
-      <c r="AA21" s="107"/>
-      <c r="AB21" s="99"/>
-      <c r="AC21" s="101"/>
-      <c r="AD21" s="99"/>
-      <c r="AE21" s="100"/>
-      <c r="AF21" s="100"/>
+      <c r="Z21" s="84"/>
+      <c r="AA21" s="85"/>
+      <c r="AB21" s="86"/>
+      <c r="AC21" s="107"/>
+      <c r="AD21" s="107"/>
+      <c r="AE21" s="99"/>
+      <c r="AF21" s="99"/>
       <c r="AG21" s="100"/>
       <c r="AH21" s="100"/>
-      <c r="AI21" s="101"/>
-    </row>
-    <row r="22" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI21" s="100"/>
+      <c r="AJ21" s="100"/>
+      <c r="AK21" s="101"/>
+    </row>
+    <row r="22" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>2018</v>
       </c>
@@ -5112,38 +5280,40 @@
       <c r="C22" s="84"/>
       <c r="D22" s="85"/>
       <c r="E22" s="86"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="86"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
       <c r="K22" s="84"/>
       <c r="L22" s="85"/>
-      <c r="M22" s="85"/>
-      <c r="N22" s="85"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="117"/>
       <c r="O22" s="85"/>
-      <c r="P22" s="85"/>
-      <c r="Q22" s="85"/>
+      <c r="P22" s="86"/>
+      <c r="Q22" s="84"/>
       <c r="R22" s="85"/>
-      <c r="S22" s="86"/>
-      <c r="T22" s="84"/>
+      <c r="S22" s="85"/>
+      <c r="T22" s="85"/>
       <c r="U22" s="85"/>
       <c r="V22" s="86"/>
       <c r="W22" s="84"/>
       <c r="X22" s="85"/>
       <c r="Y22" s="86"/>
-      <c r="Z22" s="107"/>
-      <c r="AA22" s="107"/>
-      <c r="AB22" s="99"/>
-      <c r="AC22" s="101"/>
-      <c r="AD22" s="99"/>
-      <c r="AE22" s="100"/>
-      <c r="AF22" s="100"/>
+      <c r="Z22" s="84"/>
+      <c r="AA22" s="85"/>
+      <c r="AB22" s="86"/>
+      <c r="AC22" s="107"/>
+      <c r="AD22" s="107"/>
+      <c r="AE22" s="99"/>
+      <c r="AF22" s="99"/>
       <c r="AG22" s="100"/>
       <c r="AH22" s="100"/>
-      <c r="AI22" s="101"/>
-    </row>
-    <row r="23" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI22" s="100"/>
+      <c r="AJ22" s="100"/>
+      <c r="AK22" s="101"/>
+    </row>
+    <row r="23" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>2019</v>
       </c>
@@ -5151,38 +5321,40 @@
       <c r="C23" s="84"/>
       <c r="D23" s="85"/>
       <c r="E23" s="86"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="86"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
       <c r="K23" s="84"/>
       <c r="L23" s="85"/>
-      <c r="M23" s="85"/>
-      <c r="N23" s="85"/>
+      <c r="M23" s="112"/>
+      <c r="N23" s="117"/>
       <c r="O23" s="85"/>
-      <c r="P23" s="85"/>
-      <c r="Q23" s="85"/>
+      <c r="P23" s="86"/>
+      <c r="Q23" s="84"/>
       <c r="R23" s="85"/>
-      <c r="S23" s="86"/>
-      <c r="T23" s="84"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="85"/>
       <c r="U23" s="85"/>
       <c r="V23" s="86"/>
       <c r="W23" s="84"/>
       <c r="X23" s="85"/>
       <c r="Y23" s="86"/>
-      <c r="Z23" s="107"/>
-      <c r="AA23" s="107"/>
-      <c r="AB23" s="99"/>
-      <c r="AC23" s="101"/>
-      <c r="AD23" s="99"/>
-      <c r="AE23" s="100"/>
-      <c r="AF23" s="100"/>
+      <c r="Z23" s="84"/>
+      <c r="AA23" s="85"/>
+      <c r="AB23" s="86"/>
+      <c r="AC23" s="107"/>
+      <c r="AD23" s="107"/>
+      <c r="AE23" s="99"/>
+      <c r="AF23" s="99"/>
       <c r="AG23" s="100"/>
       <c r="AH23" s="100"/>
-      <c r="AI23" s="101"/>
-    </row>
-    <row r="24" spans="1:35" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI23" s="100"/>
+      <c r="AJ23" s="100"/>
+      <c r="AK23" s="101"/>
+    </row>
+    <row r="24" spans="1:37" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="72">
         <v>2020</v>
       </c>
@@ -5190,96 +5362,98 @@
       <c r="C24" s="87"/>
       <c r="D24" s="88"/>
       <c r="E24" s="89"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="89"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
       <c r="K24" s="87"/>
       <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
+      <c r="M24" s="113"/>
+      <c r="N24" s="118"/>
       <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="88"/>
+      <c r="P24" s="89"/>
+      <c r="Q24" s="87"/>
       <c r="R24" s="88"/>
-      <c r="S24" s="89"/>
-      <c r="T24" s="87"/>
+      <c r="S24" s="88"/>
+      <c r="T24" s="88"/>
       <c r="U24" s="88"/>
       <c r="V24" s="89"/>
       <c r="W24" s="87"/>
       <c r="X24" s="88"/>
       <c r="Y24" s="89"/>
-      <c r="Z24" s="108"/>
-      <c r="AA24" s="108"/>
-      <c r="AB24" s="102"/>
-      <c r="AC24" s="104"/>
-      <c r="AD24" s="102"/>
-      <c r="AE24" s="103"/>
-      <c r="AF24" s="103"/>
+      <c r="Z24" s="87"/>
+      <c r="AA24" s="88"/>
+      <c r="AB24" s="89"/>
+      <c r="AC24" s="108"/>
+      <c r="AD24" s="108"/>
+      <c r="AE24" s="102"/>
+      <c r="AF24" s="102"/>
       <c r="AG24" s="103"/>
       <c r="AH24" s="103"/>
-      <c r="AI24" s="104"/>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI24" s="103"/>
+      <c r="AJ24" s="103"/>
+      <c r="AK24" s="104"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>2021</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>2022</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>2023</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
         <v>2024</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="72">
         <v>2025</v>
       </c>
-      <c r="U29" s="69">
+      <c r="X29" s="69">
         <v>0.95</v>
       </c>
-      <c r="V29" s="69">
+      <c r="Y29" s="69">
         <v>0.95</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
         <v>2026</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
         <v>2027</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
         <v>2028</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
         <v>2029</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="72">
         <v>2030</v>
       </c>
-      <c r="U34" s="69">
+      <c r="X34" s="69">
         <v>0.99</v>
       </c>
-      <c r="V34" s="69">
+      <c r="Y34" s="69">
         <v>0.99</v>
       </c>
     </row>
@@ -5307,21 +5481,21 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="38"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -5461,27 +5635,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15" style="69" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="52"/>
+    <col min="3" max="3" width="14.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="75" t="s">
         <v>75</v>
@@ -5498,22 +5671,13 @@
       <c r="F1" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="78" t="s">
         <v>76</v>
@@ -5522,60 +5686,42 @@
         <v>76</v>
       </c>
       <c r="D2" s="79" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E2" s="79" t="s">
         <v>77</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="G2" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="78" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="F3" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="80" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>2000</v>
       </c>
@@ -5584,12 +5730,9 @@
       <c r="D4" s="82"/>
       <c r="E4" s="82"/>
       <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="83"/>
-    </row>
-    <row r="5" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="83"/>
+    </row>
+    <row r="5" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>2001</v>
       </c>
@@ -5598,12 +5741,9 @@
       <c r="D5" s="85"/>
       <c r="E5" s="85"/>
       <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
-    </row>
-    <row r="6" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="86"/>
+    </row>
+    <row r="6" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>2002</v>
       </c>
@@ -5612,12 +5752,9 @@
       <c r="D6" s="85"/>
       <c r="E6" s="85"/>
       <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
-    </row>
-    <row r="7" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="86"/>
+    </row>
+    <row r="7" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>2003</v>
       </c>
@@ -5626,12 +5763,9 @@
       <c r="D7" s="85"/>
       <c r="E7" s="85"/>
       <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="86"/>
-    </row>
-    <row r="8" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="86"/>
+    </row>
+    <row r="8" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>2004</v>
       </c>
@@ -5640,12 +5774,9 @@
       <c r="D8" s="85"/>
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="86"/>
-    </row>
-    <row r="9" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="86"/>
+    </row>
+    <row r="9" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>2005</v>
       </c>
@@ -5654,12 +5785,9 @@
       <c r="D9" s="85"/>
       <c r="E9" s="85"/>
       <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="86"/>
-    </row>
-    <row r="10" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="86"/>
+    </row>
+    <row r="10" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>2006</v>
       </c>
@@ -5668,12 +5796,9 @@
       <c r="D10" s="85"/>
       <c r="E10" s="85"/>
       <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="86"/>
-    </row>
-    <row r="11" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="86"/>
+    </row>
+    <row r="11" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>2007</v>
       </c>
@@ -5682,12 +5807,9 @@
       <c r="D11" s="85"/>
       <c r="E11" s="85"/>
       <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="86"/>
-    </row>
-    <row r="12" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="86"/>
+    </row>
+    <row r="12" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>2008</v>
       </c>
@@ -5696,12 +5818,9 @@
       <c r="D12" s="85"/>
       <c r="E12" s="85"/>
       <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="86"/>
-    </row>
-    <row r="13" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="86"/>
+    </row>
+    <row r="13" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>2009</v>
       </c>
@@ -5710,12 +5829,9 @@
       <c r="D13" s="85"/>
       <c r="E13" s="85"/>
       <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="86"/>
-    </row>
-    <row r="14" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="86"/>
+    </row>
+    <row r="14" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>2010</v>
       </c>
@@ -5724,12 +5840,9 @@
       <c r="D14" s="85"/>
       <c r="E14" s="85"/>
       <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="86"/>
-    </row>
-    <row r="15" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="86"/>
+    </row>
+    <row r="15" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>2011</v>
       </c>
@@ -5738,12 +5851,9 @@
       <c r="D15" s="85"/>
       <c r="E15" s="85"/>
       <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="85"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="86"/>
-    </row>
-    <row r="16" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="86"/>
+    </row>
+    <row r="16" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>2012</v>
       </c>
@@ -5752,12 +5862,9 @@
       <c r="D16" s="85"/>
       <c r="E16" s="85"/>
       <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="86"/>
-    </row>
-    <row r="17" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="86"/>
+    </row>
+    <row r="17" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>2013</v>
       </c>
@@ -5766,12 +5873,9 @@
       <c r="D17" s="85"/>
       <c r="E17" s="85"/>
       <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="86"/>
-    </row>
-    <row r="18" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="86"/>
+    </row>
+    <row r="18" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
         <v>2014</v>
       </c>
@@ -5780,12 +5884,9 @@
       <c r="D18" s="85"/>
       <c r="E18" s="85"/>
       <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="86"/>
-    </row>
-    <row r="19" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="86"/>
+    </row>
+    <row r="19" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
         <v>2015</v>
       </c>
@@ -5793,31 +5894,22 @@
         <v>0.5</v>
       </c>
       <c r="C19" s="85">
+        <v>5</v>
+      </c>
+      <c r="D19" s="85">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="85">
         <v>2</v>
       </c>
-      <c r="D19" s="85">
-        <v>5</v>
-      </c>
-      <c r="E19" s="85">
-        <v>0.25</v>
-      </c>
       <c r="F19" s="85">
-        <v>2</v>
-      </c>
-      <c r="G19" s="85">
-        <v>2</v>
-      </c>
-      <c r="H19" s="85">
         <v>0.125</v>
       </c>
-      <c r="I19" s="85">
+      <c r="G19" s="86">
         <v>0.125</v>
       </c>
-      <c r="J19" s="86">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>2016</v>
       </c>
@@ -5826,12 +5918,9 @@
       <c r="D20" s="85"/>
       <c r="E20" s="85"/>
       <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="86"/>
-    </row>
-    <row r="21" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="86"/>
+    </row>
+    <row r="21" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
         <v>2017</v>
       </c>
@@ -5840,12 +5929,9 @@
       <c r="D21" s="85"/>
       <c r="E21" s="85"/>
       <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="86"/>
-    </row>
-    <row r="22" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="86"/>
+    </row>
+    <row r="22" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>2018</v>
       </c>
@@ -5854,12 +5940,9 @@
       <c r="D22" s="85"/>
       <c r="E22" s="85"/>
       <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="86"/>
-    </row>
-    <row r="23" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="86"/>
+    </row>
+    <row r="23" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>2019</v>
       </c>
@@ -5868,12 +5951,9 @@
       <c r="D23" s="85"/>
       <c r="E23" s="85"/>
       <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="86"/>
-    </row>
-    <row r="24" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="86"/>
+    </row>
+    <row r="24" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="72">
         <v>2020</v>
       </c>
@@ -5882,10 +5962,7 @@
       <c r="D24" s="88"/>
       <c r="E24" s="88"/>
       <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="89"/>
+      <c r="G24" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Restructured data tab of data_sti.xlsx
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -216,7 +216,7 @@
     <author>Michael Traeger</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="1" shapeId="0">
+    <comment ref="K1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -317,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -442,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -468,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -497,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -523,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -595,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -619,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -643,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="1" shapeId="0">
+    <comment ref="H11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -671,7 +671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U11" authorId="1" shapeId="0">
+    <comment ref="AB11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -719,7 +719,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0">
+    <comment ref="P12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1399,7 +1399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
   <si>
     <t>Waiting list</t>
   </si>
@@ -1467,18 +1467,9 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Total PLHIV</t>
-  </si>
-  <si>
-    <t>New diagnoses</t>
-  </si>
-  <si>
     <t>eff_condom</t>
   </si>
   <si>
-    <t>Total MSM</t>
-  </si>
-  <si>
     <t>prop_prep_base</t>
   </si>
   <si>
@@ -1587,15 +1578,6 @@
     <t>Total Gon cases HIV+</t>
   </si>
   <si>
-    <t>Prop HIV diagnosed</t>
-  </si>
-  <si>
-    <t>Prop HIV on treatment</t>
-  </si>
-  <si>
-    <t>Prop HIV virally suppressed</t>
-  </si>
-  <si>
     <t>Gon prev: HIV- all</t>
   </si>
   <si>
@@ -1714,6 +1696,42 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>PLHIV_int</t>
+  </si>
+  <si>
+    <t>PLHIV_tot</t>
+  </si>
+  <si>
+    <t>HIV_diag_tot</t>
+  </si>
+  <si>
+    <t>HIV_diag_aus</t>
+  </si>
+  <si>
+    <t>HIV_diag_int</t>
+  </si>
+  <si>
+    <t>PLHIV_aus</t>
+  </si>
+  <si>
+    <t>pop_tot</t>
+  </si>
+  <si>
+    <t>pop_aus</t>
+  </si>
+  <si>
+    <t>pop_int</t>
+  </si>
+  <si>
+    <t>prop_HIV_diagnosed</t>
+  </si>
+  <si>
+    <t>prop_HIV_treated</t>
+  </si>
+  <si>
+    <t>prop_HIV_virally_suppressed</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2225,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2383,6 +2401,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -2747,10 +2774,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2771,12 +2798,12 @@
       </c>
       <c r="L2" s="59"/>
       <c r="M2" s="52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>13</v>
@@ -2794,7 +2821,7 @@
       </c>
       <c r="L3" s="61"/>
       <c r="M3" s="52" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2818,7 +2845,7 @@
       </c>
       <c r="L4" s="57"/>
       <c r="M4" s="52" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2842,7 +2869,7 @@
       </c>
       <c r="L5" s="27"/>
       <c r="M5" s="52" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2873,7 +2900,7 @@
       </c>
       <c r="L6" s="67"/>
       <c r="M6" s="52" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2898,11 +2925,11 @@
         <v>6</v>
       </c>
       <c r="I7" s="46">
-        <f>((data!G12/data!G2) ^ (C2/((data!A12-data!A2))) - 1)</f>
+        <f>((data!K12/data!K2) ^ (C2/((data!A12-data!A2))) - 1)</f>
         <v>4.0741237836483535E-3</v>
       </c>
       <c r="J7" s="52">
-        <f>(data!G7-data!G2)/(data!A7-data!A2)/data!G2*C2</f>
+        <f>(data!K7-data!K2)/(data!A7-data!A2)/data!K2*C2</f>
         <v>4.6046927083333387E-3</v>
       </c>
     </row>
@@ -2927,10 +2954,10 @@
     </row>
     <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C9" s="28">
         <v>0.4</v>
@@ -2946,10 +2973,10 @@
     </row>
     <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C10" s="28">
         <v>0.4</v>
@@ -2965,10 +2992,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="66">
         <v>0</v>
@@ -2978,10 +3005,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="62">
         <f>6.2</f>
@@ -2998,10 +3025,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="28">
         <v>7</v>
@@ -3017,10 +3044,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="54">
         <v>0.1</v>
@@ -3036,10 +3063,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="54">
         <v>0.17</v>
@@ -3055,10 +3082,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="63">
         <v>0.38800000000000001</v>
@@ -3074,10 +3101,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="64">
         <v>0.45</v>
@@ -3093,10 +3120,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" s="31">
         <v>1</v>
@@ -3112,10 +3139,10 @@
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C19" s="60">
         <f>1-C17</f>
@@ -3132,10 +3159,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C20" s="58">
         <v>0.5</v>
@@ -3151,10 +3178,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C21" s="53">
         <v>2007</v>
@@ -3162,10 +3189,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C22" s="53">
         <v>42714</v>
@@ -3183,904 +3210,1092 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:AC24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <selection pane="topRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11" style="52" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.28515625" style="52" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>22</v>
+      <c r="B1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="119"/>
+      <c r="O1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="U1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="15"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB1" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="15"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>2007</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="35">
-        <f>G2*7.2/100</f>
+      <c r="C2" s="11"/>
+      <c r="E2" s="35">
+        <f>K2*7.2/100</f>
         <v>3075.4079999999999</v>
       </c>
-      <c r="D2" s="12">
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="12">
         <v>0.7</v>
       </c>
-      <c r="E2" s="12">
+      <c r="I2" s="12">
         <v>0.75</v>
       </c>
-      <c r="F2" s="12">
+      <c r="J2" s="12">
         <v>0.8</v>
       </c>
-      <c r="G2" s="33">
+      <c r="K2" s="33">
         <f>42714</f>
         <v>42714</v>
       </c>
-      <c r="H2" s="48">
+      <c r="L2" s="35">
+        <f>K2-M2</f>
+        <v>41714</v>
+      </c>
+      <c r="M2" s="33">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="120"/>
+      <c r="O2" s="48">
         <v>2.32876712328767E-2</v>
       </c>
-      <c r="I2" s="48">
+      <c r="P2" s="48">
         <v>3.4931506849315071E-2</v>
       </c>
-      <c r="J2" s="35">
-        <f>G2-K2</f>
+      <c r="Q2" s="35">
+        <f>K2-R2</f>
         <v>39638.591999999997</v>
       </c>
-      <c r="K2" s="35">
-        <f>C2</f>
+      <c r="R2" s="35">
+        <f>E2</f>
         <v>3075.4079999999999</v>
       </c>
-      <c r="L2" s="40">
-        <f>ROUND(H2*J2,0)</f>
+      <c r="S2" s="40">
+        <f>ROUND(O2*Q2,0)</f>
         <v>923</v>
       </c>
-      <c r="M2" s="40">
-        <f t="shared" ref="M2" si="0">ROUND(I2*K2,0)</f>
+      <c r="T2" s="40">
+        <f t="shared" ref="T2" si="0">ROUND(P2*R2,0)</f>
         <v>107</v>
       </c>
-      <c r="N2" s="12">
+      <c r="U2" s="12">
         <v>1007</v>
       </c>
-      <c r="O2" s="44">
+      <c r="V2" s="44">
         <v>0.81</v>
       </c>
-      <c r="P2" s="44">
+      <c r="W2" s="44">
         <v>0.82</v>
       </c>
-      <c r="Q2" s="45">
-        <f>N2*O2*P2</f>
+      <c r="X2" s="45">
+        <f>U2*V2*W2</f>
         <v>668.84940000000006</v>
       </c>
-      <c r="R2" s="41">
+      <c r="Y2" s="41">
         <v>0.17</v>
       </c>
-      <c r="S2" s="43">
-        <f>Q2-T2</f>
+      <c r="Z2" s="43">
+        <f>X2-AA2</f>
         <v>555.14500200000009</v>
       </c>
-      <c r="T2" s="43">
-        <f>Q2*R2</f>
+      <c r="AA2" s="43">
+        <f>X2*Y2</f>
         <v>113.70439800000001</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2008</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" s="35">
-        <f t="shared" ref="C3:C12" si="1">G3*7.2/100</f>
+      <c r="C3" s="11"/>
+      <c r="E3" s="35">
+        <f t="shared" ref="E3:E12" si="1">K3*7.2/100</f>
         <v>3229.1784000000002</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="35">
-        <f>1.05*G2</f>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="35">
+        <f>1.05*K2</f>
         <v>44849.700000000004</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="35">
-        <f>G3-K3</f>
+      <c r="L3" s="35">
+        <f t="shared" ref="L3:L13" si="2">K3-M3</f>
+        <v>43599.700000000004</v>
+      </c>
+      <c r="M3" s="35">
+        <f>M2*1.25</f>
+        <v>1250</v>
+      </c>
+      <c r="N3" s="121"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="35">
+        <f>K3-R3</f>
         <v>41620.521600000007</v>
       </c>
-      <c r="K3" s="35">
-        <f>C3</f>
+      <c r="R3" s="35">
+        <f>E3</f>
         <v>3229.1784000000002</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="12">
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="12">
         <v>922</v>
       </c>
-      <c r="O3" s="44">
+      <c r="V3" s="44">
         <v>0.81</v>
       </c>
-      <c r="P3" s="44">
+      <c r="W3" s="44">
         <v>0.82</v>
       </c>
-      <c r="Q3" s="45">
-        <f t="shared" ref="Q3:Q12" si="2">N3*O3*P3</f>
+      <c r="X3" s="45">
+        <f t="shared" ref="X3:X12" si="3">U3*V3*W3</f>
         <v>612.39239999999995</v>
       </c>
-      <c r="R3" s="41">
+      <c r="Y3" s="41">
         <v>0.17</v>
       </c>
-      <c r="S3" s="43">
-        <f t="shared" ref="S3:S12" si="3">Q3-T3</f>
+      <c r="Z3" s="43">
+        <f t="shared" ref="Z3:Z12" si="4">X3-AA3</f>
         <v>508.28569199999993</v>
       </c>
-      <c r="T3" s="43">
-        <f t="shared" ref="T3:T12" si="4">Q3*R3</f>
+      <c r="AA3" s="43">
+        <f t="shared" ref="AA3:AA12" si="5">X3*Y3</f>
         <v>104.106708</v>
       </c>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2009</v>
       </c>
       <c r="B4" s="13"/>
-      <c r="C4" s="35">
+      <c r="C4" s="11"/>
+      <c r="E4" s="35">
         <f t="shared" si="1"/>
         <v>3390.6373200000003</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="35">
-        <f t="shared" ref="G4:G11" si="5">1.05*G3</f>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="35">
+        <f t="shared" ref="K4:K11" si="6">1.05*K3</f>
         <v>47092.185000000005</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="35">
-        <f>G4-K4</f>
+      <c r="L4" s="35">
+        <f t="shared" si="2"/>
+        <v>45529.685000000005</v>
+      </c>
+      <c r="M4" s="35">
+        <f t="shared" ref="M4:M12" si="7">M3*1.25</f>
+        <v>1562.5</v>
+      </c>
+      <c r="N4" s="121"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="35">
+        <f>K4-R4</f>
         <v>43701.547680000003</v>
       </c>
-      <c r="K4" s="35">
-        <f>C4</f>
+      <c r="R4" s="35">
+        <f>E4</f>
         <v>3390.6373200000003</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="12">
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="12">
         <v>1480</v>
       </c>
-      <c r="O4" s="44">
+      <c r="V4" s="44">
         <v>0.81</v>
       </c>
-      <c r="P4" s="44">
+      <c r="W4" s="44">
         <v>0.82</v>
       </c>
-      <c r="Q4" s="45">
-        <f t="shared" si="2"/>
+      <c r="X4" s="45">
+        <f t="shared" si="3"/>
         <v>983.01600000000008</v>
       </c>
-      <c r="R4" s="41">
+      <c r="Y4" s="41">
         <v>0.17</v>
       </c>
-      <c r="S4" s="43">
-        <f t="shared" si="3"/>
+      <c r="Z4" s="43">
+        <f t="shared" si="4"/>
         <v>815.90328</v>
       </c>
-      <c r="T4" s="43">
-        <f t="shared" si="4"/>
+      <c r="AA4" s="43">
+        <f t="shared" si="5"/>
         <v>167.11272000000002</v>
       </c>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2010</v>
       </c>
       <c r="B5" s="12">
         <v>178</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="11"/>
+      <c r="E5" s="35">
         <f t="shared" si="1"/>
         <v>3560.1691860000005</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
         <v>0.75</v>
       </c>
-      <c r="F5" s="12">
+      <c r="J5" s="12">
         <v>0.8</v>
       </c>
-      <c r="G5" s="35">
+      <c r="K5" s="35">
+        <f t="shared" si="6"/>
+        <v>49446.794250000006</v>
+      </c>
+      <c r="L5" s="35">
+        <f t="shared" si="2"/>
+        <v>47493.669250000006</v>
+      </c>
+      <c r="M5" s="35">
+        <f t="shared" si="7"/>
+        <v>1953.125</v>
+      </c>
+      <c r="N5" s="121"/>
+      <c r="O5" s="48">
+        <v>4.0273972602739724E-2</v>
+      </c>
+      <c r="P5" s="48">
+        <v>4.3150684931506846E-2</v>
+      </c>
+      <c r="Q5" s="35">
+        <f>K5-R5</f>
+        <v>45886.625064000007</v>
+      </c>
+      <c r="R5" s="35">
+        <f>E5</f>
+        <v>3560.1691860000005</v>
+      </c>
+      <c r="S5" s="39">
+        <f t="shared" ref="S5:S11" si="8">ROUND(O5*Q5,0)</f>
+        <v>1848</v>
+      </c>
+      <c r="T5" s="39">
+        <f t="shared" ref="T5:T12" si="9">ROUND(P5*R5,0)</f>
+        <v>154</v>
+      </c>
+      <c r="U5" s="12">
+        <v>1758</v>
+      </c>
+      <c r="V5" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W5" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X5" s="45">
+        <f t="shared" si="3"/>
+        <v>1167.6635999999999</v>
+      </c>
+      <c r="Y5" s="41">
+        <v>0.17</v>
+      </c>
+      <c r="Z5" s="43">
+        <f t="shared" si="4"/>
+        <v>969.16078799999991</v>
+      </c>
+      <c r="AA5" s="43">
         <f t="shared" si="5"/>
-        <v>49446.794250000006</v>
-      </c>
-      <c r="H5" s="48">
-        <v>4.0273972602739724E-2</v>
-      </c>
-      <c r="I5" s="48">
-        <v>4.3150684931506846E-2</v>
-      </c>
-      <c r="J5" s="35">
-        <f>G5-K5</f>
-        <v>45886.625064000007</v>
-      </c>
-      <c r="K5" s="35">
-        <f>C5</f>
-        <v>3560.1691860000005</v>
-      </c>
-      <c r="L5" s="39">
-        <f t="shared" ref="L5:L11" si="6">ROUND(H5*J5,0)</f>
-        <v>1848</v>
-      </c>
-      <c r="M5" s="39">
-        <f t="shared" ref="M5:M12" si="7">ROUND(I5*K5,0)</f>
-        <v>154</v>
-      </c>
-      <c r="N5" s="12">
-        <v>1758</v>
-      </c>
-      <c r="O5" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P5" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q5" s="45">
-        <f t="shared" si="2"/>
-        <v>1167.6635999999999</v>
-      </c>
-      <c r="R5" s="41">
-        <v>0.17</v>
-      </c>
-      <c r="S5" s="43">
-        <f t="shared" si="3"/>
-        <v>969.16078799999991</v>
-      </c>
-      <c r="T5" s="43">
-        <f t="shared" si="4"/>
         <v>198.50281199999998</v>
       </c>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>2011</v>
       </c>
       <c r="B6" s="12">
         <v>218</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="11"/>
+      <c r="E6" s="35">
         <f t="shared" si="1"/>
         <v>3738.1776453000011</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="35">
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="35">
+        <f t="shared" si="6"/>
+        <v>51919.133962500011</v>
+      </c>
+      <c r="L6" s="35">
+        <f t="shared" si="2"/>
+        <v>49477.727712500011</v>
+      </c>
+      <c r="M6" s="35">
+        <f t="shared" si="7"/>
+        <v>2441.40625</v>
+      </c>
+      <c r="N6" s="121"/>
+      <c r="O6" s="48">
+        <v>3.7534246575342468E-2</v>
+      </c>
+      <c r="P6" s="48">
+        <v>4.726027397260274E-2</v>
+      </c>
+      <c r="Q6" s="35">
+        <f>K6-R6</f>
+        <v>48180.956317200013</v>
+      </c>
+      <c r="R6" s="35">
+        <f>E6</f>
+        <v>3738.1776453000011</v>
+      </c>
+      <c r="S6" s="39">
+        <f t="shared" si="8"/>
+        <v>1808</v>
+      </c>
+      <c r="T6" s="39">
+        <f t="shared" si="9"/>
+        <v>177</v>
+      </c>
+      <c r="U6" s="12">
+        <v>1863</v>
+      </c>
+      <c r="V6" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W6" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X6" s="45">
+        <f t="shared" si="3"/>
+        <v>1237.4046000000001</v>
+      </c>
+      <c r="Y6" s="41">
+        <v>0.17</v>
+      </c>
+      <c r="Z6" s="43">
+        <f t="shared" si="4"/>
+        <v>1027.0458180000001</v>
+      </c>
+      <c r="AA6" s="43">
         <f t="shared" si="5"/>
-        <v>51919.133962500011</v>
-      </c>
-      <c r="H6" s="48">
-        <v>3.7534246575342468E-2</v>
-      </c>
-      <c r="I6" s="48">
-        <v>4.726027397260274E-2</v>
-      </c>
-      <c r="J6" s="35">
-        <f>G6-K6</f>
-        <v>48180.956317200013</v>
-      </c>
-      <c r="K6" s="35">
-        <f>C6</f>
-        <v>3738.1776453000011</v>
-      </c>
-      <c r="L6" s="39">
-        <f t="shared" si="6"/>
-        <v>1808</v>
-      </c>
-      <c r="M6" s="39">
-        <f t="shared" si="7"/>
-        <v>177</v>
-      </c>
-      <c r="N6" s="12">
-        <v>1863</v>
-      </c>
-      <c r="O6" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P6" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q6" s="45">
-        <f t="shared" si="2"/>
-        <v>1237.4046000000001</v>
-      </c>
-      <c r="R6" s="41">
-        <v>0.17</v>
-      </c>
-      <c r="S6" s="43">
-        <f t="shared" si="3"/>
-        <v>1027.0458180000001</v>
-      </c>
-      <c r="T6" s="43">
-        <f t="shared" si="4"/>
         <v>210.35878200000002</v>
       </c>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>2012</v>
       </c>
       <c r="B7" s="12">
         <v>200</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="11"/>
+      <c r="E7" s="35">
         <f t="shared" si="1"/>
         <v>3925.0865275650012</v>
       </c>
-      <c r="D7" s="12">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="12">
         <v>0.91200000000000003</v>
       </c>
-      <c r="E7" s="12">
+      <c r="I7" s="12">
         <v>0.82</v>
       </c>
-      <c r="F7" s="12">
+      <c r="J7" s="12">
         <v>0.88</v>
       </c>
-      <c r="G7" s="35">
+      <c r="K7" s="35">
+        <f t="shared" si="6"/>
+        <v>54515.090660625014</v>
+      </c>
+      <c r="L7" s="35">
+        <f t="shared" si="2"/>
+        <v>51463.332848125014</v>
+      </c>
+      <c r="M7" s="35">
+        <f t="shared" si="7"/>
+        <v>3051.7578125</v>
+      </c>
+      <c r="N7" s="121"/>
+      <c r="O7" s="48">
+        <v>4.876712328767123E-2</v>
+      </c>
+      <c r="P7" s="48">
+        <v>5.3835616438356167E-2</v>
+      </c>
+      <c r="Q7" s="35">
+        <f>K7-R7</f>
+        <v>50590.004133060014</v>
+      </c>
+      <c r="R7" s="35">
+        <f>E7</f>
+        <v>3925.0865275650012</v>
+      </c>
+      <c r="S7" s="39">
+        <f t="shared" si="8"/>
+        <v>2467</v>
+      </c>
+      <c r="T7" s="39">
+        <f t="shared" si="9"/>
+        <v>211</v>
+      </c>
+      <c r="U7" s="12">
+        <v>2436</v>
+      </c>
+      <c r="V7" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W7" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X7" s="45">
+        <f t="shared" si="3"/>
+        <v>1617.9911999999999</v>
+      </c>
+      <c r="Y7" s="41">
+        <v>0.17</v>
+      </c>
+      <c r="Z7" s="43">
+        <f t="shared" si="4"/>
+        <v>1342.9326959999999</v>
+      </c>
+      <c r="AA7" s="43">
         <f t="shared" si="5"/>
-        <v>54515.090660625014</v>
-      </c>
-      <c r="H7" s="48">
-        <v>4.876712328767123E-2</v>
-      </c>
-      <c r="I7" s="48">
-        <v>5.3835616438356167E-2</v>
-      </c>
-      <c r="J7" s="35">
-        <f>G7-K7</f>
-        <v>50590.004133060014</v>
-      </c>
-      <c r="K7" s="35">
-        <f>C7</f>
-        <v>3925.0865275650012</v>
-      </c>
-      <c r="L7" s="39">
-        <f t="shared" si="6"/>
-        <v>2467</v>
-      </c>
-      <c r="M7" s="39">
-        <f t="shared" si="7"/>
-        <v>211</v>
-      </c>
-      <c r="N7" s="12">
-        <v>2436</v>
-      </c>
-      <c r="O7" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P7" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q7" s="45">
-        <f t="shared" si="2"/>
-        <v>1617.9911999999999</v>
-      </c>
-      <c r="R7" s="41">
-        <v>0.17</v>
-      </c>
-      <c r="S7" s="43">
-        <f t="shared" si="3"/>
-        <v>1342.9326959999999</v>
-      </c>
-      <c r="T7" s="43">
-        <f t="shared" si="4"/>
         <v>275.05850400000003</v>
       </c>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>2013</v>
       </c>
       <c r="B8" s="12">
         <v>218</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="11"/>
+      <c r="E8" s="35">
         <f t="shared" si="1"/>
         <v>4121.3408539432512</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="34">
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="34">
         <v>0.86</v>
       </c>
-      <c r="F8" s="12">
+      <c r="J8" s="12">
         <v>0.9</v>
       </c>
-      <c r="G8" s="35">
+      <c r="K8" s="35">
+        <f t="shared" si="6"/>
+        <v>57240.845193656263</v>
+      </c>
+      <c r="L8" s="35">
+        <f t="shared" si="2"/>
+        <v>53426.147928031263</v>
+      </c>
+      <c r="M8" s="35">
+        <f t="shared" si="7"/>
+        <v>3814.697265625</v>
+      </c>
+      <c r="N8" s="121"/>
+      <c r="O8" s="48">
+        <v>5.2876712328767124E-2</v>
+      </c>
+      <c r="P8" s="48">
+        <v>6.2671232876712321E-2</v>
+      </c>
+      <c r="Q8" s="35">
+        <f>K8-R8</f>
+        <v>53119.504339713014</v>
+      </c>
+      <c r="R8" s="35">
+        <f>E8</f>
+        <v>4121.3408539432512</v>
+      </c>
+      <c r="S8" s="39">
+        <f t="shared" si="8"/>
+        <v>2809</v>
+      </c>
+      <c r="T8" s="39">
+        <f t="shared" si="9"/>
+        <v>258</v>
+      </c>
+      <c r="U8" s="12">
+        <v>2978</v>
+      </c>
+      <c r="V8" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W8" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X8" s="45">
+        <f t="shared" si="3"/>
+        <v>1977.9876000000002</v>
+      </c>
+      <c r="Y8" s="41">
+        <v>0.17</v>
+      </c>
+      <c r="Z8" s="43">
+        <f t="shared" si="4"/>
+        <v>1641.7297080000001</v>
+      </c>
+      <c r="AA8" s="43">
         <f t="shared" si="5"/>
-        <v>57240.845193656263</v>
-      </c>
-      <c r="H8" s="48">
-        <v>5.2876712328767124E-2</v>
-      </c>
-      <c r="I8" s="48">
-        <v>6.2671232876712321E-2</v>
-      </c>
-      <c r="J8" s="35">
-        <f>G8-K8</f>
-        <v>53119.504339713014</v>
-      </c>
-      <c r="K8" s="35">
-        <f>C8</f>
-        <v>4121.3408539432512</v>
-      </c>
-      <c r="L8" s="39">
-        <f t="shared" si="6"/>
-        <v>2809</v>
-      </c>
-      <c r="M8" s="39">
-        <f t="shared" si="7"/>
-        <v>258</v>
-      </c>
-      <c r="N8" s="12">
-        <v>2978</v>
-      </c>
-      <c r="O8" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P8" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q8" s="45">
-        <f t="shared" si="2"/>
-        <v>1977.9876000000002</v>
-      </c>
-      <c r="R8" s="41">
-        <v>0.17</v>
-      </c>
-      <c r="S8" s="43">
-        <f t="shared" si="3"/>
-        <v>1641.7297080000001</v>
-      </c>
-      <c r="T8" s="43">
-        <f t="shared" si="4"/>
         <v>336.25789200000003</v>
       </c>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>2014</v>
       </c>
       <c r="B9" s="12">
         <v>219</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="11"/>
+      <c r="E9" s="35">
         <f t="shared" si="1"/>
         <v>4327.407896640414</v>
       </c>
-      <c r="D9" s="12">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="12">
         <v>0.88</v>
       </c>
-      <c r="E9" s="34">
+      <c r="I9" s="34">
         <v>0.89</v>
       </c>
-      <c r="F9" s="34">
+      <c r="J9" s="34">
         <v>0.9</v>
       </c>
-      <c r="G9" s="35">
+      <c r="K9" s="35">
+        <f t="shared" si="6"/>
+        <v>60102.887453339077</v>
+      </c>
+      <c r="L9" s="35">
+        <f t="shared" si="2"/>
+        <v>55334.515871307827</v>
+      </c>
+      <c r="M9" s="35">
+        <f t="shared" si="7"/>
+        <v>4768.37158203125</v>
+      </c>
+      <c r="N9" s="121"/>
+      <c r="O9" s="48">
+        <v>5.1506849315068493E-2</v>
+      </c>
+      <c r="P9" s="48">
+        <v>5.321917808219178E-2</v>
+      </c>
+      <c r="Q9" s="35">
+        <f>K9-R9</f>
+        <v>55775.479556698665</v>
+      </c>
+      <c r="R9" s="35">
+        <f>E9</f>
+        <v>4327.407896640414</v>
+      </c>
+      <c r="S9" s="39">
+        <f t="shared" si="8"/>
+        <v>2873</v>
+      </c>
+      <c r="T9" s="39">
+        <f t="shared" si="9"/>
+        <v>230</v>
+      </c>
+      <c r="U9" s="12">
+        <v>3269</v>
+      </c>
+      <c r="V9" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W9" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X9" s="45">
+        <f t="shared" si="3"/>
+        <v>2171.2698</v>
+      </c>
+      <c r="Y9" s="41">
+        <v>0.17</v>
+      </c>
+      <c r="Z9" s="43">
+        <f t="shared" si="4"/>
+        <v>1802.1539339999999</v>
+      </c>
+      <c r="AA9" s="43">
         <f t="shared" si="5"/>
-        <v>60102.887453339077</v>
-      </c>
-      <c r="H9" s="48">
-        <v>5.1506849315068493E-2</v>
-      </c>
-      <c r="I9" s="48">
-        <v>5.321917808219178E-2</v>
-      </c>
-      <c r="J9" s="35">
-        <f>G9-K9</f>
-        <v>55775.479556698665</v>
-      </c>
-      <c r="K9" s="35">
-        <f>C9</f>
-        <v>4327.407896640414</v>
-      </c>
-      <c r="L9" s="39">
-        <f t="shared" si="6"/>
-        <v>2873</v>
-      </c>
-      <c r="M9" s="39">
-        <f t="shared" si="7"/>
-        <v>230</v>
-      </c>
-      <c r="N9" s="12">
-        <v>3269</v>
-      </c>
-      <c r="O9" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P9" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q9" s="45">
-        <f t="shared" si="2"/>
-        <v>2171.2698</v>
-      </c>
-      <c r="R9" s="41">
-        <v>0.17</v>
-      </c>
-      <c r="S9" s="43">
-        <f t="shared" si="3"/>
-        <v>1802.1539339999999</v>
-      </c>
-      <c r="T9" s="43">
-        <f t="shared" si="4"/>
         <v>369.11586600000004</v>
       </c>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>2015</v>
       </c>
       <c r="B10" s="12">
         <v>206</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="11"/>
+      <c r="E10" s="35">
         <f t="shared" si="1"/>
         <v>4543.7782914724339</v>
       </c>
-      <c r="D10" s="12">
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="12">
         <v>0.88</v>
       </c>
-      <c r="E10" s="12">
+      <c r="I10" s="12">
         <v>0.92</v>
       </c>
-      <c r="F10" s="12">
+      <c r="J10" s="12">
         <v>0.92</v>
       </c>
-      <c r="G10" s="35">
+      <c r="K10" s="35">
+        <f t="shared" si="6"/>
+        <v>63108.03182600603</v>
+      </c>
+      <c r="L10" s="35">
+        <f t="shared" si="2"/>
+        <v>57147.567348466968</v>
+      </c>
+      <c r="M10" s="35">
+        <f t="shared" si="7"/>
+        <v>5960.4644775390625</v>
+      </c>
+      <c r="N10" s="121"/>
+      <c r="O10" s="48">
+        <v>6.6575342465753418E-2</v>
+      </c>
+      <c r="P10" s="48">
+        <v>6.7191780821917804E-2</v>
+      </c>
+      <c r="Q10" s="35">
+        <f>K10-R10</f>
+        <v>58564.253534533593</v>
+      </c>
+      <c r="R10" s="35">
+        <f>E10</f>
+        <v>4543.7782914724339</v>
+      </c>
+      <c r="S10" s="39">
+        <f t="shared" si="8"/>
+        <v>3899</v>
+      </c>
+      <c r="T10" s="39">
+        <f t="shared" si="9"/>
+        <v>305</v>
+      </c>
+      <c r="U10" s="12">
+        <v>4865</v>
+      </c>
+      <c r="V10" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W10" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X10" s="45">
+        <f t="shared" si="3"/>
+        <v>3231.3330000000001</v>
+      </c>
+      <c r="Y10" s="42">
+        <v>0.17</v>
+      </c>
+      <c r="Z10" s="43">
+        <f t="shared" si="4"/>
+        <v>2682.00639</v>
+      </c>
+      <c r="AA10" s="43">
         <f t="shared" si="5"/>
-        <v>63108.03182600603</v>
-      </c>
-      <c r="H10" s="48">
-        <v>6.6575342465753418E-2</v>
-      </c>
-      <c r="I10" s="48">
-        <v>6.7191780821917804E-2</v>
-      </c>
-      <c r="J10" s="35">
-        <f>G10-K10</f>
-        <v>58564.253534533593</v>
-      </c>
-      <c r="K10" s="35">
-        <f>C10</f>
-        <v>4543.7782914724339</v>
-      </c>
-      <c r="L10" s="39">
-        <f t="shared" si="6"/>
-        <v>3899</v>
-      </c>
-      <c r="M10" s="39">
-        <f t="shared" si="7"/>
-        <v>305</v>
-      </c>
-      <c r="N10" s="12">
-        <v>4865</v>
-      </c>
-      <c r="O10" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P10" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q10" s="45">
-        <f t="shared" si="2"/>
-        <v>3231.3330000000001</v>
-      </c>
-      <c r="R10" s="42">
-        <v>0.17</v>
-      </c>
-      <c r="S10" s="43">
-        <f t="shared" si="3"/>
-        <v>2682.00639</v>
-      </c>
-      <c r="T10" s="43">
-        <f t="shared" si="4"/>
         <v>549.32661000000007</v>
       </c>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>2016</v>
       </c>
       <c r="B11" s="12">
         <v>233</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="11"/>
+      <c r="E11" s="35">
         <f t="shared" si="1"/>
         <v>4770.9672060460571</v>
       </c>
-      <c r="D11" s="12">
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="12">
         <v>0.89</v>
       </c>
-      <c r="E11" s="12">
+      <c r="I11" s="12">
         <v>0.95</v>
       </c>
-      <c r="F11" s="12">
+      <c r="J11" s="12">
         <v>0.94</v>
       </c>
-      <c r="G11" s="35">
+      <c r="K11" s="35">
+        <f t="shared" si="6"/>
+        <v>66263.43341730634</v>
+      </c>
+      <c r="L11" s="35">
+        <f t="shared" si="2"/>
+        <v>58812.852820382512</v>
+      </c>
+      <c r="M11" s="35">
+        <f t="shared" si="7"/>
+        <v>7450.5805969238281</v>
+      </c>
+      <c r="N11" s="121"/>
+      <c r="O11" s="48">
+        <v>6.3287671232876708E-2</v>
+      </c>
+      <c r="P11" s="48">
+        <v>6.9246575342465755E-2</v>
+      </c>
+      <c r="Q11" s="35">
+        <f>K11-R11</f>
+        <v>61492.466211260282</v>
+      </c>
+      <c r="R11" s="35">
+        <f>E11</f>
+        <v>4770.9672060460571</v>
+      </c>
+      <c r="S11" s="39">
+        <f t="shared" si="8"/>
+        <v>3892</v>
+      </c>
+      <c r="T11" s="39">
+        <f t="shared" si="9"/>
+        <v>330</v>
+      </c>
+      <c r="U11" s="12">
+        <v>6265</v>
+      </c>
+      <c r="V11" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="W11" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="X11" s="45">
+        <f t="shared" si="3"/>
+        <v>4161.2130000000006</v>
+      </c>
+      <c r="Y11" s="42">
+        <v>0.13</v>
+      </c>
+      <c r="Z11" s="43">
+        <f t="shared" si="4"/>
+        <v>3620.2553100000005</v>
+      </c>
+      <c r="AA11" s="43">
         <f t="shared" si="5"/>
-        <v>66263.43341730634</v>
-      </c>
-      <c r="H11" s="48">
-        <v>6.3287671232876708E-2</v>
-      </c>
-      <c r="I11" s="48">
-        <v>6.9246575342465755E-2</v>
-      </c>
-      <c r="J11" s="35">
-        <f>G11-K11</f>
-        <v>61492.466211260282</v>
-      </c>
-      <c r="K11" s="35">
-        <f>C11</f>
-        <v>4770.9672060460571</v>
-      </c>
-      <c r="L11" s="39">
-        <f t="shared" si="6"/>
-        <v>3892</v>
-      </c>
-      <c r="M11" s="39">
-        <f t="shared" si="7"/>
-        <v>330</v>
-      </c>
-      <c r="N11" s="12">
-        <v>6265</v>
-      </c>
-      <c r="O11" s="44">
-        <v>0.81</v>
-      </c>
-      <c r="P11" s="44">
-        <v>0.82</v>
-      </c>
-      <c r="Q11" s="45">
-        <f t="shared" si="2"/>
-        <v>4161.2130000000006</v>
-      </c>
-      <c r="R11" s="42">
-        <v>0.13</v>
-      </c>
-      <c r="S11" s="43">
-        <f t="shared" si="3"/>
-        <v>3620.2553100000005</v>
-      </c>
-      <c r="T11" s="43">
-        <f t="shared" si="4"/>
         <v>540.95769000000007</v>
       </c>
-      <c r="U11" s="51">
+      <c r="AB11" s="51">
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
       <c r="B12" s="12">
         <v>194</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="11"/>
+      <c r="E12" s="35">
         <f t="shared" si="1"/>
         <v>5009.5155663483602</v>
       </c>
-      <c r="D12" s="11">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="11">
         <v>0.9</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="35">
-        <f>1.05*G11</f>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="35">
+        <f>1.05*K11</f>
         <v>69576.605088171666</v>
       </c>
-      <c r="H12" s="48" t="e">
+      <c r="L12" s="35">
+        <f t="shared" si="2"/>
+        <v>60263.37934201688</v>
+      </c>
+      <c r="M12" s="35">
+        <f t="shared" si="7"/>
+        <v>9313.2257461547852</v>
+      </c>
+      <c r="N12" s="121"/>
+      <c r="O12" s="48" t="e">
         <f>0.01*(#REF!*#REF!+#REF!*#REF!)/(#REF!+#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I12" s="48">
+      <c r="P12" s="48">
         <v>4.6699999999999998E-2</v>
       </c>
-      <c r="J12" s="35">
-        <f>G12-K12</f>
+      <c r="Q12" s="35">
+        <f>K12-R12</f>
         <v>64567.089521823305</v>
       </c>
-      <c r="K12" s="35">
-        <f>C12</f>
+      <c r="R12" s="35">
+        <f>E12</f>
         <v>5009.5155663483602</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="39">
-        <f t="shared" si="7"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="39">
+        <f t="shared" si="9"/>
         <v>234</v>
       </c>
-      <c r="N12" s="12">
+      <c r="U12" s="12">
         <v>7289</v>
       </c>
-      <c r="O12" s="44">
+      <c r="V12" s="44">
         <v>0.81</v>
       </c>
-      <c r="P12" s="44">
+      <c r="W12" s="44">
         <v>0.7</v>
       </c>
-      <c r="Q12" s="45">
-        <f t="shared" si="2"/>
+      <c r="X12" s="45">
+        <f t="shared" si="3"/>
         <v>4132.8630000000003</v>
       </c>
-      <c r="R12" s="41">
+      <c r="Y12" s="41">
         <v>0.1</v>
       </c>
-      <c r="S12" s="43">
-        <f t="shared" si="3"/>
+      <c r="Z12" s="43">
+        <f t="shared" si="4"/>
         <v>3719.5767000000001</v>
       </c>
-      <c r="T12" s="43">
-        <f t="shared" si="4"/>
+      <c r="AA12" s="43">
+        <f t="shared" si="5"/>
         <v>413.28630000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>2018</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="12">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="12">
         <v>0.9</v>
       </c>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="J14" s="47"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="J15" s="47"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="11"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="121"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D14" s="11"/>
+      <c r="Q14" s="47"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D15" s="11"/>
+      <c r="Q15" s="47"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4133,177 +4348,177 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F1" s="75" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G1" s="76" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H1" s="77" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K1" s="75" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L1" s="76" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M1" s="109" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N1" s="114" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O1" s="76" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="P1" s="77" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="75" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="R1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="S1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="T1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="U1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V1" s="77" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="W1" s="75" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="X1" s="76" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Y1" s="77" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Z1" s="75" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AA1" s="76" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB1" s="77" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AC1" s="105" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AD1" s="105" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AE1" s="90" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF1" s="90" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AG1" s="91" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AH1" s="91" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AI1" s="91" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AJ1" s="91" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AK1" s="92" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="78" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2" s="80" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F2" s="78" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H2" s="80" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
       <c r="K2" s="78" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M2" s="110" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="N2" s="115" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="P2" s="80" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="78" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="R2" s="79" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="S2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="T2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="U2" s="79" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="V2" s="80" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="W2" s="78"/>
       <c r="X2" s="79"/>
@@ -4313,105 +4528,105 @@
       <c r="AB2" s="80"/>
       <c r="AE2" s="93"/>
       <c r="AF2" s="93" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AG2" s="94" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="AH2" s="94" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AI2" s="94" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AJ2" s="94" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="AK2" s="95" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="78" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E3" s="80" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F3" s="78" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G3" s="79" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H3" s="80" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I3" s="38"/>
       <c r="J3" s="38"/>
       <c r="K3" s="78" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L3" s="79" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="M3" s="110" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="N3" s="115" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="O3" s="79" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="P3" s="80" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="Q3" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="T3" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="U3" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="V3" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="W3" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="79" t="s">
+      <c r="X3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="S3" s="79" t="s">
+      <c r="Y3" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z3" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="T3" s="79" t="s">
+      <c r="AA3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="U3" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="V3" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="W3" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="X3" s="79" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y3" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z3" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA3" s="79" t="s">
-        <v>86</v>
-      </c>
       <c r="AB3" s="80" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AE3" s="93" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="AF3" s="93"/>
       <c r="AG3" s="94"/>
@@ -5481,21 +5696,21 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B2" s="38"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -5654,71 +5869,71 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F1" s="76" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G1" s="77" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2" s="79" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G2" s="80" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B3" s="78" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E3" s="79" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F3" s="79" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G3" s="80" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced relative_foi with eff_prep
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -803,7 +803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -823,7 +823,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Relative force of infection multiplier for each risk group </t>
+Number of people on PrEP. Seemed to make more sense than proportion of people on PrEP</t>
         </r>
       </text>
     </comment>
@@ -847,11 +847,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Relative force of infection multiplier for each risk group </t>
+Effectiveness of condoms. This number doesn't actually matter because it gets absorbed into the force of infection. But its needed for a gel condom analysis</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -871,11 +871,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Number of people on PrEP. Seemed to make more sense than proportion of people on PrEP</t>
+Time between HIV tests (in years)</t>
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -895,11 +895,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Effectiveness of condoms. This number doesn't actually matter because it gets absorbed into the force of infection. But its needed for a gel condom analysis</t>
+Effectiveness of each care stage in reducing infectiousness. The number of people in each infected compartment are multiplied by these values to get an overall relative proportion positive</t>
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -919,11 +919,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time between HIV tests (in years)</t>
+Relative force of infection multiplier for each risk group </t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -943,11 +943,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Effectiveness of each care stage in reducing infectiousness. The number of people in each infected compartment are multiplied by these values to get an overall relative proportion positive</t>
+Relative force of infection multiplier for each risk group </t>
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -971,7 +971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -992,30 +992,6 @@
           </rPr>
           <t xml:space="preserve">
 Condom usage between risk groups. Might be set this to zero then absorb any relative risk into the relative_foi parameter</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AE1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the time (in years) in each undiagnosed group before people move on to the next one (if they don't get diagnosed). i.e. people spend 1 year in the "&lt;1 year since infection" group, then 2 years in the "1-3 years since infection" group, then stay in the "3+ years since infection" group until they get diagnosed</t>
         </r>
       </text>
     </comment>
@@ -1039,11 +1015,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Proportions of people changing to gel condoms. From the geldom analysis. Can just leave at 0.</t>
+This is the time (in years) in each undiagnosed group before people move on to the next one (if they don't get diagnosed). i.e. people spend 1 year in the "&lt;1 year since infection" group, then 2 years in the "1-3 years since infection" group, then stay in the "3+ years since infection" group until they get diagnosed</t>
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="AG1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Proportions of people changing to gel condoms. From the geldom analysis. Can just leave at 0.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1064,6 +1064,30 @@
           </rPr>
           <t xml:space="preserve">
 Time between tests for people within 1 year of infection</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Time between tests for people infected over 3 years ago</t>
         </r>
       </text>
     </comment>
@@ -1087,11 +1111,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time between tests for people infected over 3 years ago</t>
+Proportion of diagnosed PLHIV who are on treatment</t>
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1111,11 +1135,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Proportion of diagnosed PLHIV who are on treatment</t>
+Proportion of PLHIV on treatment who are virally suppressed</t>
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
+    <comment ref="T4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1135,35 +1159,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Proportion of PLHIV on treatment who are virally suppressed</t>
+i.e. PrEP is 97% effective</t>
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-i.e. PrEP is 97% effective</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="W4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1308,7 +1308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="118">
   <si>
     <t>Waiting list</t>
   </si>
@@ -1660,6 +1660,9 @@
   <si>
     <t>e.g. the first row represents the weighting with which low risk people who are medicare eligible interact with other groups.
 i.e. all 1's means that a low risk medicare eligible person is mixing uniformly with everyone</t>
+  </si>
+  <si>
+    <t>eff_prep</t>
   </si>
 </sst>
 </file>
@@ -2546,7 +2549,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2839,6 +2842,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -4916,435 +4929,441 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK34"/>
+  <dimension ref="A1:AL34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="60" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="60" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28" style="60" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28" style="60" bestFit="1" customWidth="1"/>
-    <col min="23" max="28" width="16" style="60" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="28" style="60" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="11" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="60" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15" style="60" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" style="60" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28" style="60" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="60" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" style="60" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="24" max="29" width="16" style="60" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="28" style="60" customWidth="1"/>
+    <col min="32" max="32" width="13.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15" style="60" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" style="60" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15" style="60" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" style="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="172" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="173" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="172" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="173" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="S1" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="172" t="s">
+      <c r="T1" s="182" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="173" t="s">
+      <c r="U1" s="183" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="V1" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="W1" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="172" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="173" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="172" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" s="173" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="U1" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="W1" s="81" t="s">
+      <c r="X1" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="82" t="s">
+      <c r="Y1" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" s="162" t="s">
+      <c r="Z1" s="162" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="163" t="s">
+      <c r="AA1" s="163" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="82" t="s">
+      <c r="AB1" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="83" t="s">
+      <c r="AC1" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="AC1" s="98" t="s">
+      <c r="AD1" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="AD1" s="98" t="s">
+      <c r="AE1" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="AE1" s="81" t="s">
+      <c r="AF1" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="AF1" s="81" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG1" s="82" t="s">
+      <c r="AG1" s="81" t="s">
         <v>76</v>
       </c>
       <c r="AH1" s="82" t="s">
         <v>76</v>
       </c>
       <c r="AI1" s="82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AJ1" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="AK1" s="83" t="s">
+      <c r="AK1" s="82" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL1" s="83" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="44"/>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="H2" s="174" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="175" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="174" t="s">
+      <c r="J2" s="174" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="175" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="175" t="s">
+      <c r="L2" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="S2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="T2" s="184" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="69" t="s">
+      <c r="U2" s="185" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="174" t="s">
+      <c r="V2" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="86" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="175" t="s">
+      <c r="Y2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="174" t="s">
+      <c r="Z2" s="164" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="165" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="175" t="s">
+      <c r="AC2" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="71" t="s">
+      <c r="AD2" s="99"/>
+      <c r="AE2" s="99"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH2" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI2" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="R2" s="70"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="84" t="s">
+      <c r="AJ2" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="X2" s="85" t="s">
+      <c r="AK2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="Y2" s="164" t="s">
+      <c r="AL2" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="Z2" s="165" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA2" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB2" s="86" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC2" s="99"/>
-      <c r="AD2" s="99"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG2" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH2" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI2" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ2" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK2" s="86" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
       <c r="B3" s="44"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="E3" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="174" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="175" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="174" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="175" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="P3" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q3" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="174" t="s">
+      <c r="S3" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="175" t="s">
+      <c r="T3" s="184" t="s">
+        <v>97</v>
+      </c>
+      <c r="U3" s="185" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="V3" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="W3" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="X3" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="Y3" s="85" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z3" s="164" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA3" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="M3" s="174" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" s="175" t="s">
-        <v>73</v>
-      </c>
-      <c r="O3" s="174" t="s">
-        <v>74</v>
-      </c>
-      <c r="P3" s="175" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="S3" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="T3" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="V3" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="W3" s="84" t="s">
-        <v>97</v>
-      </c>
-      <c r="X3" s="85" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y3" s="164" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z3" s="165" t="s">
+      <c r="AB3" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="AA3" s="85" t="s">
+      <c r="AC3" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC3" s="99"/>
       <c r="AD3" s="99"/>
-      <c r="AE3" s="84" t="s">
+      <c r="AE3" s="99"/>
+      <c r="AF3" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="AF3" s="84"/>
-      <c r="AG3" s="85"/>
+      <c r="AG3" s="84"/>
       <c r="AH3" s="85"/>
       <c r="AI3" s="85"/>
       <c r="AJ3" s="85"/>
-      <c r="AK3" s="86"/>
-    </row>
-    <row r="4" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK3" s="85"/>
+      <c r="AL3" s="86"/>
+    </row>
+    <row r="4" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2000</v>
       </c>
       <c r="B4" s="29">
         <v>0.13</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="29">
+        <v>0.97</v>
+      </c>
+      <c r="D4" s="72"/>
+      <c r="E4" s="74">
+        <v>0</v>
+      </c>
+      <c r="F4" s="65">
+        <v>0.7</v>
+      </c>
+      <c r="G4" s="72">
         <v>1</v>
       </c>
-      <c r="D4" s="73">
-        <v>1</v>
-      </c>
-      <c r="E4" s="176">
-        <v>0.03</v>
-      </c>
-      <c r="F4" s="177">
-        <v>1</v>
-      </c>
-      <c r="G4" s="73">
-        <v>1</v>
-      </c>
-      <c r="H4" s="74">
-        <v>0.03</v>
-      </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="74">
-        <v>0</v>
-      </c>
-      <c r="K4" s="65">
-        <v>0.7</v>
-      </c>
-      <c r="L4" s="72">
-        <v>1</v>
-      </c>
-      <c r="M4" s="176">
+      <c r="H4" s="176">
         <v>10</v>
       </c>
-      <c r="N4" s="177">
+      <c r="I4" s="177">
         <v>0.5</v>
       </c>
-      <c r="O4" s="176">
+      <c r="J4" s="176">
         <v>4</v>
       </c>
-      <c r="P4" s="177">
+      <c r="K4" s="177">
         <f>3/12</f>
         <v>0.25</v>
       </c>
-      <c r="Q4" s="74">
+      <c r="L4" s="74">
         <f>3/12</f>
         <v>0.25</v>
       </c>
-      <c r="R4" s="73"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="72">
+      <c r="M4" s="73"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="72">
         <v>1</v>
       </c>
-      <c r="U4" s="73">
+      <c r="P4" s="73">
         <v>1</v>
       </c>
-      <c r="V4" s="74">
+      <c r="Q4" s="74">
         <v>0.04</v>
       </c>
-      <c r="W4" s="87">
+      <c r="R4" s="87">
         <v>1</v>
       </c>
-      <c r="X4" s="88">
+      <c r="S4" s="88">
+        <v>1</v>
+      </c>
+      <c r="T4" s="186">
+        <v>0.03</v>
+      </c>
+      <c r="U4" s="187">
+        <v>1</v>
+      </c>
+      <c r="V4" s="88">
+        <v>1</v>
+      </c>
+      <c r="W4" s="89">
+        <v>0.03</v>
+      </c>
+      <c r="X4" s="87">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="88">
         <v>0</v>
       </c>
-      <c r="Y4" s="166">
+      <c r="Z4" s="166">
         <v>0</v>
       </c>
-      <c r="Z4" s="167">
+      <c r="AA4" s="167">
         <v>1</v>
       </c>
-      <c r="AA4" s="88">
+      <c r="AB4" s="88">
         <v>0</v>
       </c>
-      <c r="AB4" s="89">
+      <c r="AC4" s="89">
         <v>0</v>
-      </c>
-      <c r="AC4" s="100">
-        <v>1</v>
       </c>
       <c r="AD4" s="100">
         <v>1</v>
       </c>
-      <c r="AE4" s="87">
+      <c r="AE4" s="100">
         <v>1</v>
       </c>
       <c r="AF4" s="87">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="88">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="87">
         <v>0</v>
       </c>
       <c r="AH4" s="88">
@@ -5356,929 +5375,952 @@
       <c r="AJ4" s="88">
         <v>0</v>
       </c>
-      <c r="AK4" s="89">
+      <c r="AK4" s="88">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AL4" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2001</v>
       </c>
       <c r="B5" s="44"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="178"/>
-      <c r="F5" s="179"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="178"/>
-      <c r="N5" s="179"/>
-      <c r="O5" s="178"/>
-      <c r="P5" s="179"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="178"/>
+      <c r="I5" s="179"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="179"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="77"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="76"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="168"/>
-      <c r="Z5" s="169"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="92"/>
-      <c r="AC5" s="101"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="188"/>
+      <c r="U5" s="189"/>
+      <c r="V5" s="91"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="90"/>
+      <c r="Y5" s="91"/>
+      <c r="Z5" s="168"/>
+      <c r="AA5" s="169"/>
+      <c r="AB5" s="91"/>
+      <c r="AC5" s="92"/>
       <c r="AD5" s="101"/>
-      <c r="AE5" s="90"/>
+      <c r="AE5" s="101"/>
       <c r="AF5" s="90"/>
-      <c r="AG5" s="91"/>
+      <c r="AG5" s="90"/>
       <c r="AH5" s="91"/>
       <c r="AI5" s="91"/>
       <c r="AJ5" s="91"/>
-      <c r="AK5" s="92"/>
-    </row>
-    <row r="6" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK5" s="91"/>
+      <c r="AL5" s="92"/>
+    </row>
+    <row r="6" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>2002</v>
       </c>
       <c r="B6" s="44"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="178"/>
-      <c r="F6" s="179"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="178"/>
-      <c r="N6" s="179"/>
-      <c r="O6" s="178"/>
-      <c r="P6" s="179"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="76"/>
       <c r="Q6" s="77"/>
-      <c r="R6" s="76"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="76"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="91"/>
-      <c r="Y6" s="168"/>
-      <c r="Z6" s="169"/>
-      <c r="AA6" s="91"/>
-      <c r="AB6" s="92"/>
-      <c r="AC6" s="101"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="188"/>
+      <c r="U6" s="189"/>
+      <c r="V6" s="91"/>
+      <c r="W6" s="92"/>
+      <c r="X6" s="90"/>
+      <c r="Y6" s="91"/>
+      <c r="Z6" s="168"/>
+      <c r="AA6" s="169"/>
+      <c r="AB6" s="91"/>
+      <c r="AC6" s="92"/>
       <c r="AD6" s="101"/>
-      <c r="AE6" s="90"/>
+      <c r="AE6" s="101"/>
       <c r="AF6" s="90"/>
-      <c r="AG6" s="91"/>
+      <c r="AG6" s="90"/>
       <c r="AH6" s="91"/>
       <c r="AI6" s="91"/>
       <c r="AJ6" s="91"/>
-      <c r="AK6" s="92"/>
-    </row>
-    <row r="7" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK6" s="91"/>
+      <c r="AL6" s="92"/>
+    </row>
+    <row r="7" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>2003</v>
       </c>
       <c r="B7" s="44"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="179"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="179"/>
-      <c r="O7" s="178"/>
-      <c r="P7" s="179"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="178"/>
+      <c r="I7" s="179"/>
+      <c r="J7" s="178"/>
+      <c r="K7" s="179"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="77"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="75"/>
-      <c r="U7" s="76"/>
-      <c r="V7" s="77"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="168"/>
-      <c r="Z7" s="169"/>
-      <c r="AA7" s="91"/>
-      <c r="AB7" s="92"/>
-      <c r="AC7" s="101"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="188"/>
+      <c r="U7" s="189"/>
+      <c r="V7" s="91"/>
+      <c r="W7" s="92"/>
+      <c r="X7" s="90"/>
+      <c r="Y7" s="91"/>
+      <c r="Z7" s="168"/>
+      <c r="AA7" s="169"/>
+      <c r="AB7" s="91"/>
+      <c r="AC7" s="92"/>
       <c r="AD7" s="101"/>
-      <c r="AE7" s="90"/>
+      <c r="AE7" s="101"/>
       <c r="AF7" s="90"/>
-      <c r="AG7" s="91"/>
+      <c r="AG7" s="90"/>
       <c r="AH7" s="91"/>
       <c r="AI7" s="91"/>
       <c r="AJ7" s="91"/>
-      <c r="AK7" s="92"/>
-    </row>
-    <row r="8" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK7" s="91"/>
+      <c r="AL7" s="92"/>
+    </row>
+    <row r="8" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>2004</v>
       </c>
       <c r="B8" s="44"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="178"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="178"/>
-      <c r="N8" s="179"/>
-      <c r="O8" s="178"/>
-      <c r="P8" s="179"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="178"/>
+      <c r="K8" s="179"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="76"/>
       <c r="Q8" s="77"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="90"/>
-      <c r="X8" s="91"/>
-      <c r="Y8" s="168"/>
-      <c r="Z8" s="169"/>
-      <c r="AA8" s="91"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="101"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="91"/>
+      <c r="T8" s="188"/>
+      <c r="U8" s="189"/>
+      <c r="V8" s="91"/>
+      <c r="W8" s="92"/>
+      <c r="X8" s="90"/>
+      <c r="Y8" s="91"/>
+      <c r="Z8" s="168"/>
+      <c r="AA8" s="169"/>
+      <c r="AB8" s="91"/>
+      <c r="AC8" s="92"/>
       <c r="AD8" s="101"/>
-      <c r="AE8" s="90"/>
+      <c r="AE8" s="101"/>
       <c r="AF8" s="90"/>
-      <c r="AG8" s="91"/>
+      <c r="AG8" s="90"/>
       <c r="AH8" s="91"/>
       <c r="AI8" s="91"/>
       <c r="AJ8" s="91"/>
-      <c r="AK8" s="92"/>
-    </row>
-    <row r="9" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK8" s="91"/>
+      <c r="AL8" s="92"/>
+    </row>
+    <row r="9" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>2005</v>
       </c>
       <c r="B9" s="44"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="178"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="178"/>
-      <c r="N9" s="179"/>
-      <c r="O9" s="178"/>
-      <c r="P9" s="179"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="178"/>
+      <c r="K9" s="179"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="76"/>
       <c r="Q9" s="77"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="77"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="77"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="91"/>
-      <c r="Y9" s="168"/>
-      <c r="Z9" s="169"/>
-      <c r="AA9" s="91"/>
-      <c r="AB9" s="92"/>
-      <c r="AC9" s="101"/>
+      <c r="R9" s="90"/>
+      <c r="S9" s="91"/>
+      <c r="T9" s="188"/>
+      <c r="U9" s="189"/>
+      <c r="V9" s="91"/>
+      <c r="W9" s="92"/>
+      <c r="X9" s="90"/>
+      <c r="Y9" s="91"/>
+      <c r="Z9" s="168"/>
+      <c r="AA9" s="169"/>
+      <c r="AB9" s="91"/>
+      <c r="AC9" s="92"/>
       <c r="AD9" s="101"/>
-      <c r="AE9" s="90"/>
+      <c r="AE9" s="101"/>
       <c r="AF9" s="90"/>
-      <c r="AG9" s="91"/>
+      <c r="AG9" s="90"/>
       <c r="AH9" s="91"/>
       <c r="AI9" s="91"/>
       <c r="AJ9" s="91"/>
-      <c r="AK9" s="92"/>
-    </row>
-    <row r="10" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK9" s="91"/>
+      <c r="AL9" s="92"/>
+    </row>
+    <row r="10" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2006</v>
       </c>
       <c r="B10" s="44"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="179"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="178"/>
-      <c r="N10" s="179"/>
-      <c r="O10" s="178"/>
-      <c r="P10" s="179"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="179"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="76"/>
       <c r="Q10" s="77"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="77"/>
-      <c r="T10" s="75"/>
-      <c r="U10" s="76"/>
-      <c r="V10" s="77"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="91"/>
-      <c r="Y10" s="168"/>
-      <c r="Z10" s="169"/>
-      <c r="AA10" s="91"/>
-      <c r="AB10" s="92"/>
-      <c r="AC10" s="101"/>
+      <c r="R10" s="90"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="188"/>
+      <c r="U10" s="189"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="92"/>
+      <c r="X10" s="90"/>
+      <c r="Y10" s="91"/>
+      <c r="Z10" s="168"/>
+      <c r="AA10" s="169"/>
+      <c r="AB10" s="91"/>
+      <c r="AC10" s="92"/>
       <c r="AD10" s="101"/>
-      <c r="AE10" s="90"/>
+      <c r="AE10" s="101"/>
       <c r="AF10" s="90"/>
-      <c r="AG10" s="91"/>
+      <c r="AG10" s="90"/>
       <c r="AH10" s="91"/>
       <c r="AI10" s="91"/>
       <c r="AJ10" s="91"/>
-      <c r="AK10" s="92"/>
-    </row>
-    <row r="11" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK10" s="91"/>
+      <c r="AL10" s="92"/>
+    </row>
+    <row r="11" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2007</v>
       </c>
       <c r="B11" s="44"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="179"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="178"/>
-      <c r="N11" s="179"/>
-      <c r="O11" s="178"/>
-      <c r="P11" s="179"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="178"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="178"/>
+      <c r="K11" s="179"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="76">
+        <v>0.75</v>
+      </c>
+      <c r="N11" s="77">
+        <v>0.8</v>
+      </c>
+      <c r="O11" s="75"/>
+      <c r="P11" s="76"/>
       <c r="Q11" s="77"/>
-      <c r="R11" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="S11" s="77">
-        <v>0.8</v>
-      </c>
-      <c r="T11" s="75"/>
-      <c r="U11" s="76"/>
-      <c r="V11" s="77"/>
-      <c r="W11" s="90"/>
-      <c r="X11" s="91"/>
-      <c r="Y11" s="168"/>
-      <c r="Z11" s="169"/>
-      <c r="AA11" s="91"/>
-      <c r="AB11" s="92"/>
-      <c r="AC11" s="101"/>
+      <c r="R11" s="90"/>
+      <c r="S11" s="91"/>
+      <c r="T11" s="188"/>
+      <c r="U11" s="189"/>
+      <c r="V11" s="91"/>
+      <c r="W11" s="92"/>
+      <c r="X11" s="90"/>
+      <c r="Y11" s="91"/>
+      <c r="Z11" s="168"/>
+      <c r="AA11" s="169"/>
+      <c r="AB11" s="91"/>
+      <c r="AC11" s="92"/>
       <c r="AD11" s="101"/>
-      <c r="AE11" s="90"/>
+      <c r="AE11" s="101"/>
       <c r="AF11" s="90"/>
-      <c r="AG11" s="91"/>
+      <c r="AG11" s="90"/>
       <c r="AH11" s="91"/>
       <c r="AI11" s="91"/>
       <c r="AJ11" s="91"/>
-      <c r="AK11" s="92"/>
-    </row>
-    <row r="12" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK11" s="91"/>
+      <c r="AL11" s="92"/>
+    </row>
+    <row r="12" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2008</v>
       </c>
       <c r="B12" s="44"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="179"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="178"/>
-      <c r="N12" s="179"/>
-      <c r="O12" s="178"/>
-      <c r="P12" s="179"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="179"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="76"/>
       <c r="Q12" s="77"/>
-      <c r="R12" s="76"/>
-      <c r="S12" s="77"/>
-      <c r="T12" s="75"/>
-      <c r="U12" s="76"/>
-      <c r="V12" s="77"/>
-      <c r="W12" s="90"/>
-      <c r="X12" s="91"/>
-      <c r="Y12" s="168"/>
-      <c r="Z12" s="169"/>
-      <c r="AA12" s="91"/>
-      <c r="AB12" s="92"/>
-      <c r="AC12" s="101"/>
+      <c r="R12" s="90"/>
+      <c r="S12" s="91"/>
+      <c r="T12" s="188"/>
+      <c r="U12" s="189"/>
+      <c r="V12" s="91"/>
+      <c r="W12" s="92"/>
+      <c r="X12" s="90"/>
+      <c r="Y12" s="91"/>
+      <c r="Z12" s="168"/>
+      <c r="AA12" s="169"/>
+      <c r="AB12" s="91"/>
+      <c r="AC12" s="92"/>
       <c r="AD12" s="101"/>
-      <c r="AE12" s="90"/>
+      <c r="AE12" s="101"/>
       <c r="AF12" s="90"/>
-      <c r="AG12" s="91"/>
+      <c r="AG12" s="90"/>
       <c r="AH12" s="91"/>
       <c r="AI12" s="91"/>
       <c r="AJ12" s="91"/>
-      <c r="AK12" s="92"/>
-    </row>
-    <row r="13" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK12" s="91"/>
+      <c r="AL12" s="92"/>
+    </row>
+    <row r="13" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2009</v>
       </c>
       <c r="B13" s="44"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="179"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="75">
+      <c r="C13" s="44"/>
+      <c r="D13" s="75">
         <v>0</v>
       </c>
-      <c r="J13" s="77"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="178"/>
-      <c r="N13" s="179"/>
-      <c r="O13" s="178"/>
-      <c r="P13" s="179"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="179"/>
+      <c r="J13" s="178"/>
+      <c r="K13" s="179"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="76"/>
       <c r="Q13" s="77"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="77"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="76"/>
-      <c r="V13" s="77"/>
-      <c r="W13" s="90"/>
-      <c r="X13" s="91"/>
-      <c r="Y13" s="168"/>
-      <c r="Z13" s="169"/>
-      <c r="AA13" s="91"/>
-      <c r="AB13" s="92"/>
-      <c r="AC13" s="101"/>
+      <c r="R13" s="90"/>
+      <c r="S13" s="91"/>
+      <c r="T13" s="188"/>
+      <c r="U13" s="189"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="92"/>
+      <c r="X13" s="90"/>
+      <c r="Y13" s="91"/>
+      <c r="Z13" s="168"/>
+      <c r="AA13" s="169"/>
+      <c r="AB13" s="91"/>
+      <c r="AC13" s="92"/>
       <c r="AD13" s="101"/>
-      <c r="AE13" s="90"/>
+      <c r="AE13" s="101"/>
       <c r="AF13" s="90"/>
-      <c r="AG13" s="91"/>
+      <c r="AG13" s="90"/>
       <c r="AH13" s="91"/>
       <c r="AI13" s="91"/>
       <c r="AJ13" s="91"/>
-      <c r="AK13" s="92"/>
-    </row>
-    <row r="14" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK13" s="91"/>
+      <c r="AL13" s="92"/>
+    </row>
+    <row r="14" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>2010</v>
       </c>
       <c r="B14" s="44"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="178"/>
-      <c r="F14" s="179"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="75">
+      <c r="C14" s="44"/>
+      <c r="D14" s="75">
         <v>1500</v>
       </c>
-      <c r="J14" s="77">
+      <c r="E14" s="77">
         <v>0</v>
       </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="178"/>
-      <c r="N14" s="179"/>
-      <c r="O14" s="178"/>
-      <c r="P14" s="179"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="179"/>
+      <c r="J14" s="178"/>
+      <c r="K14" s="179"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="76">
+        <v>0.75</v>
+      </c>
+      <c r="N14" s="77">
+        <v>0.8</v>
+      </c>
+      <c r="O14" s="75"/>
+      <c r="P14" s="76"/>
       <c r="Q14" s="77"/>
-      <c r="R14" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="S14" s="77">
-        <v>0.8</v>
-      </c>
-      <c r="T14" s="75"/>
-      <c r="U14" s="76"/>
-      <c r="V14" s="77"/>
-      <c r="W14" s="90"/>
-      <c r="X14" s="91"/>
-      <c r="Y14" s="168"/>
-      <c r="Z14" s="169"/>
-      <c r="AA14" s="91"/>
-      <c r="AB14" s="92"/>
-      <c r="AC14" s="101"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="188"/>
+      <c r="U14" s="189"/>
+      <c r="V14" s="91"/>
+      <c r="W14" s="92"/>
+      <c r="X14" s="90"/>
+      <c r="Y14" s="91"/>
+      <c r="Z14" s="168"/>
+      <c r="AA14" s="169"/>
+      <c r="AB14" s="91"/>
+      <c r="AC14" s="92"/>
       <c r="AD14" s="101"/>
-      <c r="AE14" s="90"/>
+      <c r="AE14" s="101"/>
       <c r="AF14" s="90"/>
-      <c r="AG14" s="91"/>
+      <c r="AG14" s="90"/>
       <c r="AH14" s="91"/>
       <c r="AI14" s="91"/>
       <c r="AJ14" s="91"/>
-      <c r="AK14" s="92"/>
-    </row>
-    <row r="15" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK14" s="91"/>
+      <c r="AL14" s="92"/>
+    </row>
+    <row r="15" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>2011</v>
       </c>
       <c r="B15" s="44"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="178"/>
-      <c r="F15" s="179"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="77">
+      <c r="C15" s="44"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="77">
         <v>110</v>
       </c>
-      <c r="K15" s="62"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="178"/>
-      <c r="N15" s="179"/>
-      <c r="O15" s="178"/>
-      <c r="P15" s="179"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="179"/>
+      <c r="J15" s="178"/>
+      <c r="K15" s="179"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="76"/>
       <c r="Q15" s="77"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="77"/>
-      <c r="T15" s="75"/>
-      <c r="U15" s="76"/>
-      <c r="V15" s="77"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="91"/>
-      <c r="Y15" s="168"/>
-      <c r="Z15" s="169"/>
-      <c r="AA15" s="91"/>
-      <c r="AB15" s="92"/>
-      <c r="AC15" s="101"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="188"/>
+      <c r="U15" s="189"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="90"/>
+      <c r="Y15" s="91"/>
+      <c r="Z15" s="168"/>
+      <c r="AA15" s="169"/>
+      <c r="AB15" s="91"/>
+      <c r="AC15" s="92"/>
       <c r="AD15" s="101"/>
-      <c r="AE15" s="90"/>
+      <c r="AE15" s="101"/>
       <c r="AF15" s="90"/>
-      <c r="AG15" s="91"/>
+      <c r="AG15" s="90"/>
       <c r="AH15" s="91"/>
       <c r="AI15" s="91"/>
       <c r="AJ15" s="91"/>
-      <c r="AK15" s="92"/>
-    </row>
-    <row r="16" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK15" s="91"/>
+      <c r="AL15" s="92"/>
+    </row>
+    <row r="16" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>2012</v>
       </c>
       <c r="B16" s="44"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="179"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="178"/>
-      <c r="N16" s="179"/>
-      <c r="O16" s="178"/>
-      <c r="P16" s="179"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="179"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="179"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="76">
+        <v>0.82</v>
+      </c>
+      <c r="N16" s="77">
+        <v>0.88</v>
+      </c>
+      <c r="O16" s="75"/>
+      <c r="P16" s="76"/>
       <c r="Q16" s="77"/>
-      <c r="R16" s="76">
-        <v>0.82</v>
-      </c>
-      <c r="S16" s="77">
-        <v>0.88</v>
-      </c>
-      <c r="T16" s="75"/>
-      <c r="U16" s="76"/>
-      <c r="V16" s="77"/>
-      <c r="W16" s="90"/>
-      <c r="X16" s="91"/>
-      <c r="Y16" s="168"/>
-      <c r="Z16" s="169"/>
-      <c r="AA16" s="91"/>
-      <c r="AB16" s="92"/>
-      <c r="AC16" s="101"/>
+      <c r="R16" s="90"/>
+      <c r="S16" s="91"/>
+      <c r="T16" s="188"/>
+      <c r="U16" s="189"/>
+      <c r="V16" s="91"/>
+      <c r="W16" s="92"/>
+      <c r="X16" s="90"/>
+      <c r="Y16" s="91"/>
+      <c r="Z16" s="168"/>
+      <c r="AA16" s="169"/>
+      <c r="AB16" s="91"/>
+      <c r="AC16" s="92"/>
       <c r="AD16" s="101"/>
-      <c r="AE16" s="90"/>
+      <c r="AE16" s="101"/>
       <c r="AF16" s="90"/>
-      <c r="AG16" s="91"/>
+      <c r="AG16" s="90"/>
       <c r="AH16" s="91"/>
       <c r="AI16" s="91"/>
       <c r="AJ16" s="91"/>
-      <c r="AK16" s="92"/>
-    </row>
-    <row r="17" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK16" s="91"/>
+      <c r="AL16" s="92"/>
+    </row>
+    <row r="17" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>2013</v>
       </c>
       <c r="B17" s="44"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="178"/>
-      <c r="F17" s="179"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="178"/>
-      <c r="N17" s="179"/>
-      <c r="O17" s="178"/>
-      <c r="P17" s="179"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="179"/>
+      <c r="J17" s="178"/>
+      <c r="K17" s="179"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="76">
+        <v>0.86</v>
+      </c>
+      <c r="N17" s="77">
+        <v>0.9</v>
+      </c>
+      <c r="O17" s="75"/>
+      <c r="P17" s="76"/>
       <c r="Q17" s="77"/>
-      <c r="R17" s="76">
-        <v>0.86</v>
-      </c>
-      <c r="S17" s="77">
-        <v>0.9</v>
-      </c>
-      <c r="T17" s="75"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="77"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="91"/>
-      <c r="Y17" s="168"/>
-      <c r="Z17" s="169"/>
-      <c r="AA17" s="91"/>
-      <c r="AB17" s="92"/>
-      <c r="AC17" s="101"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="91"/>
+      <c r="T17" s="188"/>
+      <c r="U17" s="189"/>
+      <c r="V17" s="91"/>
+      <c r="W17" s="92"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="91"/>
+      <c r="Z17" s="168"/>
+      <c r="AA17" s="169"/>
+      <c r="AB17" s="91"/>
+      <c r="AC17" s="92"/>
       <c r="AD17" s="101"/>
-      <c r="AE17" s="90"/>
+      <c r="AE17" s="101"/>
       <c r="AF17" s="90"/>
-      <c r="AG17" s="91"/>
+      <c r="AG17" s="90"/>
       <c r="AH17" s="91"/>
       <c r="AI17" s="91"/>
       <c r="AJ17" s="91"/>
-      <c r="AK17" s="92"/>
-    </row>
-    <row r="18" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK17" s="91"/>
+      <c r="AL17" s="92"/>
+    </row>
+    <row r="18" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>2014</v>
       </c>
       <c r="B18" s="44"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="179"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="178"/>
-      <c r="N18" s="179"/>
-      <c r="O18" s="178"/>
-      <c r="P18" s="179"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="178"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="178"/>
+      <c r="K18" s="179"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="76">
+        <v>0.89</v>
+      </c>
+      <c r="N18" s="77">
+        <v>0.9</v>
+      </c>
+      <c r="O18" s="75"/>
+      <c r="P18" s="76"/>
       <c r="Q18" s="77"/>
-      <c r="R18" s="76">
-        <v>0.89</v>
-      </c>
-      <c r="S18" s="77">
-        <v>0.9</v>
-      </c>
-      <c r="T18" s="75"/>
-      <c r="U18" s="76"/>
-      <c r="V18" s="77"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="91"/>
-      <c r="Y18" s="168"/>
-      <c r="Z18" s="169"/>
-      <c r="AA18" s="91"/>
-      <c r="AB18" s="92"/>
-      <c r="AC18" s="101"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="91"/>
+      <c r="T18" s="188"/>
+      <c r="U18" s="189"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="92"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="91"/>
+      <c r="Z18" s="168"/>
+      <c r="AA18" s="169"/>
+      <c r="AB18" s="91"/>
+      <c r="AC18" s="92"/>
       <c r="AD18" s="101"/>
-      <c r="AE18" s="90"/>
+      <c r="AE18" s="101"/>
       <c r="AF18" s="90"/>
-      <c r="AG18" s="91"/>
+      <c r="AG18" s="90"/>
       <c r="AH18" s="91"/>
       <c r="AI18" s="91"/>
       <c r="AJ18" s="91"/>
-      <c r="AK18" s="92"/>
-    </row>
-    <row r="19" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK18" s="91"/>
+      <c r="AL18" s="92"/>
+    </row>
+    <row r="19" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>2015</v>
       </c>
       <c r="B19" s="44"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="179"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="178"/>
-      <c r="N19" s="179"/>
-      <c r="O19" s="178"/>
-      <c r="P19" s="179"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="179"/>
+      <c r="J19" s="178"/>
+      <c r="K19" s="179"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="76">
+        <v>0.92</v>
+      </c>
+      <c r="N19" s="77">
+        <v>0.92</v>
+      </c>
+      <c r="O19" s="75"/>
+      <c r="P19" s="76"/>
       <c r="Q19" s="77"/>
-      <c r="R19" s="76">
-        <v>0.92</v>
-      </c>
-      <c r="S19" s="77">
-        <v>0.92</v>
-      </c>
-      <c r="T19" s="75"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="77"/>
-      <c r="W19" s="90"/>
-      <c r="X19" s="91"/>
-      <c r="Y19" s="168"/>
-      <c r="Z19" s="169"/>
-      <c r="AA19" s="91"/>
-      <c r="AB19" s="92"/>
-      <c r="AC19" s="101"/>
+      <c r="R19" s="90"/>
+      <c r="S19" s="91"/>
+      <c r="T19" s="188"/>
+      <c r="U19" s="189"/>
+      <c r="V19" s="91"/>
+      <c r="W19" s="92"/>
+      <c r="X19" s="90"/>
+      <c r="Y19" s="91"/>
+      <c r="Z19" s="168"/>
+      <c r="AA19" s="169"/>
+      <c r="AB19" s="91"/>
+      <c r="AC19" s="92"/>
       <c r="AD19" s="101"/>
-      <c r="AE19" s="90"/>
+      <c r="AE19" s="101"/>
       <c r="AF19" s="90"/>
-      <c r="AG19" s="91"/>
+      <c r="AG19" s="90"/>
       <c r="AH19" s="91"/>
       <c r="AI19" s="91"/>
       <c r="AJ19" s="91"/>
-      <c r="AK19" s="92"/>
-    </row>
-    <row r="20" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK19" s="91"/>
+      <c r="AL19" s="92"/>
+    </row>
+    <row r="20" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2016</v>
       </c>
       <c r="B20" s="44"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="178"/>
-      <c r="F20" s="179"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="75">
+      <c r="C20" s="44"/>
+      <c r="D20" s="75">
         <v>4000</v>
       </c>
-      <c r="J20" s="77">
+      <c r="E20" s="77">
         <v>200</v>
       </c>
-      <c r="K20" s="62"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="178"/>
-      <c r="N20" s="179"/>
-      <c r="O20" s="178"/>
-      <c r="P20" s="179"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="179"/>
+      <c r="J20" s="178"/>
+      <c r="K20" s="179"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="76">
+        <v>0.95</v>
+      </c>
+      <c r="N20" s="77">
+        <v>0.94</v>
+      </c>
+      <c r="O20" s="75"/>
+      <c r="P20" s="76"/>
       <c r="Q20" s="77"/>
-      <c r="R20" s="76">
-        <v>0.95</v>
-      </c>
-      <c r="S20" s="77">
-        <v>0.94</v>
-      </c>
-      <c r="T20" s="75"/>
-      <c r="U20" s="76"/>
-      <c r="V20" s="77"/>
-      <c r="W20" s="90"/>
-      <c r="X20" s="91"/>
-      <c r="Y20" s="168"/>
-      <c r="Z20" s="169"/>
-      <c r="AA20" s="91"/>
-      <c r="AB20" s="92"/>
-      <c r="AC20" s="101"/>
+      <c r="R20" s="90"/>
+      <c r="S20" s="91"/>
+      <c r="T20" s="188"/>
+      <c r="U20" s="189"/>
+      <c r="V20" s="91"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="90"/>
+      <c r="Y20" s="91"/>
+      <c r="Z20" s="168"/>
+      <c r="AA20" s="169"/>
+      <c r="AB20" s="91"/>
+      <c r="AC20" s="92"/>
       <c r="AD20" s="101"/>
-      <c r="AE20" s="90"/>
+      <c r="AE20" s="101"/>
       <c r="AF20" s="90"/>
-      <c r="AG20" s="91"/>
+      <c r="AG20" s="90"/>
       <c r="AH20" s="91"/>
       <c r="AI20" s="91"/>
       <c r="AJ20" s="91"/>
-      <c r="AK20" s="92"/>
-    </row>
-    <row r="21" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK20" s="91"/>
+      <c r="AL20" s="92"/>
+    </row>
+    <row r="21" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>2017</v>
       </c>
       <c r="B21" s="44"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="178"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="178"/>
-      <c r="N21" s="179"/>
-      <c r="O21" s="178"/>
-      <c r="P21" s="179"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="179"/>
+      <c r="J21" s="178"/>
+      <c r="K21" s="179"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="76"/>
       <c r="Q21" s="77"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="77"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="76"/>
-      <c r="V21" s="77"/>
-      <c r="W21" s="90"/>
-      <c r="X21" s="91"/>
-      <c r="Y21" s="168"/>
-      <c r="Z21" s="169"/>
-      <c r="AA21" s="91"/>
-      <c r="AB21" s="92"/>
-      <c r="AC21" s="101"/>
+      <c r="R21" s="90"/>
+      <c r="S21" s="91"/>
+      <c r="T21" s="188"/>
+      <c r="U21" s="189"/>
+      <c r="V21" s="91"/>
+      <c r="W21" s="92"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="91"/>
+      <c r="Z21" s="168"/>
+      <c r="AA21" s="169"/>
+      <c r="AB21" s="91"/>
+      <c r="AC21" s="92"/>
       <c r="AD21" s="101"/>
-      <c r="AE21" s="90"/>
+      <c r="AE21" s="101"/>
       <c r="AF21" s="90"/>
-      <c r="AG21" s="91"/>
+      <c r="AG21" s="90"/>
       <c r="AH21" s="91"/>
       <c r="AI21" s="91"/>
       <c r="AJ21" s="91"/>
-      <c r="AK21" s="92"/>
-    </row>
-    <row r="22" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK21" s="91"/>
+      <c r="AL21" s="92"/>
+    </row>
+    <row r="22" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>2018</v>
       </c>
       <c r="B22" s="44"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="179"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="178"/>
-      <c r="N22" s="179"/>
-      <c r="O22" s="178"/>
-      <c r="P22" s="179"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="179"/>
+      <c r="J22" s="178"/>
+      <c r="K22" s="179"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="77"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="76"/>
       <c r="Q22" s="77"/>
-      <c r="R22" s="76"/>
-      <c r="S22" s="77"/>
-      <c r="T22" s="75"/>
-      <c r="U22" s="76"/>
-      <c r="V22" s="77"/>
-      <c r="W22" s="90"/>
-      <c r="X22" s="91"/>
-      <c r="Y22" s="168"/>
-      <c r="Z22" s="169"/>
-      <c r="AA22" s="91"/>
-      <c r="AB22" s="92"/>
-      <c r="AC22" s="101"/>
+      <c r="R22" s="90"/>
+      <c r="S22" s="91"/>
+      <c r="T22" s="188"/>
+      <c r="U22" s="189"/>
+      <c r="V22" s="91"/>
+      <c r="W22" s="92"/>
+      <c r="X22" s="90"/>
+      <c r="Y22" s="91"/>
+      <c r="Z22" s="168"/>
+      <c r="AA22" s="169"/>
+      <c r="AB22" s="91"/>
+      <c r="AC22" s="92"/>
       <c r="AD22" s="101"/>
-      <c r="AE22" s="90"/>
+      <c r="AE22" s="101"/>
       <c r="AF22" s="90"/>
-      <c r="AG22" s="91"/>
+      <c r="AG22" s="90"/>
       <c r="AH22" s="91"/>
       <c r="AI22" s="91"/>
       <c r="AJ22" s="91"/>
-      <c r="AK22" s="92"/>
-    </row>
-    <row r="23" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK22" s="91"/>
+      <c r="AL22" s="92"/>
+    </row>
+    <row r="23" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>2019</v>
       </c>
       <c r="B23" s="44"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="178"/>
-      <c r="F23" s="179"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="178"/>
-      <c r="N23" s="179"/>
-      <c r="O23" s="178"/>
-      <c r="P23" s="179"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="179"/>
+      <c r="J23" s="178"/>
+      <c r="K23" s="179"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="75"/>
+      <c r="P23" s="76"/>
       <c r="Q23" s="77"/>
-      <c r="R23" s="76"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="75"/>
-      <c r="U23" s="76"/>
-      <c r="V23" s="77"/>
-      <c r="W23" s="90"/>
-      <c r="X23" s="91"/>
-      <c r="Y23" s="168"/>
-      <c r="Z23" s="169"/>
-      <c r="AA23" s="91"/>
-      <c r="AB23" s="92"/>
-      <c r="AC23" s="101"/>
+      <c r="R23" s="90"/>
+      <c r="S23" s="91"/>
+      <c r="T23" s="188"/>
+      <c r="U23" s="189"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="92"/>
+      <c r="X23" s="90"/>
+      <c r="Y23" s="91"/>
+      <c r="Z23" s="168"/>
+      <c r="AA23" s="169"/>
+      <c r="AB23" s="91"/>
+      <c r="AC23" s="92"/>
       <c r="AD23" s="101"/>
-      <c r="AE23" s="90"/>
+      <c r="AE23" s="101"/>
       <c r="AF23" s="90"/>
-      <c r="AG23" s="91"/>
+      <c r="AG23" s="90"/>
       <c r="AH23" s="91"/>
       <c r="AI23" s="91"/>
       <c r="AJ23" s="91"/>
-      <c r="AK23" s="92"/>
-    </row>
-    <row r="24" spans="1:37" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK23" s="91"/>
+      <c r="AL23" s="92"/>
+    </row>
+    <row r="24" spans="1:38" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="63">
         <v>2020</v>
       </c>
       <c r="B24" s="61"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="180"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="180"/>
-      <c r="N24" s="181"/>
-      <c r="O24" s="180"/>
-      <c r="P24" s="181"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="181"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="78"/>
+      <c r="P24" s="79"/>
       <c r="Q24" s="80"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="80"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="79"/>
-      <c r="V24" s="80"/>
-      <c r="W24" s="93"/>
-      <c r="X24" s="94"/>
-      <c r="Y24" s="170"/>
-      <c r="Z24" s="171"/>
-      <c r="AA24" s="94"/>
-      <c r="AB24" s="95"/>
-      <c r="AC24" s="102"/>
+      <c r="R24" s="93"/>
+      <c r="S24" s="94"/>
+      <c r="T24" s="190"/>
+      <c r="U24" s="191"/>
+      <c r="V24" s="94"/>
+      <c r="W24" s="95"/>
+      <c r="X24" s="93"/>
+      <c r="Y24" s="94"/>
+      <c r="Z24" s="170"/>
+      <c r="AA24" s="171"/>
+      <c r="AB24" s="94"/>
+      <c r="AC24" s="95"/>
       <c r="AD24" s="102"/>
-      <c r="AE24" s="93"/>
+      <c r="AE24" s="102"/>
       <c r="AF24" s="93"/>
-      <c r="AG24" s="94"/>
+      <c r="AG24" s="93"/>
       <c r="AH24" s="94"/>
       <c r="AI24" s="94"/>
       <c r="AJ24" s="94"/>
-      <c r="AK24" s="95"/>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AK24" s="94"/>
+      <c r="AL24" s="95"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="31">
         <v>2021</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>2022</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
         <v>2023</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
         <v>2024</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="63">
         <v>2025</v>
       </c>
-      <c r="R29" s="60">
+      <c r="M29" s="60">
         <v>0.95</v>
       </c>
-      <c r="S29" s="60">
+      <c r="N29" s="60">
         <v>0.95</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="31">
         <v>2026</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
         <v>2027</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="31">
         <v>2028</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="31">
         <v>2029</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="63">
         <v>2030</v>
       </c>
-      <c r="R34" s="60">
+      <c r="M34" s="60">
         <v>0.99</v>
       </c>
-      <c r="S34" s="60">
+      <c r="N34" s="60">
         <v>0.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slightly generalised diagnosed compartment
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -5173,8 +5173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8592,7 +8592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Seperated diagnosed compartments by risk category
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
     <sheet name="data" sheetId="5" r:id="rId2"/>
     <sheet name="mixing" sheetId="27" r:id="rId3"/>
-    <sheet name="timepars_short" sheetId="28" r:id="rId4"/>
+    <sheet name="timepars" sheetId="28" r:id="rId4"/>
     <sheet name="scen_1" sheetId="25" r:id="rId5"/>
     <sheet name="scen_2" sheetId="26" r:id="rId6"/>
     <sheet name="timepars_all" sheetId="20" r:id="rId7"/>
-    <sheet name="timepars" sheetId="30" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1535,234 +1534,8 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Tom Tidhar</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Proportion of the susceptible population that is at high risk</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Number of people on PrEP. Seemed to make more sense than proportion of people on PrEP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Effectiveness of condoms. This number doesn't actually matter because it gets absorbed into the force of infection. But its needed for a gel condom analysis</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between HIV tests (in years)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Effectiveness of each care stage in reducing infectiousness. The number of people in each infected compartment are multiplied by these values to get an overall relative proportion positive</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people within 1 year of infection</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people infected over 3 years ago</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Proportion of diagnosed PLHIV who are on treatment</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Proportion of PLHIV on treatment who are virally suppressed</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="118">
   <si>
     <t>Waiting list</t>
   </si>
@@ -5173,7 +4946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -5385,8 +5158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5561,16 +5334,16 @@
         <v>0.7</v>
       </c>
       <c r="G4" s="72">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H4" s="175">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="I4" s="176">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J4" s="175">
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="K4" s="176">
         <f>3/12</f>
@@ -6485,7 +6258,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6741,13 +6514,13 @@
         <v>0.5</v>
       </c>
       <c r="C19" s="76">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D19" s="76">
         <v>0.25</v>
       </c>
       <c r="E19" s="76">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="F19" s="76">
         <v>0.125</v>
@@ -8586,900 +8359,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
-  <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9" style="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="60" customWidth="1"/>
-    <col min="4" max="4" width="11" style="60" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="60" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15" style="60" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28" style="60" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28" style="60" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="43"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="171" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="172" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="171" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="172" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="P1" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="68" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="173" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="174" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="173" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="174" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="70"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="69" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="173" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="174" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="173" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="174" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="O3" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="71" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
-        <v>2000</v>
-      </c>
-      <c r="B4" s="29">
-        <v>0.13</v>
-      </c>
-      <c r="C4" s="29">
-        <v>0.97</v>
-      </c>
-      <c r="D4" s="72"/>
-      <c r="E4" s="74">
-        <v>0</v>
-      </c>
-      <c r="F4" s="65">
-        <v>0.7</v>
-      </c>
-      <c r="G4" s="72">
-        <v>1</v>
-      </c>
-      <c r="H4" s="175">
-        <v>10</v>
-      </c>
-      <c r="I4" s="176">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="175">
-        <v>4</v>
-      </c>
-      <c r="K4" s="176">
-        <f>3/12</f>
-        <v>0.25</v>
-      </c>
-      <c r="L4" s="74">
-        <f>3/12</f>
-        <v>0.25</v>
-      </c>
-      <c r="M4" s="73"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="72">
-        <v>1</v>
-      </c>
-      <c r="P4" s="73">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="74">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
-        <v>2001</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="178"/>
-      <c r="J5" s="177"/>
-      <c r="K5" s="178"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="77"/>
-    </row>
-    <row r="6" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
-        <v>2002</v>
-      </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="177"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="177"/>
-      <c r="K6" s="178"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="77"/>
-    </row>
-    <row r="7" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>2003</v>
-      </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="177"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="77"/>
-    </row>
-    <row r="8" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
-        <v>2004</v>
-      </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="177"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="177"/>
-      <c r="K8" s="178"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="77"/>
-    </row>
-    <row r="9" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>2005</v>
-      </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="177"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="177"/>
-      <c r="K9" s="178"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="77"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="77"/>
-    </row>
-    <row r="10" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>2006</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="177"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="177"/>
-      <c r="K10" s="178"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="77"/>
-    </row>
-    <row r="11" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
-        <v>2007</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="177"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="177"/>
-      <c r="K11" s="178"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="N11" s="77">
-        <v>0.8</v>
-      </c>
-      <c r="O11" s="75"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="77"/>
-    </row>
-    <row r="12" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
-        <v>2008</v>
-      </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="177"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="177"/>
-      <c r="K12" s="178"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="77"/>
-    </row>
-    <row r="13" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>2009</v>
-      </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="75">
-        <v>0</v>
-      </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="177"/>
-      <c r="K13" s="178"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="76"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="77"/>
-    </row>
-    <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
-        <v>2010</v>
-      </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="75">
-        <v>1500</v>
-      </c>
-      <c r="E14" s="77">
-        <v>0</v>
-      </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="177"/>
-      <c r="I14" s="178"/>
-      <c r="J14" s="177"/>
-      <c r="K14" s="178"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="N14" s="77">
-        <v>0.8</v>
-      </c>
-      <c r="O14" s="75"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="77"/>
-    </row>
-    <row r="15" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
-        <v>2011</v>
-      </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="77">
-        <v>110</v>
-      </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="177"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="177"/>
-      <c r="K15" s="178"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="77"/>
-    </row>
-    <row r="16" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
-        <v>2012</v>
-      </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="177"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="177"/>
-      <c r="K16" s="178"/>
-      <c r="L16" s="77"/>
-      <c r="M16" s="76">
-        <v>0.82</v>
-      </c>
-      <c r="N16" s="77">
-        <v>0.88</v>
-      </c>
-      <c r="O16" s="75"/>
-      <c r="P16" s="76"/>
-      <c r="Q16" s="77"/>
-    </row>
-    <row r="17" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
-        <v>2013</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="177"/>
-      <c r="I17" s="178"/>
-      <c r="J17" s="177"/>
-      <c r="K17" s="178"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="76">
-        <v>0.86</v>
-      </c>
-      <c r="N17" s="77">
-        <v>0.9</v>
-      </c>
-      <c r="O17" s="75"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="77"/>
-    </row>
-    <row r="18" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31">
-        <v>2014</v>
-      </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="177"/>
-      <c r="I18" s="178"/>
-      <c r="J18" s="177"/>
-      <c r="K18" s="178"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="76">
-        <v>0.89</v>
-      </c>
-      <c r="N18" s="77">
-        <v>0.9</v>
-      </c>
-      <c r="O18" s="75"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="77"/>
-    </row>
-    <row r="19" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
-        <v>2015</v>
-      </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="178"/>
-      <c r="J19" s="177"/>
-      <c r="K19" s="178"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="76">
-        <v>0.92</v>
-      </c>
-      <c r="N19" s="77">
-        <v>0.92</v>
-      </c>
-      <c r="O19" s="75"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="77"/>
-    </row>
-    <row r="20" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31">
-        <v>2016</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="75">
-        <v>4000</v>
-      </c>
-      <c r="E20" s="77">
-        <v>200</v>
-      </c>
-      <c r="F20" s="62"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="177"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="177"/>
-      <c r="K20" s="178"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="76">
-        <v>0.95</v>
-      </c>
-      <c r="N20" s="77">
-        <v>0.94</v>
-      </c>
-      <c r="O20" s="75"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="77"/>
-    </row>
-    <row r="21" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
-        <v>2017</v>
-      </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="177"/>
-      <c r="I21" s="178"/>
-      <c r="J21" s="177"/>
-      <c r="K21" s="178"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="76"/>
-      <c r="Q21" s="77"/>
-    </row>
-    <row r="22" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31">
-        <v>2018</v>
-      </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="177"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="177"/>
-      <c r="K22" s="178"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="76"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="75"/>
-      <c r="P22" s="76"/>
-      <c r="Q22" s="77"/>
-    </row>
-    <row r="23" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31">
-        <v>2019</v>
-      </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="177"/>
-      <c r="I23" s="178"/>
-      <c r="J23" s="177"/>
-      <c r="K23" s="178"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="75"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="77"/>
-    </row>
-    <row r="24" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31">
-        <v>2020</v>
-      </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="177"/>
-      <c r="I24" s="178"/>
-      <c r="J24" s="177"/>
-      <c r="K24" s="178"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="76"/>
-      <c r="Q24" s="77"/>
-    </row>
-    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31">
-        <v>2021</v>
-      </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="177"/>
-      <c r="I25" s="178"/>
-      <c r="J25" s="177"/>
-      <c r="K25" s="178"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="75"/>
-      <c r="P25" s="76"/>
-      <c r="Q25" s="77"/>
-    </row>
-    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31">
-        <v>2022</v>
-      </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="177"/>
-      <c r="I26" s="178"/>
-      <c r="J26" s="177"/>
-      <c r="K26" s="178"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="76"/>
-      <c r="Q26" s="77"/>
-    </row>
-    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31">
-        <v>2023</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="177"/>
-      <c r="I27" s="178"/>
-      <c r="J27" s="177"/>
-      <c r="K27" s="178"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="76"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="75"/>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="77"/>
-    </row>
-    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31">
-        <v>2024</v>
-      </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="177"/>
-      <c r="I28" s="178"/>
-      <c r="J28" s="177"/>
-      <c r="K28" s="178"/>
-      <c r="L28" s="77"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="77"/>
-      <c r="O28" s="75"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="77"/>
-    </row>
-    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31">
-        <v>2025</v>
-      </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="177"/>
-      <c r="I29" s="178"/>
-      <c r="J29" s="177"/>
-      <c r="K29" s="178"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="76">
-        <v>0.95</v>
-      </c>
-      <c r="N29" s="77">
-        <v>0.95</v>
-      </c>
-      <c r="O29" s="75"/>
-      <c r="P29" s="76"/>
-      <c r="Q29" s="77"/>
-    </row>
-    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31">
-        <v>2026</v>
-      </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="177"/>
-      <c r="I30" s="178"/>
-      <c r="J30" s="177"/>
-      <c r="K30" s="178"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="77"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="76"/>
-      <c r="Q30" s="77"/>
-    </row>
-    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31">
-        <v>2027</v>
-      </c>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="177"/>
-      <c r="I31" s="178"/>
-      <c r="J31" s="177"/>
-      <c r="K31" s="178"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="76"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="75"/>
-      <c r="P31" s="76"/>
-      <c r="Q31" s="77"/>
-    </row>
-    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31">
-        <v>2028</v>
-      </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="177"/>
-      <c r="I32" s="178"/>
-      <c r="J32" s="177"/>
-      <c r="K32" s="178"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="75"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="77"/>
-    </row>
-    <row r="33" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31">
-        <v>2029</v>
-      </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="177"/>
-      <c r="I33" s="178"/>
-      <c r="J33" s="177"/>
-      <c r="K33" s="178"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="76"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="75"/>
-      <c r="P33" s="76"/>
-      <c r="Q33" s="77"/>
-    </row>
-    <row r="34" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="63">
-        <v>2030</v>
-      </c>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="179"/>
-      <c r="I34" s="180"/>
-      <c r="J34" s="179"/>
-      <c r="K34" s="180"/>
-      <c r="L34" s="80"/>
-      <c r="M34" s="79">
-        <v>0.99</v>
-      </c>
-      <c r="N34" s="80">
-        <v>0.99</v>
-      </c>
-      <c r="O34" s="78"/>
-      <c r="P34" s="79"/>
-      <c r="Q34" s="80"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added prevalence by risk plot
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -18,7 +18,7 @@
     <sheet name="timepars" sheetId="28" r:id="rId4"/>
     <sheet name="scen_1" sheetId="25" r:id="rId5"/>
     <sheet name="scen_2" sheetId="26" r:id="rId6"/>
-    <sheet name="timepars_all" sheetId="20" r:id="rId7"/>
+    <sheet name="timepars_old" sheetId="20" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -801,6 +801,30 @@
           </rPr>
           <t xml:space="preserve">
 Proportion of the susceptible population that is at high risk</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Effectiveness of PrEP</t>
         </r>
       </text>
     </comment>
@@ -5159,7 +5183,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5340,10 +5364,10 @@
         <v>1.5</v>
       </c>
       <c r="I4" s="176">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J4" s="175">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K4" s="176">
         <f>3/12</f>

</xml_diff>

<commit_message>
Medicare ineligible people can now leave/become eligible
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -1795,7 +1795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="132">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2186,6 +2186,12 @@
   </si>
   <si>
     <t>pr_old</t>
+  </si>
+  <si>
+    <t>ineligibility_duration</t>
+  </si>
+  <si>
+    <t>proportion_stay</t>
   </si>
 </sst>
 </file>
@@ -4263,7 +4269,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J11" sqref="J11"/>
+      <selection pane="topRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5857,10 +5863,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5888,10 +5894,12 @@
     <col min="21" max="21" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="28" style="60" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="43"/>
+    <col min="24" max="24" width="20" style="43" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
@@ -5961,8 +5969,14 @@
       <c r="W1" s="68" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y1" s="68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>84</v>
       </c>
@@ -6012,8 +6026,10 @@
       <c r="U2" s="69"/>
       <c r="V2" s="70"/>
       <c r="W2" s="71"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="70"/>
+      <c r="Y2" s="71"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
@@ -6077,8 +6093,14 @@
       <c r="W3" s="71" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X3" s="70" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y3" s="71" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2000</v>
       </c>
@@ -6126,8 +6148,14 @@
       <c r="W4" s="74">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="73">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="74">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2001</v>
       </c>
@@ -6153,8 +6181,10 @@
       <c r="U5" s="75"/>
       <c r="V5" s="76"/>
       <c r="W5" s="77"/>
-    </row>
-    <row r="6" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X5" s="76"/>
+      <c r="Y5" s="77"/>
+    </row>
+    <row r="6" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>2002</v>
       </c>
@@ -6180,8 +6210,10 @@
       <c r="U6" s="75"/>
       <c r="V6" s="76"/>
       <c r="W6" s="77"/>
-    </row>
-    <row r="7" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X6" s="76"/>
+      <c r="Y6" s="77"/>
+    </row>
+    <row r="7" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>2003</v>
       </c>
@@ -6209,8 +6241,10 @@
       <c r="U7" s="75"/>
       <c r="V7" s="76"/>
       <c r="W7" s="77"/>
-    </row>
-    <row r="8" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X7" s="76"/>
+      <c r="Y7" s="77"/>
+    </row>
+    <row r="8" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>2004</v>
       </c>
@@ -6238,8 +6272,10 @@
       <c r="U8" s="75"/>
       <c r="V8" s="76"/>
       <c r="W8" s="77"/>
-    </row>
-    <row r="9" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X8" s="76"/>
+      <c r="Y8" s="77"/>
+    </row>
+    <row r="9" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>2005</v>
       </c>
@@ -6267,8 +6303,10 @@
       <c r="U9" s="75"/>
       <c r="V9" s="76"/>
       <c r="W9" s="77"/>
-    </row>
-    <row r="10" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X9" s="76"/>
+      <c r="Y9" s="77"/>
+    </row>
+    <row r="10" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2006</v>
       </c>
@@ -6296,8 +6334,10 @@
       <c r="U10" s="75"/>
       <c r="V10" s="76"/>
       <c r="W10" s="77"/>
-    </row>
-    <row r="11" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X10" s="76"/>
+      <c r="Y10" s="77"/>
+    </row>
+    <row r="11" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2007</v>
       </c>
@@ -6329,8 +6369,10 @@
       <c r="U11" s="75"/>
       <c r="V11" s="76"/>
       <c r="W11" s="77"/>
-    </row>
-    <row r="12" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X11" s="76"/>
+      <c r="Y11" s="77"/>
+    </row>
+    <row r="12" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2008</v>
       </c>
@@ -6358,8 +6400,10 @@
       <c r="U12" s="75"/>
       <c r="V12" s="76"/>
       <c r="W12" s="77"/>
-    </row>
-    <row r="13" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="76"/>
+      <c r="Y12" s="77"/>
+    </row>
+    <row r="13" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2009</v>
       </c>
@@ -6388,8 +6432,10 @@
       <c r="U13" s="75"/>
       <c r="V13" s="76"/>
       <c r="W13" s="77"/>
-    </row>
-    <row r="14" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="76"/>
+      <c r="Y13" s="77"/>
+    </row>
+    <row r="14" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>2010</v>
       </c>
@@ -6422,8 +6468,10 @@
       <c r="U14" s="75"/>
       <c r="V14" s="76"/>
       <c r="W14" s="77"/>
-    </row>
-    <row r="15" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X14" s="76"/>
+      <c r="Y14" s="77"/>
+    </row>
+    <row r="15" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>2011</v>
       </c>
@@ -6452,8 +6500,10 @@
       <c r="U15" s="75"/>
       <c r="V15" s="76"/>
       <c r="W15" s="77"/>
-    </row>
-    <row r="16" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X15" s="76"/>
+      <c r="Y15" s="77"/>
+    </row>
+    <row r="16" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>2012</v>
       </c>
@@ -6502,8 +6552,10 @@
       <c r="U16" s="75"/>
       <c r="V16" s="76"/>
       <c r="W16" s="77"/>
-    </row>
-    <row r="17" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X16" s="76"/>
+      <c r="Y16" s="77"/>
+    </row>
+    <row r="17" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>2013</v>
       </c>
@@ -6552,8 +6604,10 @@
       <c r="U17" s="75"/>
       <c r="V17" s="76"/>
       <c r="W17" s="77"/>
-    </row>
-    <row r="18" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="76"/>
+      <c r="Y17" s="77"/>
+    </row>
+    <row r="18" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>2014</v>
       </c>
@@ -6603,8 +6657,10 @@
       <c r="U18" s="75"/>
       <c r="V18" s="76"/>
       <c r="W18" s="77"/>
-    </row>
-    <row r="19" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X18" s="76"/>
+      <c r="Y18" s="77"/>
+    </row>
+    <row r="19" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>2015</v>
       </c>
@@ -6654,8 +6710,10 @@
       <c r="U19" s="75"/>
       <c r="V19" s="76"/>
       <c r="W19" s="77"/>
-    </row>
-    <row r="20" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="76"/>
+      <c r="Y19" s="77"/>
+    </row>
+    <row r="20" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2016</v>
       </c>
@@ -6708,8 +6766,10 @@
       <c r="U20" s="75"/>
       <c r="V20" s="76"/>
       <c r="W20" s="77"/>
-    </row>
-    <row r="21" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X20" s="76"/>
+      <c r="Y20" s="77"/>
+    </row>
+    <row r="21" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>2017</v>
       </c>
@@ -6758,8 +6818,10 @@
       <c r="U21" s="75"/>
       <c r="V21" s="76"/>
       <c r="W21" s="77"/>
-    </row>
-    <row r="22" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="76"/>
+      <c r="Y21" s="77"/>
+    </row>
+    <row r="22" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>2018</v>
       </c>
@@ -6806,8 +6868,10 @@
       <c r="U22" s="75"/>
       <c r="V22" s="76"/>
       <c r="W22" s="77"/>
-    </row>
-    <row r="23" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X22" s="76"/>
+      <c r="Y22" s="77"/>
+    </row>
+    <row r="23" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>2019</v>
       </c>
@@ -6854,8 +6918,10 @@
       <c r="U23" s="75"/>
       <c r="V23" s="76"/>
       <c r="W23" s="77"/>
-    </row>
-    <row r="24" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="76"/>
+      <c r="Y23" s="77"/>
+    </row>
+    <row r="24" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31">
         <v>2020</v>
       </c>
@@ -6881,8 +6947,10 @@
       <c r="U24" s="75"/>
       <c r="V24" s="76"/>
       <c r="W24" s="77"/>
-    </row>
-    <row r="25" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X24" s="76"/>
+      <c r="Y24" s="77"/>
+    </row>
+    <row r="25" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31">
         <v>2021</v>
       </c>
@@ -6908,8 +6976,10 @@
       <c r="U25" s="75"/>
       <c r="V25" s="76"/>
       <c r="W25" s="77"/>
-    </row>
-    <row r="26" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X25" s="76"/>
+      <c r="Y25" s="77"/>
+    </row>
+    <row r="26" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>2022</v>
       </c>
@@ -6935,8 +7005,10 @@
       <c r="U26" s="75"/>
       <c r="V26" s="76"/>
       <c r="W26" s="77"/>
-    </row>
-    <row r="27" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X26" s="76"/>
+      <c r="Y26" s="77"/>
+    </row>
+    <row r="27" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
         <v>2023</v>
       </c>
@@ -6962,8 +7034,10 @@
       <c r="U27" s="75"/>
       <c r="V27" s="76"/>
       <c r="W27" s="77"/>
-    </row>
-    <row r="28" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X27" s="76"/>
+      <c r="Y27" s="77"/>
+    </row>
+    <row r="28" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
         <v>2024</v>
       </c>
@@ -6989,8 +7063,10 @@
       <c r="U28" s="75"/>
       <c r="V28" s="76"/>
       <c r="W28" s="77"/>
-    </row>
-    <row r="29" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X28" s="76"/>
+      <c r="Y28" s="77"/>
+    </row>
+    <row r="29" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
         <v>2025</v>
       </c>
@@ -7020,8 +7096,10 @@
       <c r="U29" s="75"/>
       <c r="V29" s="76"/>
       <c r="W29" s="77"/>
-    </row>
-    <row r="30" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X29" s="76"/>
+      <c r="Y29" s="77"/>
+    </row>
+    <row r="30" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31">
         <v>2026</v>
       </c>
@@ -7047,8 +7125,10 @@
       <c r="U30" s="75"/>
       <c r="V30" s="76"/>
       <c r="W30" s="77"/>
-    </row>
-    <row r="31" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X30" s="76"/>
+      <c r="Y30" s="77"/>
+    </row>
+    <row r="31" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
         <v>2027</v>
       </c>
@@ -7074,8 +7154,10 @@
       <c r="U31" s="75"/>
       <c r="V31" s="76"/>
       <c r="W31" s="77"/>
-    </row>
-    <row r="32" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X31" s="76"/>
+      <c r="Y31" s="77"/>
+    </row>
+    <row r="32" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31">
         <v>2028</v>
       </c>
@@ -7101,8 +7183,10 @@
       <c r="U32" s="75"/>
       <c r="V32" s="76"/>
       <c r="W32" s="77"/>
-    </row>
-    <row r="33" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X32" s="76"/>
+      <c r="Y32" s="77"/>
+    </row>
+    <row r="33" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31">
         <v>2029</v>
       </c>
@@ -7128,8 +7212,10 @@
       <c r="U33" s="75"/>
       <c r="V33" s="76"/>
       <c r="W33" s="77"/>
-    </row>
-    <row r="34" spans="1:23" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X33" s="76"/>
+      <c r="Y33" s="77"/>
+    </row>
+    <row r="34" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="63">
         <v>2030</v>
       </c>
@@ -7159,6 +7245,8 @@
       <c r="U34" s="78"/>
       <c r="V34" s="79"/>
       <c r="W34" s="80"/>
+      <c r="X34" s="79"/>
+      <c r="Y34" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated data and scenarios
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -1300,7 +1300,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1320,11 +1320,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Time between HIV tests (in years)</t>
+Proportion of diagnosed PLHIV who are on treatment</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1344,103 +1344,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Time between HIV tests (in years)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people within 1 year of infection</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people infected over 3 years ago</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people within 1 year of infection</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom Tidhar:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Time between tests for people infected over 3 years ago</t>
+Proportion of PLHIV on treatment who are virally suppressed</t>
         </r>
       </text>
     </comment>
@@ -1867,7 +1771,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="132">
   <si>
     <t>Waiting list</t>
   </si>
@@ -5937,8 +5841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:R1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6587,31 +6491,31 @@
         <v>0</v>
       </c>
       <c r="F16" s="62"/>
-      <c r="G16" s="194">
-        <v>0.6</v>
-      </c>
-      <c r="H16" s="195">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I16" s="196">
-        <v>0.6</v>
-      </c>
-      <c r="J16" s="195">
-        <v>4.4000000000000004</v>
+      <c r="G16" s="43">
+        <v>1.91</v>
+      </c>
+      <c r="H16" s="43">
+        <v>1.91</v>
+      </c>
+      <c r="I16" s="43">
+        <v>1.91</v>
+      </c>
+      <c r="J16" s="43">
+        <v>1.91</v>
       </c>
       <c r="K16" s="216"/>
       <c r="L16" s="218"/>
-      <c r="M16" s="194">
-        <v>0.5</v>
-      </c>
-      <c r="N16" s="195">
-        <v>3.3</v>
-      </c>
-      <c r="O16" s="196">
-        <v>0.5</v>
-      </c>
-      <c r="P16" s="195">
-        <v>3.3</v>
+      <c r="M16" s="43">
+        <v>2.37</v>
+      </c>
+      <c r="N16" s="43">
+        <v>2.37</v>
+      </c>
+      <c r="O16" s="43">
+        <v>2.37</v>
+      </c>
+      <c r="P16" s="43">
+        <v>2.37</v>
       </c>
       <c r="Q16" s="216"/>
       <c r="R16" s="77"/>
@@ -6639,31 +6543,31 @@
         <v>0</v>
       </c>
       <c r="F17" s="62"/>
-      <c r="G17" s="194">
-        <v>0.9</v>
-      </c>
-      <c r="H17" s="195">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="I17" s="196">
-        <v>0.9</v>
-      </c>
-      <c r="J17" s="195">
-        <v>4.9000000000000004</v>
+      <c r="G17" s="43">
+        <v>2.34</v>
+      </c>
+      <c r="H17" s="43">
+        <v>2.34</v>
+      </c>
+      <c r="I17" s="43">
+        <v>2.34</v>
+      </c>
+      <c r="J17" s="43">
+        <v>2.34</v>
       </c>
       <c r="K17" s="216"/>
       <c r="L17" s="218"/>
-      <c r="M17" s="194">
-        <v>0.6</v>
-      </c>
-      <c r="N17" s="195">
-        <v>4.2</v>
-      </c>
-      <c r="O17" s="196">
-        <v>0.6</v>
-      </c>
-      <c r="P17" s="195">
-        <v>4.2</v>
+      <c r="M17" s="43">
+        <v>2.84</v>
+      </c>
+      <c r="N17" s="43">
+        <v>2.84</v>
+      </c>
+      <c r="O17" s="43">
+        <v>2.84</v>
+      </c>
+      <c r="P17" s="43">
+        <v>2.84</v>
       </c>
       <c r="Q17" s="216"/>
       <c r="R17" s="77"/>
@@ -6692,31 +6596,31 @@
         <v>0</v>
       </c>
       <c r="F18" s="62"/>
-      <c r="G18" s="194">
-        <v>0.8</v>
-      </c>
-      <c r="H18" s="195">
-        <v>3.5</v>
-      </c>
-      <c r="I18" s="196">
-        <v>0.8</v>
-      </c>
-      <c r="J18" s="195">
-        <v>3.5</v>
+      <c r="G18" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="I18" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="J18" s="43">
+        <v>1.5</v>
       </c>
       <c r="K18" s="216"/>
       <c r="L18" s="218"/>
-      <c r="M18" s="194">
-        <v>0.8</v>
-      </c>
-      <c r="N18" s="195">
-        <v>1.7</v>
-      </c>
-      <c r="O18" s="196">
-        <v>0.8</v>
-      </c>
-      <c r="P18" s="195">
-        <v>1.7</v>
+      <c r="M18" s="43">
+        <v>0.96</v>
+      </c>
+      <c r="N18" s="43">
+        <v>0.96</v>
+      </c>
+      <c r="O18" s="43">
+        <v>0.96</v>
+      </c>
+      <c r="P18" s="43">
+        <v>0.96</v>
       </c>
       <c r="Q18" s="216"/>
       <c r="R18" s="77"/>
@@ -6745,31 +6649,31 @@
         <v>0</v>
       </c>
       <c r="F19" s="62"/>
-      <c r="G19" s="194">
-        <v>1.2</v>
-      </c>
-      <c r="H19" s="195">
-        <v>3.9</v>
-      </c>
-      <c r="I19" s="196">
-        <v>1.2</v>
-      </c>
-      <c r="J19" s="195">
-        <v>3.9</v>
+      <c r="G19" s="43">
+        <v>2.08</v>
+      </c>
+      <c r="H19" s="43">
+        <v>2.08</v>
+      </c>
+      <c r="I19" s="43">
+        <v>2.08</v>
+      </c>
+      <c r="J19" s="43">
+        <v>2.08</v>
       </c>
       <c r="K19" s="216"/>
       <c r="L19" s="218"/>
-      <c r="M19" s="194">
-        <v>0.9</v>
-      </c>
-      <c r="N19" s="195">
-        <v>2.4</v>
-      </c>
-      <c r="O19" s="196">
-        <v>0.9</v>
-      </c>
-      <c r="P19" s="195">
-        <v>2.4</v>
+      <c r="M19" s="43">
+        <v>1.45</v>
+      </c>
+      <c r="N19" s="43">
+        <v>1.45</v>
+      </c>
+      <c r="O19" s="43">
+        <v>1.45</v>
+      </c>
+      <c r="P19" s="43">
+        <v>1.45</v>
       </c>
       <c r="Q19" s="216"/>
       <c r="R19" s="77"/>
@@ -6801,31 +6705,31 @@
         <v>49.394274000000003</v>
       </c>
       <c r="F20" s="62"/>
-      <c r="G20" s="194">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H20" s="195">
-        <v>5.8</v>
-      </c>
-      <c r="I20" s="196">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J20" s="195">
-        <v>5.8</v>
+      <c r="G20" s="43">
+        <v>2.73</v>
+      </c>
+      <c r="H20" s="43">
+        <v>2.73</v>
+      </c>
+      <c r="I20" s="43">
+        <v>2.73</v>
+      </c>
+      <c r="J20" s="43">
+        <v>2.73</v>
       </c>
       <c r="K20" s="216"/>
       <c r="L20" s="218"/>
-      <c r="M20" s="194">
-        <v>2</v>
-      </c>
-      <c r="N20" s="195">
-        <v>3.5</v>
-      </c>
-      <c r="O20" s="196">
-        <v>2</v>
-      </c>
-      <c r="P20" s="195">
-        <v>3.5</v>
+      <c r="M20" s="43">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N20" s="43">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="O20" s="43">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="P20" s="43">
+        <v>2.5499999999999998</v>
       </c>
       <c r="Q20" s="216"/>
       <c r="R20" s="77"/>
@@ -6857,31 +6761,31 @@
         <v>131.75528800000001</v>
       </c>
       <c r="F21" s="62"/>
-      <c r="G21" s="194">
-        <v>1.7</v>
-      </c>
-      <c r="H21" s="195">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I21" s="196">
-        <v>1.7</v>
-      </c>
-      <c r="J21" s="195">
-        <v>4.0999999999999996</v>
+      <c r="G21" s="43">
+        <v>2.71</v>
+      </c>
+      <c r="H21" s="43">
+        <v>2.71</v>
+      </c>
+      <c r="I21" s="43">
+        <v>2.71</v>
+      </c>
+      <c r="J21" s="43">
+        <v>2.71</v>
       </c>
       <c r="K21" s="216"/>
       <c r="L21" s="218"/>
-      <c r="M21" s="194">
-        <v>0.9</v>
-      </c>
-      <c r="N21" s="195">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O21" s="196">
-        <v>0.9</v>
-      </c>
-      <c r="P21" s="195">
-        <v>4.0999999999999996</v>
+      <c r="M21" s="43">
+        <v>2.23</v>
+      </c>
+      <c r="N21" s="43">
+        <v>2.23</v>
+      </c>
+      <c r="O21" s="43">
+        <v>2.23</v>
+      </c>
+      <c r="P21" s="43">
+        <v>2.23</v>
       </c>
       <c r="Q21" s="216"/>
       <c r="R21" s="217"/>
@@ -6907,31 +6811,31 @@
         <v>149.30809600000001</v>
       </c>
       <c r="F22" s="62"/>
-      <c r="G22" s="194">
-        <v>1.4</v>
-      </c>
-      <c r="H22" s="195">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="I22" s="196">
-        <v>1.4</v>
-      </c>
-      <c r="J22" s="195">
-        <v>4.5999999999999996</v>
+      <c r="G22" s="43">
+        <v>2.75</v>
+      </c>
+      <c r="H22" s="43">
+        <v>2.75</v>
+      </c>
+      <c r="I22" s="43">
+        <v>2.75</v>
+      </c>
+      <c r="J22" s="43">
+        <v>2.75</v>
       </c>
       <c r="K22" s="216"/>
       <c r="L22" s="218"/>
-      <c r="M22" s="194">
-        <v>0.6</v>
-      </c>
-      <c r="N22" s="195">
-        <v>4</v>
-      </c>
-      <c r="O22" s="196">
-        <v>0.6</v>
-      </c>
-      <c r="P22" s="195">
-        <v>4</v>
+      <c r="M22" s="43">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="N22" s="43">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="O22" s="43">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="P22" s="43">
+        <v>2.2599999999999998</v>
       </c>
       <c r="Q22" s="216"/>
       <c r="R22" s="77"/>
@@ -6957,32 +6861,16 @@
         <v>164.58356600000002</v>
       </c>
       <c r="F23" s="62"/>
-      <c r="G23" s="194">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H23" s="195">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I23" s="196">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J23" s="195">
-        <v>4.0999999999999996</v>
-      </c>
+      <c r="G23" s="194"/>
+      <c r="H23" s="195"/>
+      <c r="I23" s="196"/>
+      <c r="J23" s="195"/>
       <c r="K23" s="216"/>
       <c r="L23" s="218"/>
-      <c r="M23" s="194">
-        <v>0.5</v>
-      </c>
-      <c r="N23" s="195">
-        <v>3.6</v>
-      </c>
-      <c r="O23" s="196">
-        <v>0.5</v>
-      </c>
-      <c r="P23" s="195">
-        <v>3.6</v>
-      </c>
+      <c r="M23" s="194"/>
+      <c r="N23" s="195"/>
+      <c r="O23" s="196"/>
+      <c r="P23" s="195"/>
       <c r="Q23" s="216"/>
       <c r="R23" s="77"/>
       <c r="S23" s="76"/>
@@ -7532,533 +7420,219 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="43"/>
+    <col min="2" max="2" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="163" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="164" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="163" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="164" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="163" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="164" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="163" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="164" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="68" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="165" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="166" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="165" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="166" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="I2" s="165" t="s">
-        <v>125</v>
-      </c>
-      <c r="J2" s="166" t="s">
-        <v>126</v>
-      </c>
-      <c r="K2" s="165" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" s="166" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" s="71" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="70"/>
+      <c r="C2" s="71"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="219" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="220" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="221" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" s="220" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" s="221" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="222" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2000</v>
       </c>
-      <c r="B4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="C4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="D4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="F4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="G4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="H4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="I4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="J4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="K4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="L4" s="168">
-        <v>0.25</v>
-      </c>
-      <c r="M4" s="168">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+    </row>
+    <row r="5" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2001</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="169"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="169"/>
-      <c r="L5" s="170"/>
-      <c r="M5" s="77"/>
-    </row>
-    <row r="6" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+    </row>
+    <row r="6" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>2002</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="169"/>
-      <c r="J6" s="170"/>
-      <c r="K6" s="169"/>
-      <c r="L6" s="170"/>
-      <c r="M6" s="77"/>
-    </row>
-    <row r="7" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="76"/>
+      <c r="C6" s="77"/>
+    </row>
+    <row r="7" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>2003</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="169"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="169"/>
-      <c r="L7" s="170"/>
-      <c r="M7" s="77"/>
-    </row>
-    <row r="8" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="76"/>
+      <c r="C7" s="77"/>
+    </row>
+    <row r="8" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>2004</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="169"/>
-      <c r="J8" s="170"/>
-      <c r="K8" s="169"/>
-      <c r="L8" s="170"/>
-      <c r="M8" s="77"/>
-    </row>
-    <row r="9" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
+    </row>
+    <row r="9" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>2005</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="169"/>
-      <c r="J9" s="170"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="170"/>
-      <c r="M9" s="77"/>
-    </row>
-    <row r="10" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="76"/>
+      <c r="C9" s="77"/>
+    </row>
+    <row r="10" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2006</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="169"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="169"/>
-      <c r="J10" s="170"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="170"/>
-      <c r="M10" s="77"/>
-    </row>
-    <row r="11" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="76"/>
+      <c r="C10" s="77"/>
+    </row>
+    <row r="11" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2007</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="169"/>
-      <c r="D11" s="170"/>
-      <c r="E11" s="169"/>
-      <c r="F11" s="170"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="169"/>
-      <c r="J11" s="170"/>
-      <c r="K11" s="169"/>
-      <c r="L11" s="170"/>
-      <c r="M11" s="77"/>
-    </row>
-    <row r="12" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="76">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2008</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="169"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="169"/>
-      <c r="F12" s="170"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="169"/>
-      <c r="J12" s="170"/>
-      <c r="K12" s="169"/>
-      <c r="L12" s="170"/>
-      <c r="M12" s="77"/>
-    </row>
-    <row r="13" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="76"/>
+      <c r="C12" s="77"/>
+    </row>
+    <row r="13" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2009</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="169"/>
-      <c r="D13" s="170"/>
-      <c r="E13" s="169"/>
-      <c r="F13" s="170"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="169"/>
-      <c r="J13" s="170"/>
-      <c r="K13" s="169"/>
-      <c r="L13" s="216"/>
-      <c r="M13" s="217"/>
-    </row>
-    <row r="14" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="76"/>
+      <c r="C13" s="77"/>
+    </row>
+    <row r="14" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>2010</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="169"/>
-      <c r="D14" s="170"/>
-      <c r="E14" s="169"/>
-      <c r="F14" s="216"/>
-      <c r="G14" s="217"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="169"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="169"/>
-      <c r="L14" s="216"/>
-      <c r="M14" s="217"/>
-    </row>
-    <row r="15" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="76">
+        <v>0.75</v>
+      </c>
+      <c r="C14" s="77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>2011</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="170"/>
-      <c r="E15" s="169"/>
-      <c r="F15" s="216"/>
-      <c r="G15" s="217"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="169"/>
-      <c r="J15" s="170"/>
-      <c r="K15" s="169"/>
-      <c r="L15" s="216"/>
-      <c r="M15" s="217"/>
-    </row>
-    <row r="16" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="76"/>
+      <c r="C15" s="77"/>
+    </row>
+    <row r="16" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>2012</v>
       </c>
-      <c r="B16" s="194"/>
-      <c r="C16" s="195"/>
-      <c r="D16" s="196"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="216"/>
-      <c r="G16" s="218"/>
-      <c r="H16" s="194"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="196"/>
-      <c r="K16" s="195"/>
-      <c r="L16" s="216"/>
-      <c r="M16" s="77"/>
-    </row>
-    <row r="17" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="76">
+        <v>0.82</v>
+      </c>
+      <c r="C16" s="77">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>2013</v>
       </c>
-      <c r="B17" s="194"/>
-      <c r="C17" s="195"/>
-      <c r="D17" s="196"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="216"/>
-      <c r="G17" s="218"/>
-      <c r="H17" s="194"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="196"/>
-      <c r="K17" s="195"/>
-      <c r="L17" s="216"/>
-      <c r="M17" s="77"/>
-    </row>
-    <row r="18" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="76">
+        <v>0.86</v>
+      </c>
+      <c r="C17" s="77">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>2014</v>
       </c>
-      <c r="B18" s="194"/>
-      <c r="C18" s="195"/>
-      <c r="D18" s="196"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="216"/>
-      <c r="G18" s="218"/>
-      <c r="H18" s="194"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="196"/>
-      <c r="K18" s="195"/>
-      <c r="L18" s="216"/>
-      <c r="M18" s="77"/>
-    </row>
-    <row r="19" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="76">
+        <v>0.89</v>
+      </c>
+      <c r="C18" s="77">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>2015</v>
       </c>
-      <c r="B19" s="194"/>
-      <c r="C19" s="195"/>
-      <c r="D19" s="196"/>
-      <c r="E19" s="195"/>
-      <c r="F19" s="216"/>
-      <c r="G19" s="218"/>
-      <c r="H19" s="194"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="196"/>
-      <c r="K19" s="195"/>
-      <c r="L19" s="216"/>
-      <c r="M19" s="77"/>
-    </row>
-    <row r="20" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="76">
+        <v>0.92</v>
+      </c>
+      <c r="C19" s="77">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2016</v>
       </c>
-      <c r="B20" s="194"/>
-      <c r="C20" s="195"/>
-      <c r="D20" s="196"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="216"/>
-      <c r="G20" s="218"/>
-      <c r="H20" s="194"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="196"/>
-      <c r="K20" s="195"/>
-      <c r="L20" s="216"/>
-      <c r="M20" s="77"/>
-    </row>
-    <row r="21" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="76"/>
+      <c r="C20" s="77"/>
+    </row>
+    <row r="21" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>2017</v>
       </c>
-      <c r="B21" s="194"/>
-      <c r="C21" s="195"/>
-      <c r="D21" s="196"/>
-      <c r="E21" s="195"/>
-      <c r="F21" s="216"/>
-      <c r="G21" s="218"/>
-      <c r="H21" s="194"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="196"/>
-      <c r="K21" s="195"/>
-      <c r="L21" s="216"/>
-      <c r="M21" s="217"/>
-    </row>
-    <row r="22" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="76"/>
+      <c r="C21" s="77"/>
+    </row>
+    <row r="22" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>2018</v>
       </c>
-      <c r="B22" s="194"/>
-      <c r="C22" s="195"/>
-      <c r="D22" s="196"/>
-      <c r="E22" s="195"/>
-      <c r="F22" s="216"/>
-      <c r="G22" s="218"/>
-      <c r="H22" s="194"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="196"/>
-      <c r="K22" s="195"/>
-      <c r="L22" s="216"/>
-      <c r="M22" s="77"/>
-    </row>
-    <row r="23" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="76"/>
+      <c r="C22" s="77"/>
+    </row>
+    <row r="23" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>2019</v>
       </c>
-      <c r="B23" s="194"/>
-      <c r="C23" s="195"/>
-      <c r="D23" s="196"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="216"/>
-      <c r="G23" s="218"/>
-      <c r="H23" s="194"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="196"/>
-      <c r="K23" s="195"/>
-      <c r="L23" s="216"/>
-      <c r="M23" s="77"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="76"/>
+      <c r="C23" s="77"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="44">
         <v>2020</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="171"/>
-      <c r="D24" s="172"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="171"/>
-      <c r="J24" s="172"/>
-      <c r="K24" s="171"/>
-      <c r="L24" s="172"/>
-      <c r="M24" s="80"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="77"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated data and calibration
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -5841,8 +5841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6108,10 +6108,10 @@
       <c r="O4" s="168"/>
       <c r="P4" s="167"/>
       <c r="Q4" s="168">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R4" s="74">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S4" s="73"/>
       <c r="T4" s="74"/>

</xml_diff>

<commit_message>
Added in Kat's data
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -1062,6 +1062,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="X1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kathleen Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+source: https://research.treasury.gov.au/external-paper/shaping-a-nation/</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1300,6 +1324,30 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Time between HIV tests (in years)</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1320,7 +1368,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Proportion of diagnosed PLHIV who are on treatment</t>
+Time between tests for people within 1 year of infection</t>
         </r>
       </text>
     </comment>
@@ -1344,7 +1392,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Proportion of PLHIV on treatment who are virally suppressed</t>
+Time between tests for people infected over 3 years ago</t>
         </r>
       </text>
     </comment>
@@ -1771,7 +1819,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="132">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2180,7 +2228,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2233,12 +2281,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2302,6 +2344,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3063,11 +3130,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3092,17 +3159,17 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="13" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3124,27 +3191,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="13" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="13" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="8" fillId="4" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -3204,10 +3271,10 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3215,67 +3282,66 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
@@ -3296,21 +3362,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3343,77 +3409,77 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
@@ -3430,6 +3496,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4245,7 +4323,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4281,139 +4359,153 @@
     <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+    <row r="1" spans="1:32" s="118" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="110" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="111" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="113" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="115" t="s">
+      <c r="F1" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="112" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="115" t="s">
+      <c r="I1" s="114" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="112" t="s">
+      <c r="J1" s="111" t="s">
         <v>122</v>
       </c>
-      <c r="K1" s="113" t="s">
+      <c r="K1" s="112" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="111" t="s">
+      <c r="L1" s="110" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="112" t="s">
+      <c r="M1" s="111" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="113" t="s">
+      <c r="N1" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="149" t="s">
+      <c r="O1" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="117" t="s">
+      <c r="P1" s="115"/>
+      <c r="Q1" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="117" t="s">
+      <c r="R1" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="117" t="s">
+      <c r="S1" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="117" t="s">
+      <c r="T1" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="117" t="s">
+      <c r="U1" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="117" t="s">
+      <c r="V1" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="W1" s="117" t="s">
+      <c r="W1" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="117" t="s">
+      <c r="X1" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="117" t="s">
+      <c r="Y1" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="117" t="s">
+      <c r="Z1" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="117" t="s">
+      <c r="AA1" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="117" t="s">
+      <c r="AB1" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="117" t="s">
+      <c r="AC1" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="118" t="s">
+      <c r="AD1" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="197" t="s">
+      <c r="AE1" s="196" t="s">
         <v>115</v>
       </c>
-      <c r="AF1" s="197" t="s">
+      <c r="AF1" s="196" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="200">
+      <c r="A2" s="199">
         <v>2006</v>
       </c>
-      <c r="B2" s="201"/>
-      <c r="C2" s="211"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="204"/>
-      <c r="I2" s="205"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="203"/>
-      <c r="L2" s="201"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="203"/>
-      <c r="O2" s="206"/>
-      <c r="P2" s="207"/>
-      <c r="Q2" s="208"/>
-      <c r="R2" s="208"/>
-      <c r="S2" s="208"/>
-      <c r="T2" s="208"/>
-      <c r="U2" s="208"/>
-      <c r="V2" s="208"/>
-      <c r="W2" s="208"/>
-      <c r="X2" s="208"/>
-      <c r="Y2" s="208"/>
-      <c r="Z2" s="208"/>
-      <c r="AA2" s="208"/>
-      <c r="AB2" s="208"/>
-      <c r="AC2" s="208"/>
-      <c r="AD2" s="209"/>
-      <c r="AE2" s="193">
+      <c r="B2" s="200"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="103">
+        <v>199</v>
+      </c>
+      <c r="F2" s="104">
+        <v>186</v>
+      </c>
+      <c r="G2" s="223">
+        <v>13</v>
+      </c>
+      <c r="H2" s="203">
+        <v>81</v>
+      </c>
+      <c r="I2" s="204">
+        <v>105</v>
+      </c>
+      <c r="J2" s="201">
+        <v>6</v>
+      </c>
+      <c r="K2" s="202">
+        <v>7</v>
+      </c>
+      <c r="L2" s="200"/>
+      <c r="M2" s="201"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="205"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="207"/>
+      <c r="R2" s="207"/>
+      <c r="S2" s="207"/>
+      <c r="T2" s="207"/>
+      <c r="U2" s="207"/>
+      <c r="V2" s="207"/>
+      <c r="W2" s="207"/>
+      <c r="X2" s="207"/>
+      <c r="Y2" s="207"/>
+      <c r="Z2" s="207"/>
+      <c r="AA2" s="207"/>
+      <c r="AB2" s="207"/>
+      <c r="AC2" s="207"/>
+      <c r="AD2" s="208"/>
+      <c r="AE2" s="192">
         <v>30713</v>
       </c>
-      <c r="AF2" s="193">
+      <c r="AF2" s="192">
         <v>30713</v>
       </c>
     </row>
@@ -4421,20 +4513,34 @@
       <c r="A3" s="10">
         <v>2007</v>
       </c>
-      <c r="B3" s="189"/>
-      <c r="C3" s="211"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="212"/>
-      <c r="K3" s="105"/>
+      <c r="B3" s="188"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="103">
+        <v>184</v>
+      </c>
+      <c r="F3" s="104">
+        <v>167</v>
+      </c>
+      <c r="G3" s="224">
+        <v>17</v>
+      </c>
+      <c r="H3" s="103">
+        <v>69</v>
+      </c>
+      <c r="I3" s="104">
+        <v>98</v>
+      </c>
+      <c r="J3" s="211">
+        <v>7</v>
+      </c>
+      <c r="K3" s="105">
+        <v>10</v>
+      </c>
       <c r="L3" s="106"/>
       <c r="M3" s="107"/>
       <c r="N3" s="108"/>
-      <c r="O3" s="150">
+      <c r="O3" s="149">
         <v>0.7</v>
       </c>
       <c r="P3" s="96"/>
@@ -4485,8 +4591,8 @@
         <v>113.70439800000001</v>
       </c>
       <c r="AD3" s="13"/>
-      <c r="AE3" s="199"/>
-      <c r="AF3" s="210">
+      <c r="AE3" s="198"/>
+      <c r="AF3" s="209">
         <f>AF2+532.4</f>
         <v>31245.4</v>
       </c>
@@ -4495,34 +4601,48 @@
       <c r="A4" s="10">
         <v>2008</v>
       </c>
-      <c r="B4" s="189">
+      <c r="B4" s="188">
         <f>SUM(C4:D4)</f>
         <v>27291.800000000003</v>
       </c>
-      <c r="C4" s="211">
+      <c r="C4" s="210">
         <f t="shared" ref="C4:C15" si="3">AF4-(D4+L4)</f>
         <v>27291.800000000003</v>
       </c>
-      <c r="D4" s="183"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="212"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="189">
+      <c r="D4" s="182"/>
+      <c r="E4" s="226">
+        <v>181</v>
+      </c>
+      <c r="F4" s="104">
+        <v>165</v>
+      </c>
+      <c r="G4" s="224">
+        <v>16</v>
+      </c>
+      <c r="H4" s="103">
+        <v>71</v>
+      </c>
+      <c r="I4" s="104">
+        <v>94</v>
+      </c>
+      <c r="J4" s="211">
+        <v>8</v>
+      </c>
+      <c r="K4" s="105">
+        <v>8</v>
+      </c>
+      <c r="L4" s="188">
         <v>4486</v>
       </c>
-      <c r="M4" s="193">
+      <c r="M4" s="192">
         <f>L4*0.78</f>
         <v>3499.08</v>
       </c>
-      <c r="N4" s="183">
+      <c r="N4" s="182">
         <f>L4*0.22</f>
         <v>986.92</v>
       </c>
-      <c r="O4" s="151"/>
+      <c r="O4" s="150"/>
       <c r="P4" s="97"/>
       <c r="Q4" s="40"/>
       <c r="R4" s="40"/>
@@ -4561,8 +4681,8 @@
         <v>104.106708</v>
       </c>
       <c r="AD4" s="13"/>
-      <c r="AE4" s="199"/>
-      <c r="AF4" s="210">
+      <c r="AE4" s="198"/>
+      <c r="AF4" s="209">
         <f t="shared" ref="AF4:AF7" si="7">AF3+532.4</f>
         <v>31777.800000000003</v>
       </c>
@@ -4571,34 +4691,48 @@
       <c r="A5" s="10">
         <v>2009</v>
       </c>
-      <c r="B5" s="189">
+      <c r="B5" s="188">
         <f t="shared" ref="B5:B15" si="8">SUM(C5:D5)</f>
         <v>27545.200000000004</v>
       </c>
-      <c r="C5" s="211">
+      <c r="C5" s="210">
         <f t="shared" si="3"/>
         <v>27545.200000000004</v>
       </c>
-      <c r="D5" s="183"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="212"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="189">
+      <c r="D5" s="182"/>
+      <c r="E5" s="225">
+        <v>197</v>
+      </c>
+      <c r="F5" s="104">
+        <v>183</v>
+      </c>
+      <c r="G5" s="224">
+        <v>14</v>
+      </c>
+      <c r="H5" s="103">
+        <v>85</v>
+      </c>
+      <c r="I5" s="104">
+        <v>98</v>
+      </c>
+      <c r="J5" s="211">
+        <v>7</v>
+      </c>
+      <c r="K5" s="105">
+        <v>7</v>
+      </c>
+      <c r="L5" s="188">
         <v>4765</v>
       </c>
-      <c r="M5" s="193">
+      <c r="M5" s="192">
         <f t="shared" ref="M5:M14" si="9">L5*0.78</f>
         <v>3716.7000000000003</v>
       </c>
-      <c r="N5" s="183">
+      <c r="N5" s="182">
         <f t="shared" ref="N5:N14" si="10">L5*0.22</f>
         <v>1048.3</v>
       </c>
-      <c r="O5" s="151"/>
+      <c r="O5" s="150"/>
       <c r="P5" s="97"/>
       <c r="Q5" s="40"/>
       <c r="R5" s="40"/>
@@ -4637,8 +4771,8 @@
         <v>167.11272000000002</v>
       </c>
       <c r="AD5" s="14"/>
-      <c r="AE5" s="199"/>
-      <c r="AF5" s="210">
+      <c r="AE5" s="198"/>
+      <c r="AF5" s="209">
         <f t="shared" si="7"/>
         <v>32310.200000000004</v>
       </c>
@@ -4647,36 +4781,50 @@
       <c r="A6" s="10">
         <v>2010</v>
       </c>
-      <c r="B6" s="189">
+      <c r="B6" s="188">
         <f t="shared" si="8"/>
         <v>27788.600000000006</v>
       </c>
-      <c r="C6" s="211">
+      <c r="C6" s="210">
         <f t="shared" si="3"/>
         <v>26472.496600000006</v>
       </c>
-      <c r="D6" s="184">
+      <c r="D6" s="183">
         <v>1316.1034</v>
       </c>
-      <c r="E6" s="120"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="212"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="189">
+      <c r="E6" s="119">
+        <v>174</v>
+      </c>
+      <c r="F6" s="104">
+        <v>153</v>
+      </c>
+      <c r="G6" s="224">
+        <v>21</v>
+      </c>
+      <c r="H6" s="103">
+        <v>85</v>
+      </c>
+      <c r="I6" s="104">
+        <v>68</v>
+      </c>
+      <c r="J6" s="211">
+        <v>7</v>
+      </c>
+      <c r="K6" s="105">
+        <v>14</v>
+      </c>
+      <c r="L6" s="188">
         <v>5054</v>
       </c>
-      <c r="M6" s="193">
+      <c r="M6" s="192">
         <f t="shared" si="9"/>
         <v>3942.1200000000003</v>
       </c>
-      <c r="N6" s="183">
+      <c r="N6" s="182">
         <f t="shared" si="10"/>
         <v>1111.8800000000001</v>
       </c>
-      <c r="O6" s="150"/>
+      <c r="O6" s="149"/>
       <c r="P6" s="97"/>
       <c r="Q6" s="40">
         <v>4.0273972602739724E-2</v>
@@ -4725,8 +4873,8 @@
         <v>198.50281199999998</v>
       </c>
       <c r="AD6" s="14"/>
-      <c r="AE6" s="199"/>
-      <c r="AF6" s="210">
+      <c r="AE6" s="198"/>
+      <c r="AF6" s="209">
         <f t="shared" si="7"/>
         <v>32842.600000000006</v>
       </c>
@@ -4735,36 +4883,50 @@
       <c r="A7" s="10">
         <v>2011</v>
       </c>
-      <c r="B7" s="189">
+      <c r="B7" s="188">
         <f>SUM(C7:D7)</f>
         <v>28074.000000000007</v>
       </c>
-      <c r="C7" s="211">
+      <c r="C7" s="210">
         <f t="shared" si="3"/>
         <v>26900.372400000007</v>
       </c>
-      <c r="D7" s="184">
+      <c r="D7" s="183">
         <v>1173.6276</v>
       </c>
-      <c r="E7" s="120"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="213"/>
-      <c r="K7" s="214"/>
-      <c r="L7" s="189">
+      <c r="E7" s="119">
+        <v>210</v>
+      </c>
+      <c r="F7" s="104">
+        <v>190</v>
+      </c>
+      <c r="G7" s="224">
+        <v>20</v>
+      </c>
+      <c r="H7" s="119">
+        <v>99</v>
+      </c>
+      <c r="I7" s="121">
+        <v>91</v>
+      </c>
+      <c r="J7" s="212">
+        <v>7</v>
+      </c>
+      <c r="K7" s="213">
+        <v>13</v>
+      </c>
+      <c r="L7" s="188">
         <v>5301</v>
       </c>
-      <c r="M7" s="193">
+      <c r="M7" s="192">
         <f t="shared" si="9"/>
         <v>4134.78</v>
       </c>
-      <c r="N7" s="183">
+      <c r="N7" s="182">
         <f t="shared" si="10"/>
         <v>1166.22</v>
       </c>
-      <c r="O7" s="151"/>
+      <c r="O7" s="150"/>
       <c r="P7" s="97"/>
       <c r="Q7" s="40">
         <v>3.7534246575342468E-2</v>
@@ -4813,10 +4975,10 @@
         <v>210.35878200000002</v>
       </c>
       <c r="AD7" s="14"/>
-      <c r="AE7" s="193">
+      <c r="AE7" s="192">
         <v>33375</v>
       </c>
-      <c r="AF7" s="210">
+      <c r="AF7" s="209">
         <f t="shared" si="7"/>
         <v>33375.000000000007</v>
       </c>
@@ -4825,50 +4987,50 @@
       <c r="A8" s="10">
         <v>2012</v>
       </c>
-      <c r="B8" s="189">
+      <c r="B8" s="188">
         <f t="shared" si="8"/>
         <v>28353.000000000007</v>
       </c>
-      <c r="C8" s="211">
+      <c r="C8" s="210">
         <f t="shared" si="3"/>
         <v>27248.744400000007</v>
       </c>
-      <c r="D8" s="184">
+      <c r="D8" s="183">
         <v>1104.2556</v>
       </c>
-      <c r="E8" s="185">
+      <c r="E8" s="184">
         <v>206</v>
       </c>
-      <c r="F8" s="186">
+      <c r="F8" s="185">
         <v>172</v>
       </c>
-      <c r="G8" s="187">
+      <c r="G8" s="186">
         <v>34</v>
       </c>
       <c r="H8" s="185">
+        <v>101</v>
+      </c>
+      <c r="I8" s="184">
         <v>71</v>
       </c>
-      <c r="I8" s="186">
-        <v>101</v>
-      </c>
-      <c r="J8" s="223">
+      <c r="J8" s="186">
+        <v>10</v>
+      </c>
+      <c r="K8" s="222">
         <v>24</v>
       </c>
-      <c r="K8" s="187">
-        <v>10</v>
-      </c>
-      <c r="L8" s="189">
+      <c r="L8" s="188">
         <v>5610</v>
       </c>
-      <c r="M8" s="193">
+      <c r="M8" s="192">
         <f t="shared" si="9"/>
         <v>4375.8</v>
       </c>
-      <c r="N8" s="183">
+      <c r="N8" s="182">
         <f t="shared" si="10"/>
         <v>1234.2</v>
       </c>
-      <c r="O8" s="150">
+      <c r="O8" s="149">
         <v>0.91200000000000003</v>
       </c>
       <c r="P8" s="97"/>
@@ -4919,8 +5081,8 @@
         <v>275.05850400000003</v>
       </c>
       <c r="AD8" s="14"/>
-      <c r="AE8" s="199"/>
-      <c r="AF8" s="199">
+      <c r="AE8" s="198"/>
+      <c r="AF8" s="198">
         <f>AF7+588</f>
         <v>33963.000000000007</v>
       </c>
@@ -4929,50 +5091,50 @@
       <c r="A9" s="10">
         <v>2013</v>
       </c>
-      <c r="B9" s="189">
+      <c r="B9" s="188">
         <f t="shared" si="8"/>
         <v>28657.000000000007</v>
       </c>
-      <c r="C9" s="211">
+      <c r="C9" s="210">
         <f t="shared" si="3"/>
         <v>27511.205800000007</v>
       </c>
-      <c r="D9" s="184">
+      <c r="D9" s="183">
         <v>1145.7942</v>
       </c>
-      <c r="E9" s="185">
+      <c r="E9" s="184">
         <v>233</v>
       </c>
-      <c r="F9" s="186">
+      <c r="F9" s="185">
         <v>184</v>
       </c>
-      <c r="G9" s="187">
+      <c r="G9" s="186">
         <v>49</v>
       </c>
       <c r="H9" s="185">
+        <v>106</v>
+      </c>
+      <c r="I9" s="184">
         <v>78</v>
       </c>
-      <c r="I9" s="186">
-        <v>106</v>
-      </c>
-      <c r="J9" s="223">
+      <c r="J9" s="186">
+        <v>14</v>
+      </c>
+      <c r="K9" s="222">
         <v>35</v>
       </c>
-      <c r="K9" s="187">
-        <v>14</v>
-      </c>
-      <c r="L9" s="189">
+      <c r="L9" s="188">
         <v>5894</v>
       </c>
-      <c r="M9" s="193">
+      <c r="M9" s="192">
         <f t="shared" si="9"/>
         <v>4597.32</v>
       </c>
-      <c r="N9" s="183">
+      <c r="N9" s="182">
         <f t="shared" si="10"/>
         <v>1296.68</v>
       </c>
-      <c r="O9" s="150"/>
+      <c r="O9" s="149"/>
       <c r="P9" s="97"/>
       <c r="Q9" s="40">
         <v>5.2876712328767124E-2</v>
@@ -5021,8 +5183,8 @@
         <v>336.25789200000003</v>
       </c>
       <c r="AD9" s="14"/>
-      <c r="AE9" s="199"/>
-      <c r="AF9" s="199">
+      <c r="AE9" s="198"/>
+      <c r="AF9" s="198">
         <f t="shared" ref="AF9:AF15" si="13">AF8+588</f>
         <v>34551.000000000007</v>
       </c>
@@ -5031,50 +5193,50 @@
       <c r="A10" s="10">
         <v>2014</v>
       </c>
-      <c r="B10" s="189">
+      <c r="B10" s="188">
         <f t="shared" si="8"/>
         <v>28939.000000000007</v>
       </c>
-      <c r="C10" s="211">
+      <c r="C10" s="210">
         <f t="shared" si="3"/>
         <v>27635.934400000006</v>
       </c>
-      <c r="D10" s="184">
+      <c r="D10" s="183">
         <v>1303.0656000000001</v>
       </c>
-      <c r="E10" s="185">
+      <c r="E10" s="184">
         <v>235</v>
       </c>
-      <c r="F10" s="186">
+      <c r="F10" s="185">
         <v>200</v>
       </c>
-      <c r="G10" s="187">
+      <c r="G10" s="186">
         <v>35</v>
       </c>
       <c r="H10" s="185">
+        <v>133</v>
+      </c>
+      <c r="I10" s="184">
         <v>67</v>
       </c>
-      <c r="I10" s="186">
-        <v>133</v>
-      </c>
-      <c r="J10" s="223">
+      <c r="J10" s="186">
+        <v>25</v>
+      </c>
+      <c r="K10" s="222">
         <v>10</v>
       </c>
-      <c r="K10" s="187">
-        <v>25</v>
-      </c>
-      <c r="L10" s="189">
+      <c r="L10" s="188">
         <v>6200</v>
       </c>
-      <c r="M10" s="193">
+      <c r="M10" s="192">
         <f t="shared" si="9"/>
         <v>4836</v>
       </c>
-      <c r="N10" s="183">
+      <c r="N10" s="182">
         <f t="shared" si="10"/>
         <v>1364</v>
       </c>
-      <c r="O10" s="150">
+      <c r="O10" s="149">
         <v>0.88</v>
       </c>
       <c r="P10" s="97"/>
@@ -5125,8 +5287,8 @@
         <v>369.11586600000004</v>
       </c>
       <c r="AD10" s="14"/>
-      <c r="AE10" s="199"/>
-      <c r="AF10" s="199">
+      <c r="AE10" s="198"/>
+      <c r="AF10" s="198">
         <f t="shared" si="13"/>
         <v>35139.000000000007</v>
       </c>
@@ -5135,50 +5297,50 @@
       <c r="A11" s="10">
         <v>2015</v>
       </c>
-      <c r="B11" s="189">
+      <c r="B11" s="188">
         <f t="shared" si="8"/>
         <v>29178.000000000007</v>
       </c>
-      <c r="C11" s="211">
+      <c r="C11" s="210">
         <f t="shared" si="3"/>
         <v>27722.579200000007</v>
       </c>
-      <c r="D11" s="184">
+      <c r="D11" s="183">
         <v>1455.4208000000001</v>
       </c>
-      <c r="E11" s="185">
+      <c r="E11" s="184">
         <v>218</v>
       </c>
-      <c r="F11" s="186">
+      <c r="F11" s="185">
         <v>177</v>
       </c>
-      <c r="G11" s="187">
+      <c r="G11" s="186">
         <v>41</v>
       </c>
       <c r="H11" s="185">
+        <v>115</v>
+      </c>
+      <c r="I11" s="184">
         <v>62</v>
       </c>
-      <c r="I11" s="186">
-        <v>115</v>
-      </c>
-      <c r="J11" s="223">
+      <c r="J11" s="186">
+        <v>23</v>
+      </c>
+      <c r="K11" s="222">
         <v>18</v>
       </c>
-      <c r="K11" s="187">
-        <v>23</v>
-      </c>
-      <c r="L11" s="189">
+      <c r="L11" s="188">
         <v>6549</v>
       </c>
-      <c r="M11" s="193">
+      <c r="M11" s="192">
         <f t="shared" si="9"/>
         <v>5108.22</v>
       </c>
-      <c r="N11" s="183">
+      <c r="N11" s="182">
         <f t="shared" si="10"/>
         <v>1440.78</v>
       </c>
-      <c r="O11" s="150">
+      <c r="O11" s="149">
         <v>0.88</v>
       </c>
       <c r="P11" s="97"/>
@@ -5229,8 +5391,8 @@
         <v>549.32661000000007</v>
       </c>
       <c r="AD11" s="14"/>
-      <c r="AE11" s="199"/>
-      <c r="AF11" s="199">
+      <c r="AE11" s="198"/>
+      <c r="AF11" s="198">
         <f t="shared" si="13"/>
         <v>35727.000000000007</v>
       </c>
@@ -5239,50 +5401,50 @@
       <c r="A12" s="10">
         <v>2016</v>
       </c>
-      <c r="B12" s="189">
+      <c r="B12" s="188">
         <f>SUM(C12:D12)</f>
         <v>29456.000000000007</v>
       </c>
-      <c r="C12" s="211">
+      <c r="C12" s="210">
         <f t="shared" si="3"/>
         <v>27809.524200000007</v>
       </c>
-      <c r="D12" s="184">
+      <c r="D12" s="183">
         <v>1646.4758000000002</v>
       </c>
-      <c r="E12" s="185">
+      <c r="E12" s="184">
         <v>244</v>
       </c>
-      <c r="F12" s="186">
+      <c r="F12" s="185">
         <v>180</v>
       </c>
-      <c r="G12" s="187">
+      <c r="G12" s="186">
         <v>64</v>
       </c>
       <c r="H12" s="185">
+        <v>102</v>
+      </c>
+      <c r="I12" s="184">
         <v>78</v>
       </c>
-      <c r="I12" s="186">
-        <v>102</v>
-      </c>
-      <c r="J12" s="223">
+      <c r="J12" s="186">
         <v>32</v>
       </c>
-      <c r="K12" s="187">
+      <c r="K12" s="222">
         <v>32</v>
       </c>
-      <c r="L12" s="189">
+      <c r="L12" s="188">
         <v>6859</v>
       </c>
-      <c r="M12" s="193">
+      <c r="M12" s="192">
         <f t="shared" si="9"/>
         <v>5350.02</v>
       </c>
-      <c r="N12" s="183">
+      <c r="N12" s="182">
         <f t="shared" si="10"/>
         <v>1508.98</v>
       </c>
-      <c r="O12" s="150">
+      <c r="O12" s="149">
         <v>0.89</v>
       </c>
       <c r="P12" s="97"/>
@@ -5335,10 +5497,10 @@
       <c r="AD12" s="42">
         <v>0.18</v>
       </c>
-      <c r="AE12" s="193">
+      <c r="AE12" s="192">
         <v>36315</v>
       </c>
-      <c r="AF12" s="199">
+      <c r="AF12" s="198">
         <f t="shared" si="13"/>
         <v>36315.000000000007</v>
       </c>
@@ -5347,50 +5509,50 @@
       <c r="A13" s="10">
         <v>2017</v>
       </c>
-      <c r="B13" s="189">
+      <c r="B13" s="188">
         <f t="shared" si="8"/>
         <v>29684.000000000011</v>
       </c>
-      <c r="C13" s="211">
+      <c r="C13" s="210">
         <f t="shared" si="3"/>
         <v>27801.781600000009</v>
       </c>
-      <c r="D13" s="184">
+      <c r="D13" s="183">
         <v>1882.2184</v>
       </c>
-      <c r="E13" s="185">
+      <c r="E13" s="184">
         <v>207</v>
       </c>
-      <c r="F13" s="186">
+      <c r="F13" s="185">
         <v>147</v>
       </c>
-      <c r="G13" s="187">
+      <c r="G13" s="186">
         <v>60</v>
       </c>
       <c r="H13" s="185">
+        <v>74</v>
+      </c>
+      <c r="I13" s="184">
         <v>73</v>
       </c>
-      <c r="I13" s="186">
-        <v>74</v>
-      </c>
-      <c r="J13" s="223">
+      <c r="J13" s="186">
+        <v>27</v>
+      </c>
+      <c r="K13" s="222">
         <v>33</v>
       </c>
-      <c r="K13" s="187">
-        <v>27</v>
-      </c>
-      <c r="L13" s="189">
+      <c r="L13" s="188">
         <v>7219</v>
       </c>
-      <c r="M13" s="193">
+      <c r="M13" s="192">
         <f t="shared" si="9"/>
         <v>5630.8200000000006</v>
       </c>
-      <c r="N13" s="183">
+      <c r="N13" s="182">
         <f t="shared" si="10"/>
         <v>1588.18</v>
       </c>
-      <c r="O13" s="151">
+      <c r="O13" s="150">
         <v>0.9</v>
       </c>
       <c r="P13" s="97"/>
@@ -5438,8 +5600,8 @@
         <f t="shared" si="6"/>
         <v>413.28630000000004</v>
       </c>
-      <c r="AE13" s="199"/>
-      <c r="AF13" s="199">
+      <c r="AE13" s="198"/>
+      <c r="AF13" s="198">
         <f>AF12+588</f>
         <v>36903.000000000007</v>
       </c>
@@ -5448,103 +5610,103 @@
       <c r="A14" s="10">
         <v>2018</v>
       </c>
-      <c r="B14" s="189">
+      <c r="B14" s="188">
         <f t="shared" si="8"/>
         <v>29987.000000000007</v>
       </c>
-      <c r="C14" s="211">
+      <c r="C14" s="210">
         <f t="shared" si="3"/>
         <v>27854.027200000008</v>
       </c>
-      <c r="D14" s="184">
+      <c r="D14" s="183">
         <v>2132.9728</v>
       </c>
-      <c r="E14" s="185">
+      <c r="E14" s="184">
         <v>174</v>
       </c>
-      <c r="F14" s="186">
+      <c r="F14" s="185">
         <v>120</v>
       </c>
-      <c r="G14" s="188">
+      <c r="G14" s="187">
         <v>54</v>
       </c>
       <c r="H14" s="185">
         <v>60</v>
       </c>
-      <c r="I14" s="186">
+      <c r="I14" s="184">
         <v>60</v>
       </c>
-      <c r="J14" s="186">
+      <c r="J14" s="187">
+        <v>19</v>
+      </c>
+      <c r="K14" s="185">
         <v>35</v>
       </c>
-      <c r="K14" s="188">
-        <v>19</v>
-      </c>
-      <c r="L14" s="189">
+      <c r="L14" s="188">
         <v>7504</v>
       </c>
-      <c r="M14" s="193">
+      <c r="M14" s="192">
         <f t="shared" si="9"/>
         <v>5853.12</v>
       </c>
-      <c r="N14" s="183">
+      <c r="N14" s="182">
         <f t="shared" si="10"/>
         <v>1650.88</v>
       </c>
-      <c r="O14" s="150">
+      <c r="O14" s="149">
         <v>0.9</v>
       </c>
-      <c r="P14" s="124"/>
+      <c r="P14" s="123"/>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
         <v>7504</v>
       </c>
-      <c r="AE14" s="198"/>
-      <c r="AF14" s="199">
+      <c r="AE14" s="197"/>
+      <c r="AF14" s="198">
         <f t="shared" si="13"/>
         <v>37491.000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121">
+      <c r="A15" s="120">
         <v>2019</v>
       </c>
-      <c r="B15" s="189">
+      <c r="B15" s="188">
         <f t="shared" si="8"/>
         <v>38079.000000000007</v>
       </c>
-      <c r="C15" s="211">
+      <c r="C15" s="210">
         <f t="shared" si="3"/>
         <v>35727.806200000006</v>
       </c>
-      <c r="D15" s="184">
+      <c r="D15" s="183">
         <v>2351.1938</v>
       </c>
-      <c r="E15" s="120"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="122"/>
-      <c r="J15" s="122"/>
-      <c r="K15" s="123"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="122"/>
       <c r="L15" s="106"/>
       <c r="M15" s="107"/>
       <c r="N15" s="108"/>
-      <c r="O15" s="152"/>
-      <c r="P15" s="124"/>
-      <c r="AE15" s="199"/>
-      <c r="AF15" s="199">
+      <c r="O15" s="151"/>
+      <c r="P15" s="123"/>
+      <c r="AE15" s="198"/>
+      <c r="AF15" s="198">
         <f t="shared" si="13"/>
         <v>38079.000000000007</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G16" s="10"/>
-      <c r="H16" s="215"/>
-      <c r="I16" s="215"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="121"/>
-      <c r="S16" s="125"/>
+      <c r="H16" s="214"/>
+      <c r="I16" s="214"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="S16" s="124"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
@@ -5561,7 +5723,6 @@
       <c r="D18" s="10"/>
       <c r="G18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -5570,7 +5731,6 @@
       <c r="D19" s="10"/>
       <c r="G19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
       <c r="P19" s="10"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -5579,7 +5739,6 @@
       <c r="D20" s="10"/>
       <c r="G20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -5588,7 +5747,6 @@
       <c r="D21" s="10"/>
       <c r="G21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
       <c r="P21" s="10"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -5597,7 +5755,6 @@
       <c r="D22" s="10"/>
       <c r="G22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
       <c r="P22" s="10"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
@@ -5636,195 +5793,195 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126"/>
-      <c r="B1" s="127" t="s">
+      <c r="A1" s="125"/>
+      <c r="B1" s="126" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="128" t="s">
+      <c r="C1" s="127" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="128" t="s">
+      <c r="D1" s="127" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="142" t="s">
+      <c r="E1" s="141" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="128" t="s">
+      <c r="F1" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="129" t="s">
+      <c r="G1" s="128" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="131">
+      <c r="B2" s="130">
         <v>1</v>
       </c>
-      <c r="C2" s="132">
+      <c r="C2" s="131">
         <v>1</v>
       </c>
-      <c r="D2" s="132">
+      <c r="D2" s="131">
         <v>1</v>
       </c>
-      <c r="E2" s="147">
+      <c r="E2" s="146">
         <v>1</v>
       </c>
-      <c r="F2" s="132">
+      <c r="F2" s="131">
         <v>1</v>
       </c>
-      <c r="G2" s="133">
+      <c r="G2" s="132">
         <v>1</v>
       </c>
-      <c r="I2" s="224" t="s">
+      <c r="I2" s="227" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
-      <c r="M2" s="224"/>
-      <c r="N2" s="224"/>
-      <c r="O2" s="224"/>
-      <c r="P2" s="224"/>
+      <c r="J2" s="227"/>
+      <c r="K2" s="227"/>
+      <c r="L2" s="227"/>
+      <c r="M2" s="227"/>
+      <c r="N2" s="227"/>
+      <c r="O2" s="227"/>
+      <c r="P2" s="227"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="134" t="s">
+      <c r="A3" s="133" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="135">
+      <c r="B3" s="134">
         <v>1</v>
       </c>
-      <c r="C3" s="136">
+      <c r="C3" s="135">
         <v>1</v>
       </c>
-      <c r="D3" s="136">
+      <c r="D3" s="135">
         <v>1</v>
       </c>
-      <c r="E3" s="145">
+      <c r="E3" s="144">
         <v>1</v>
       </c>
-      <c r="F3" s="136">
+      <c r="F3" s="135">
         <v>1</v>
       </c>
-      <c r="G3" s="137">
+      <c r="G3" s="136">
         <v>1</v>
       </c>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="224"/>
-      <c r="L3" s="224"/>
-      <c r="M3" s="224"/>
-      <c r="N3" s="224"/>
-      <c r="O3" s="224"/>
-      <c r="P3" s="224"/>
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="227"/>
+      <c r="M3" s="227"/>
+      <c r="N3" s="227"/>
+      <c r="O3" s="227"/>
+      <c r="P3" s="227"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="134" t="s">
+      <c r="A4" s="133" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="135">
+      <c r="B4" s="134">
         <v>1</v>
       </c>
-      <c r="C4" s="136">
+      <c r="C4" s="135">
         <v>1</v>
       </c>
-      <c r="D4" s="136">
+      <c r="D4" s="135">
         <v>1</v>
       </c>
-      <c r="E4" s="145">
+      <c r="E4" s="144">
         <v>1</v>
       </c>
-      <c r="F4" s="136">
+      <c r="F4" s="135">
         <v>1</v>
       </c>
-      <c r="G4" s="137">
+      <c r="G4" s="136">
         <v>1</v>
       </c>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
-      <c r="L4" s="224"/>
-      <c r="M4" s="224"/>
-      <c r="N4" s="224"/>
-      <c r="O4" s="224"/>
-      <c r="P4" s="224"/>
+      <c r="I4" s="227"/>
+      <c r="J4" s="227"/>
+      <c r="K4" s="227"/>
+      <c r="L4" s="227"/>
+      <c r="M4" s="227"/>
+      <c r="N4" s="227"/>
+      <c r="O4" s="227"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="143" t="s">
+      <c r="A5" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="144">
+      <c r="B5" s="143">
         <v>1</v>
       </c>
-      <c r="C5" s="145">
+      <c r="C5" s="144">
         <v>1</v>
       </c>
-      <c r="D5" s="145">
+      <c r="D5" s="144">
         <v>1</v>
       </c>
-      <c r="E5" s="145">
+      <c r="E5" s="144">
         <v>1</v>
       </c>
-      <c r="F5" s="145">
+      <c r="F5" s="144">
         <v>1</v>
       </c>
-      <c r="G5" s="146">
+      <c r="G5" s="145">
         <v>1</v>
       </c>
-      <c r="I5" s="224"/>
-      <c r="J5" s="224"/>
-      <c r="K5" s="224"/>
-      <c r="L5" s="224"/>
-      <c r="M5" s="224"/>
-      <c r="N5" s="224"/>
-      <c r="O5" s="224"/>
-      <c r="P5" s="224"/>
+      <c r="I5" s="227"/>
+      <c r="J5" s="227"/>
+      <c r="K5" s="227"/>
+      <c r="L5" s="227"/>
+      <c r="M5" s="227"/>
+      <c r="N5" s="227"/>
+      <c r="O5" s="227"/>
+      <c r="P5" s="227"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="134" t="s">
+      <c r="A6" s="133" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="135">
+      <c r="B6" s="134">
         <v>1</v>
       </c>
-      <c r="C6" s="136">
+      <c r="C6" s="135">
         <v>1</v>
       </c>
-      <c r="D6" s="136">
+      <c r="D6" s="135">
         <v>1</v>
       </c>
-      <c r="E6" s="145">
+      <c r="E6" s="144">
         <v>1</v>
       </c>
-      <c r="F6" s="136">
+      <c r="F6" s="135">
         <v>1</v>
       </c>
-      <c r="G6" s="137">
+      <c r="G6" s="136">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="138" t="s">
+      <c r="A7" s="137" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="139">
+      <c r="B7" s="138">
         <v>1</v>
       </c>
-      <c r="C7" s="140">
+      <c r="C7" s="139">
         <v>1</v>
       </c>
-      <c r="D7" s="140">
+      <c r="D7" s="139">
         <v>1</v>
       </c>
-      <c r="E7" s="148">
+      <c r="E7" s="147">
         <v>1</v>
       </c>
-      <c r="F7" s="140">
+      <c r="F7" s="139">
         <v>1</v>
       </c>
-      <c r="G7" s="141">
+      <c r="G7" s="140">
         <v>1</v>
       </c>
     </row>
@@ -5842,7 +5999,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5897,16 +6054,16 @@
       <c r="G1" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="163" t="s">
+      <c r="H1" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="164" t="s">
+      <c r="I1" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="163" t="s">
+      <c r="J1" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="164" t="s">
+      <c r="K1" s="163" t="s">
         <v>69</v>
       </c>
       <c r="L1" s="68" t="s">
@@ -5915,16 +6072,16 @@
       <c r="M1" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="163" t="s">
+      <c r="N1" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="164" t="s">
+      <c r="O1" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="163" t="s">
+      <c r="P1" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="164" t="s">
+      <c r="Q1" s="163" t="s">
         <v>69</v>
       </c>
       <c r="R1" s="68" t="s">
@@ -5964,16 +6121,16 @@
       <c r="G2" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="165" t="s">
+      <c r="H2" s="164" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="165" t="s">
         <v>126</v>
       </c>
-      <c r="J2" s="165" t="s">
+      <c r="J2" s="164" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="166" t="s">
+      <c r="K2" s="165" t="s">
         <v>128</v>
       </c>
       <c r="L2" s="71" t="s">
@@ -5982,16 +6139,16 @@
       <c r="M2" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="165" t="s">
+      <c r="N2" s="164" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="166" t="s">
+      <c r="O2" s="165" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="165" t="s">
+      <c r="P2" s="164" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" s="166" t="s">
+      <c r="Q2" s="165" t="s">
         <v>128</v>
       </c>
       <c r="R2" s="71" t="s">
@@ -6036,22 +6193,22 @@
       <c r="L3" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="219" t="s">
+      <c r="M3" s="218" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="220" t="s">
+      <c r="N3" s="219" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="221" t="s">
+      <c r="O3" s="220" t="s">
         <v>98</v>
       </c>
-      <c r="P3" s="220" t="s">
+      <c r="P3" s="219" t="s">
         <v>98</v>
       </c>
-      <c r="Q3" s="221" t="s">
+      <c r="Q3" s="220" t="s">
         <v>98</v>
       </c>
-      <c r="R3" s="222" t="s">
+      <c r="R3" s="221" t="s">
         <v>98</v>
       </c>
       <c r="S3" s="70" t="s">
@@ -6094,24 +6251,24 @@
         <v>0.7</v>
       </c>
       <c r="G4" s="72"/>
-      <c r="H4" s="167"/>
-      <c r="I4" s="168"/>
-      <c r="J4" s="167"/>
-      <c r="K4" s="168">
+      <c r="H4" s="166"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="167">
         <v>0.25</v>
       </c>
       <c r="L4" s="74">
         <v>0.25</v>
       </c>
       <c r="M4" s="72"/>
-      <c r="N4" s="167"/>
-      <c r="O4" s="168"/>
-      <c r="P4" s="167"/>
-      <c r="Q4" s="168">
-        <v>0.5</v>
+      <c r="N4" s="166"/>
+      <c r="O4" s="167"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167">
+        <v>0.25</v>
       </c>
       <c r="R4" s="74">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S4" s="73"/>
       <c r="T4" s="74"/>
@@ -6125,10 +6282,10 @@
         <v>0.04</v>
       </c>
       <c r="X4" s="73">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="Y4" s="74">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
@@ -6141,16 +6298,16 @@
       <c r="E5" s="77"/>
       <c r="F5" s="62"/>
       <c r="G5" s="75"/>
-      <c r="H5" s="169"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="169"/>
-      <c r="K5" s="170"/>
+      <c r="H5" s="168"/>
+      <c r="I5" s="169"/>
+      <c r="J5" s="168"/>
+      <c r="K5" s="169"/>
       <c r="L5" s="77"/>
       <c r="M5" s="75"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="170"/>
+      <c r="N5" s="168"/>
+      <c r="O5" s="169"/>
+      <c r="P5" s="168"/>
+      <c r="Q5" s="169"/>
       <c r="R5" s="77"/>
       <c r="S5" s="76"/>
       <c r="T5" s="77"/>
@@ -6170,16 +6327,16 @@
       <c r="E6" s="77"/>
       <c r="F6" s="62"/>
       <c r="G6" s="75"/>
-      <c r="H6" s="169"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="169"/>
-      <c r="K6" s="170"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="169"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="169"/>
       <c r="L6" s="77"/>
       <c r="M6" s="75"/>
-      <c r="N6" s="169"/>
-      <c r="O6" s="170"/>
-      <c r="P6" s="169"/>
-      <c r="Q6" s="170"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="169"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="169"/>
       <c r="R6" s="77"/>
       <c r="S6" s="76"/>
       <c r="T6" s="77"/>
@@ -6193,7 +6350,7 @@
       <c r="A7" s="31">
         <v>2003</v>
       </c>
-      <c r="B7" s="191">
+      <c r="B7" s="190">
         <v>0.26</v>
       </c>
       <c r="C7" s="44"/>
@@ -6201,16 +6358,16 @@
       <c r="E7" s="77"/>
       <c r="F7" s="62"/>
       <c r="G7" s="75"/>
-      <c r="H7" s="169"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="169"/>
-      <c r="K7" s="170"/>
+      <c r="H7" s="168"/>
+      <c r="I7" s="169"/>
+      <c r="J7" s="168"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="77"/>
       <c r="M7" s="75"/>
-      <c r="N7" s="169"/>
-      <c r="O7" s="170"/>
-      <c r="P7" s="169"/>
-      <c r="Q7" s="170"/>
+      <c r="N7" s="168"/>
+      <c r="O7" s="169"/>
+      <c r="P7" s="168"/>
+      <c r="Q7" s="169"/>
       <c r="R7" s="77"/>
       <c r="S7" s="76"/>
       <c r="T7" s="77"/>
@@ -6224,7 +6381,7 @@
       <c r="A8" s="31">
         <v>2004</v>
       </c>
-      <c r="B8" s="191">
+      <c r="B8" s="190">
         <v>0.24</v>
       </c>
       <c r="C8" s="44"/>
@@ -6232,16 +6389,16 @@
       <c r="E8" s="77"/>
       <c r="F8" s="62"/>
       <c r="G8" s="75"/>
-      <c r="H8" s="169"/>
-      <c r="I8" s="170"/>
-      <c r="J8" s="169"/>
-      <c r="K8" s="170"/>
+      <c r="H8" s="168"/>
+      <c r="I8" s="169"/>
+      <c r="J8" s="168"/>
+      <c r="K8" s="169"/>
       <c r="L8" s="77"/>
       <c r="M8" s="75"/>
-      <c r="N8" s="169"/>
-      <c r="O8" s="170"/>
-      <c r="P8" s="169"/>
-      <c r="Q8" s="170"/>
+      <c r="N8" s="168"/>
+      <c r="O8" s="169"/>
+      <c r="P8" s="168"/>
+      <c r="Q8" s="169"/>
       <c r="R8" s="77"/>
       <c r="S8" s="76"/>
       <c r="T8" s="77"/>
@@ -6255,7 +6412,7 @@
       <c r="A9" s="31">
         <v>2005</v>
       </c>
-      <c r="B9" s="191">
+      <c r="B9" s="190">
         <v>0.28000000000000003</v>
       </c>
       <c r="C9" s="44"/>
@@ -6263,16 +6420,16 @@
       <c r="E9" s="77"/>
       <c r="F9" s="62"/>
       <c r="G9" s="75"/>
-      <c r="H9" s="169"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="170"/>
+      <c r="H9" s="168"/>
+      <c r="I9" s="169"/>
+      <c r="J9" s="168"/>
+      <c r="K9" s="169"/>
       <c r="L9" s="77"/>
       <c r="M9" s="75"/>
-      <c r="N9" s="169"/>
-      <c r="O9" s="170"/>
-      <c r="P9" s="169"/>
-      <c r="Q9" s="170"/>
+      <c r="N9" s="168"/>
+      <c r="O9" s="169"/>
+      <c r="P9" s="168"/>
+      <c r="Q9" s="169"/>
       <c r="R9" s="77"/>
       <c r="S9" s="76"/>
       <c r="T9" s="77"/>
@@ -6286,24 +6443,40 @@
       <c r="A10" s="31">
         <v>2006</v>
       </c>
-      <c r="B10" s="191">
+      <c r="B10" s="190">
         <v>0.26</v>
       </c>
       <c r="C10" s="44"/>
       <c r="D10" s="75"/>
       <c r="E10" s="77"/>
       <c r="F10" s="62"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="170"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="170"/>
+      <c r="G10" s="75">
+        <v>2.82</v>
+      </c>
+      <c r="H10" s="75">
+        <v>2.82</v>
+      </c>
+      <c r="I10" s="75">
+        <v>2.82</v>
+      </c>
+      <c r="J10" s="75">
+        <v>2.82</v>
+      </c>
+      <c r="K10" s="169"/>
       <c r="L10" s="77"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="169"/>
-      <c r="O10" s="170"/>
-      <c r="P10" s="169"/>
-      <c r="Q10" s="170"/>
+      <c r="M10" s="75">
+        <v>2.46</v>
+      </c>
+      <c r="N10" s="75">
+        <v>2.46</v>
+      </c>
+      <c r="O10" s="75">
+        <v>2.46</v>
+      </c>
+      <c r="P10" s="75">
+        <v>2.46</v>
+      </c>
+      <c r="Q10" s="169"/>
       <c r="R10" s="77"/>
       <c r="S10" s="76"/>
       <c r="T10" s="77"/>
@@ -6317,24 +6490,40 @@
       <c r="A11" s="31">
         <v>2007</v>
       </c>
-      <c r="B11" s="191">
+      <c r="B11" s="190">
         <v>0.26</v>
       </c>
       <c r="C11" s="44"/>
       <c r="D11" s="75"/>
       <c r="E11" s="77"/>
       <c r="F11" s="62"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="169"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="169"/>
-      <c r="K11" s="170"/>
+      <c r="G11" s="75">
+        <v>3.06</v>
+      </c>
+      <c r="H11" s="75">
+        <v>3.06</v>
+      </c>
+      <c r="I11" s="75">
+        <v>3.06</v>
+      </c>
+      <c r="J11" s="75">
+        <v>3.06</v>
+      </c>
+      <c r="K11" s="169"/>
       <c r="L11" s="77"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="169"/>
-      <c r="O11" s="170"/>
-      <c r="P11" s="169"/>
-      <c r="Q11" s="170"/>
+      <c r="M11" s="75">
+        <v>2.77</v>
+      </c>
+      <c r="N11" s="75">
+        <v>2.77</v>
+      </c>
+      <c r="O11" s="75">
+        <v>2.77</v>
+      </c>
+      <c r="P11" s="75">
+        <v>2.77</v>
+      </c>
+      <c r="Q11" s="169"/>
       <c r="R11" s="77"/>
       <c r="S11" s="76">
         <v>0.75</v>
@@ -6352,24 +6541,40 @@
       <c r="A12" s="31">
         <v>2008</v>
       </c>
-      <c r="B12" s="191">
+      <c r="B12" s="190">
         <v>0.27</v>
       </c>
       <c r="C12" s="44"/>
       <c r="D12" s="75"/>
       <c r="E12" s="77"/>
       <c r="F12" s="62"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="169"/>
-      <c r="K12" s="170"/>
+      <c r="G12" s="75">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H12" s="75">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I12" s="75">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="J12" s="75">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="K12" s="169"/>
       <c r="L12" s="77"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="169"/>
-      <c r="O12" s="170"/>
-      <c r="P12" s="169"/>
-      <c r="Q12" s="170"/>
+      <c r="M12" s="75">
+        <v>2.91</v>
+      </c>
+      <c r="N12" s="75">
+        <v>2.91</v>
+      </c>
+      <c r="O12" s="75">
+        <v>2.91</v>
+      </c>
+      <c r="P12" s="75">
+        <v>2.91</v>
+      </c>
+      <c r="Q12" s="169"/>
       <c r="R12" s="77"/>
       <c r="S12" s="76"/>
       <c r="T12" s="77"/>
@@ -6383,26 +6588,42 @@
       <c r="A13" s="31">
         <v>2009</v>
       </c>
-      <c r="B13" s="191">
+      <c r="B13" s="190">
         <v>0.28999999999999998</v>
       </c>
       <c r="C13" s="44"/>
-      <c r="D13" s="190">
+      <c r="D13" s="189">
         <v>0</v>
       </c>
       <c r="F13" s="62"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="169"/>
-      <c r="K13" s="170"/>
+      <c r="G13" s="75">
+        <v>2.65</v>
+      </c>
+      <c r="H13" s="75">
+        <v>2.65</v>
+      </c>
+      <c r="I13" s="75">
+        <v>2.65</v>
+      </c>
+      <c r="J13" s="75">
+        <v>2.65</v>
+      </c>
+      <c r="K13" s="169"/>
       <c r="L13" s="77"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="169"/>
-      <c r="O13" s="170"/>
-      <c r="P13" s="169"/>
-      <c r="Q13" s="216"/>
-      <c r="R13" s="217"/>
+      <c r="M13" s="75">
+        <v>1.07</v>
+      </c>
+      <c r="N13" s="75">
+        <v>1.07</v>
+      </c>
+      <c r="O13" s="75">
+        <v>1.07</v>
+      </c>
+      <c r="P13" s="75">
+        <v>1.07</v>
+      </c>
+      <c r="Q13" s="215"/>
+      <c r="R13" s="216"/>
       <c r="S13" s="76"/>
       <c r="T13" s="77"/>
       <c r="U13" s="75"/>
@@ -6415,26 +6636,42 @@
       <c r="A14" s="31">
         <v>2010</v>
       </c>
-      <c r="B14" s="191">
+      <c r="B14" s="190">
         <v>0.32</v>
       </c>
       <c r="C14" s="44"/>
-      <c r="D14" s="190">
+      <c r="D14" s="189">
         <v>0</v>
       </c>
       <c r="F14" s="62"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="169"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="169"/>
-      <c r="K14" s="216"/>
-      <c r="L14" s="217"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="169"/>
-      <c r="O14" s="170"/>
-      <c r="P14" s="169"/>
-      <c r="Q14" s="216"/>
-      <c r="R14" s="217"/>
+      <c r="G14" s="75">
+        <v>2.23</v>
+      </c>
+      <c r="H14" s="75">
+        <v>2.23</v>
+      </c>
+      <c r="I14" s="75">
+        <v>2.23</v>
+      </c>
+      <c r="J14" s="75">
+        <v>2.23</v>
+      </c>
+      <c r="K14" s="215"/>
+      <c r="L14" s="216"/>
+      <c r="M14" s="75">
+        <v>2.71</v>
+      </c>
+      <c r="N14" s="75">
+        <v>2.71</v>
+      </c>
+      <c r="O14" s="75">
+        <v>2.71</v>
+      </c>
+      <c r="P14" s="75">
+        <v>2.71</v>
+      </c>
+      <c r="Q14" s="215"/>
+      <c r="R14" s="216"/>
       <c r="S14" s="76">
         <v>0.75</v>
       </c>
@@ -6451,26 +6688,42 @@
       <c r="A15" s="31">
         <v>2011</v>
       </c>
-      <c r="B15" s="191">
+      <c r="B15" s="190">
         <v>0.31</v>
       </c>
       <c r="C15" s="44"/>
-      <c r="D15" s="190">
+      <c r="D15" s="189">
         <v>0</v>
       </c>
       <c r="F15" s="62"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="169"/>
-      <c r="K15" s="216"/>
-      <c r="L15" s="217"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="169"/>
-      <c r="O15" s="170"/>
-      <c r="P15" s="169"/>
-      <c r="Q15" s="216"/>
-      <c r="R15" s="217"/>
+      <c r="G15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="H15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="I15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="J15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="K15" s="215"/>
+      <c r="L15" s="216"/>
+      <c r="M15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="N15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="O15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="P15" s="75">
+        <v>1.92</v>
+      </c>
+      <c r="Q15" s="215"/>
+      <c r="R15" s="216"/>
       <c r="S15" s="76"/>
       <c r="T15" s="77"/>
       <c r="U15" s="75"/>
@@ -6483,11 +6736,11 @@
       <c r="A16" s="31">
         <v>2012</v>
       </c>
-      <c r="B16" s="191">
+      <c r="B16" s="190">
         <v>0.28000000000000003</v>
       </c>
       <c r="C16" s="44"/>
-      <c r="D16" s="190">
+      <c r="D16" s="189">
         <v>0</v>
       </c>
       <c r="F16" s="62"/>
@@ -6503,8 +6756,8 @@
       <c r="J16" s="43">
         <v>1.91</v>
       </c>
-      <c r="K16" s="216"/>
-      <c r="L16" s="218"/>
+      <c r="K16" s="215"/>
+      <c r="L16" s="217"/>
       <c r="M16" s="43">
         <v>2.37</v>
       </c>
@@ -6517,7 +6770,7 @@
       <c r="P16" s="43">
         <v>2.37</v>
       </c>
-      <c r="Q16" s="216"/>
+      <c r="Q16" s="215"/>
       <c r="R16" s="77"/>
       <c r="S16" s="76">
         <v>0.82</v>
@@ -6535,11 +6788,11 @@
       <c r="A17" s="31">
         <v>2013</v>
       </c>
-      <c r="B17" s="191">
+      <c r="B17" s="190">
         <v>0.3</v>
       </c>
       <c r="C17" s="44"/>
-      <c r="D17" s="190">
+      <c r="D17" s="189">
         <v>0</v>
       </c>
       <c r="F17" s="62"/>
@@ -6555,8 +6808,8 @@
       <c r="J17" s="43">
         <v>2.34</v>
       </c>
-      <c r="K17" s="216"/>
-      <c r="L17" s="218"/>
+      <c r="K17" s="215"/>
+      <c r="L17" s="217"/>
       <c r="M17" s="43">
         <v>2.84</v>
       </c>
@@ -6569,7 +6822,7 @@
       <c r="P17" s="43">
         <v>2.84</v>
       </c>
-      <c r="Q17" s="216"/>
+      <c r="Q17" s="215"/>
       <c r="R17" s="77"/>
       <c r="S17" s="76">
         <v>0.86</v>
@@ -6587,12 +6840,14 @@
       <c r="A18" s="31">
         <v>2014</v>
       </c>
-      <c r="B18" s="191"/>
+      <c r="B18" s="190">
+        <v>0.32</v>
+      </c>
       <c r="C18" s="44"/>
-      <c r="D18" s="190">
+      <c r="D18" s="189">
         <v>143</v>
       </c>
-      <c r="E18" s="192">
+      <c r="E18" s="191">
         <v>0</v>
       </c>
       <c r="F18" s="62"/>
@@ -6608,8 +6863,8 @@
       <c r="J18" s="43">
         <v>1.5</v>
       </c>
-      <c r="K18" s="216"/>
-      <c r="L18" s="218"/>
+      <c r="K18" s="215"/>
+      <c r="L18" s="217"/>
       <c r="M18" s="43">
         <v>0.96</v>
       </c>
@@ -6622,7 +6877,7 @@
       <c r="P18" s="43">
         <v>0.96</v>
       </c>
-      <c r="Q18" s="216"/>
+      <c r="Q18" s="215"/>
       <c r="R18" s="77"/>
       <c r="S18" s="76">
         <v>0.89</v>
@@ -6640,12 +6895,14 @@
       <c r="A19" s="31">
         <v>2015</v>
       </c>
-      <c r="B19" s="191"/>
+      <c r="B19" s="190">
+        <v>0.35</v>
+      </c>
       <c r="C19" s="44"/>
-      <c r="D19" s="190">
+      <c r="D19" s="189">
         <v>143</v>
       </c>
-      <c r="E19" s="192">
+      <c r="E19" s="191">
         <v>0</v>
       </c>
       <c r="F19" s="62"/>
@@ -6661,8 +6918,8 @@
       <c r="J19" s="43">
         <v>2.08</v>
       </c>
-      <c r="K19" s="216"/>
-      <c r="L19" s="218"/>
+      <c r="K19" s="215"/>
+      <c r="L19" s="217"/>
       <c r="M19" s="43">
         <v>1.45</v>
       </c>
@@ -6675,7 +6932,7 @@
       <c r="P19" s="43">
         <v>1.45</v>
       </c>
-      <c r="Q19" s="216"/>
+      <c r="Q19" s="215"/>
       <c r="R19" s="77"/>
       <c r="S19" s="76">
         <v>0.92</v>
@@ -6693,14 +6950,14 @@
       <c r="A20" s="31">
         <v>2016</v>
       </c>
-      <c r="B20" s="192">
-        <v>0.31</v>
+      <c r="B20" s="191">
+        <v>0.37</v>
       </c>
       <c r="C20" s="44"/>
-      <c r="D20" s="190">
+      <c r="D20" s="189">
         <v>2841</v>
       </c>
-      <c r="E20" s="192">
+      <c r="E20" s="191">
         <f>data!D12*0.03</f>
         <v>49.394274000000003</v>
       </c>
@@ -6717,8 +6974,8 @@
       <c r="J20" s="43">
         <v>2.73</v>
       </c>
-      <c r="K20" s="216"/>
-      <c r="L20" s="218"/>
+      <c r="K20" s="215"/>
+      <c r="L20" s="217"/>
       <c r="M20" s="43">
         <v>2.5499999999999998</v>
       </c>
@@ -6731,7 +6988,7 @@
       <c r="P20" s="43">
         <v>2.5499999999999998</v>
       </c>
-      <c r="Q20" s="216"/>
+      <c r="Q20" s="215"/>
       <c r="R20" s="77"/>
       <c r="S20" s="76">
         <v>0.95</v>
@@ -6749,14 +7006,14 @@
       <c r="A21" s="31">
         <v>2017</v>
       </c>
-      <c r="B21" s="191">
-        <v>0.28999999999999998</v>
+      <c r="B21" s="190">
+        <v>0.4</v>
       </c>
       <c r="C21" s="44"/>
-      <c r="D21" s="190">
+      <c r="D21" s="189">
         <v>3727</v>
       </c>
-      <c r="E21" s="192">
+      <c r="E21" s="191">
         <f>data!D13*0.07</f>
         <v>131.75528800000001</v>
       </c>
@@ -6773,8 +7030,8 @@
       <c r="J21" s="43">
         <v>2.71</v>
       </c>
-      <c r="K21" s="216"/>
-      <c r="L21" s="218"/>
+      <c r="K21" s="215"/>
+      <c r="L21" s="217"/>
       <c r="M21" s="43">
         <v>2.23</v>
       </c>
@@ -6787,8 +7044,8 @@
       <c r="P21" s="43">
         <v>2.23</v>
       </c>
-      <c r="Q21" s="216"/>
-      <c r="R21" s="217"/>
+      <c r="Q21" s="215"/>
+      <c r="R21" s="216"/>
       <c r="S21" s="76"/>
       <c r="T21" s="77"/>
       <c r="U21" s="75"/>
@@ -6801,12 +7058,14 @@
       <c r="A22" s="31">
         <v>2018</v>
       </c>
-      <c r="B22" s="44"/>
+      <c r="B22" s="44">
+        <v>0.4</v>
+      </c>
       <c r="C22" s="44"/>
-      <c r="D22" s="190">
+      <c r="D22" s="189">
         <v>3995</v>
       </c>
-      <c r="E22" s="192">
+      <c r="E22" s="191">
         <f>data!D14*0.07</f>
         <v>149.30809600000001</v>
       </c>
@@ -6823,8 +7082,8 @@
       <c r="J22" s="43">
         <v>2.75</v>
       </c>
-      <c r="K22" s="216"/>
-      <c r="L22" s="218"/>
+      <c r="K22" s="215"/>
+      <c r="L22" s="217"/>
       <c r="M22" s="43">
         <v>2.2599999999999998</v>
       </c>
@@ -6837,7 +7096,7 @@
       <c r="P22" s="43">
         <v>2.2599999999999998</v>
       </c>
-      <c r="Q22" s="216"/>
+      <c r="Q22" s="215"/>
       <c r="R22" s="77"/>
       <c r="S22" s="76"/>
       <c r="T22" s="77"/>
@@ -6853,25 +7112,25 @@
       </c>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
-      <c r="D23" s="190">
+      <c r="D23" s="189">
         <v>4525</v>
       </c>
-      <c r="E23" s="192">
+      <c r="E23" s="191">
         <f>data!D15*0.07</f>
         <v>164.58356600000002</v>
       </c>
       <c r="F23" s="62"/>
-      <c r="G23" s="194"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="195"/>
-      <c r="K23" s="216"/>
-      <c r="L23" s="218"/>
-      <c r="M23" s="194"/>
-      <c r="N23" s="195"/>
-      <c r="O23" s="196"/>
-      <c r="P23" s="195"/>
-      <c r="Q23" s="216"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="194"/>
+      <c r="I23" s="195"/>
+      <c r="J23" s="194"/>
+      <c r="K23" s="215"/>
+      <c r="L23" s="217"/>
+      <c r="M23" s="193"/>
+      <c r="N23" s="194"/>
+      <c r="O23" s="195"/>
+      <c r="P23" s="194"/>
+      <c r="Q23" s="215"/>
       <c r="R23" s="77"/>
       <c r="S23" s="76"/>
       <c r="T23" s="77"/>
@@ -6891,16 +7150,16 @@
       <c r="E24" s="77"/>
       <c r="F24" s="62"/>
       <c r="G24" s="75"/>
-      <c r="H24" s="169"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="169"/>
-      <c r="K24" s="216"/>
-      <c r="L24" s="217"/>
+      <c r="H24" s="168"/>
+      <c r="I24" s="169"/>
+      <c r="J24" s="168"/>
+      <c r="K24" s="215"/>
+      <c r="L24" s="216"/>
       <c r="M24" s="75"/>
-      <c r="N24" s="169"/>
-      <c r="O24" s="170"/>
-      <c r="P24" s="169"/>
-      <c r="Q24" s="216"/>
+      <c r="N24" s="168"/>
+      <c r="O24" s="169"/>
+      <c r="P24" s="168"/>
+      <c r="Q24" s="215"/>
       <c r="R24" s="77"/>
       <c r="S24" s="76"/>
       <c r="T24" s="77"/>
@@ -6920,16 +7179,16 @@
       <c r="E25" s="77"/>
       <c r="F25" s="62"/>
       <c r="G25" s="75"/>
-      <c r="H25" s="169"/>
-      <c r="I25" s="170"/>
-      <c r="J25" s="169"/>
-      <c r="K25" s="170"/>
+      <c r="H25" s="168"/>
+      <c r="I25" s="169"/>
+      <c r="J25" s="168"/>
+      <c r="K25" s="169"/>
       <c r="L25" s="77"/>
       <c r="M25" s="75"/>
-      <c r="N25" s="169"/>
-      <c r="O25" s="170"/>
-      <c r="P25" s="169"/>
-      <c r="Q25" s="170"/>
+      <c r="N25" s="168"/>
+      <c r="O25" s="169"/>
+      <c r="P25" s="168"/>
+      <c r="Q25" s="169"/>
       <c r="R25" s="77"/>
       <c r="S25" s="76"/>
       <c r="T25" s="77"/>
@@ -6949,16 +7208,16 @@
       <c r="E26" s="77"/>
       <c r="F26" s="62"/>
       <c r="G26" s="75"/>
-      <c r="H26" s="169"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="169"/>
-      <c r="K26" s="170"/>
+      <c r="H26" s="168"/>
+      <c r="I26" s="169"/>
+      <c r="J26" s="168"/>
+      <c r="K26" s="169"/>
       <c r="L26" s="77"/>
       <c r="M26" s="75"/>
-      <c r="N26" s="169"/>
-      <c r="O26" s="170"/>
-      <c r="P26" s="169"/>
-      <c r="Q26" s="170"/>
+      <c r="N26" s="168"/>
+      <c r="O26" s="169"/>
+      <c r="P26" s="168"/>
+      <c r="Q26" s="169"/>
       <c r="R26" s="77"/>
       <c r="S26" s="76"/>
       <c r="T26" s="77"/>
@@ -6978,16 +7237,16 @@
       <c r="E27" s="77"/>
       <c r="F27" s="62"/>
       <c r="G27" s="75"/>
-      <c r="H27" s="169"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="169"/>
-      <c r="K27" s="170"/>
+      <c r="H27" s="168"/>
+      <c r="I27" s="169"/>
+      <c r="J27" s="168"/>
+      <c r="K27" s="169"/>
       <c r="L27" s="77"/>
       <c r="M27" s="75"/>
-      <c r="N27" s="169"/>
-      <c r="O27" s="170"/>
-      <c r="P27" s="169"/>
-      <c r="Q27" s="170"/>
+      <c r="N27" s="168"/>
+      <c r="O27" s="169"/>
+      <c r="P27" s="168"/>
+      <c r="Q27" s="169"/>
       <c r="R27" s="77"/>
       <c r="S27" s="76"/>
       <c r="T27" s="77"/>
@@ -7007,16 +7266,16 @@
       <c r="E28" s="77"/>
       <c r="F28" s="62"/>
       <c r="G28" s="75"/>
-      <c r="H28" s="169"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="169"/>
-      <c r="K28" s="170"/>
+      <c r="H28" s="168"/>
+      <c r="I28" s="169"/>
+      <c r="J28" s="168"/>
+      <c r="K28" s="169"/>
       <c r="L28" s="77"/>
       <c r="M28" s="75"/>
-      <c r="N28" s="169"/>
-      <c r="O28" s="170"/>
-      <c r="P28" s="169"/>
-      <c r="Q28" s="170"/>
+      <c r="N28" s="168"/>
+      <c r="O28" s="169"/>
+      <c r="P28" s="168"/>
+      <c r="Q28" s="169"/>
       <c r="R28" s="77"/>
       <c r="S28" s="76"/>
       <c r="T28" s="77"/>
@@ -7036,16 +7295,16 @@
       <c r="E29" s="77"/>
       <c r="F29" s="62"/>
       <c r="G29" s="75"/>
-      <c r="H29" s="169"/>
-      <c r="I29" s="170"/>
-      <c r="J29" s="169"/>
-      <c r="K29" s="170"/>
+      <c r="H29" s="168"/>
+      <c r="I29" s="169"/>
+      <c r="J29" s="168"/>
+      <c r="K29" s="169"/>
       <c r="L29" s="77"/>
       <c r="M29" s="75"/>
-      <c r="N29" s="169"/>
-      <c r="O29" s="170"/>
-      <c r="P29" s="169"/>
-      <c r="Q29" s="170"/>
+      <c r="N29" s="168"/>
+      <c r="O29" s="169"/>
+      <c r="P29" s="168"/>
+      <c r="Q29" s="169"/>
       <c r="R29" s="77"/>
       <c r="S29" s="76">
         <v>0.95</v>
@@ -7069,16 +7328,16 @@
       <c r="E30" s="77"/>
       <c r="F30" s="62"/>
       <c r="G30" s="75"/>
-      <c r="H30" s="169"/>
-      <c r="I30" s="170"/>
-      <c r="J30" s="169"/>
-      <c r="K30" s="170"/>
+      <c r="H30" s="168"/>
+      <c r="I30" s="169"/>
+      <c r="J30" s="168"/>
+      <c r="K30" s="169"/>
       <c r="L30" s="77"/>
       <c r="M30" s="75"/>
-      <c r="N30" s="169"/>
-      <c r="O30" s="170"/>
-      <c r="P30" s="169"/>
-      <c r="Q30" s="170"/>
+      <c r="N30" s="168"/>
+      <c r="O30" s="169"/>
+      <c r="P30" s="168"/>
+      <c r="Q30" s="169"/>
       <c r="R30" s="77"/>
       <c r="S30" s="76"/>
       <c r="T30" s="77"/>
@@ -7098,16 +7357,16 @@
       <c r="E31" s="77"/>
       <c r="F31" s="62"/>
       <c r="G31" s="75"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="170"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="170"/>
+      <c r="H31" s="168"/>
+      <c r="I31" s="169"/>
+      <c r="J31" s="168"/>
+      <c r="K31" s="169"/>
       <c r="L31" s="77"/>
       <c r="M31" s="75"/>
-      <c r="N31" s="169"/>
-      <c r="O31" s="170"/>
-      <c r="P31" s="169"/>
-      <c r="Q31" s="170"/>
+      <c r="N31" s="168"/>
+      <c r="O31" s="169"/>
+      <c r="P31" s="168"/>
+      <c r="Q31" s="169"/>
       <c r="R31" s="77"/>
       <c r="S31" s="76"/>
       <c r="T31" s="77"/>
@@ -7127,16 +7386,16 @@
       <c r="E32" s="77"/>
       <c r="F32" s="62"/>
       <c r="G32" s="75"/>
-      <c r="H32" s="169"/>
-      <c r="I32" s="170"/>
-      <c r="J32" s="169"/>
-      <c r="K32" s="170"/>
+      <c r="H32" s="168"/>
+      <c r="I32" s="169"/>
+      <c r="J32" s="168"/>
+      <c r="K32" s="169"/>
       <c r="L32" s="77"/>
       <c r="M32" s="75"/>
-      <c r="N32" s="169"/>
-      <c r="O32" s="170"/>
-      <c r="P32" s="169"/>
-      <c r="Q32" s="170"/>
+      <c r="N32" s="168"/>
+      <c r="O32" s="169"/>
+      <c r="P32" s="168"/>
+      <c r="Q32" s="169"/>
       <c r="R32" s="77"/>
       <c r="S32" s="76"/>
       <c r="T32" s="77"/>
@@ -7156,16 +7415,16 @@
       <c r="E33" s="77"/>
       <c r="F33" s="62"/>
       <c r="G33" s="75"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="170"/>
-      <c r="J33" s="169"/>
-      <c r="K33" s="170"/>
+      <c r="H33" s="168"/>
+      <c r="I33" s="169"/>
+      <c r="J33" s="168"/>
+      <c r="K33" s="169"/>
       <c r="L33" s="77"/>
       <c r="M33" s="75"/>
-      <c r="N33" s="169"/>
-      <c r="O33" s="170"/>
-      <c r="P33" s="169"/>
-      <c r="Q33" s="170"/>
+      <c r="N33" s="168"/>
+      <c r="O33" s="169"/>
+      <c r="P33" s="168"/>
+      <c r="Q33" s="169"/>
       <c r="R33" s="77"/>
       <c r="S33" s="76"/>
       <c r="T33" s="77"/>
@@ -7185,16 +7444,16 @@
       <c r="E34" s="80"/>
       <c r="F34" s="64"/>
       <c r="G34" s="78"/>
-      <c r="H34" s="171"/>
-      <c r="I34" s="172"/>
-      <c r="J34" s="171"/>
-      <c r="K34" s="172"/>
+      <c r="H34" s="170"/>
+      <c r="I34" s="171"/>
+      <c r="J34" s="170"/>
+      <c r="K34" s="171"/>
       <c r="L34" s="80"/>
       <c r="M34" s="78"/>
-      <c r="N34" s="171"/>
-      <c r="O34" s="172"/>
-      <c r="P34" s="171"/>
-      <c r="Q34" s="172"/>
+      <c r="N34" s="170"/>
+      <c r="O34" s="171"/>
+      <c r="P34" s="170"/>
+      <c r="Q34" s="171"/>
       <c r="R34" s="80"/>
       <c r="S34" s="79">
         <v>0.99</v>
@@ -7220,7 +7479,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7420,219 +7679,334 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" style="60" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="43"/>
+    <col min="2" max="2" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="68" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="71" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2000</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-    </row>
-    <row r="5" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="72"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2001</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-    </row>
-    <row r="6" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
+    </row>
+    <row r="6" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>2002</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="77"/>
-    </row>
-    <row r="7" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="77"/>
+    </row>
+    <row r="7" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>2003</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="77"/>
-    </row>
-    <row r="8" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="75"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="77"/>
+    </row>
+    <row r="8" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>2004</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
-    </row>
-    <row r="9" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
+    </row>
+    <row r="9" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>2005</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="77"/>
-    </row>
-    <row r="10" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="75"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
+    </row>
+    <row r="10" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2006</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="77"/>
-    </row>
-    <row r="11" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="77"/>
+    </row>
+    <row r="11" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2007</v>
       </c>
-      <c r="B11" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="C11" s="77">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="75"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
+    </row>
+    <row r="12" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2008</v>
       </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="77"/>
-    </row>
-    <row r="13" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="77"/>
+    </row>
+    <row r="13" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2009</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="77"/>
-    </row>
-    <row r="14" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="75"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="77"/>
+    </row>
+    <row r="14" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>2010</v>
       </c>
-      <c r="B14" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="C14" s="77">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="75"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="77"/>
+    </row>
+    <row r="15" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>2011</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="77"/>
-    </row>
-    <row r="16" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="75"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
+    </row>
+    <row r="16" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>2012</v>
       </c>
-      <c r="B16" s="76">
-        <v>0.82</v>
-      </c>
-      <c r="C16" s="77">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="75"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="77"/>
+    </row>
+    <row r="17" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>2013</v>
       </c>
-      <c r="B17" s="76">
-        <v>0.86</v>
-      </c>
-      <c r="C17" s="77">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="77"/>
+    </row>
+    <row r="18" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>2014</v>
       </c>
-      <c r="B18" s="76">
-        <v>0.89</v>
-      </c>
-      <c r="C18" s="77">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="77"/>
+    </row>
+    <row r="19" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>2015</v>
       </c>
-      <c r="B19" s="76">
-        <v>0.92</v>
-      </c>
-      <c r="C19" s="77">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="76">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="76">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="76">
+        <v>0.25</v>
+      </c>
+      <c r="F19" s="76">
+        <v>0.125</v>
+      </c>
+      <c r="G19" s="77">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2016</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="77"/>
-    </row>
-    <row r="21" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="75"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="77"/>
+    </row>
+    <row r="21" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>2017</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="77"/>
-    </row>
-    <row r="22" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="75"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
+    </row>
+    <row r="22" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>2018</v>
       </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="77"/>
-    </row>
-    <row r="23" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="75"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="77"/>
+    </row>
+    <row r="23" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>2019</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="77"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="44">
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="77"/>
+    </row>
+    <row r="24" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="63">
         <v>2020</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7706,16 +8080,16 @@
       <c r="G1" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="163" t="s">
+      <c r="H1" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="164" t="s">
+      <c r="I1" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="163" t="s">
+      <c r="J1" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="164" t="s">
+      <c r="K1" s="163" t="s">
         <v>69</v>
       </c>
       <c r="L1" s="68" t="s">
@@ -7742,10 +8116,10 @@
       <c r="S1" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="173" t="s">
+      <c r="T1" s="172" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="174" t="s">
+      <c r="U1" s="173" t="s">
         <v>92</v>
       </c>
       <c r="V1" s="82" t="s">
@@ -7760,10 +8134,10 @@
       <c r="Y1" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="153" t="s">
+      <c r="Z1" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="154" t="s">
+      <c r="AA1" s="153" t="s">
         <v>75</v>
       </c>
       <c r="AB1" s="82" t="s">
@@ -7812,16 +8186,16 @@
       <c r="G2" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="165" t="s">
+      <c r="H2" s="164" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="165" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="165" t="s">
+      <c r="J2" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="166" t="s">
+      <c r="K2" s="165" t="s">
         <v>72</v>
       </c>
       <c r="L2" s="71" t="s">
@@ -7838,10 +8212,10 @@
       <c r="S2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="175" t="s">
+      <c r="T2" s="174" t="s">
         <v>72</v>
       </c>
-      <c r="U2" s="176" t="s">
+      <c r="U2" s="175" t="s">
         <v>70</v>
       </c>
       <c r="V2" s="85" t="s">
@@ -7856,10 +8230,10 @@
       <c r="Y2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="Z2" s="155" t="s">
+      <c r="Z2" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="AA2" s="156" t="s">
+      <c r="AA2" s="155" t="s">
         <v>70</v>
       </c>
       <c r="AB2" s="85" t="s">
@@ -7906,16 +8280,16 @@
       <c r="G3" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="165" t="s">
+      <c r="H3" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="166" t="s">
+      <c r="I3" s="165" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="165" t="s">
+      <c r="J3" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="166" t="s">
+      <c r="K3" s="165" t="s">
         <v>73</v>
       </c>
       <c r="L3" s="71" t="s">
@@ -7942,10 +8316,10 @@
       <c r="S3" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="T3" s="175" t="s">
+      <c r="T3" s="174" t="s">
         <v>97</v>
       </c>
-      <c r="U3" s="176" t="s">
+      <c r="U3" s="175" t="s">
         <v>98</v>
       </c>
       <c r="V3" s="85" t="s">
@@ -7960,10 +8334,10 @@
       <c r="Y3" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="Z3" s="155" t="s">
+      <c r="Z3" s="154" t="s">
         <v>97</v>
       </c>
-      <c r="AA3" s="156" t="s">
+      <c r="AA3" s="155" t="s">
         <v>98</v>
       </c>
       <c r="AB3" s="85" t="s">
@@ -8004,16 +8378,16 @@
       <c r="G4" s="72">
         <v>1</v>
       </c>
-      <c r="H4" s="167">
+      <c r="H4" s="166">
         <v>10</v>
       </c>
-      <c r="I4" s="168">
+      <c r="I4" s="167">
         <v>0.5</v>
       </c>
-      <c r="J4" s="167">
+      <c r="J4" s="166">
         <v>4</v>
       </c>
-      <c r="K4" s="168">
+      <c r="K4" s="167">
         <f>3/12</f>
         <v>0.25</v>
       </c>
@@ -8038,10 +8412,10 @@
       <c r="S4" s="88">
         <v>1</v>
       </c>
-      <c r="T4" s="177">
+      <c r="T4" s="176">
         <v>0.03</v>
       </c>
-      <c r="U4" s="178">
+      <c r="U4" s="177">
         <v>1</v>
       </c>
       <c r="V4" s="88">
@@ -8056,10 +8430,10 @@
       <c r="Y4" s="88">
         <v>0</v>
       </c>
-      <c r="Z4" s="157">
+      <c r="Z4" s="156">
         <v>0</v>
       </c>
-      <c r="AA4" s="158">
+      <c r="AA4" s="157">
         <v>1</v>
       </c>
       <c r="AB4" s="88">
@@ -8106,10 +8480,10 @@
       <c r="E5" s="77"/>
       <c r="F5" s="62"/>
       <c r="G5" s="75"/>
-      <c r="H5" s="169"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="169"/>
-      <c r="K5" s="170"/>
+      <c r="H5" s="168"/>
+      <c r="I5" s="169"/>
+      <c r="J5" s="168"/>
+      <c r="K5" s="169"/>
       <c r="L5" s="77"/>
       <c r="M5" s="76"/>
       <c r="N5" s="77"/>
@@ -8118,14 +8492,14 @@
       <c r="Q5" s="77"/>
       <c r="R5" s="90"/>
       <c r="S5" s="91"/>
-      <c r="T5" s="179"/>
-      <c r="U5" s="180"/>
+      <c r="T5" s="178"/>
+      <c r="U5" s="179"/>
       <c r="V5" s="91"/>
       <c r="W5" s="92"/>
       <c r="X5" s="90"/>
       <c r="Y5" s="91"/>
-      <c r="Z5" s="159"/>
-      <c r="AA5" s="160"/>
+      <c r="Z5" s="158"/>
+      <c r="AA5" s="159"/>
       <c r="AB5" s="91"/>
       <c r="AC5" s="92"/>
       <c r="AD5" s="101"/>
@@ -8148,10 +8522,10 @@
       <c r="E6" s="77"/>
       <c r="F6" s="62"/>
       <c r="G6" s="75"/>
-      <c r="H6" s="169"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="169"/>
-      <c r="K6" s="170"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="169"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="169"/>
       <c r="L6" s="77"/>
       <c r="M6" s="76"/>
       <c r="N6" s="77"/>
@@ -8160,14 +8534,14 @@
       <c r="Q6" s="77"/>
       <c r="R6" s="90"/>
       <c r="S6" s="91"/>
-      <c r="T6" s="179"/>
-      <c r="U6" s="180"/>
+      <c r="T6" s="178"/>
+      <c r="U6" s="179"/>
       <c r="V6" s="91"/>
       <c r="W6" s="92"/>
       <c r="X6" s="90"/>
       <c r="Y6" s="91"/>
-      <c r="Z6" s="159"/>
-      <c r="AA6" s="160"/>
+      <c r="Z6" s="158"/>
+      <c r="AA6" s="159"/>
       <c r="AB6" s="91"/>
       <c r="AC6" s="92"/>
       <c r="AD6" s="101"/>
@@ -8190,10 +8564,10 @@
       <c r="E7" s="77"/>
       <c r="F7" s="62"/>
       <c r="G7" s="75"/>
-      <c r="H7" s="169"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="169"/>
-      <c r="K7" s="170"/>
+      <c r="H7" s="168"/>
+      <c r="I7" s="169"/>
+      <c r="J7" s="168"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="77"/>
       <c r="M7" s="76"/>
       <c r="N7" s="77"/>
@@ -8202,14 +8576,14 @@
       <c r="Q7" s="77"/>
       <c r="R7" s="90"/>
       <c r="S7" s="91"/>
-      <c r="T7" s="179"/>
-      <c r="U7" s="180"/>
+      <c r="T7" s="178"/>
+      <c r="U7" s="179"/>
       <c r="V7" s="91"/>
       <c r="W7" s="92"/>
       <c r="X7" s="90"/>
       <c r="Y7" s="91"/>
-      <c r="Z7" s="159"/>
-      <c r="AA7" s="160"/>
+      <c r="Z7" s="158"/>
+      <c r="AA7" s="159"/>
       <c r="AB7" s="91"/>
       <c r="AC7" s="92"/>
       <c r="AD7" s="101"/>
@@ -8232,10 +8606,10 @@
       <c r="E8" s="77"/>
       <c r="F8" s="62"/>
       <c r="G8" s="75"/>
-      <c r="H8" s="169"/>
-      <c r="I8" s="170"/>
-      <c r="J8" s="169"/>
-      <c r="K8" s="170"/>
+      <c r="H8" s="168"/>
+      <c r="I8" s="169"/>
+      <c r="J8" s="168"/>
+      <c r="K8" s="169"/>
       <c r="L8" s="77"/>
       <c r="M8" s="76"/>
       <c r="N8" s="77"/>
@@ -8244,14 +8618,14 @@
       <c r="Q8" s="77"/>
       <c r="R8" s="90"/>
       <c r="S8" s="91"/>
-      <c r="T8" s="179"/>
-      <c r="U8" s="180"/>
+      <c r="T8" s="178"/>
+      <c r="U8" s="179"/>
       <c r="V8" s="91"/>
       <c r="W8" s="92"/>
       <c r="X8" s="90"/>
       <c r="Y8" s="91"/>
-      <c r="Z8" s="159"/>
-      <c r="AA8" s="160"/>
+      <c r="Z8" s="158"/>
+      <c r="AA8" s="159"/>
       <c r="AB8" s="91"/>
       <c r="AC8" s="92"/>
       <c r="AD8" s="101"/>
@@ -8274,10 +8648,10 @@
       <c r="E9" s="77"/>
       <c r="F9" s="62"/>
       <c r="G9" s="75"/>
-      <c r="H9" s="169"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="170"/>
+      <c r="H9" s="168"/>
+      <c r="I9" s="169"/>
+      <c r="J9" s="168"/>
+      <c r="K9" s="169"/>
       <c r="L9" s="77"/>
       <c r="M9" s="76"/>
       <c r="N9" s="77"/>
@@ -8286,14 +8660,14 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="90"/>
       <c r="S9" s="91"/>
-      <c r="T9" s="179"/>
-      <c r="U9" s="180"/>
+      <c r="T9" s="178"/>
+      <c r="U9" s="179"/>
       <c r="V9" s="91"/>
       <c r="W9" s="92"/>
       <c r="X9" s="90"/>
       <c r="Y9" s="91"/>
-      <c r="Z9" s="159"/>
-      <c r="AA9" s="160"/>
+      <c r="Z9" s="158"/>
+      <c r="AA9" s="159"/>
       <c r="AB9" s="91"/>
       <c r="AC9" s="92"/>
       <c r="AD9" s="101"/>
@@ -8316,10 +8690,10 @@
       <c r="E10" s="77"/>
       <c r="F10" s="62"/>
       <c r="G10" s="75"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="170"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="170"/>
+      <c r="H10" s="168"/>
+      <c r="I10" s="169"/>
+      <c r="J10" s="168"/>
+      <c r="K10" s="169"/>
       <c r="L10" s="77"/>
       <c r="M10" s="76"/>
       <c r="N10" s="77"/>
@@ -8328,14 +8702,14 @@
       <c r="Q10" s="77"/>
       <c r="R10" s="90"/>
       <c r="S10" s="91"/>
-      <c r="T10" s="179"/>
-      <c r="U10" s="180"/>
+      <c r="T10" s="178"/>
+      <c r="U10" s="179"/>
       <c r="V10" s="91"/>
       <c r="W10" s="92"/>
       <c r="X10" s="90"/>
       <c r="Y10" s="91"/>
-      <c r="Z10" s="159"/>
-      <c r="AA10" s="160"/>
+      <c r="Z10" s="158"/>
+      <c r="AA10" s="159"/>
       <c r="AB10" s="91"/>
       <c r="AC10" s="92"/>
       <c r="AD10" s="101"/>
@@ -8358,10 +8732,10 @@
       <c r="E11" s="77"/>
       <c r="F11" s="62"/>
       <c r="G11" s="75"/>
-      <c r="H11" s="169"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="169"/>
-      <c r="K11" s="170"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="169"/>
+      <c r="J11" s="168"/>
+      <c r="K11" s="169"/>
       <c r="L11" s="77"/>
       <c r="M11" s="76">
         <v>0.75</v>
@@ -8374,14 +8748,14 @@
       <c r="Q11" s="77"/>
       <c r="R11" s="90"/>
       <c r="S11" s="91"/>
-      <c r="T11" s="179"/>
-      <c r="U11" s="180"/>
+      <c r="T11" s="178"/>
+      <c r="U11" s="179"/>
       <c r="V11" s="91"/>
       <c r="W11" s="92"/>
       <c r="X11" s="90"/>
       <c r="Y11" s="91"/>
-      <c r="Z11" s="159"/>
-      <c r="AA11" s="160"/>
+      <c r="Z11" s="158"/>
+      <c r="AA11" s="159"/>
       <c r="AB11" s="91"/>
       <c r="AC11" s="92"/>
       <c r="AD11" s="101"/>
@@ -8404,10 +8778,10 @@
       <c r="E12" s="77"/>
       <c r="F12" s="62"/>
       <c r="G12" s="75"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="169"/>
-      <c r="K12" s="170"/>
+      <c r="H12" s="168"/>
+      <c r="I12" s="169"/>
+      <c r="J12" s="168"/>
+      <c r="K12" s="169"/>
       <c r="L12" s="77"/>
       <c r="M12" s="76"/>
       <c r="N12" s="77"/>
@@ -8416,14 +8790,14 @@
       <c r="Q12" s="77"/>
       <c r="R12" s="90"/>
       <c r="S12" s="91"/>
-      <c r="T12" s="179"/>
-      <c r="U12" s="180"/>
+      <c r="T12" s="178"/>
+      <c r="U12" s="179"/>
       <c r="V12" s="91"/>
       <c r="W12" s="92"/>
       <c r="X12" s="90"/>
       <c r="Y12" s="91"/>
-      <c r="Z12" s="159"/>
-      <c r="AA12" s="160"/>
+      <c r="Z12" s="158"/>
+      <c r="AA12" s="159"/>
       <c r="AB12" s="91"/>
       <c r="AC12" s="92"/>
       <c r="AD12" s="101"/>
@@ -8448,10 +8822,10 @@
       <c r="E13" s="77"/>
       <c r="F13" s="62"/>
       <c r="G13" s="75"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="169"/>
-      <c r="K13" s="170"/>
+      <c r="H13" s="168"/>
+      <c r="I13" s="169"/>
+      <c r="J13" s="168"/>
+      <c r="K13" s="169"/>
       <c r="L13" s="77"/>
       <c r="M13" s="76"/>
       <c r="N13" s="77"/>
@@ -8460,14 +8834,14 @@
       <c r="Q13" s="77"/>
       <c r="R13" s="90"/>
       <c r="S13" s="91"/>
-      <c r="T13" s="179"/>
-      <c r="U13" s="180"/>
+      <c r="T13" s="178"/>
+      <c r="U13" s="179"/>
       <c r="V13" s="91"/>
       <c r="W13" s="92"/>
       <c r="X13" s="90"/>
       <c r="Y13" s="91"/>
-      <c r="Z13" s="159"/>
-      <c r="AA13" s="160"/>
+      <c r="Z13" s="158"/>
+      <c r="AA13" s="159"/>
       <c r="AB13" s="91"/>
       <c r="AC13" s="92"/>
       <c r="AD13" s="101"/>
@@ -8494,10 +8868,10 @@
       </c>
       <c r="F14" s="62"/>
       <c r="G14" s="75"/>
-      <c r="H14" s="169"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="169"/>
-      <c r="K14" s="170"/>
+      <c r="H14" s="168"/>
+      <c r="I14" s="169"/>
+      <c r="J14" s="168"/>
+      <c r="K14" s="169"/>
       <c r="L14" s="77"/>
       <c r="M14" s="76">
         <v>0.75</v>
@@ -8510,14 +8884,14 @@
       <c r="Q14" s="77"/>
       <c r="R14" s="90"/>
       <c r="S14" s="91"/>
-      <c r="T14" s="179"/>
-      <c r="U14" s="180"/>
+      <c r="T14" s="178"/>
+      <c r="U14" s="179"/>
       <c r="V14" s="91"/>
       <c r="W14" s="92"/>
       <c r="X14" s="90"/>
       <c r="Y14" s="91"/>
-      <c r="Z14" s="159"/>
-      <c r="AA14" s="160"/>
+      <c r="Z14" s="158"/>
+      <c r="AA14" s="159"/>
       <c r="AB14" s="91"/>
       <c r="AC14" s="92"/>
       <c r="AD14" s="101"/>
@@ -8542,10 +8916,10 @@
       </c>
       <c r="F15" s="62"/>
       <c r="G15" s="75"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="169"/>
-      <c r="K15" s="170"/>
+      <c r="H15" s="168"/>
+      <c r="I15" s="169"/>
+      <c r="J15" s="168"/>
+      <c r="K15" s="169"/>
       <c r="L15" s="77"/>
       <c r="M15" s="76"/>
       <c r="N15" s="77"/>
@@ -8554,14 +8928,14 @@
       <c r="Q15" s="77"/>
       <c r="R15" s="90"/>
       <c r="S15" s="91"/>
-      <c r="T15" s="179"/>
-      <c r="U15" s="180"/>
+      <c r="T15" s="178"/>
+      <c r="U15" s="179"/>
       <c r="V15" s="91"/>
       <c r="W15" s="92"/>
       <c r="X15" s="90"/>
       <c r="Y15" s="91"/>
-      <c r="Z15" s="159"/>
-      <c r="AA15" s="160"/>
+      <c r="Z15" s="158"/>
+      <c r="AA15" s="159"/>
       <c r="AB15" s="91"/>
       <c r="AC15" s="92"/>
       <c r="AD15" s="101"/>
@@ -8584,10 +8958,10 @@
       <c r="E16" s="77"/>
       <c r="F16" s="62"/>
       <c r="G16" s="75"/>
-      <c r="H16" s="169"/>
-      <c r="I16" s="170"/>
-      <c r="J16" s="169"/>
-      <c r="K16" s="170"/>
+      <c r="H16" s="168"/>
+      <c r="I16" s="169"/>
+      <c r="J16" s="168"/>
+      <c r="K16" s="169"/>
       <c r="L16" s="77"/>
       <c r="M16" s="76">
         <v>0.82</v>
@@ -8600,14 +8974,14 @@
       <c r="Q16" s="77"/>
       <c r="R16" s="90"/>
       <c r="S16" s="91"/>
-      <c r="T16" s="179"/>
-      <c r="U16" s="180"/>
+      <c r="T16" s="178"/>
+      <c r="U16" s="179"/>
       <c r="V16" s="91"/>
       <c r="W16" s="92"/>
       <c r="X16" s="90"/>
       <c r="Y16" s="91"/>
-      <c r="Z16" s="159"/>
-      <c r="AA16" s="160"/>
+      <c r="Z16" s="158"/>
+      <c r="AA16" s="159"/>
       <c r="AB16" s="91"/>
       <c r="AC16" s="92"/>
       <c r="AD16" s="101"/>
@@ -8630,10 +9004,10 @@
       <c r="E17" s="77"/>
       <c r="F17" s="62"/>
       <c r="G17" s="75"/>
-      <c r="H17" s="169"/>
-      <c r="I17" s="170"/>
-      <c r="J17" s="169"/>
-      <c r="K17" s="170"/>
+      <c r="H17" s="168"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="168"/>
+      <c r="K17" s="169"/>
       <c r="L17" s="77"/>
       <c r="M17" s="76">
         <v>0.86</v>
@@ -8646,14 +9020,14 @@
       <c r="Q17" s="77"/>
       <c r="R17" s="90"/>
       <c r="S17" s="91"/>
-      <c r="T17" s="179"/>
-      <c r="U17" s="180"/>
+      <c r="T17" s="178"/>
+      <c r="U17" s="179"/>
       <c r="V17" s="91"/>
       <c r="W17" s="92"/>
       <c r="X17" s="90"/>
       <c r="Y17" s="91"/>
-      <c r="Z17" s="159"/>
-      <c r="AA17" s="160"/>
+      <c r="Z17" s="158"/>
+      <c r="AA17" s="159"/>
       <c r="AB17" s="91"/>
       <c r="AC17" s="92"/>
       <c r="AD17" s="101"/>
@@ -8676,10 +9050,10 @@
       <c r="E18" s="77"/>
       <c r="F18" s="62"/>
       <c r="G18" s="75"/>
-      <c r="H18" s="169"/>
-      <c r="I18" s="170"/>
-      <c r="J18" s="169"/>
-      <c r="K18" s="170"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="169"/>
+      <c r="J18" s="168"/>
+      <c r="K18" s="169"/>
       <c r="L18" s="77"/>
       <c r="M18" s="76">
         <v>0.89</v>
@@ -8692,14 +9066,14 @@
       <c r="Q18" s="77"/>
       <c r="R18" s="90"/>
       <c r="S18" s="91"/>
-      <c r="T18" s="179"/>
-      <c r="U18" s="180"/>
+      <c r="T18" s="178"/>
+      <c r="U18" s="179"/>
       <c r="V18" s="91"/>
       <c r="W18" s="92"/>
       <c r="X18" s="90"/>
       <c r="Y18" s="91"/>
-      <c r="Z18" s="159"/>
-      <c r="AA18" s="160"/>
+      <c r="Z18" s="158"/>
+      <c r="AA18" s="159"/>
       <c r="AB18" s="91"/>
       <c r="AC18" s="92"/>
       <c r="AD18" s="101"/>
@@ -8722,10 +9096,10 @@
       <c r="E19" s="77"/>
       <c r="F19" s="62"/>
       <c r="G19" s="75"/>
-      <c r="H19" s="169"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="169"/>
-      <c r="K19" s="170"/>
+      <c r="H19" s="168"/>
+      <c r="I19" s="169"/>
+      <c r="J19" s="168"/>
+      <c r="K19" s="169"/>
       <c r="L19" s="77"/>
       <c r="M19" s="76">
         <v>0.92</v>
@@ -8738,14 +9112,14 @@
       <c r="Q19" s="77"/>
       <c r="R19" s="90"/>
       <c r="S19" s="91"/>
-      <c r="T19" s="179"/>
-      <c r="U19" s="180"/>
+      <c r="T19" s="178"/>
+      <c r="U19" s="179"/>
       <c r="V19" s="91"/>
       <c r="W19" s="92"/>
       <c r="X19" s="90"/>
       <c r="Y19" s="91"/>
-      <c r="Z19" s="159"/>
-      <c r="AA19" s="160"/>
+      <c r="Z19" s="158"/>
+      <c r="AA19" s="159"/>
       <c r="AB19" s="91"/>
       <c r="AC19" s="92"/>
       <c r="AD19" s="101"/>
@@ -8772,10 +9146,10 @@
       </c>
       <c r="F20" s="62"/>
       <c r="G20" s="75"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="169"/>
-      <c r="K20" s="170"/>
+      <c r="H20" s="168"/>
+      <c r="I20" s="169"/>
+      <c r="J20" s="168"/>
+      <c r="K20" s="169"/>
       <c r="L20" s="77"/>
       <c r="M20" s="76">
         <v>0.95</v>
@@ -8788,14 +9162,14 @@
       <c r="Q20" s="77"/>
       <c r="R20" s="90"/>
       <c r="S20" s="91"/>
-      <c r="T20" s="179"/>
-      <c r="U20" s="180"/>
+      <c r="T20" s="178"/>
+      <c r="U20" s="179"/>
       <c r="V20" s="91"/>
       <c r="W20" s="92"/>
       <c r="X20" s="90"/>
       <c r="Y20" s="91"/>
-      <c r="Z20" s="159"/>
-      <c r="AA20" s="160"/>
+      <c r="Z20" s="158"/>
+      <c r="AA20" s="159"/>
       <c r="AB20" s="91"/>
       <c r="AC20" s="92"/>
       <c r="AD20" s="101"/>
@@ -8818,10 +9192,10 @@
       <c r="E21" s="77"/>
       <c r="F21" s="62"/>
       <c r="G21" s="75"/>
-      <c r="H21" s="169"/>
-      <c r="I21" s="170"/>
-      <c r="J21" s="169"/>
-      <c r="K21" s="170"/>
+      <c r="H21" s="168"/>
+      <c r="I21" s="169"/>
+      <c r="J21" s="168"/>
+      <c r="K21" s="169"/>
       <c r="L21" s="77"/>
       <c r="M21" s="76"/>
       <c r="N21" s="77"/>
@@ -8830,14 +9204,14 @@
       <c r="Q21" s="77"/>
       <c r="R21" s="90"/>
       <c r="S21" s="91"/>
-      <c r="T21" s="179"/>
-      <c r="U21" s="180"/>
+      <c r="T21" s="178"/>
+      <c r="U21" s="179"/>
       <c r="V21" s="91"/>
       <c r="W21" s="92"/>
       <c r="X21" s="90"/>
       <c r="Y21" s="91"/>
-      <c r="Z21" s="159"/>
-      <c r="AA21" s="160"/>
+      <c r="Z21" s="158"/>
+      <c r="AA21" s="159"/>
       <c r="AB21" s="91"/>
       <c r="AC21" s="92"/>
       <c r="AD21" s="101"/>
@@ -8860,10 +9234,10 @@
       <c r="E22" s="77"/>
       <c r="F22" s="62"/>
       <c r="G22" s="75"/>
-      <c r="H22" s="169"/>
-      <c r="I22" s="170"/>
-      <c r="J22" s="169"/>
-      <c r="K22" s="170"/>
+      <c r="H22" s="168"/>
+      <c r="I22" s="169"/>
+      <c r="J22" s="168"/>
+      <c r="K22" s="169"/>
       <c r="L22" s="77"/>
       <c r="M22" s="76"/>
       <c r="N22" s="77"/>
@@ -8872,14 +9246,14 @@
       <c r="Q22" s="77"/>
       <c r="R22" s="90"/>
       <c r="S22" s="91"/>
-      <c r="T22" s="179"/>
-      <c r="U22" s="180"/>
+      <c r="T22" s="178"/>
+      <c r="U22" s="179"/>
       <c r="V22" s="91"/>
       <c r="W22" s="92"/>
       <c r="X22" s="90"/>
       <c r="Y22" s="91"/>
-      <c r="Z22" s="159"/>
-      <c r="AA22" s="160"/>
+      <c r="Z22" s="158"/>
+      <c r="AA22" s="159"/>
       <c r="AB22" s="91"/>
       <c r="AC22" s="92"/>
       <c r="AD22" s="101"/>
@@ -8902,10 +9276,10 @@
       <c r="E23" s="77"/>
       <c r="F23" s="62"/>
       <c r="G23" s="75"/>
-      <c r="H23" s="169"/>
-      <c r="I23" s="170"/>
-      <c r="J23" s="169"/>
-      <c r="K23" s="170"/>
+      <c r="H23" s="168"/>
+      <c r="I23" s="169"/>
+      <c r="J23" s="168"/>
+      <c r="K23" s="169"/>
       <c r="L23" s="77"/>
       <c r="M23" s="76"/>
       <c r="N23" s="77"/>
@@ -8914,14 +9288,14 @@
       <c r="Q23" s="77"/>
       <c r="R23" s="90"/>
       <c r="S23" s="91"/>
-      <c r="T23" s="179"/>
-      <c r="U23" s="180"/>
+      <c r="T23" s="178"/>
+      <c r="U23" s="179"/>
       <c r="V23" s="91"/>
       <c r="W23" s="92"/>
       <c r="X23" s="90"/>
       <c r="Y23" s="91"/>
-      <c r="Z23" s="159"/>
-      <c r="AA23" s="160"/>
+      <c r="Z23" s="158"/>
+      <c r="AA23" s="159"/>
       <c r="AB23" s="91"/>
       <c r="AC23" s="92"/>
       <c r="AD23" s="101"/>
@@ -8944,10 +9318,10 @@
       <c r="E24" s="77"/>
       <c r="F24" s="62"/>
       <c r="G24" s="75"/>
-      <c r="H24" s="169"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="169"/>
-      <c r="K24" s="170"/>
+      <c r="H24" s="168"/>
+      <c r="I24" s="169"/>
+      <c r="J24" s="168"/>
+      <c r="K24" s="169"/>
       <c r="L24" s="77"/>
       <c r="M24" s="76"/>
       <c r="N24" s="77"/>
@@ -8956,14 +9330,14 @@
       <c r="Q24" s="77"/>
       <c r="R24" s="90"/>
       <c r="S24" s="91"/>
-      <c r="T24" s="179"/>
-      <c r="U24" s="180"/>
+      <c r="T24" s="178"/>
+      <c r="U24" s="179"/>
       <c r="V24" s="91"/>
       <c r="W24" s="92"/>
       <c r="X24" s="90"/>
       <c r="Y24" s="91"/>
-      <c r="Z24" s="159"/>
-      <c r="AA24" s="160"/>
+      <c r="Z24" s="158"/>
+      <c r="AA24" s="159"/>
       <c r="AB24" s="91"/>
       <c r="AC24" s="92"/>
       <c r="AD24" s="101"/>
@@ -8986,10 +9360,10 @@
       <c r="E25" s="77"/>
       <c r="F25" s="62"/>
       <c r="G25" s="75"/>
-      <c r="H25" s="169"/>
-      <c r="I25" s="170"/>
-      <c r="J25" s="169"/>
-      <c r="K25" s="170"/>
+      <c r="H25" s="168"/>
+      <c r="I25" s="169"/>
+      <c r="J25" s="168"/>
+      <c r="K25" s="169"/>
       <c r="L25" s="77"/>
       <c r="M25" s="76"/>
       <c r="N25" s="77"/>
@@ -8998,14 +9372,14 @@
       <c r="Q25" s="77"/>
       <c r="R25" s="90"/>
       <c r="S25" s="91"/>
-      <c r="T25" s="179"/>
-      <c r="U25" s="180"/>
+      <c r="T25" s="178"/>
+      <c r="U25" s="179"/>
       <c r="V25" s="91"/>
       <c r="W25" s="92"/>
       <c r="X25" s="90"/>
       <c r="Y25" s="91"/>
-      <c r="Z25" s="159"/>
-      <c r="AA25" s="160"/>
+      <c r="Z25" s="158"/>
+      <c r="AA25" s="159"/>
       <c r="AB25" s="91"/>
       <c r="AC25" s="92"/>
       <c r="AD25" s="101"/>
@@ -9028,10 +9402,10 @@
       <c r="E26" s="77"/>
       <c r="F26" s="62"/>
       <c r="G26" s="75"/>
-      <c r="H26" s="169"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="169"/>
-      <c r="K26" s="170"/>
+      <c r="H26" s="168"/>
+      <c r="I26" s="169"/>
+      <c r="J26" s="168"/>
+      <c r="K26" s="169"/>
       <c r="L26" s="77"/>
       <c r="M26" s="76"/>
       <c r="N26" s="77"/>
@@ -9040,14 +9414,14 @@
       <c r="Q26" s="77"/>
       <c r="R26" s="90"/>
       <c r="S26" s="91"/>
-      <c r="T26" s="179"/>
-      <c r="U26" s="180"/>
+      <c r="T26" s="178"/>
+      <c r="U26" s="179"/>
       <c r="V26" s="91"/>
       <c r="W26" s="92"/>
       <c r="X26" s="90"/>
       <c r="Y26" s="91"/>
-      <c r="Z26" s="159"/>
-      <c r="AA26" s="160"/>
+      <c r="Z26" s="158"/>
+      <c r="AA26" s="159"/>
       <c r="AB26" s="91"/>
       <c r="AC26" s="92"/>
       <c r="AD26" s="101"/>
@@ -9070,10 +9444,10 @@
       <c r="E27" s="77"/>
       <c r="F27" s="62"/>
       <c r="G27" s="75"/>
-      <c r="H27" s="169"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="169"/>
-      <c r="K27" s="170"/>
+      <c r="H27" s="168"/>
+      <c r="I27" s="169"/>
+      <c r="J27" s="168"/>
+      <c r="K27" s="169"/>
       <c r="L27" s="77"/>
       <c r="M27" s="76"/>
       <c r="N27" s="77"/>
@@ -9082,14 +9456,14 @@
       <c r="Q27" s="77"/>
       <c r="R27" s="90"/>
       <c r="S27" s="91"/>
-      <c r="T27" s="179"/>
-      <c r="U27" s="180"/>
+      <c r="T27" s="178"/>
+      <c r="U27" s="179"/>
       <c r="V27" s="91"/>
       <c r="W27" s="92"/>
       <c r="X27" s="90"/>
       <c r="Y27" s="91"/>
-      <c r="Z27" s="159"/>
-      <c r="AA27" s="160"/>
+      <c r="Z27" s="158"/>
+      <c r="AA27" s="159"/>
       <c r="AB27" s="91"/>
       <c r="AC27" s="92"/>
       <c r="AD27" s="101"/>
@@ -9112,10 +9486,10 @@
       <c r="E28" s="77"/>
       <c r="F28" s="62"/>
       <c r="G28" s="75"/>
-      <c r="H28" s="169"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="169"/>
-      <c r="K28" s="170"/>
+      <c r="H28" s="168"/>
+      <c r="I28" s="169"/>
+      <c r="J28" s="168"/>
+      <c r="K28" s="169"/>
       <c r="L28" s="77"/>
       <c r="M28" s="76"/>
       <c r="N28" s="77"/>
@@ -9124,14 +9498,14 @@
       <c r="Q28" s="77"/>
       <c r="R28" s="90"/>
       <c r="S28" s="91"/>
-      <c r="T28" s="179"/>
-      <c r="U28" s="180"/>
+      <c r="T28" s="178"/>
+      <c r="U28" s="179"/>
       <c r="V28" s="91"/>
       <c r="W28" s="92"/>
       <c r="X28" s="90"/>
       <c r="Y28" s="91"/>
-      <c r="Z28" s="159"/>
-      <c r="AA28" s="160"/>
+      <c r="Z28" s="158"/>
+      <c r="AA28" s="159"/>
       <c r="AB28" s="91"/>
       <c r="AC28" s="92"/>
       <c r="AD28" s="101"/>
@@ -9154,10 +9528,10 @@
       <c r="E29" s="77"/>
       <c r="F29" s="62"/>
       <c r="G29" s="75"/>
-      <c r="H29" s="169"/>
-      <c r="I29" s="170"/>
-      <c r="J29" s="169"/>
-      <c r="K29" s="170"/>
+      <c r="H29" s="168"/>
+      <c r="I29" s="169"/>
+      <c r="J29" s="168"/>
+      <c r="K29" s="169"/>
       <c r="L29" s="77"/>
       <c r="M29" s="76">
         <v>0.95</v>
@@ -9170,14 +9544,14 @@
       <c r="Q29" s="77"/>
       <c r="R29" s="90"/>
       <c r="S29" s="91"/>
-      <c r="T29" s="179"/>
-      <c r="U29" s="180"/>
+      <c r="T29" s="178"/>
+      <c r="U29" s="179"/>
       <c r="V29" s="91"/>
       <c r="W29" s="92"/>
       <c r="X29" s="90"/>
       <c r="Y29" s="91"/>
-      <c r="Z29" s="159"/>
-      <c r="AA29" s="160"/>
+      <c r="Z29" s="158"/>
+      <c r="AA29" s="159"/>
       <c r="AB29" s="91"/>
       <c r="AC29" s="92"/>
       <c r="AD29" s="101"/>
@@ -9200,10 +9574,10 @@
       <c r="E30" s="77"/>
       <c r="F30" s="62"/>
       <c r="G30" s="75"/>
-      <c r="H30" s="169"/>
-      <c r="I30" s="170"/>
-      <c r="J30" s="169"/>
-      <c r="K30" s="170"/>
+      <c r="H30" s="168"/>
+      <c r="I30" s="169"/>
+      <c r="J30" s="168"/>
+      <c r="K30" s="169"/>
       <c r="L30" s="77"/>
       <c r="M30" s="76"/>
       <c r="N30" s="77"/>
@@ -9212,14 +9586,14 @@
       <c r="Q30" s="77"/>
       <c r="R30" s="90"/>
       <c r="S30" s="91"/>
-      <c r="T30" s="179"/>
-      <c r="U30" s="180"/>
+      <c r="T30" s="178"/>
+      <c r="U30" s="179"/>
       <c r="V30" s="91"/>
       <c r="W30" s="92"/>
       <c r="X30" s="90"/>
       <c r="Y30" s="91"/>
-      <c r="Z30" s="159"/>
-      <c r="AA30" s="160"/>
+      <c r="Z30" s="158"/>
+      <c r="AA30" s="159"/>
       <c r="AB30" s="91"/>
       <c r="AC30" s="92"/>
       <c r="AD30" s="101"/>
@@ -9242,10 +9616,10 @@
       <c r="E31" s="77"/>
       <c r="F31" s="62"/>
       <c r="G31" s="75"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="170"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="170"/>
+      <c r="H31" s="168"/>
+      <c r="I31" s="169"/>
+      <c r="J31" s="168"/>
+      <c r="K31" s="169"/>
       <c r="L31" s="77"/>
       <c r="M31" s="76"/>
       <c r="N31" s="77"/>
@@ -9254,14 +9628,14 @@
       <c r="Q31" s="77"/>
       <c r="R31" s="90"/>
       <c r="S31" s="91"/>
-      <c r="T31" s="179"/>
-      <c r="U31" s="180"/>
+      <c r="T31" s="178"/>
+      <c r="U31" s="179"/>
       <c r="V31" s="91"/>
       <c r="W31" s="92"/>
       <c r="X31" s="90"/>
       <c r="Y31" s="91"/>
-      <c r="Z31" s="159"/>
-      <c r="AA31" s="160"/>
+      <c r="Z31" s="158"/>
+      <c r="AA31" s="159"/>
       <c r="AB31" s="91"/>
       <c r="AC31" s="92"/>
       <c r="AD31" s="101"/>
@@ -9284,10 +9658,10 @@
       <c r="E32" s="77"/>
       <c r="F32" s="62"/>
       <c r="G32" s="75"/>
-      <c r="H32" s="169"/>
-      <c r="I32" s="170"/>
-      <c r="J32" s="169"/>
-      <c r="K32" s="170"/>
+      <c r="H32" s="168"/>
+      <c r="I32" s="169"/>
+      <c r="J32" s="168"/>
+      <c r="K32" s="169"/>
       <c r="L32" s="77"/>
       <c r="M32" s="76"/>
       <c r="N32" s="77"/>
@@ -9296,14 +9670,14 @@
       <c r="Q32" s="77"/>
       <c r="R32" s="90"/>
       <c r="S32" s="91"/>
-      <c r="T32" s="179"/>
-      <c r="U32" s="180"/>
+      <c r="T32" s="178"/>
+      <c r="U32" s="179"/>
       <c r="V32" s="91"/>
       <c r="W32" s="92"/>
       <c r="X32" s="90"/>
       <c r="Y32" s="91"/>
-      <c r="Z32" s="159"/>
-      <c r="AA32" s="160"/>
+      <c r="Z32" s="158"/>
+      <c r="AA32" s="159"/>
       <c r="AB32" s="91"/>
       <c r="AC32" s="92"/>
       <c r="AD32" s="101"/>
@@ -9326,10 +9700,10 @@
       <c r="E33" s="77"/>
       <c r="F33" s="62"/>
       <c r="G33" s="75"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="170"/>
-      <c r="J33" s="169"/>
-      <c r="K33" s="170"/>
+      <c r="H33" s="168"/>
+      <c r="I33" s="169"/>
+      <c r="J33" s="168"/>
+      <c r="K33" s="169"/>
       <c r="L33" s="77"/>
       <c r="M33" s="76"/>
       <c r="N33" s="77"/>
@@ -9338,14 +9712,14 @@
       <c r="Q33" s="77"/>
       <c r="R33" s="90"/>
       <c r="S33" s="91"/>
-      <c r="T33" s="179"/>
-      <c r="U33" s="180"/>
+      <c r="T33" s="178"/>
+      <c r="U33" s="179"/>
       <c r="V33" s="91"/>
       <c r="W33" s="92"/>
       <c r="X33" s="90"/>
       <c r="Y33" s="91"/>
-      <c r="Z33" s="159"/>
-      <c r="AA33" s="160"/>
+      <c r="Z33" s="158"/>
+      <c r="AA33" s="159"/>
       <c r="AB33" s="91"/>
       <c r="AC33" s="92"/>
       <c r="AD33" s="101"/>
@@ -9368,10 +9742,10 @@
       <c r="E34" s="80"/>
       <c r="F34" s="64"/>
       <c r="G34" s="78"/>
-      <c r="H34" s="171"/>
-      <c r="I34" s="172"/>
-      <c r="J34" s="171"/>
-      <c r="K34" s="172"/>
+      <c r="H34" s="170"/>
+      <c r="I34" s="171"/>
+      <c r="J34" s="170"/>
+      <c r="K34" s="171"/>
       <c r="L34" s="80"/>
       <c r="M34" s="79">
         <v>0.99</v>
@@ -9384,14 +9758,14 @@
       <c r="Q34" s="80"/>
       <c r="R34" s="93"/>
       <c r="S34" s="94"/>
-      <c r="T34" s="181"/>
-      <c r="U34" s="182"/>
+      <c r="T34" s="180"/>
+      <c r="U34" s="181"/>
       <c r="V34" s="94"/>
       <c r="W34" s="95"/>
       <c r="X34" s="93"/>
       <c r="Y34" s="94"/>
-      <c r="Z34" s="161"/>
-      <c r="AA34" s="162"/>
+      <c r="Z34" s="160"/>
+      <c r="AA34" s="161"/>
       <c r="AB34" s="94"/>
       <c r="AC34" s="95"/>
       <c r="AD34" s="102"/>

</xml_diff>

<commit_message>
Updated data, plots and results
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="scen_2" sheetId="26" r:id="rId6"/>
     <sheet name="timepars_old" sheetId="20" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1795,7 +1795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="133">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2192,6 +2192,9 @@
   </si>
   <si>
     <t>proportion_stay</t>
+  </si>
+  <si>
+    <t>years each person is in model</t>
   </si>
 </sst>
 </file>
@@ -3814,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,16 +3917,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="47">
-        <f>0.001*12*C2</f>
-        <v>1E-3</v>
+        <f>1 - EXP(-$C$2 / $H$8)</f>
+        <v>1.8501382321644E-3</v>
       </c>
       <c r="D4" s="19">
         <f t="shared" si="0"/>
-        <v>9.5E-4</v>
+        <v>1.7576313205561801E-3</v>
       </c>
       <c r="E4" s="16">
         <f t="shared" si="1"/>
-        <v>1.0499999999999999E-3</v>
+        <v>1.9426451437726199E-3</v>
       </c>
       <c r="L4" s="48"/>
       <c r="M4" s="43" t="s">
@@ -4032,6 +4035,12 @@
       <c r="E8" s="18">
         <f t="shared" si="1"/>
         <v>0.13650000000000001</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="43">
+        <v>45</v>
       </c>
       <c r="J8" s="43" t="s">
         <v>106</v>
@@ -5981,7 +5990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S29" sqref="S29:T29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added in Kat's updated data
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom.tidhar\Documents\GitHub\STI-HIV-coinfection\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <sheet name="scen_2" sheetId="26" r:id="rId6"/>
     <sheet name="timepars_old" sheetId="20" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -31,7 +26,7 @@
     <author>Michael Traeger</author>
   </authors>
   <commentList>
-    <comment ref="M4" authorId="0" shapeId="0">
+    <comment ref="M4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,10 +50,10 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="1" shapeId="0">
+    <comment ref="C8" authorId="1">
       <text/>
     </comment>
-    <comment ref="C11" authorId="1" shapeId="0">
+    <comment ref="C11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -82,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0">
+    <comment ref="C18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +214,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0">
+    <comment ref="C1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -277,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0">
+    <comment ref="D1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -304,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -328,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="2" shapeId="0">
+    <comment ref="L1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -355,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" shapeId="0">
+    <comment ref="M1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -379,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="2" shapeId="0">
+    <comment ref="O1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -403,7 +398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="2" shapeId="0">
+    <comment ref="Q1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -429,7 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="2" shapeId="0">
+    <comment ref="S1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -453,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="2" shapeId="0">
+    <comment ref="T1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -477,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="2" shapeId="0">
+    <comment ref="U1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -501,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="2" shapeId="0">
+    <comment ref="W1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -529,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="2" shapeId="0">
+    <comment ref="X1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -554,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="2" shapeId="0">
+    <comment ref="Y1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -580,7 +575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="2" shapeId="0">
+    <comment ref="Z1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -609,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="2" shapeId="0">
+    <comment ref="AA1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -635,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="2" shapeId="0">
+    <comment ref="AB1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -659,7 +654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="2" shapeId="0">
+    <comment ref="AC1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -683,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE2" authorId="1" shapeId="0">
+    <comment ref="AE2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -707,7 +702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="2" shapeId="0">
+    <comment ref="O8" authorId="2">
       <text>
         <r>
           <rPr>
@@ -731,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="2" shapeId="0">
+    <comment ref="O9" authorId="2">
       <text>
         <r>
           <rPr>
@@ -755,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O12" authorId="0" shapeId="0">
+    <comment ref="O12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -783,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD12" authorId="0" shapeId="0">
+    <comment ref="AD12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -807,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="2" shapeId="0">
+    <comment ref="R13" authorId="2">
       <text>
         <r>
           <rPr>
@@ -831,7 +826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="2" shapeId="0">
+    <comment ref="A14" authorId="2">
       <text>
         <r>
           <rPr>
@@ -867,7 +862,7 @@
     <author>Kathleen Ryan</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -891,7 +886,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -915,7 +910,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -939,7 +934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -966,7 +961,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -990,7 +985,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1014,7 +1009,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1038,7 +1033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1062,7 +1057,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" shapeId="0">
+    <comment ref="X1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1086,7 +1081,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1110,7 +1105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1134,7 +1129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0">
+    <comment ref="M2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1158,7 +1153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0">
+    <comment ref="N2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1182,7 +1177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="1" shapeId="0">
+    <comment ref="B3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1207,7 +1202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1231,7 +1226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="T3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1255,7 +1250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="1" shapeId="0">
+    <comment ref="D18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1290,7 +1285,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1324,7 +1319,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1348,7 +1343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1382,7 +1377,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1406,7 +1401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1430,7 +1425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1454,7 +1449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1478,7 +1473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1502,7 +1497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1526,7 +1521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1550,7 +1545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1574,7 +1569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1598,7 +1593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1622,7 +1617,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1646,7 +1641,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
+    <comment ref="G3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1670,7 +1665,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1694,7 +1689,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1718,7 +1713,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
+    <comment ref="N3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1742,7 +1737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="0" shapeId="0">
+    <comment ref="T4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1766,7 +1761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W4" authorId="0" shapeId="0">
+    <comment ref="W4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2200,7 +2195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -3113,7 +3108,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3490,6 +3485,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -3817,7 +3814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -4308,7 +4305,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <selection pane="topRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4468,7 +4465,9 @@
       <c r="K2" s="202">
         <v>7</v>
       </c>
-      <c r="L2" s="200"/>
+      <c r="L2" s="200">
+        <v>4216</v>
+      </c>
       <c r="M2" s="201"/>
       <c r="N2" s="202"/>
       <c r="O2" s="205"/>
@@ -4522,7 +4521,9 @@
       <c r="K3" s="105">
         <v>10</v>
       </c>
-      <c r="L3" s="106"/>
+      <c r="L3" s="106">
+        <v>4491</v>
+      </c>
       <c r="M3" s="107"/>
       <c r="N3" s="108"/>
       <c r="O3" s="149">
@@ -4537,19 +4538,19 @@
       </c>
       <c r="S3" s="28">
         <f t="shared" ref="S3:S13" si="0">B3-T3</f>
-        <v>0</v>
+        <v>-4491</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ref="T3:T14" si="1">L3</f>
-        <v>0</v>
+        <v>4491</v>
       </c>
       <c r="U3" s="33">
         <f>ROUND(Q3*S3,0)</f>
-        <v>0</v>
+        <v>-105</v>
       </c>
       <c r="V3" s="33">
         <f t="shared" ref="V3" si="2">ROUND(R3*T3,0)</f>
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="W3" s="11">
         <v>1007</v>
@@ -4588,11 +4589,11 @@
       </c>
       <c r="B4" s="188">
         <f>SUM(C4:D4)</f>
-        <v>27291.800000000003</v>
+        <v>27007.800000000003</v>
       </c>
       <c r="C4" s="210">
         <f t="shared" ref="C4:C15" si="3">AF4-(D4+L4)</f>
-        <v>27291.800000000003</v>
+        <v>27007.800000000003</v>
       </c>
       <c r="D4" s="182"/>
       <c r="E4" s="226">
@@ -4617,27 +4618,21 @@
         <v>8</v>
       </c>
       <c r="L4" s="188">
-        <v>4486</v>
-      </c>
-      <c r="M4" s="192">
-        <f>L4*0.78</f>
-        <v>3499.08</v>
-      </c>
-      <c r="N4" s="182">
-        <f>L4*0.22</f>
-        <v>986.92</v>
-      </c>
+        <v>4770</v>
+      </c>
+      <c r="M4" s="192"/>
+      <c r="N4" s="182"/>
       <c r="O4" s="150"/>
       <c r="P4" s="97"/>
       <c r="Q4" s="40"/>
       <c r="R4" s="40"/>
       <c r="S4" s="28">
         <f t="shared" si="0"/>
-        <v>22805.800000000003</v>
+        <v>22237.800000000003</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" si="1"/>
-        <v>4486</v>
+        <v>4770</v>
       </c>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
@@ -4678,11 +4673,11 @@
       </c>
       <c r="B5" s="188">
         <f t="shared" ref="B5:B15" si="8">SUM(C5:D5)</f>
-        <v>27545.200000000004</v>
+        <v>27251.200000000004</v>
       </c>
       <c r="C5" s="210">
         <f t="shared" si="3"/>
-        <v>27545.200000000004</v>
+        <v>27251.200000000004</v>
       </c>
       <c r="D5" s="182"/>
       <c r="E5" s="225">
@@ -4707,27 +4702,21 @@
         <v>7</v>
       </c>
       <c r="L5" s="188">
-        <v>4765</v>
-      </c>
-      <c r="M5" s="192">
-        <f t="shared" ref="M5:M14" si="9">L5*0.78</f>
-        <v>3716.7000000000003</v>
-      </c>
-      <c r="N5" s="182">
-        <f t="shared" ref="N5:N14" si="10">L5*0.22</f>
-        <v>1048.3</v>
-      </c>
+        <v>5059</v>
+      </c>
+      <c r="M5" s="192"/>
+      <c r="N5" s="182"/>
       <c r="O5" s="150"/>
       <c r="P5" s="97"/>
       <c r="Q5" s="40"/>
       <c r="R5" s="40"/>
       <c r="S5" s="28">
         <f t="shared" si="0"/>
-        <v>22780.200000000004</v>
+        <v>22192.200000000004</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" si="1"/>
-        <v>4765</v>
+        <v>5059</v>
       </c>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
@@ -4768,11 +4757,11 @@
       </c>
       <c r="B6" s="188">
         <f t="shared" si="8"/>
-        <v>27788.600000000006</v>
+        <v>27536.600000000006</v>
       </c>
       <c r="C6" s="210">
         <f t="shared" si="3"/>
-        <v>26472.496600000006</v>
+        <v>26220.496600000006</v>
       </c>
       <c r="D6" s="183">
         <v>1316.1034</v>
@@ -4799,16 +4788,10 @@
         <v>14</v>
       </c>
       <c r="L6" s="188">
-        <v>5054</v>
-      </c>
-      <c r="M6" s="192">
-        <f t="shared" si="9"/>
-        <v>3942.1200000000003</v>
-      </c>
-      <c r="N6" s="182">
-        <f t="shared" si="10"/>
-        <v>1111.8800000000001</v>
-      </c>
+        <v>5306</v>
+      </c>
+      <c r="M6" s="192"/>
+      <c r="N6" s="182"/>
       <c r="O6" s="149"/>
       <c r="P6" s="97"/>
       <c r="Q6" s="40">
@@ -4819,19 +4802,19 @@
       </c>
       <c r="S6" s="28">
         <f t="shared" si="0"/>
-        <v>22734.600000000006</v>
+        <v>22230.600000000006</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>5054</v>
+        <v>5306</v>
       </c>
       <c r="U6" s="32">
-        <f t="shared" ref="U6:U12" si="11">ROUND(Q6*S6,0)</f>
-        <v>916</v>
+        <f t="shared" ref="U6:U12" si="9">ROUND(Q6*S6,0)</f>
+        <v>895</v>
       </c>
       <c r="V6" s="32">
-        <f t="shared" ref="V6:V13" si="12">ROUND(R6*T6,0)</f>
-        <v>218</v>
+        <f t="shared" ref="V6:V13" si="10">ROUND(R6*T6,0)</f>
+        <v>229</v>
       </c>
       <c r="W6" s="11">
         <v>1758</v>
@@ -4870,11 +4853,11 @@
       </c>
       <c r="B7" s="188">
         <f>SUM(C7:D7)</f>
-        <v>28074.000000000007</v>
+        <v>27760.000000000007</v>
       </c>
       <c r="C7" s="210">
         <f t="shared" si="3"/>
-        <v>26900.372400000007</v>
+        <v>26586.372400000007</v>
       </c>
       <c r="D7" s="183">
         <v>1173.6276</v>
@@ -4901,16 +4884,10 @@
         <v>13</v>
       </c>
       <c r="L7" s="188">
-        <v>5301</v>
-      </c>
-      <c r="M7" s="192">
-        <f t="shared" si="9"/>
-        <v>4134.78</v>
-      </c>
-      <c r="N7" s="182">
-        <f t="shared" si="10"/>
-        <v>1166.22</v>
-      </c>
+        <v>5615</v>
+      </c>
+      <c r="M7" s="192"/>
+      <c r="N7" s="182"/>
       <c r="O7" s="150"/>
       <c r="P7" s="97"/>
       <c r="Q7" s="40">
@@ -4921,19 +4898,19 @@
       </c>
       <c r="S7" s="28">
         <f t="shared" si="0"/>
-        <v>22773.000000000007</v>
+        <v>22145.000000000007</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" si="1"/>
-        <v>5301</v>
+        <v>5615</v>
       </c>
       <c r="U7" s="32">
-        <f t="shared" si="11"/>
-        <v>855</v>
+        <f t="shared" si="9"/>
+        <v>831</v>
       </c>
       <c r="V7" s="32">
-        <f t="shared" si="12"/>
-        <v>251</v>
+        <f t="shared" si="10"/>
+        <v>265</v>
       </c>
       <c r="W7" s="11">
         <v>1863</v>
@@ -4974,11 +4951,11 @@
       </c>
       <c r="B8" s="188">
         <f t="shared" si="8"/>
-        <v>28353.000000000007</v>
+        <v>28064.000000000007</v>
       </c>
       <c r="C8" s="210">
         <f t="shared" si="3"/>
-        <v>27248.744400000007</v>
+        <v>26959.744400000007</v>
       </c>
       <c r="D8" s="183">
         <v>1104.2556</v>
@@ -5005,16 +4982,10 @@
         <v>24</v>
       </c>
       <c r="L8" s="188">
-        <v>5610</v>
-      </c>
-      <c r="M8" s="192">
-        <f t="shared" si="9"/>
-        <v>4375.8</v>
-      </c>
-      <c r="N8" s="182">
-        <f t="shared" si="10"/>
-        <v>1234.2</v>
-      </c>
+        <v>5899</v>
+      </c>
+      <c r="M8" s="192"/>
+      <c r="N8" s="182"/>
       <c r="O8" s="149">
         <v>0.91200000000000003</v>
       </c>
@@ -5027,19 +4998,19 @@
       </c>
       <c r="S8" s="28">
         <f t="shared" si="0"/>
-        <v>22743.000000000007</v>
+        <v>22165.000000000007</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>5610</v>
+        <v>5899</v>
       </c>
       <c r="U8" s="32">
-        <f t="shared" si="11"/>
-        <v>1109</v>
+        <f t="shared" si="9"/>
+        <v>1081</v>
       </c>
       <c r="V8" s="32">
-        <f t="shared" si="12"/>
-        <v>302</v>
+        <f t="shared" si="10"/>
+        <v>318</v>
       </c>
       <c r="W8" s="11">
         <v>2436</v>
@@ -5078,11 +5049,11 @@
       </c>
       <c r="B9" s="188">
         <f t="shared" si="8"/>
-        <v>28657.000000000007</v>
+        <v>28346.000000000007</v>
       </c>
       <c r="C9" s="210">
         <f t="shared" si="3"/>
-        <v>27511.205800000007</v>
+        <v>27200.205800000007</v>
       </c>
       <c r="D9" s="183">
         <v>1145.7942</v>
@@ -5109,16 +5080,10 @@
         <v>35</v>
       </c>
       <c r="L9" s="188">
-        <v>5894</v>
-      </c>
-      <c r="M9" s="192">
-        <f t="shared" si="9"/>
-        <v>4597.32</v>
-      </c>
-      <c r="N9" s="182">
-        <f t="shared" si="10"/>
-        <v>1296.68</v>
-      </c>
+        <v>6205</v>
+      </c>
+      <c r="M9" s="192"/>
+      <c r="N9" s="182"/>
       <c r="O9" s="149"/>
       <c r="P9" s="97"/>
       <c r="Q9" s="40">
@@ -5129,19 +5094,19 @@
       </c>
       <c r="S9" s="28">
         <f t="shared" si="0"/>
-        <v>22763.000000000007</v>
+        <v>22141.000000000007</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" si="1"/>
-        <v>5894</v>
+        <v>6205</v>
       </c>
       <c r="U9" s="32">
-        <f t="shared" si="11"/>
-        <v>1204</v>
+        <f t="shared" si="9"/>
+        <v>1171</v>
       </c>
       <c r="V9" s="32">
-        <f t="shared" si="12"/>
-        <v>369</v>
+        <f t="shared" si="10"/>
+        <v>389</v>
       </c>
       <c r="W9" s="11">
         <v>2978</v>
@@ -5170,7 +5135,7 @@
       <c r="AD9" s="14"/>
       <c r="AE9" s="198"/>
       <c r="AF9" s="198">
-        <f t="shared" ref="AF9:AF15" si="13">AF8+588</f>
+        <f t="shared" ref="AF9:AF15" si="11">AF8+588</f>
         <v>34551.000000000007</v>
       </c>
     </row>
@@ -5180,11 +5145,11 @@
       </c>
       <c r="B10" s="188">
         <f t="shared" si="8"/>
-        <v>28939.000000000007</v>
+        <v>28585.000000000007</v>
       </c>
       <c r="C10" s="210">
         <f t="shared" si="3"/>
-        <v>27635.934400000006</v>
+        <v>27281.934400000006</v>
       </c>
       <c r="D10" s="183">
         <v>1303.0656000000001</v>
@@ -5211,16 +5176,10 @@
         <v>10</v>
       </c>
       <c r="L10" s="188">
-        <v>6200</v>
-      </c>
-      <c r="M10" s="192">
-        <f t="shared" si="9"/>
-        <v>4836</v>
-      </c>
-      <c r="N10" s="182">
-        <f t="shared" si="10"/>
-        <v>1364</v>
-      </c>
+        <v>6554</v>
+      </c>
+      <c r="M10" s="192"/>
+      <c r="N10" s="182"/>
       <c r="O10" s="149">
         <v>0.88</v>
       </c>
@@ -5233,19 +5192,19 @@
       </c>
       <c r="S10" s="28">
         <f t="shared" si="0"/>
-        <v>22739.000000000007</v>
+        <v>22031.000000000007</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>6200</v>
+        <v>6554</v>
       </c>
       <c r="U10" s="32">
-        <f t="shared" si="11"/>
-        <v>1171</v>
+        <f t="shared" si="9"/>
+        <v>1135</v>
       </c>
       <c r="V10" s="32">
-        <f t="shared" si="12"/>
-        <v>330</v>
+        <f t="shared" si="10"/>
+        <v>349</v>
       </c>
       <c r="W10" s="11">
         <v>3269</v>
@@ -5274,7 +5233,7 @@
       <c r="AD10" s="14"/>
       <c r="AE10" s="198"/>
       <c r="AF10" s="198">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>35139.000000000007</v>
       </c>
     </row>
@@ -5284,11 +5243,11 @@
       </c>
       <c r="B11" s="188">
         <f t="shared" si="8"/>
-        <v>29178.000000000007</v>
+        <v>28863.000000000007</v>
       </c>
       <c r="C11" s="210">
         <f t="shared" si="3"/>
-        <v>27722.579200000007</v>
+        <v>27407.579200000007</v>
       </c>
       <c r="D11" s="183">
         <v>1455.4208000000001</v>
@@ -5315,16 +5274,10 @@
         <v>18</v>
       </c>
       <c r="L11" s="188">
-        <v>6549</v>
-      </c>
-      <c r="M11" s="192">
-        <f t="shared" si="9"/>
-        <v>5108.22</v>
-      </c>
-      <c r="N11" s="182">
-        <f t="shared" si="10"/>
-        <v>1440.78</v>
-      </c>
+        <v>6864</v>
+      </c>
+      <c r="M11" s="192"/>
+      <c r="N11" s="182"/>
       <c r="O11" s="149">
         <v>0.88</v>
       </c>
@@ -5337,19 +5290,19 @@
       </c>
       <c r="S11" s="28">
         <f t="shared" si="0"/>
-        <v>22629.000000000007</v>
+        <v>21999.000000000007</v>
       </c>
       <c r="T11" s="28">
         <f t="shared" si="1"/>
-        <v>6549</v>
+        <v>6864</v>
       </c>
       <c r="U11" s="32">
-        <f t="shared" si="11"/>
-        <v>1507</v>
+        <f t="shared" si="9"/>
+        <v>1465</v>
       </c>
       <c r="V11" s="32">
-        <f t="shared" si="12"/>
-        <v>440</v>
+        <f t="shared" si="10"/>
+        <v>461</v>
       </c>
       <c r="W11" s="11">
         <v>4865</v>
@@ -5378,7 +5331,7 @@
       <c r="AD11" s="14"/>
       <c r="AE11" s="198"/>
       <c r="AF11" s="198">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>35727.000000000007</v>
       </c>
     </row>
@@ -5388,11 +5341,11 @@
       </c>
       <c r="B12" s="188">
         <f>SUM(C12:D12)</f>
-        <v>29456.000000000007</v>
+        <v>29091.000000000007</v>
       </c>
       <c r="C12" s="210">
         <f t="shared" si="3"/>
-        <v>27809.524200000007</v>
+        <v>27444.524200000007</v>
       </c>
       <c r="D12" s="183">
         <v>1646.4758000000002</v>
@@ -5419,16 +5372,10 @@
         <v>32</v>
       </c>
       <c r="L12" s="188">
-        <v>6859</v>
-      </c>
-      <c r="M12" s="192">
-        <f t="shared" si="9"/>
-        <v>5350.02</v>
-      </c>
-      <c r="N12" s="182">
-        <f t="shared" si="10"/>
-        <v>1508.98</v>
-      </c>
+        <v>7224</v>
+      </c>
+      <c r="M12" s="192"/>
+      <c r="N12" s="182"/>
       <c r="O12" s="149">
         <v>0.89</v>
       </c>
@@ -5441,19 +5388,19 @@
       </c>
       <c r="S12" s="28">
         <f t="shared" si="0"/>
-        <v>22597.000000000007</v>
+        <v>21867.000000000007</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>6859</v>
+        <v>7224</v>
       </c>
       <c r="U12" s="32">
-        <f t="shared" si="11"/>
-        <v>1430</v>
+        <f t="shared" si="9"/>
+        <v>1384</v>
       </c>
       <c r="V12" s="32">
-        <f t="shared" si="12"/>
-        <v>475</v>
+        <f t="shared" si="10"/>
+        <v>500</v>
       </c>
       <c r="W12" s="11">
         <v>6265</v>
@@ -5486,7 +5433,7 @@
         <v>36315</v>
       </c>
       <c r="AF12" s="198">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>36315.000000000007</v>
       </c>
     </row>
@@ -5496,11 +5443,11 @@
       </c>
       <c r="B13" s="188">
         <f t="shared" si="8"/>
-        <v>29684.000000000011</v>
+        <v>29394.000000000011</v>
       </c>
       <c r="C13" s="210">
         <f t="shared" si="3"/>
-        <v>27801.781600000009</v>
+        <v>27511.781600000009</v>
       </c>
       <c r="D13" s="183">
         <v>1882.2184</v>
@@ -5527,16 +5474,10 @@
         <v>33</v>
       </c>
       <c r="L13" s="188">
-        <v>7219</v>
-      </c>
-      <c r="M13" s="192">
-        <f t="shared" si="9"/>
-        <v>5630.8200000000006</v>
-      </c>
-      <c r="N13" s="182">
-        <f t="shared" si="10"/>
-        <v>1588.18</v>
-      </c>
+        <v>7509</v>
+      </c>
+      <c r="M13" s="192"/>
+      <c r="N13" s="182"/>
       <c r="O13" s="150">
         <v>0.9</v>
       </c>
@@ -5550,16 +5491,16 @@
       </c>
       <c r="S13" s="28">
         <f t="shared" si="0"/>
-        <v>22465.000000000011</v>
+        <v>21885.000000000011</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>7219</v>
+        <v>7509</v>
       </c>
       <c r="U13" s="12"/>
       <c r="V13" s="32">
-        <f t="shared" si="12"/>
-        <v>337</v>
+        <f t="shared" si="10"/>
+        <v>351</v>
       </c>
       <c r="W13" s="11">
         <v>7289</v>
@@ -5597,11 +5538,11 @@
       </c>
       <c r="B14" s="188">
         <f t="shared" si="8"/>
-        <v>29987.000000000007</v>
+        <v>37491.000000000007</v>
       </c>
       <c r="C14" s="210">
         <f t="shared" si="3"/>
-        <v>27854.027200000008</v>
+        <v>35358.027200000004</v>
       </c>
       <c r="D14" s="183">
         <v>2132.9728</v>
@@ -5627,28 +5568,20 @@
       <c r="K14" s="185">
         <v>35</v>
       </c>
-      <c r="L14" s="188">
-        <v>7504</v>
-      </c>
-      <c r="M14" s="192">
-        <f t="shared" si="9"/>
-        <v>5853.12</v>
-      </c>
-      <c r="N14" s="182">
-        <f t="shared" si="10"/>
-        <v>1650.88</v>
-      </c>
+      <c r="L14" s="188"/>
+      <c r="M14" s="192"/>
+      <c r="N14" s="182"/>
       <c r="O14" s="149">
         <v>0.9</v>
       </c>
       <c r="P14" s="123"/>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
-        <v>7504</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="197"/>
       <c r="AF14" s="198">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>37491.000000000007</v>
       </c>
     </row>
@@ -5681,7 +5614,7 @@
       <c r="P15" s="123"/>
       <c r="AE15" s="198"/>
       <c r="AF15" s="198">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>38079.000000000007</v>
       </c>
     </row>
@@ -5990,8 +5923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29:T29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6832,8 +6765,8 @@
       <c r="A18" s="31">
         <v>2014</v>
       </c>
-      <c r="B18" s="190">
-        <v>0.32</v>
+      <c r="B18" s="228">
+        <v>0.32297447280799113</v>
       </c>
       <c r="C18" s="44"/>
       <c r="D18" s="189">
@@ -6887,8 +6820,8 @@
       <c r="A19" s="31">
         <v>2015</v>
       </c>
-      <c r="B19" s="190">
-        <v>0.35</v>
+      <c r="B19" s="228">
+        <v>0.35719557195571955</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="189">
@@ -6943,7 +6876,7 @@
         <v>2016</v>
       </c>
       <c r="B20" s="191">
-        <v>0.37</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="C20" s="44"/>
       <c r="D20" s="189">
@@ -6998,8 +6931,8 @@
       <c r="A21" s="31">
         <v>2017</v>
       </c>
-      <c r="B21" s="190">
-        <v>0.4</v>
+      <c r="B21" s="228">
+        <v>0.49761417859577367</v>
       </c>
       <c r="C21" s="44"/>
       <c r="D21" s="189">
@@ -7050,8 +6983,8 @@
       <c r="A22" s="31">
         <v>2018</v>
       </c>
-      <c r="B22" s="44">
-        <v>0.4</v>
+      <c r="B22" s="229">
+        <v>0.53368660105980315</v>
       </c>
       <c r="C22" s="44"/>
       <c r="D22" s="189">
@@ -7102,7 +7035,9 @@
       <c r="A23" s="31">
         <v>2019</v>
       </c>
-      <c r="B23" s="44"/>
+      <c r="B23" s="229">
+        <v>0.59571788413098237</v>
+      </c>
       <c r="C23" s="44"/>
       <c r="D23" s="189">
         <v>4525</v>

</xml_diff>

<commit_message>
Created columns for total diagnoses by time since infection
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom.tidhar\Documents\GitHub\STI-HIV-coinfection\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <sheet name="scen_2" sheetId="26" r:id="rId6"/>
     <sheet name="timepars_old" sheetId="20" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -26,7 +31,7 @@
     <author>Michael Traeger</author>
   </authors>
   <commentList>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,10 +55,10 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="1">
+    <comment ref="C8" authorId="1" shapeId="0">
       <text/>
     </comment>
-    <comment ref="C11" authorId="1">
+    <comment ref="C11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0">
+    <comment ref="C18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +219,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -241,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1">
+    <comment ref="C1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1">
+    <comment ref="D1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -299,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="2">
+    <comment ref="N1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1">
+    <comment ref="O1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="2">
+    <comment ref="Q1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -398,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="2">
+    <comment ref="S1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="2">
+    <comment ref="U1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="2">
+    <comment ref="V1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="2">
+    <comment ref="W1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="2">
+    <comment ref="Y1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -524,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="2">
+    <comment ref="Z1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -549,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="2">
+    <comment ref="AA1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -575,7 +580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="2">
+    <comment ref="AB1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -604,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="2">
+    <comment ref="AC1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -630,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="2">
+    <comment ref="AD1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -654,7 +659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="2">
+    <comment ref="AE1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -678,7 +683,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE2" authorId="1">
+    <comment ref="AG2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -702,7 +707,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="2">
+    <comment ref="Q8" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -726,7 +731,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="2">
+    <comment ref="Q9" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -750,7 +755,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O12" authorId="0">
+    <comment ref="Q12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -778,7 +783,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD12" authorId="0">
+    <comment ref="AF12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -802,7 +807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="2">
+    <comment ref="T13" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -826,7 +831,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="2">
+    <comment ref="A14" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -862,7 +867,7 @@
     <author>Kathleen Ryan</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -886,7 +891,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -910,7 +915,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -934,7 +939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -961,7 +966,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -985,7 +990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1009,7 +1014,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1033,7 +1038,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1057,7 +1062,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1">
+    <comment ref="X1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1081,7 +1086,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1105,7 +1110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1129,7 +1134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1153,7 +1158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1177,7 +1182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="1">
+    <comment ref="B3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1202,7 +1207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1226,7 +1231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0">
+    <comment ref="T3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1250,7 +1255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="1">
+    <comment ref="D18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1285,7 +1290,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1319,7 +1324,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1377,7 +1382,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1401,7 +1406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1425,7 +1430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1449,7 +1454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1473,7 +1478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1497,7 +1502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1521,7 +1526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1545,7 +1550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1569,7 +1574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1593,7 +1598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AF1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1617,7 +1622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AG1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1641,7 +1646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1665,7 +1670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1689,7 +1694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1713,7 +1718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1737,7 +1742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="0">
+    <comment ref="T4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1761,7 +1766,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W4" authorId="0">
+    <comment ref="W4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1790,7 +1795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="135">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2190,12 +2195,18 @@
   </si>
   <si>
     <t>years each person is in model</t>
+  </si>
+  <si>
+    <t>HIV_diag_new_tot</t>
+  </si>
+  <si>
+    <t>HIV_diag_old_tot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -3108,7 +3119,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3482,11 +3493,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -4301,11 +4315,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF25"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M19" sqref="M19"/>
+      <selection pane="topRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4316,32 +4330,34 @@
     <col min="5" max="5" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="43" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11" style="43" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="43" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="62.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11" style="43" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="43" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="118" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="118" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="109" t="s">
         <v>21</v>
       </c>
@@ -4363,81 +4379,87 @@
       <c r="G1" s="112" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="116" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="116" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="K1" s="114" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="111" t="s">
+      <c r="L1" s="111" t="s">
         <v>122</v>
       </c>
-      <c r="K1" s="112" t="s">
+      <c r="M1" s="112" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="110" t="s">
+      <c r="N1" s="110" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="111" t="s">
+      <c r="O1" s="111" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="112" t="s">
+      <c r="P1" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="148" t="s">
+      <c r="Q1" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="116" t="s">
+      <c r="R1" s="115"/>
+      <c r="S1" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="116" t="s">
+      <c r="T1" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="116" t="s">
+      <c r="U1" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="116" t="s">
+      <c r="V1" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="116" t="s">
+      <c r="W1" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="116" t="s">
+      <c r="X1" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="W1" s="116" t="s">
+      <c r="Y1" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="116" t="s">
+      <c r="Z1" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="116" t="s">
+      <c r="AA1" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="116" t="s">
+      <c r="AB1" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="116" t="s">
+      <c r="AC1" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="116" t="s">
+      <c r="AD1" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="116" t="s">
+      <c r="AE1" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="117" t="s">
+      <c r="AF1" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="196" t="s">
+      <c r="AG1" s="196" t="s">
         <v>115</v>
       </c>
-      <c r="AF1" s="196" t="s">
+      <c r="AH1" s="196" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="199">
         <v>2006</v>
       </c>
@@ -4453,27 +4475,33 @@
       <c r="G2" s="223">
         <v>13</v>
       </c>
-      <c r="H2" s="203">
+      <c r="H2" s="230">
+        <f>J2+L2</f>
+        <v>87</v>
+      </c>
+      <c r="I2" s="230">
+        <f>K2+M2</f>
+        <v>112</v>
+      </c>
+      <c r="J2" s="203">
         <v>81</v>
       </c>
-      <c r="I2" s="204">
+      <c r="K2" s="204">
         <v>105</v>
       </c>
-      <c r="J2" s="201">
+      <c r="L2" s="201">
         <v>6</v>
       </c>
-      <c r="K2" s="202">
+      <c r="M2" s="202">
         <v>7</v>
       </c>
-      <c r="L2" s="200">
+      <c r="N2" s="200">
         <v>4216</v>
       </c>
-      <c r="M2" s="201"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="205"/>
-      <c r="P2" s="206"/>
-      <c r="Q2" s="207"/>
-      <c r="R2" s="207"/>
+      <c r="O2" s="201"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="205"/>
+      <c r="R2" s="206"/>
       <c r="S2" s="207"/>
       <c r="T2" s="207"/>
       <c r="U2" s="207"/>
@@ -4485,15 +4513,17 @@
       <c r="AA2" s="207"/>
       <c r="AB2" s="207"/>
       <c r="AC2" s="207"/>
-      <c r="AD2" s="208"/>
-      <c r="AE2" s="192">
+      <c r="AD2" s="207"/>
+      <c r="AE2" s="207"/>
+      <c r="AF2" s="208"/>
+      <c r="AG2" s="192">
         <v>30713</v>
       </c>
-      <c r="AF2" s="192">
+      <c r="AH2" s="192">
         <v>30713</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2007</v>
       </c>
@@ -4509,81 +4539,89 @@
       <c r="G3" s="224">
         <v>17</v>
       </c>
-      <c r="H3" s="103">
+      <c r="H3" s="230">
+        <f t="shared" ref="H3:H15" si="0">J3+L3</f>
+        <v>76</v>
+      </c>
+      <c r="I3" s="230">
+        <f t="shared" ref="I3:I15" si="1">K3+M3</f>
+        <v>108</v>
+      </c>
+      <c r="J3" s="103">
         <v>69</v>
       </c>
-      <c r="I3" s="104">
+      <c r="K3" s="104">
         <v>98</v>
       </c>
-      <c r="J3" s="211">
+      <c r="L3" s="211">
         <v>7</v>
       </c>
-      <c r="K3" s="105">
+      <c r="M3" s="105">
         <v>10</v>
       </c>
-      <c r="L3" s="106">
+      <c r="N3" s="106">
         <v>4491</v>
       </c>
-      <c r="M3" s="107"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="149">
+      <c r="O3" s="107"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="149">
         <v>0.7</v>
       </c>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="40">
+      <c r="R3" s="96"/>
+      <c r="S3" s="40">
         <v>2.32876712328767E-2</v>
       </c>
-      <c r="R3" s="40">
+      <c r="T3" s="40">
         <v>3.4931506849315071E-2</v>
       </c>
-      <c r="S3" s="28">
-        <f t="shared" ref="S3:S13" si="0">B3-T3</f>
+      <c r="U3" s="28">
+        <f>B3-V3</f>
         <v>-4491</v>
       </c>
-      <c r="T3" s="28">
-        <f t="shared" ref="T3:T14" si="1">L3</f>
+      <c r="V3" s="28">
+        <f t="shared" ref="V3:V14" si="2">N3</f>
         <v>4491</v>
       </c>
-      <c r="U3" s="33">
-        <f>ROUND(Q3*S3,0)</f>
+      <c r="W3" s="33">
+        <f>ROUND(S3*U3,0)</f>
         <v>-105</v>
       </c>
-      <c r="V3" s="33">
-        <f t="shared" ref="V3" si="2">ROUND(R3*T3,0)</f>
+      <c r="X3" s="33">
+        <f t="shared" ref="X3" si="3">ROUND(T3*V3,0)</f>
         <v>157</v>
       </c>
-      <c r="W3" s="11">
+      <c r="Y3" s="11">
         <v>1007</v>
       </c>
-      <c r="X3" s="37">
+      <c r="Z3" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y3" s="37">
+      <c r="AA3" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z3" s="38">
-        <f>W3*X3*Y3</f>
+      <c r="AB3" s="38">
+        <f>Y3*Z3*AA3</f>
         <v>668.84940000000006</v>
       </c>
-      <c r="AA3" s="34">
+      <c r="AC3" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB3" s="36">
-        <f>Z3-AC3</f>
+      <c r="AD3" s="36">
+        <f>AB3-AE3</f>
         <v>555.14500200000009</v>
       </c>
-      <c r="AC3" s="36">
-        <f>Z3*AA3</f>
+      <c r="AE3" s="36">
+        <f>AB3*AC3</f>
         <v>113.70439800000001</v>
       </c>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="198"/>
-      <c r="AF3" s="209">
-        <f>AF2+532.4</f>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="198"/>
+      <c r="AH3" s="209">
+        <f>AH2+532.4</f>
         <v>31245.4</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2008</v>
       </c>
@@ -4592,7 +4630,7 @@
         <v>27007.800000000003</v>
       </c>
       <c r="C4" s="210">
-        <f t="shared" ref="C4:C15" si="3">AF4-(D4+L4)</f>
+        <f>AH4-(D4+N4)</f>
         <v>27007.800000000003</v>
       </c>
       <c r="D4" s="182"/>
@@ -4605,69 +4643,77 @@
       <c r="G4" s="224">
         <v>16</v>
       </c>
-      <c r="H4" s="103">
+      <c r="H4" s="230">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="I4" s="230">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="J4" s="103">
         <v>71</v>
       </c>
-      <c r="I4" s="104">
+      <c r="K4" s="104">
         <v>94</v>
       </c>
-      <c r="J4" s="211">
+      <c r="L4" s="211">
         <v>8</v>
       </c>
-      <c r="K4" s="105">
+      <c r="M4" s="105">
         <v>8</v>
       </c>
-      <c r="L4" s="188">
+      <c r="N4" s="188">
         <v>4770</v>
       </c>
-      <c r="M4" s="192"/>
-      <c r="N4" s="182"/>
-      <c r="O4" s="150"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="28">
-        <f t="shared" si="0"/>
+      <c r="O4" s="192"/>
+      <c r="P4" s="182"/>
+      <c r="Q4" s="150"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="28">
+        <f>B4-V4</f>
         <v>22237.800000000003</v>
       </c>
-      <c r="T4" s="28">
-        <f t="shared" si="1"/>
+      <c r="V4" s="28">
+        <f t="shared" si="2"/>
         <v>4770</v>
       </c>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="11">
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="11">
         <v>922</v>
       </c>
-      <c r="X4" s="37">
+      <c r="Z4" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y4" s="37">
+      <c r="AA4" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z4" s="38">
-        <f t="shared" ref="Z4:Z13" si="4">W4*X4*Y4</f>
+      <c r="AB4" s="38">
+        <f t="shared" ref="AB4:AB13" si="4">Y4*Z4*AA4</f>
         <v>612.39239999999995</v>
       </c>
-      <c r="AA4" s="34">
+      <c r="AC4" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB4" s="36">
-        <f t="shared" ref="AB4:AB13" si="5">Z4-AC4</f>
+      <c r="AD4" s="36">
+        <f t="shared" ref="AD4:AD13" si="5">AB4-AE4</f>
         <v>508.28569199999993</v>
       </c>
-      <c r="AC4" s="36">
-        <f t="shared" ref="AC4:AC13" si="6">Z4*AA4</f>
+      <c r="AE4" s="36">
+        <f t="shared" ref="AE4:AE13" si="6">AB4*AC4</f>
         <v>104.106708</v>
       </c>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="198"/>
-      <c r="AF4" s="209">
-        <f t="shared" ref="AF4:AF7" si="7">AF3+532.4</f>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="198"/>
+      <c r="AH4" s="209">
+        <f t="shared" ref="AH4:AH7" si="7">AH3+532.4</f>
         <v>31777.800000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>2009</v>
       </c>
@@ -4676,7 +4722,7 @@
         <v>27251.200000000004</v>
       </c>
       <c r="C5" s="210">
-        <f t="shared" si="3"/>
+        <f>AH5-(D5+N5)</f>
         <v>27251.200000000004</v>
       </c>
       <c r="D5" s="182"/>
@@ -4689,69 +4735,77 @@
       <c r="G5" s="224">
         <v>14</v>
       </c>
-      <c r="H5" s="103">
+      <c r="H5" s="230">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="I5" s="230">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="J5" s="103">
         <v>85</v>
       </c>
-      <c r="I5" s="104">
+      <c r="K5" s="104">
         <v>98</v>
       </c>
-      <c r="J5" s="211">
+      <c r="L5" s="211">
         <v>7</v>
       </c>
-      <c r="K5" s="105">
+      <c r="M5" s="105">
         <v>7</v>
       </c>
-      <c r="L5" s="188">
+      <c r="N5" s="188">
         <v>5059</v>
       </c>
-      <c r="M5" s="192"/>
-      <c r="N5" s="182"/>
-      <c r="O5" s="150"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="28">
-        <f t="shared" si="0"/>
+      <c r="O5" s="192"/>
+      <c r="P5" s="182"/>
+      <c r="Q5" s="150"/>
+      <c r="R5" s="97"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="28">
+        <f>B5-V5</f>
         <v>22192.200000000004</v>
       </c>
-      <c r="T5" s="28">
-        <f t="shared" si="1"/>
+      <c r="V5" s="28">
+        <f t="shared" si="2"/>
         <v>5059</v>
       </c>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="11">
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="11">
         <v>1480</v>
       </c>
-      <c r="X5" s="37">
+      <c r="Z5" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y5" s="37">
+      <c r="AA5" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z5" s="38">
+      <c r="AB5" s="38">
         <f t="shared" si="4"/>
         <v>983.01600000000008</v>
       </c>
-      <c r="AA5" s="34">
+      <c r="AC5" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB5" s="36">
+      <c r="AD5" s="36">
         <f t="shared" si="5"/>
         <v>815.90328</v>
       </c>
-      <c r="AC5" s="36">
+      <c r="AE5" s="36">
         <f t="shared" si="6"/>
         <v>167.11272000000002</v>
       </c>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="198"/>
-      <c r="AF5" s="209">
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="198"/>
+      <c r="AH5" s="209">
         <f t="shared" si="7"/>
         <v>32310.200000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>2010</v>
       </c>
@@ -4760,7 +4814,7 @@
         <v>27536.600000000006</v>
       </c>
       <c r="C6" s="210">
-        <f t="shared" si="3"/>
+        <f>AH6-(D6+N6)</f>
         <v>26220.496600000006</v>
       </c>
       <c r="D6" s="183">
@@ -4775,79 +4829,87 @@
       <c r="G6" s="224">
         <v>21</v>
       </c>
-      <c r="H6" s="103">
+      <c r="H6" s="230">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="I6" s="230">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="J6" s="103">
         <v>85</v>
       </c>
-      <c r="I6" s="104">
+      <c r="K6" s="104">
         <v>68</v>
       </c>
-      <c r="J6" s="211">
+      <c r="L6" s="211">
         <v>7</v>
       </c>
-      <c r="K6" s="105">
+      <c r="M6" s="105">
         <v>14</v>
       </c>
-      <c r="L6" s="188">
+      <c r="N6" s="188">
         <v>5306</v>
       </c>
-      <c r="M6" s="192"/>
-      <c r="N6" s="182"/>
-      <c r="O6" s="149"/>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="40">
+      <c r="O6" s="192"/>
+      <c r="P6" s="182"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="97"/>
+      <c r="S6" s="40">
         <v>4.0273972602739724E-2</v>
       </c>
-      <c r="R6" s="40">
+      <c r="T6" s="40">
         <v>4.3150684931506846E-2</v>
       </c>
-      <c r="S6" s="28">
-        <f t="shared" si="0"/>
+      <c r="U6" s="28">
+        <f>B6-V6</f>
         <v>22230.600000000006</v>
       </c>
-      <c r="T6" s="28">
-        <f t="shared" si="1"/>
+      <c r="V6" s="28">
+        <f t="shared" si="2"/>
         <v>5306</v>
       </c>
-      <c r="U6" s="32">
-        <f t="shared" ref="U6:U12" si="9">ROUND(Q6*S6,0)</f>
+      <c r="W6" s="32">
+        <f t="shared" ref="W6:W12" si="9">ROUND(S6*U6,0)</f>
         <v>895</v>
       </c>
-      <c r="V6" s="32">
-        <f t="shared" ref="V6:V13" si="10">ROUND(R6*T6,0)</f>
+      <c r="X6" s="32">
+        <f t="shared" ref="X6:X13" si="10">ROUND(T6*V6,0)</f>
         <v>229</v>
       </c>
-      <c r="W6" s="11">
+      <c r="Y6" s="11">
         <v>1758</v>
       </c>
-      <c r="X6" s="37">
+      <c r="Z6" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y6" s="37">
+      <c r="AA6" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z6" s="38">
+      <c r="AB6" s="38">
         <f t="shared" si="4"/>
         <v>1167.6635999999999</v>
       </c>
-      <c r="AA6" s="34">
+      <c r="AC6" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB6" s="36">
+      <c r="AD6" s="36">
         <f t="shared" si="5"/>
         <v>969.16078799999991</v>
       </c>
-      <c r="AC6" s="36">
+      <c r="AE6" s="36">
         <f t="shared" si="6"/>
         <v>198.50281199999998</v>
       </c>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="198"/>
-      <c r="AF6" s="209">
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="198"/>
+      <c r="AH6" s="209">
         <f t="shared" si="7"/>
         <v>32842.600000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2011</v>
       </c>
@@ -4856,7 +4918,7 @@
         <v>27760.000000000007</v>
       </c>
       <c r="C7" s="210">
-        <f t="shared" si="3"/>
+        <f>AH7-(D7+N7)</f>
         <v>26586.372400000007</v>
       </c>
       <c r="D7" s="183">
@@ -4871,81 +4933,89 @@
       <c r="G7" s="224">
         <v>20</v>
       </c>
-      <c r="H7" s="119">
+      <c r="H7" s="230">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="I7" s="230">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="J7" s="119">
         <v>99</v>
       </c>
-      <c r="I7" s="121">
+      <c r="K7" s="121">
         <v>91</v>
       </c>
-      <c r="J7" s="212">
+      <c r="L7" s="212">
         <v>7</v>
       </c>
-      <c r="K7" s="213">
+      <c r="M7" s="213">
         <v>13</v>
       </c>
-      <c r="L7" s="188">
+      <c r="N7" s="188">
         <v>5615</v>
       </c>
-      <c r="M7" s="192"/>
-      <c r="N7" s="182"/>
-      <c r="O7" s="150"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="40">
+      <c r="O7" s="192"/>
+      <c r="P7" s="182"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="40">
         <v>3.7534246575342468E-2</v>
       </c>
-      <c r="R7" s="40">
+      <c r="T7" s="40">
         <v>4.726027397260274E-2</v>
       </c>
-      <c r="S7" s="28">
-        <f t="shared" si="0"/>
+      <c r="U7" s="28">
+        <f>B7-V7</f>
         <v>22145.000000000007</v>
       </c>
-      <c r="T7" s="28">
-        <f t="shared" si="1"/>
+      <c r="V7" s="28">
+        <f t="shared" si="2"/>
         <v>5615</v>
       </c>
-      <c r="U7" s="32">
+      <c r="W7" s="32">
         <f t="shared" si="9"/>
         <v>831</v>
       </c>
-      <c r="V7" s="32">
+      <c r="X7" s="32">
         <f t="shared" si="10"/>
         <v>265</v>
       </c>
-      <c r="W7" s="11">
+      <c r="Y7" s="11">
         <v>1863</v>
       </c>
-      <c r="X7" s="37">
+      <c r="Z7" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y7" s="37">
+      <c r="AA7" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z7" s="38">
+      <c r="AB7" s="38">
         <f t="shared" si="4"/>
         <v>1237.4046000000001</v>
       </c>
-      <c r="AA7" s="34">
+      <c r="AC7" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB7" s="36">
+      <c r="AD7" s="36">
         <f t="shared" si="5"/>
         <v>1027.0458180000001</v>
       </c>
-      <c r="AC7" s="36">
+      <c r="AE7" s="36">
         <f t="shared" si="6"/>
         <v>210.35878200000002</v>
       </c>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="192">
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="192">
         <v>33375</v>
       </c>
-      <c r="AF7" s="209">
+      <c r="AH7" s="209">
         <f t="shared" si="7"/>
         <v>33375.000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>2012</v>
       </c>
@@ -4954,7 +5024,7 @@
         <v>28064.000000000007</v>
       </c>
       <c r="C8" s="210">
-        <f t="shared" si="3"/>
+        <f>AH8-(D8+N8)</f>
         <v>26959.744400000007</v>
       </c>
       <c r="D8" s="183">
@@ -4969,81 +5039,89 @@
       <c r="G8" s="186">
         <v>34</v>
       </c>
-      <c r="H8" s="185">
+      <c r="H8" s="230">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="I8" s="230">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="J8" s="185">
         <v>101</v>
       </c>
-      <c r="I8" s="184">
+      <c r="K8" s="184">
         <v>71</v>
       </c>
-      <c r="J8" s="186">
+      <c r="L8" s="186">
         <v>10</v>
       </c>
-      <c r="K8" s="222">
+      <c r="M8" s="222">
         <v>24</v>
       </c>
-      <c r="L8" s="188">
+      <c r="N8" s="188">
         <v>5899</v>
       </c>
-      <c r="M8" s="192"/>
-      <c r="N8" s="182"/>
-      <c r="O8" s="149">
+      <c r="O8" s="192"/>
+      <c r="P8" s="182"/>
+      <c r="Q8" s="149">
         <v>0.91200000000000003</v>
       </c>
-      <c r="P8" s="97"/>
-      <c r="Q8" s="40">
+      <c r="R8" s="97"/>
+      <c r="S8" s="40">
         <v>4.876712328767123E-2</v>
       </c>
-      <c r="R8" s="40">
+      <c r="T8" s="40">
         <v>5.3835616438356167E-2</v>
       </c>
-      <c r="S8" s="28">
-        <f t="shared" si="0"/>
+      <c r="U8" s="28">
+        <f>B8-V8</f>
         <v>22165.000000000007</v>
       </c>
-      <c r="T8" s="28">
-        <f t="shared" si="1"/>
+      <c r="V8" s="28">
+        <f t="shared" si="2"/>
         <v>5899</v>
       </c>
-      <c r="U8" s="32">
+      <c r="W8" s="32">
         <f t="shared" si="9"/>
         <v>1081</v>
       </c>
-      <c r="V8" s="32">
+      <c r="X8" s="32">
         <f t="shared" si="10"/>
         <v>318</v>
       </c>
-      <c r="W8" s="11">
+      <c r="Y8" s="11">
         <v>2436</v>
       </c>
-      <c r="X8" s="37">
+      <c r="Z8" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y8" s="37">
+      <c r="AA8" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z8" s="38">
+      <c r="AB8" s="38">
         <f t="shared" si="4"/>
         <v>1617.9911999999999</v>
       </c>
-      <c r="AA8" s="34">
+      <c r="AC8" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB8" s="36">
+      <c r="AD8" s="36">
         <f t="shared" si="5"/>
         <v>1342.9326959999999</v>
       </c>
-      <c r="AC8" s="36">
+      <c r="AE8" s="36">
         <f t="shared" si="6"/>
         <v>275.05850400000003</v>
       </c>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="198"/>
-      <c r="AF8" s="198">
-        <f>AF7+588</f>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="198"/>
+      <c r="AH8" s="198">
+        <f>AH7+588</f>
         <v>33963.000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2013</v>
       </c>
@@ -5052,7 +5130,7 @@
         <v>28346.000000000007</v>
       </c>
       <c r="C9" s="210">
-        <f t="shared" si="3"/>
+        <f>AH9-(D9+N9)</f>
         <v>27200.205800000007</v>
       </c>
       <c r="D9" s="183">
@@ -5067,79 +5145,87 @@
       <c r="G9" s="186">
         <v>49</v>
       </c>
-      <c r="H9" s="185">
+      <c r="H9" s="230">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="I9" s="230">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="J9" s="185">
         <v>106</v>
       </c>
-      <c r="I9" s="184">
+      <c r="K9" s="184">
         <v>78</v>
       </c>
-      <c r="J9" s="186">
+      <c r="L9" s="186">
         <v>14</v>
       </c>
-      <c r="K9" s="222">
+      <c r="M9" s="222">
         <v>35</v>
       </c>
-      <c r="L9" s="188">
+      <c r="N9" s="188">
         <v>6205</v>
       </c>
-      <c r="M9" s="192"/>
-      <c r="N9" s="182"/>
-      <c r="O9" s="149"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="40">
+      <c r="O9" s="192"/>
+      <c r="P9" s="182"/>
+      <c r="Q9" s="149"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="40">
         <v>5.2876712328767124E-2</v>
       </c>
-      <c r="R9" s="40">
+      <c r="T9" s="40">
         <v>6.2671232876712321E-2</v>
       </c>
-      <c r="S9" s="28">
-        <f t="shared" si="0"/>
+      <c r="U9" s="28">
+        <f>B9-V9</f>
         <v>22141.000000000007</v>
       </c>
-      <c r="T9" s="28">
-        <f t="shared" si="1"/>
+      <c r="V9" s="28">
+        <f t="shared" si="2"/>
         <v>6205</v>
       </c>
-      <c r="U9" s="32">
+      <c r="W9" s="32">
         <f t="shared" si="9"/>
         <v>1171</v>
       </c>
-      <c r="V9" s="32">
+      <c r="X9" s="32">
         <f t="shared" si="10"/>
         <v>389</v>
       </c>
-      <c r="W9" s="11">
+      <c r="Y9" s="11">
         <v>2978</v>
       </c>
-      <c r="X9" s="37">
+      <c r="Z9" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y9" s="37">
+      <c r="AA9" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z9" s="38">
+      <c r="AB9" s="38">
         <f t="shared" si="4"/>
         <v>1977.9876000000002</v>
       </c>
-      <c r="AA9" s="34">
+      <c r="AC9" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB9" s="36">
+      <c r="AD9" s="36">
         <f t="shared" si="5"/>
         <v>1641.7297080000001</v>
       </c>
-      <c r="AC9" s="36">
+      <c r="AE9" s="36">
         <f t="shared" si="6"/>
         <v>336.25789200000003</v>
       </c>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="198"/>
-      <c r="AF9" s="198">
-        <f t="shared" ref="AF9:AF15" si="11">AF8+588</f>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="198"/>
+      <c r="AH9" s="198">
+        <f t="shared" ref="AH9:AH15" si="11">AH8+588</f>
         <v>34551.000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2014</v>
       </c>
@@ -5148,7 +5234,7 @@
         <v>28585.000000000007</v>
       </c>
       <c r="C10" s="210">
-        <f t="shared" si="3"/>
+        <f>AH10-(D10+N10)</f>
         <v>27281.934400000006</v>
       </c>
       <c r="D10" s="183">
@@ -5163,81 +5249,89 @@
       <c r="G10" s="186">
         <v>35</v>
       </c>
-      <c r="H10" s="185">
+      <c r="H10" s="230">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="I10" s="230">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="J10" s="185">
         <v>133</v>
       </c>
-      <c r="I10" s="184">
+      <c r="K10" s="184">
         <v>67</v>
       </c>
-      <c r="J10" s="186">
+      <c r="L10" s="186">
         <v>25</v>
       </c>
-      <c r="K10" s="222">
+      <c r="M10" s="222">
         <v>10</v>
       </c>
-      <c r="L10" s="188">
+      <c r="N10" s="188">
         <v>6554</v>
       </c>
-      <c r="M10" s="192"/>
-      <c r="N10" s="182"/>
-      <c r="O10" s="149">
+      <c r="O10" s="192"/>
+      <c r="P10" s="182"/>
+      <c r="Q10" s="149">
         <v>0.88</v>
       </c>
-      <c r="P10" s="97"/>
-      <c r="Q10" s="40">
+      <c r="R10" s="97"/>
+      <c r="S10" s="40">
         <v>5.1506849315068493E-2</v>
       </c>
-      <c r="R10" s="40">
+      <c r="T10" s="40">
         <v>5.321917808219178E-2</v>
       </c>
-      <c r="S10" s="28">
-        <f t="shared" si="0"/>
+      <c r="U10" s="28">
+        <f>B10-V10</f>
         <v>22031.000000000007</v>
       </c>
-      <c r="T10" s="28">
-        <f t="shared" si="1"/>
+      <c r="V10" s="28">
+        <f t="shared" si="2"/>
         <v>6554</v>
       </c>
-      <c r="U10" s="32">
+      <c r="W10" s="32">
         <f t="shared" si="9"/>
         <v>1135</v>
       </c>
-      <c r="V10" s="32">
+      <c r="X10" s="32">
         <f t="shared" si="10"/>
         <v>349</v>
       </c>
-      <c r="W10" s="11">
+      <c r="Y10" s="11">
         <v>3269</v>
       </c>
-      <c r="X10" s="37">
+      <c r="Z10" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y10" s="37">
+      <c r="AA10" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z10" s="38">
+      <c r="AB10" s="38">
         <f t="shared" si="4"/>
         <v>2171.2698</v>
       </c>
-      <c r="AA10" s="34">
+      <c r="AC10" s="34">
         <v>0.17</v>
       </c>
-      <c r="AB10" s="36">
+      <c r="AD10" s="36">
         <f t="shared" si="5"/>
         <v>1802.1539339999999</v>
       </c>
-      <c r="AC10" s="36">
+      <c r="AE10" s="36">
         <f t="shared" si="6"/>
         <v>369.11586600000004</v>
       </c>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="198"/>
-      <c r="AF10" s="198">
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="198"/>
+      <c r="AH10" s="198">
         <f t="shared" si="11"/>
         <v>35139.000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>2015</v>
       </c>
@@ -5246,7 +5340,7 @@
         <v>28863.000000000007</v>
       </c>
       <c r="C11" s="210">
-        <f t="shared" si="3"/>
+        <f>AH11-(D11+N11)</f>
         <v>27407.579200000007</v>
       </c>
       <c r="D11" s="183">
@@ -5261,81 +5355,89 @@
       <c r="G11" s="186">
         <v>41</v>
       </c>
-      <c r="H11" s="185">
+      <c r="H11" s="230">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="I11" s="230">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="J11" s="185">
         <v>115</v>
       </c>
-      <c r="I11" s="184">
+      <c r="K11" s="184">
         <v>62</v>
       </c>
-      <c r="J11" s="186">
+      <c r="L11" s="186">
         <v>23</v>
       </c>
-      <c r="K11" s="222">
+      <c r="M11" s="222">
         <v>18</v>
       </c>
-      <c r="L11" s="188">
+      <c r="N11" s="188">
         <v>6864</v>
       </c>
-      <c r="M11" s="192"/>
-      <c r="N11" s="182"/>
-      <c r="O11" s="149">
+      <c r="O11" s="192"/>
+      <c r="P11" s="182"/>
+      <c r="Q11" s="149">
         <v>0.88</v>
       </c>
-      <c r="P11" s="97"/>
-      <c r="Q11" s="40">
+      <c r="R11" s="97"/>
+      <c r="S11" s="40">
         <v>6.6575342465753418E-2</v>
       </c>
-      <c r="R11" s="40">
+      <c r="T11" s="40">
         <v>6.7191780821917804E-2</v>
       </c>
-      <c r="S11" s="28">
-        <f t="shared" si="0"/>
+      <c r="U11" s="28">
+        <f>B11-V11</f>
         <v>21999.000000000007</v>
       </c>
-      <c r="T11" s="28">
-        <f t="shared" si="1"/>
+      <c r="V11" s="28">
+        <f t="shared" si="2"/>
         <v>6864</v>
       </c>
-      <c r="U11" s="32">
+      <c r="W11" s="32">
         <f t="shared" si="9"/>
         <v>1465</v>
       </c>
-      <c r="V11" s="32">
+      <c r="X11" s="32">
         <f t="shared" si="10"/>
         <v>461</v>
       </c>
-      <c r="W11" s="11">
+      <c r="Y11" s="11">
         <v>4865</v>
       </c>
-      <c r="X11" s="37">
+      <c r="Z11" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y11" s="37">
+      <c r="AA11" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z11" s="38">
+      <c r="AB11" s="38">
         <f t="shared" si="4"/>
         <v>3231.3330000000001</v>
       </c>
-      <c r="AA11" s="35">
+      <c r="AC11" s="35">
         <v>0.17</v>
       </c>
-      <c r="AB11" s="36">
+      <c r="AD11" s="36">
         <f t="shared" si="5"/>
         <v>2682.00639</v>
       </c>
-      <c r="AC11" s="36">
+      <c r="AE11" s="36">
         <f t="shared" si="6"/>
         <v>549.32661000000007</v>
       </c>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="198"/>
-      <c r="AF11" s="198">
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="198"/>
+      <c r="AH11" s="198">
         <f t="shared" si="11"/>
         <v>35727.000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>2016</v>
       </c>
@@ -5344,7 +5446,7 @@
         <v>29091.000000000007</v>
       </c>
       <c r="C12" s="210">
-        <f t="shared" si="3"/>
+        <f>AH12-(D12+N12)</f>
         <v>27444.524200000007</v>
       </c>
       <c r="D12" s="183">
@@ -5359,85 +5461,93 @@
       <c r="G12" s="186">
         <v>64</v>
       </c>
-      <c r="H12" s="185">
+      <c r="H12" s="230">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="I12" s="230">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="J12" s="185">
         <v>102</v>
       </c>
-      <c r="I12" s="184">
+      <c r="K12" s="184">
         <v>78</v>
       </c>
-      <c r="J12" s="186">
+      <c r="L12" s="186">
         <v>32</v>
       </c>
-      <c r="K12" s="222">
+      <c r="M12" s="222">
         <v>32</v>
       </c>
-      <c r="L12" s="188">
+      <c r="N12" s="188">
         <v>7224</v>
       </c>
-      <c r="M12" s="192"/>
-      <c r="N12" s="182"/>
-      <c r="O12" s="149">
+      <c r="O12" s="192"/>
+      <c r="P12" s="182"/>
+      <c r="Q12" s="149">
         <v>0.89</v>
       </c>
-      <c r="P12" s="97"/>
-      <c r="Q12" s="40">
+      <c r="R12" s="97"/>
+      <c r="S12" s="40">
         <v>6.3287671232876708E-2</v>
       </c>
-      <c r="R12" s="40">
+      <c r="T12" s="40">
         <v>6.9246575342465755E-2</v>
       </c>
-      <c r="S12" s="28">
-        <f t="shared" si="0"/>
+      <c r="U12" s="28">
+        <f>B12-V12</f>
         <v>21867.000000000007</v>
       </c>
-      <c r="T12" s="28">
-        <f t="shared" si="1"/>
+      <c r="V12" s="28">
+        <f t="shared" si="2"/>
         <v>7224</v>
       </c>
-      <c r="U12" s="32">
+      <c r="W12" s="32">
         <f t="shared" si="9"/>
         <v>1384</v>
       </c>
-      <c r="V12" s="32">
+      <c r="X12" s="32">
         <f t="shared" si="10"/>
         <v>500</v>
       </c>
-      <c r="W12" s="11">
+      <c r="Y12" s="11">
         <v>6265</v>
       </c>
-      <c r="X12" s="37">
+      <c r="Z12" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y12" s="37">
+      <c r="AA12" s="37">
         <v>0.82</v>
       </c>
-      <c r="Z12" s="38">
+      <c r="AB12" s="38">
         <f t="shared" si="4"/>
         <v>4161.2130000000006</v>
       </c>
-      <c r="AA12" s="35">
+      <c r="AC12" s="35">
         <v>0.13</v>
       </c>
-      <c r="AB12" s="36">
+      <c r="AD12" s="36">
         <f t="shared" si="5"/>
         <v>3620.2553100000005</v>
       </c>
-      <c r="AC12" s="36">
+      <c r="AE12" s="36">
         <f t="shared" si="6"/>
         <v>540.95769000000007</v>
       </c>
-      <c r="AD12" s="42">
+      <c r="AF12" s="42">
         <v>0.18</v>
       </c>
-      <c r="AE12" s="192">
+      <c r="AG12" s="192">
         <v>36315</v>
       </c>
-      <c r="AF12" s="198">
+      <c r="AH12" s="198">
         <f t="shared" si="11"/>
         <v>36315.000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>2017</v>
       </c>
@@ -5446,7 +5556,7 @@
         <v>29394.000000000011</v>
       </c>
       <c r="C13" s="210">
-        <f t="shared" si="3"/>
+        <f>AH13-(D13+N13)</f>
         <v>27511.781600000009</v>
       </c>
       <c r="D13" s="183">
@@ -5461,78 +5571,86 @@
       <c r="G13" s="186">
         <v>60</v>
       </c>
-      <c r="H13" s="185">
+      <c r="H13" s="230">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="I13" s="230">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="J13" s="185">
         <v>74</v>
       </c>
-      <c r="I13" s="184">
+      <c r="K13" s="184">
         <v>73</v>
       </c>
-      <c r="J13" s="186">
+      <c r="L13" s="186">
         <v>27</v>
       </c>
-      <c r="K13" s="222">
+      <c r="M13" s="222">
         <v>33</v>
       </c>
-      <c r="L13" s="188">
+      <c r="N13" s="188">
         <v>7509</v>
       </c>
-      <c r="M13" s="192"/>
-      <c r="N13" s="182"/>
-      <c r="O13" s="150">
+      <c r="O13" s="192"/>
+      <c r="P13" s="182"/>
+      <c r="Q13" s="150">
         <v>0.9</v>
       </c>
-      <c r="P13" s="97"/>
-      <c r="Q13" s="40" t="e">
+      <c r="R13" s="97"/>
+      <c r="S13" s="40" t="e">
         <f>0.01*(#REF!*#REF!+#REF!*#REF!)/(#REF!+#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="R13" s="40">
+      <c r="T13" s="40">
         <v>4.6699999999999998E-2</v>
       </c>
-      <c r="S13" s="28">
-        <f t="shared" si="0"/>
+      <c r="U13" s="28">
+        <f>B13-V13</f>
         <v>21885.000000000011</v>
       </c>
-      <c r="T13" s="28">
-        <f t="shared" si="1"/>
+      <c r="V13" s="28">
+        <f t="shared" si="2"/>
         <v>7509</v>
       </c>
-      <c r="U13" s="12"/>
-      <c r="V13" s="32">
+      <c r="W13" s="12"/>
+      <c r="X13" s="32">
         <f t="shared" si="10"/>
         <v>351</v>
       </c>
-      <c r="W13" s="11">
+      <c r="Y13" s="11">
         <v>7289</v>
       </c>
-      <c r="X13" s="37">
+      <c r="Z13" s="37">
         <v>0.81</v>
       </c>
-      <c r="Y13" s="37">
+      <c r="AA13" s="37">
         <v>0.7</v>
       </c>
-      <c r="Z13" s="38">
+      <c r="AB13" s="38">
         <f t="shared" si="4"/>
         <v>4132.8630000000003</v>
       </c>
-      <c r="AA13" s="34">
+      <c r="AC13" s="34">
         <v>0.1</v>
       </c>
-      <c r="AB13" s="36">
+      <c r="AD13" s="36">
         <f t="shared" si="5"/>
         <v>3719.5767000000001</v>
       </c>
-      <c r="AC13" s="36">
+      <c r="AE13" s="36">
         <f t="shared" si="6"/>
         <v>413.28630000000004</v>
       </c>
-      <c r="AE13" s="198"/>
-      <c r="AF13" s="198">
-        <f>AF12+588</f>
+      <c r="AG13" s="198"/>
+      <c r="AH13" s="198">
+        <f>AH12+588</f>
         <v>36903.000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>2018</v>
       </c>
@@ -5541,7 +5659,7 @@
         <v>37491.000000000007</v>
       </c>
       <c r="C14" s="210">
-        <f t="shared" si="3"/>
+        <f>AH14-(D14+N14)</f>
         <v>35358.027200000004</v>
       </c>
       <c r="D14" s="183">
@@ -5556,36 +5674,44 @@
       <c r="G14" s="187">
         <v>54</v>
       </c>
-      <c r="H14" s="185">
+      <c r="H14" s="230">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="I14" s="230">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="J14" s="185">
         <v>60</v>
       </c>
-      <c r="I14" s="184">
+      <c r="K14" s="184">
         <v>60</v>
       </c>
-      <c r="J14" s="187">
+      <c r="L14" s="187">
         <v>19</v>
       </c>
-      <c r="K14" s="185">
+      <c r="M14" s="185">
         <v>35</v>
       </c>
-      <c r="L14" s="188"/>
-      <c r="M14" s="192"/>
-      <c r="N14" s="182"/>
-      <c r="O14" s="149">
+      <c r="N14" s="188"/>
+      <c r="O14" s="192"/>
+      <c r="P14" s="182"/>
+      <c r="Q14" s="149">
         <v>0.9</v>
       </c>
-      <c r="P14" s="123"/>
-      <c r="T14" s="28">
-        <f t="shared" si="1"/>
+      <c r="R14" s="123"/>
+      <c r="V14" s="28">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE14" s="197"/>
-      <c r="AF14" s="198">
+      <c r="AG14" s="197"/>
+      <c r="AH14" s="198">
         <f t="shared" si="11"/>
         <v>37491.000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="120">
         <v>2019</v>
       </c>
@@ -5594,7 +5720,7 @@
         <v>38079.000000000007</v>
       </c>
       <c r="C15" s="210">
-        <f t="shared" si="3"/>
+        <f>AH15-(D15+N15)</f>
         <v>35727.806200000006</v>
       </c>
       <c r="D15" s="183">
@@ -5603,102 +5729,118 @@
       <c r="E15" s="119"/>
       <c r="F15" s="121"/>
       <c r="G15" s="122"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="121"/>
-      <c r="J15" s="121"/>
-      <c r="K15" s="122"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="107"/>
-      <c r="N15" s="108"/>
-      <c r="O15" s="151"/>
-      <c r="P15" s="123"/>
-      <c r="AE15" s="198"/>
-      <c r="AF15" s="198">
+      <c r="H15" s="230"/>
+      <c r="I15" s="230"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="121"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="106"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="151"/>
+      <c r="R15" s="123"/>
+      <c r="AG15" s="198"/>
+      <c r="AH15" s="198">
         <f t="shared" si="11"/>
         <v>38079.000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G16" s="10"/>
-      <c r="H16" s="214"/>
-      <c r="I16" s="214"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="S16" s="124"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="214"/>
+      <c r="K16" s="214"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="U16" s="124"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="R17" s="10"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="R18" s="10"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="L19" s="43"/>
-      <c r="P19" s="10"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="N19" s="43"/>
+      <c r="R19" s="10"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="L20" s="43"/>
-      <c r="P20" s="10"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="N20" s="43"/>
+      <c r="R20" s="10"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="L21" s="43"/>
-      <c r="P21" s="10"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="N21" s="43"/>
+      <c r="R21" s="10"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="L22" s="43"/>
-      <c r="P22" s="10"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="N22" s="43"/>
+      <c r="R22" s="10"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-      <c r="L23" s="43"/>
-      <c r="P23" s="10"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="43"/>
+      <c r="R23" s="10"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="L24" s="43"/>
-      <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N24" s="43"/>
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="L25" s="43"/>
-      <c r="P25" s="10"/>
+      <c r="N25" s="43"/>
+      <c r="R25" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5760,16 +5902,16 @@
       <c r="G2" s="132">
         <v>1</v>
       </c>
-      <c r="I2" s="227" t="s">
+      <c r="I2" s="229" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="227"/>
-      <c r="K2" s="227"/>
-      <c r="L2" s="227"/>
-      <c r="M2" s="227"/>
-      <c r="N2" s="227"/>
-      <c r="O2" s="227"/>
-      <c r="P2" s="227"/>
+      <c r="J2" s="229"/>
+      <c r="K2" s="229"/>
+      <c r="L2" s="229"/>
+      <c r="M2" s="229"/>
+      <c r="N2" s="229"/>
+      <c r="O2" s="229"/>
+      <c r="P2" s="229"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="133" t="s">
@@ -5793,14 +5935,14 @@
       <c r="G3" s="136">
         <v>1</v>
       </c>
-      <c r="I3" s="227"/>
-      <c r="J3" s="227"/>
-      <c r="K3" s="227"/>
-      <c r="L3" s="227"/>
-      <c r="M3" s="227"/>
-      <c r="N3" s="227"/>
-      <c r="O3" s="227"/>
-      <c r="P3" s="227"/>
+      <c r="I3" s="229"/>
+      <c r="J3" s="229"/>
+      <c r="K3" s="229"/>
+      <c r="L3" s="229"/>
+      <c r="M3" s="229"/>
+      <c r="N3" s="229"/>
+      <c r="O3" s="229"/>
+      <c r="P3" s="229"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="133" t="s">
@@ -5824,14 +5966,14 @@
       <c r="G4" s="136">
         <v>1</v>
       </c>
-      <c r="I4" s="227"/>
-      <c r="J4" s="227"/>
-      <c r="K4" s="227"/>
-      <c r="L4" s="227"/>
-      <c r="M4" s="227"/>
-      <c r="N4" s="227"/>
-      <c r="O4" s="227"/>
-      <c r="P4" s="227"/>
+      <c r="I4" s="229"/>
+      <c r="J4" s="229"/>
+      <c r="K4" s="229"/>
+      <c r="L4" s="229"/>
+      <c r="M4" s="229"/>
+      <c r="N4" s="229"/>
+      <c r="O4" s="229"/>
+      <c r="P4" s="229"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="142" t="s">
@@ -5855,14 +5997,14 @@
       <c r="G5" s="145">
         <v>1</v>
       </c>
-      <c r="I5" s="227"/>
-      <c r="J5" s="227"/>
-      <c r="K5" s="227"/>
-      <c r="L5" s="227"/>
-      <c r="M5" s="227"/>
-      <c r="N5" s="227"/>
-      <c r="O5" s="227"/>
-      <c r="P5" s="227"/>
+      <c r="I5" s="229"/>
+      <c r="J5" s="229"/>
+      <c r="K5" s="229"/>
+      <c r="L5" s="229"/>
+      <c r="M5" s="229"/>
+      <c r="N5" s="229"/>
+      <c r="O5" s="229"/>
+      <c r="P5" s="229"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="133" t="s">
@@ -5923,7 +6065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -6765,7 +6907,7 @@
       <c r="A18" s="31">
         <v>2014</v>
       </c>
-      <c r="B18" s="228">
+      <c r="B18" s="227">
         <v>0.32297447280799113</v>
       </c>
       <c r="C18" s="44"/>
@@ -6820,7 +6962,7 @@
       <c r="A19" s="31">
         <v>2015</v>
       </c>
-      <c r="B19" s="228">
+      <c r="B19" s="227">
         <v>0.35719557195571955</v>
       </c>
       <c r="C19" s="44"/>
@@ -6931,7 +7073,7 @@
       <c r="A21" s="31">
         <v>2017</v>
       </c>
-      <c r="B21" s="228">
+      <c r="B21" s="227">
         <v>0.49761417859577367</v>
       </c>
       <c r="C21" s="44"/>
@@ -6983,7 +7125,7 @@
       <c r="A22" s="31">
         <v>2018</v>
       </c>
-      <c r="B22" s="229">
+      <c r="B22" s="228">
         <v>0.53368660105980315</v>
       </c>
       <c r="C22" s="44"/>
@@ -7035,7 +7177,7 @@
       <c r="A23" s="31">
         <v>2019</v>
       </c>
-      <c r="B23" s="229">
+      <c r="B23" s="228">
         <v>0.59571788413098237</v>
       </c>
       <c r="C23" s="44"/>

</xml_diff>

<commit_message>
Calibration bounds are now in spreadsheet
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -13,12 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
-    <sheet name="data" sheetId="5" r:id="rId2"/>
-    <sheet name="mixing" sheetId="27" r:id="rId3"/>
-    <sheet name="timepars" sheetId="28" r:id="rId4"/>
-    <sheet name="scen_1" sheetId="25" r:id="rId5"/>
-    <sheet name="scen_2" sheetId="26" r:id="rId6"/>
-    <sheet name="timepars_old" sheetId="20" r:id="rId7"/>
+    <sheet name="calibration" sheetId="29" r:id="rId2"/>
+    <sheet name="data" sheetId="5" r:id="rId3"/>
+    <sheet name="mixing" sheetId="27" r:id="rId4"/>
+    <sheet name="timepars" sheetId="28" r:id="rId5"/>
+    <sheet name="scen_1" sheetId="25" r:id="rId6"/>
+    <sheet name="scen_2" sheetId="26" r:id="rId7"/>
+    <sheet name="timepars_old" sheetId="20" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1795,7 +1796,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="146">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2201,6 +2202,39 @@
   </si>
   <si>
     <t>HIV_diag_old_tot</t>
+  </si>
+  <si>
+    <t>bes</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>ubs</t>
+  </si>
+  <si>
+    <t>f_infect_HIV</t>
+  </si>
+  <si>
+    <t>int_factor</t>
+  </si>
+  <si>
+    <t>high_risk_factor</t>
+  </si>
+  <si>
+    <t>init_diag_prop</t>
+  </si>
+  <si>
+    <t>init_prev_HIV_aus</t>
+  </si>
+  <si>
+    <t>init_prev_HIV_int</t>
+  </si>
+  <si>
+    <t>init_late_prop</t>
+  </si>
+  <si>
+    <t>init_pop_aus</t>
   </si>
 </sst>
 </file>
@@ -3829,7 +3863,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4314,10 +4348,153 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="59">
+        <v>0</v>
+      </c>
+      <c r="C2" s="59">
+        <v>2.5755000000000002E-6</v>
+      </c>
+      <c r="D2" s="59">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="59">
+        <v>1</v>
+      </c>
+      <c r="C3" s="59">
+        <v>1.2</v>
+      </c>
+      <c r="D3" s="59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="59">
+        <v>1</v>
+      </c>
+      <c r="C4" s="59">
+        <v>2</v>
+      </c>
+      <c r="D4" s="59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="59">
+        <v>0</v>
+      </c>
+      <c r="C5" s="59">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="59">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="59">
+        <v>0</v>
+      </c>
+      <c r="C6" s="59">
+        <v>0.12515000000000001</v>
+      </c>
+      <c r="D6" s="59">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="59">
+        <v>0</v>
+      </c>
+      <c r="C7" s="59">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D7" s="59">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="59">
+        <v>0</v>
+      </c>
+      <c r="C8" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="59">
+        <v>1</v>
+      </c>
+      <c r="C9" s="59">
+        <v>25000</v>
+      </c>
+      <c r="D9" s="59">
+        <v>90000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L27" sqref="L27"/>
     </sheetView>
@@ -5849,7 +6026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
@@ -6061,7 +6238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
@@ -7539,7 +7716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -7742,7 +7919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -7961,7 +8138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL34"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added population growth as timepar
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -1289,6 +1289,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Tom Tidhar</author>
+    <author>Kathleen Ryan</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0">
@@ -1312,6 +1313,55 @@
           </rPr>
           <t xml:space="preserve">
 Number of people on PrEP. Seemed to make more sense than proportion of people on PrEP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom Tidhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Proportion of the susceptible population that is at high risk</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kathleen Ryan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Before PrEp was made available I have used the % of HIV -ve and untestedmen in GCPS thtat reported any CAI
+After prEP was implemented I used the % of HIV -ve men not on PrEP from paper published by Holt - only 2 years provided in paper</t>
         </r>
       </text>
     </comment>
@@ -1796,7 +1846,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2235,6 +2285,9 @@
   </si>
   <si>
     <t>init_pop_aus</t>
+  </si>
+  <si>
+    <t>annual_pop_growth</t>
   </si>
 </sst>
 </file>
@@ -3529,11 +3582,11 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -4351,8 +4404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4412,7 +4465,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="59">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4437,10 +4490,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="59">
-        <v>0.12515000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="D6" s="59">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4479,7 +4532,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="59">
-        <v>25000</v>
+        <v>40000</v>
       </c>
       <c r="D9" s="59">
         <v>90000</v>
@@ -4495,8 +4548,8 @@
   <dimension ref="A1:AH25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L27" sqref="L27"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4652,11 +4705,11 @@
       <c r="G2" s="223">
         <v>13</v>
       </c>
-      <c r="H2" s="230">
+      <c r="H2" s="229">
         <f>J2+L2</f>
         <v>87</v>
       </c>
-      <c r="I2" s="230">
+      <c r="I2" s="229">
         <f>K2+M2</f>
         <v>112</v>
       </c>
@@ -4716,12 +4769,12 @@
       <c r="G3" s="224">
         <v>17</v>
       </c>
-      <c r="H3" s="230">
-        <f t="shared" ref="H3:H15" si="0">J3+L3</f>
+      <c r="H3" s="229">
+        <f t="shared" ref="H3:H14" si="0">J3+L3</f>
         <v>76</v>
       </c>
-      <c r="I3" s="230">
-        <f t="shared" ref="I3:I15" si="1">K3+M3</f>
+      <c r="I3" s="229">
+        <f t="shared" ref="I3:I14" si="1">K3+M3</f>
         <v>108</v>
       </c>
       <c r="J3" s="103">
@@ -4752,11 +4805,11 @@
         <v>3.4931506849315071E-2</v>
       </c>
       <c r="U3" s="28">
-        <f>B3-V3</f>
+        <f t="shared" ref="U3:U13" si="2">B3-V3</f>
         <v>-4491</v>
       </c>
       <c r="V3" s="28">
-        <f t="shared" ref="V3:V14" si="2">N3</f>
+        <f t="shared" ref="V3:V14" si="3">N3</f>
         <v>4491</v>
       </c>
       <c r="W3" s="33">
@@ -4764,7 +4817,7 @@
         <v>-105</v>
       </c>
       <c r="X3" s="33">
-        <f t="shared" ref="X3" si="3">ROUND(T3*V3,0)</f>
+        <f t="shared" ref="X3" si="4">ROUND(T3*V3,0)</f>
         <v>157</v>
       </c>
       <c r="Y3" s="11">
@@ -4807,7 +4860,7 @@
         <v>27007.800000000003</v>
       </c>
       <c r="C4" s="210">
-        <f>AH4-(D4+N4)</f>
+        <f t="shared" ref="C4:C15" si="5">AH4-(D4+N4)</f>
         <v>27007.800000000003</v>
       </c>
       <c r="D4" s="182"/>
@@ -4820,11 +4873,11 @@
       <c r="G4" s="224">
         <v>16</v>
       </c>
-      <c r="H4" s="230">
+      <c r="H4" s="229">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="I4" s="230">
+      <c r="I4" s="229">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
@@ -4850,11 +4903,11 @@
       <c r="S4" s="40"/>
       <c r="T4" s="40"/>
       <c r="U4" s="28">
-        <f>B4-V4</f>
+        <f t="shared" si="2"/>
         <v>22237.800000000003</v>
       </c>
       <c r="V4" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4770</v>
       </c>
       <c r="W4" s="12"/>
@@ -4869,24 +4922,24 @@
         <v>0.82</v>
       </c>
       <c r="AB4" s="38">
-        <f t="shared" ref="AB4:AB13" si="4">Y4*Z4*AA4</f>
+        <f t="shared" ref="AB4:AB13" si="6">Y4*Z4*AA4</f>
         <v>612.39239999999995</v>
       </c>
       <c r="AC4" s="34">
         <v>0.17</v>
       </c>
       <c r="AD4" s="36">
-        <f t="shared" ref="AD4:AD13" si="5">AB4-AE4</f>
+        <f t="shared" ref="AD4:AD13" si="7">AB4-AE4</f>
         <v>508.28569199999993</v>
       </c>
       <c r="AE4" s="36">
-        <f t="shared" ref="AE4:AE13" si="6">AB4*AC4</f>
+        <f t="shared" ref="AE4:AE13" si="8">AB4*AC4</f>
         <v>104.106708</v>
       </c>
       <c r="AF4" s="13"/>
       <c r="AG4" s="198"/>
       <c r="AH4" s="209">
-        <f t="shared" ref="AH4:AH7" si="7">AH3+532.4</f>
+        <f t="shared" ref="AH4:AH7" si="9">AH3+532.4</f>
         <v>31777.800000000003</v>
       </c>
     </row>
@@ -4895,11 +4948,11 @@
         <v>2009</v>
       </c>
       <c r="B5" s="188">
-        <f t="shared" ref="B5:B15" si="8">SUM(C5:D5)</f>
+        <f t="shared" ref="B5:B15" si="10">SUM(C5:D5)</f>
         <v>27251.200000000004</v>
       </c>
       <c r="C5" s="210">
-        <f>AH5-(D5+N5)</f>
+        <f t="shared" si="5"/>
         <v>27251.200000000004</v>
       </c>
       <c r="D5" s="182"/>
@@ -4912,11 +4965,11 @@
       <c r="G5" s="224">
         <v>14</v>
       </c>
-      <c r="H5" s="230">
+      <c r="H5" s="229">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="I5" s="230">
+      <c r="I5" s="229">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
@@ -4942,11 +4995,11 @@
       <c r="S5" s="40"/>
       <c r="T5" s="40"/>
       <c r="U5" s="28">
-        <f>B5-V5</f>
+        <f t="shared" si="2"/>
         <v>22192.200000000004</v>
       </c>
       <c r="V5" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5059</v>
       </c>
       <c r="W5" s="12"/>
@@ -4961,24 +5014,24 @@
         <v>0.82</v>
       </c>
       <c r="AB5" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>983.01600000000008</v>
       </c>
       <c r="AC5" s="34">
         <v>0.17</v>
       </c>
       <c r="AD5" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>815.90328</v>
       </c>
       <c r="AE5" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>167.11272000000002</v>
       </c>
       <c r="AF5" s="14"/>
       <c r="AG5" s="198"/>
       <c r="AH5" s="209">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>32310.200000000004</v>
       </c>
     </row>
@@ -4987,11 +5040,11 @@
         <v>2010</v>
       </c>
       <c r="B6" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>27536.600000000006</v>
       </c>
       <c r="C6" s="210">
-        <f>AH6-(D6+N6)</f>
+        <f t="shared" si="5"/>
         <v>26220.496600000006</v>
       </c>
       <c r="D6" s="183">
@@ -5006,11 +5059,11 @@
       <c r="G6" s="224">
         <v>21</v>
       </c>
-      <c r="H6" s="230">
+      <c r="H6" s="229">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="I6" s="230">
+      <c r="I6" s="229">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
@@ -5040,19 +5093,19 @@
         <v>4.3150684931506846E-2</v>
       </c>
       <c r="U6" s="28">
-        <f>B6-V6</f>
+        <f t="shared" si="2"/>
         <v>22230.600000000006</v>
       </c>
       <c r="V6" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5306</v>
       </c>
       <c r="W6" s="32">
-        <f t="shared" ref="W6:W12" si="9">ROUND(S6*U6,0)</f>
+        <f t="shared" ref="W6:W12" si="11">ROUND(S6*U6,0)</f>
         <v>895</v>
       </c>
       <c r="X6" s="32">
-        <f t="shared" ref="X6:X13" si="10">ROUND(T6*V6,0)</f>
+        <f t="shared" ref="X6:X13" si="12">ROUND(T6*V6,0)</f>
         <v>229</v>
       </c>
       <c r="Y6" s="11">
@@ -5065,24 +5118,24 @@
         <v>0.82</v>
       </c>
       <c r="AB6" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1167.6635999999999</v>
       </c>
       <c r="AC6" s="34">
         <v>0.17</v>
       </c>
       <c r="AD6" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>969.16078799999991</v>
       </c>
       <c r="AE6" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>198.50281199999998</v>
       </c>
       <c r="AF6" s="14"/>
       <c r="AG6" s="198"/>
       <c r="AH6" s="209">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>32842.600000000006</v>
       </c>
     </row>
@@ -5095,7 +5148,7 @@
         <v>27760.000000000007</v>
       </c>
       <c r="C7" s="210">
-        <f>AH7-(D7+N7)</f>
+        <f t="shared" si="5"/>
         <v>26586.372400000007</v>
       </c>
       <c r="D7" s="183">
@@ -5110,11 +5163,11 @@
       <c r="G7" s="224">
         <v>20</v>
       </c>
-      <c r="H7" s="230">
+      <c r="H7" s="229">
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="I7" s="230">
+      <c r="I7" s="229">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
@@ -5144,19 +5197,19 @@
         <v>4.726027397260274E-2</v>
       </c>
       <c r="U7" s="28">
-        <f>B7-V7</f>
+        <f t="shared" si="2"/>
         <v>22145.000000000007</v>
       </c>
       <c r="V7" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5615</v>
       </c>
       <c r="W7" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>831</v>
       </c>
       <c r="X7" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>265</v>
       </c>
       <c r="Y7" s="11">
@@ -5169,18 +5222,18 @@
         <v>0.82</v>
       </c>
       <c r="AB7" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1237.4046000000001</v>
       </c>
       <c r="AC7" s="34">
         <v>0.17</v>
       </c>
       <c r="AD7" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1027.0458180000001</v>
       </c>
       <c r="AE7" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>210.35878200000002</v>
       </c>
       <c r="AF7" s="14"/>
@@ -5188,7 +5241,7 @@
         <v>33375</v>
       </c>
       <c r="AH7" s="209">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>33375.000000000007</v>
       </c>
     </row>
@@ -5197,11 +5250,11 @@
         <v>2012</v>
       </c>
       <c r="B8" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28064.000000000007</v>
       </c>
       <c r="C8" s="210">
-        <f>AH8-(D8+N8)</f>
+        <f t="shared" si="5"/>
         <v>26959.744400000007</v>
       </c>
       <c r="D8" s="183">
@@ -5216,11 +5269,11 @@
       <c r="G8" s="186">
         <v>34</v>
       </c>
-      <c r="H8" s="230">
+      <c r="H8" s="229">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="I8" s="230">
+      <c r="I8" s="229">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
@@ -5252,19 +5305,19 @@
         <v>5.3835616438356167E-2</v>
       </c>
       <c r="U8" s="28">
-        <f>B8-V8</f>
+        <f t="shared" si="2"/>
         <v>22165.000000000007</v>
       </c>
       <c r="V8" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5899</v>
       </c>
       <c r="W8" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1081</v>
       </c>
       <c r="X8" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>318</v>
       </c>
       <c r="Y8" s="11">
@@ -5277,18 +5330,18 @@
         <v>0.82</v>
       </c>
       <c r="AB8" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1617.9911999999999</v>
       </c>
       <c r="AC8" s="34">
         <v>0.17</v>
       </c>
       <c r="AD8" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1342.9326959999999</v>
       </c>
       <c r="AE8" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>275.05850400000003</v>
       </c>
       <c r="AF8" s="14"/>
@@ -5303,11 +5356,11 @@
         <v>2013</v>
       </c>
       <c r="B9" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28346.000000000007</v>
       </c>
       <c r="C9" s="210">
-        <f>AH9-(D9+N9)</f>
+        <f t="shared" si="5"/>
         <v>27200.205800000007</v>
       </c>
       <c r="D9" s="183">
@@ -5322,11 +5375,11 @@
       <c r="G9" s="186">
         <v>49</v>
       </c>
-      <c r="H9" s="230">
+      <c r="H9" s="229">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="I9" s="230">
+      <c r="I9" s="229">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
@@ -5356,19 +5409,19 @@
         <v>6.2671232876712321E-2</v>
       </c>
       <c r="U9" s="28">
-        <f>B9-V9</f>
+        <f t="shared" si="2"/>
         <v>22141.000000000007</v>
       </c>
       <c r="V9" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6205</v>
       </c>
       <c r="W9" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1171</v>
       </c>
       <c r="X9" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>389</v>
       </c>
       <c r="Y9" s="11">
@@ -5381,24 +5434,24 @@
         <v>0.82</v>
       </c>
       <c r="AB9" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1977.9876000000002</v>
       </c>
       <c r="AC9" s="34">
         <v>0.17</v>
       </c>
       <c r="AD9" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1641.7297080000001</v>
       </c>
       <c r="AE9" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>336.25789200000003</v>
       </c>
       <c r="AF9" s="14"/>
       <c r="AG9" s="198"/>
       <c r="AH9" s="198">
-        <f t="shared" ref="AH9:AH15" si="11">AH8+588</f>
+        <f t="shared" ref="AH9:AH15" si="13">AH8+588</f>
         <v>34551.000000000007</v>
       </c>
     </row>
@@ -5407,11 +5460,11 @@
         <v>2014</v>
       </c>
       <c r="B10" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28585.000000000007</v>
       </c>
       <c r="C10" s="210">
-        <f>AH10-(D10+N10)</f>
+        <f t="shared" si="5"/>
         <v>27281.934400000006</v>
       </c>
       <c r="D10" s="183">
@@ -5426,11 +5479,11 @@
       <c r="G10" s="186">
         <v>35</v>
       </c>
-      <c r="H10" s="230">
+      <c r="H10" s="229">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="I10" s="230">
+      <c r="I10" s="229">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
@@ -5462,19 +5515,19 @@
         <v>5.321917808219178E-2</v>
       </c>
       <c r="U10" s="28">
-        <f>B10-V10</f>
+        <f t="shared" si="2"/>
         <v>22031.000000000007</v>
       </c>
       <c r="V10" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6554</v>
       </c>
       <c r="W10" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1135</v>
       </c>
       <c r="X10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>349</v>
       </c>
       <c r="Y10" s="11">
@@ -5487,24 +5540,24 @@
         <v>0.82</v>
       </c>
       <c r="AB10" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2171.2698</v>
       </c>
       <c r="AC10" s="34">
         <v>0.17</v>
       </c>
       <c r="AD10" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1802.1539339999999</v>
       </c>
       <c r="AE10" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>369.11586600000004</v>
       </c>
       <c r="AF10" s="14"/>
       <c r="AG10" s="198"/>
       <c r="AH10" s="198">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>35139.000000000007</v>
       </c>
     </row>
@@ -5513,11 +5566,11 @@
         <v>2015</v>
       </c>
       <c r="B11" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28863.000000000007</v>
       </c>
       <c r="C11" s="210">
-        <f>AH11-(D11+N11)</f>
+        <f t="shared" si="5"/>
         <v>27407.579200000007</v>
       </c>
       <c r="D11" s="183">
@@ -5532,11 +5585,11 @@
       <c r="G11" s="186">
         <v>41</v>
       </c>
-      <c r="H11" s="230">
+      <c r="H11" s="229">
         <f t="shared" si="0"/>
         <v>138</v>
       </c>
-      <c r="I11" s="230">
+      <c r="I11" s="229">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
@@ -5568,19 +5621,19 @@
         <v>6.7191780821917804E-2</v>
       </c>
       <c r="U11" s="28">
-        <f>B11-V11</f>
+        <f t="shared" si="2"/>
         <v>21999.000000000007</v>
       </c>
       <c r="V11" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6864</v>
       </c>
       <c r="W11" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1465</v>
       </c>
       <c r="X11" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>461</v>
       </c>
       <c r="Y11" s="11">
@@ -5593,24 +5646,24 @@
         <v>0.82</v>
       </c>
       <c r="AB11" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3231.3330000000001</v>
       </c>
       <c r="AC11" s="35">
         <v>0.17</v>
       </c>
       <c r="AD11" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2682.00639</v>
       </c>
       <c r="AE11" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>549.32661000000007</v>
       </c>
       <c r="AF11" s="14"/>
       <c r="AG11" s="198"/>
       <c r="AH11" s="198">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>35727.000000000007</v>
       </c>
     </row>
@@ -5623,7 +5676,7 @@
         <v>29091.000000000007</v>
       </c>
       <c r="C12" s="210">
-        <f>AH12-(D12+N12)</f>
+        <f t="shared" si="5"/>
         <v>27444.524200000007</v>
       </c>
       <c r="D12" s="183">
@@ -5638,11 +5691,11 @@
       <c r="G12" s="186">
         <v>64</v>
       </c>
-      <c r="H12" s="230">
+      <c r="H12" s="229">
         <f t="shared" si="0"/>
         <v>134</v>
       </c>
-      <c r="I12" s="230">
+      <c r="I12" s="229">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
@@ -5674,19 +5727,19 @@
         <v>6.9246575342465755E-2</v>
       </c>
       <c r="U12" s="28">
-        <f>B12-V12</f>
+        <f t="shared" si="2"/>
         <v>21867.000000000007</v>
       </c>
       <c r="V12" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7224</v>
       </c>
       <c r="W12" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1384</v>
       </c>
       <c r="X12" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>500</v>
       </c>
       <c r="Y12" s="11">
@@ -5699,18 +5752,18 @@
         <v>0.82</v>
       </c>
       <c r="AB12" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4161.2130000000006</v>
       </c>
       <c r="AC12" s="35">
         <v>0.13</v>
       </c>
       <c r="AD12" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3620.2553100000005</v>
       </c>
       <c r="AE12" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>540.95769000000007</v>
       </c>
       <c r="AF12" s="42">
@@ -5720,7 +5773,7 @@
         <v>36315</v>
       </c>
       <c r="AH12" s="198">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>36315.000000000007</v>
       </c>
     </row>
@@ -5729,11 +5782,11 @@
         <v>2017</v>
       </c>
       <c r="B13" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>29394.000000000011</v>
       </c>
       <c r="C13" s="210">
-        <f>AH13-(D13+N13)</f>
+        <f t="shared" si="5"/>
         <v>27511.781600000009</v>
       </c>
       <c r="D13" s="183">
@@ -5748,11 +5801,11 @@
       <c r="G13" s="186">
         <v>60</v>
       </c>
-      <c r="H13" s="230">
+      <c r="H13" s="229">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="I13" s="230">
+      <c r="I13" s="229">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
@@ -5785,16 +5838,16 @@
         <v>4.6699999999999998E-2</v>
       </c>
       <c r="U13" s="28">
-        <f>B13-V13</f>
+        <f t="shared" si="2"/>
         <v>21885.000000000011</v>
       </c>
       <c r="V13" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7509</v>
       </c>
       <c r="W13" s="12"/>
       <c r="X13" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>351</v>
       </c>
       <c r="Y13" s="11">
@@ -5807,18 +5860,18 @@
         <v>0.7</v>
       </c>
       <c r="AB13" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4132.8630000000003</v>
       </c>
       <c r="AC13" s="34">
         <v>0.1</v>
       </c>
       <c r="AD13" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3719.5767000000001</v>
       </c>
       <c r="AE13" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>413.28630000000004</v>
       </c>
       <c r="AG13" s="198"/>
@@ -5832,11 +5885,11 @@
         <v>2018</v>
       </c>
       <c r="B14" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>37491.000000000007</v>
       </c>
       <c r="C14" s="210">
-        <f>AH14-(D14+N14)</f>
+        <f t="shared" si="5"/>
         <v>35358.027200000004</v>
       </c>
       <c r="D14" s="183">
@@ -5851,11 +5904,11 @@
       <c r="G14" s="187">
         <v>54</v>
       </c>
-      <c r="H14" s="230">
+      <c r="H14" s="229">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="I14" s="230">
+      <c r="I14" s="229">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
@@ -5879,12 +5932,12 @@
       </c>
       <c r="R14" s="123"/>
       <c r="V14" s="28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG14" s="197"/>
       <c r="AH14" s="198">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>37491.000000000007</v>
       </c>
     </row>
@@ -5893,11 +5946,11 @@
         <v>2019</v>
       </c>
       <c r="B15" s="188">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>38079.000000000007</v>
       </c>
       <c r="C15" s="210">
-        <f>AH15-(D15+N15)</f>
+        <f t="shared" si="5"/>
         <v>35727.806200000006</v>
       </c>
       <c r="D15" s="183">
@@ -5906,8 +5959,8 @@
       <c r="E15" s="119"/>
       <c r="F15" s="121"/>
       <c r="G15" s="122"/>
-      <c r="H15" s="230"/>
-      <c r="I15" s="230"/>
+      <c r="H15" s="229"/>
+      <c r="I15" s="229"/>
       <c r="J15" s="119"/>
       <c r="K15" s="121"/>
       <c r="L15" s="121"/>
@@ -5919,7 +5972,7 @@
       <c r="R15" s="123"/>
       <c r="AG15" s="198"/>
       <c r="AH15" s="198">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>38079.000000000007</v>
       </c>
     </row>
@@ -6079,16 +6132,16 @@
       <c r="G2" s="132">
         <v>1</v>
       </c>
-      <c r="I2" s="229" t="s">
+      <c r="I2" s="230" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="229"/>
-      <c r="K2" s="229"/>
-      <c r="L2" s="229"/>
-      <c r="M2" s="229"/>
-      <c r="N2" s="229"/>
-      <c r="O2" s="229"/>
-      <c r="P2" s="229"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="230"/>
+      <c r="O2" s="230"/>
+      <c r="P2" s="230"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="133" t="s">
@@ -6112,14 +6165,14 @@
       <c r="G3" s="136">
         <v>1</v>
       </c>
-      <c r="I3" s="229"/>
-      <c r="J3" s="229"/>
-      <c r="K3" s="229"/>
-      <c r="L3" s="229"/>
-      <c r="M3" s="229"/>
-      <c r="N3" s="229"/>
-      <c r="O3" s="229"/>
-      <c r="P3" s="229"/>
+      <c r="I3" s="230"/>
+      <c r="J3" s="230"/>
+      <c r="K3" s="230"/>
+      <c r="L3" s="230"/>
+      <c r="M3" s="230"/>
+      <c r="N3" s="230"/>
+      <c r="O3" s="230"/>
+      <c r="P3" s="230"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="133" t="s">
@@ -6143,14 +6196,14 @@
       <c r="G4" s="136">
         <v>1</v>
       </c>
-      <c r="I4" s="229"/>
-      <c r="J4" s="229"/>
-      <c r="K4" s="229"/>
-      <c r="L4" s="229"/>
-      <c r="M4" s="229"/>
-      <c r="N4" s="229"/>
-      <c r="O4" s="229"/>
-      <c r="P4" s="229"/>
+      <c r="I4" s="230"/>
+      <c r="J4" s="230"/>
+      <c r="K4" s="230"/>
+      <c r="L4" s="230"/>
+      <c r="M4" s="230"/>
+      <c r="N4" s="230"/>
+      <c r="O4" s="230"/>
+      <c r="P4" s="230"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="142" t="s">
@@ -6174,14 +6227,14 @@
       <c r="G5" s="145">
         <v>1</v>
       </c>
-      <c r="I5" s="229"/>
-      <c r="J5" s="229"/>
-      <c r="K5" s="229"/>
-      <c r="L5" s="229"/>
-      <c r="M5" s="229"/>
-      <c r="N5" s="229"/>
-      <c r="O5" s="229"/>
-      <c r="P5" s="229"/>
+      <c r="I5" s="230"/>
+      <c r="J5" s="230"/>
+      <c r="K5" s="230"/>
+      <c r="L5" s="230"/>
+      <c r="M5" s="230"/>
+      <c r="N5" s="230"/>
+      <c r="O5" s="230"/>
+      <c r="P5" s="230"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="133" t="s">
@@ -6240,10 +6293,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6272,11 +6325,11 @@
     <col min="22" max="22" width="19.85546875" style="60" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="28" style="60" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20" style="43" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="43"/>
+    <col min="25" max="26" width="16.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
@@ -6352,8 +6405,11 @@
       <c r="Y1" s="68" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>84</v>
       </c>
@@ -6405,8 +6461,9 @@
       <c r="W2" s="71"/>
       <c r="X2" s="70"/>
       <c r="Y2" s="71"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" s="71"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
@@ -6476,8 +6533,11 @@
       <c r="Y3" s="71" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z3" s="71" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2000</v>
       </c>
@@ -6531,8 +6591,11 @@
       <c r="Y4" s="74">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z4" s="74">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2001</v>
       </c>
@@ -6560,8 +6623,9 @@
       <c r="W5" s="77"/>
       <c r="X5" s="76"/>
       <c r="Y5" s="77"/>
-    </row>
-    <row r="6" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z5" s="77"/>
+    </row>
+    <row r="6" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>2002</v>
       </c>
@@ -6589,8 +6653,9 @@
       <c r="W6" s="77"/>
       <c r="X6" s="76"/>
       <c r="Y6" s="77"/>
-    </row>
-    <row r="7" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z6" s="77"/>
+    </row>
+    <row r="7" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>2003</v>
       </c>
@@ -6620,8 +6685,9 @@
       <c r="W7" s="77"/>
       <c r="X7" s="76"/>
       <c r="Y7" s="77"/>
-    </row>
-    <row r="8" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z7" s="77"/>
+    </row>
+    <row r="8" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>2004</v>
       </c>
@@ -6651,8 +6717,9 @@
       <c r="W8" s="77"/>
       <c r="X8" s="76"/>
       <c r="Y8" s="77"/>
-    </row>
-    <row r="9" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z8" s="77"/>
+    </row>
+    <row r="9" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>2005</v>
       </c>
@@ -6682,8 +6749,9 @@
       <c r="W9" s="77"/>
       <c r="X9" s="76"/>
       <c r="Y9" s="77"/>
-    </row>
-    <row r="10" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z9" s="77"/>
+    </row>
+    <row r="10" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2006</v>
       </c>
@@ -6729,8 +6797,9 @@
       <c r="W10" s="77"/>
       <c r="X10" s="76"/>
       <c r="Y10" s="77"/>
-    </row>
-    <row r="11" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z10" s="77"/>
+    </row>
+    <row r="11" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2007</v>
       </c>
@@ -6780,8 +6849,9 @@
       <c r="W11" s="77"/>
       <c r="X11" s="76"/>
       <c r="Y11" s="77"/>
-    </row>
-    <row r="12" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z11" s="77"/>
+    </row>
+    <row r="12" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2008</v>
       </c>
@@ -6827,8 +6897,9 @@
       <c r="W12" s="77"/>
       <c r="X12" s="76"/>
       <c r="Y12" s="77"/>
-    </row>
-    <row r="13" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z12" s="77"/>
+    </row>
+    <row r="13" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2009</v>
       </c>
@@ -6875,8 +6946,9 @@
       <c r="W13" s="77"/>
       <c r="X13" s="76"/>
       <c r="Y13" s="77"/>
-    </row>
-    <row r="14" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z13" s="77"/>
+    </row>
+    <row r="14" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>2010</v>
       </c>
@@ -6927,8 +6999,9 @@
       <c r="W14" s="77"/>
       <c r="X14" s="76"/>
       <c r="Y14" s="77"/>
-    </row>
-    <row r="15" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z14" s="77"/>
+    </row>
+    <row r="15" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>2011</v>
       </c>
@@ -6975,8 +7048,9 @@
       <c r="W15" s="77"/>
       <c r="X15" s="76"/>
       <c r="Y15" s="77"/>
-    </row>
-    <row r="16" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z15" s="77"/>
+    </row>
+    <row r="16" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>2012</v>
       </c>
@@ -7027,8 +7101,9 @@
       <c r="W16" s="77"/>
       <c r="X16" s="76"/>
       <c r="Y16" s="77"/>
-    </row>
-    <row r="17" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z16" s="77"/>
+    </row>
+    <row r="17" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>2013</v>
       </c>
@@ -7079,8 +7154,9 @@
       <c r="W17" s="77"/>
       <c r="X17" s="76"/>
       <c r="Y17" s="77"/>
-    </row>
-    <row r="18" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="77"/>
+    </row>
+    <row r="18" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>2014</v>
       </c>
@@ -7134,8 +7210,9 @@
       <c r="W18" s="77"/>
       <c r="X18" s="76"/>
       <c r="Y18" s="77"/>
-    </row>
-    <row r="19" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z18" s="77"/>
+    </row>
+    <row r="19" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>2015</v>
       </c>
@@ -7189,8 +7266,9 @@
       <c r="W19" s="77"/>
       <c r="X19" s="76"/>
       <c r="Y19" s="77"/>
-    </row>
-    <row r="20" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z19" s="77"/>
+    </row>
+    <row r="20" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2016</v>
       </c>
@@ -7245,8 +7323,9 @@
       <c r="W20" s="77"/>
       <c r="X20" s="76"/>
       <c r="Y20" s="77"/>
-    </row>
-    <row r="21" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z20" s="77"/>
+    </row>
+    <row r="21" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>2017</v>
       </c>
@@ -7297,8 +7376,9 @@
       <c r="W21" s="77"/>
       <c r="X21" s="76"/>
       <c r="Y21" s="77"/>
-    </row>
-    <row r="22" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z21" s="77"/>
+    </row>
+    <row r="22" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>2018</v>
       </c>
@@ -7349,8 +7429,9 @@
       <c r="W22" s="77"/>
       <c r="X22" s="76"/>
       <c r="Y22" s="77"/>
-    </row>
-    <row r="23" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z22" s="77"/>
+    </row>
+    <row r="23" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>2019</v>
       </c>
@@ -7385,8 +7466,9 @@
       <c r="W23" s="77"/>
       <c r="X23" s="76"/>
       <c r="Y23" s="77"/>
-    </row>
-    <row r="24" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z23" s="77"/>
+    </row>
+    <row r="24" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31">
         <v>2020</v>
       </c>
@@ -7414,8 +7496,9 @@
       <c r="W24" s="77"/>
       <c r="X24" s="76"/>
       <c r="Y24" s="77"/>
-    </row>
-    <row r="25" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z24" s="77"/>
+    </row>
+    <row r="25" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31">
         <v>2021</v>
       </c>
@@ -7443,8 +7526,9 @@
       <c r="W25" s="77"/>
       <c r="X25" s="76"/>
       <c r="Y25" s="77"/>
-    </row>
-    <row r="26" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z25" s="77"/>
+    </row>
+    <row r="26" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>2022</v>
       </c>
@@ -7472,8 +7556,9 @@
       <c r="W26" s="77"/>
       <c r="X26" s="76"/>
       <c r="Y26" s="77"/>
-    </row>
-    <row r="27" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z26" s="77"/>
+    </row>
+    <row r="27" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
         <v>2023</v>
       </c>
@@ -7501,8 +7586,9 @@
       <c r="W27" s="77"/>
       <c r="X27" s="76"/>
       <c r="Y27" s="77"/>
-    </row>
-    <row r="28" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z27" s="77"/>
+    </row>
+    <row r="28" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
         <v>2024</v>
       </c>
@@ -7530,8 +7616,9 @@
       <c r="W28" s="77"/>
       <c r="X28" s="76"/>
       <c r="Y28" s="77"/>
-    </row>
-    <row r="29" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z28" s="77"/>
+    </row>
+    <row r="29" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
         <v>2025</v>
       </c>
@@ -7559,8 +7646,9 @@
       <c r="W29" s="77"/>
       <c r="X29" s="76"/>
       <c r="Y29" s="77"/>
-    </row>
-    <row r="30" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z29" s="77"/>
+    </row>
+    <row r="30" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31">
         <v>2026</v>
       </c>
@@ -7588,8 +7676,9 @@
       <c r="W30" s="77"/>
       <c r="X30" s="76"/>
       <c r="Y30" s="77"/>
-    </row>
-    <row r="31" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z30" s="77"/>
+    </row>
+    <row r="31" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
         <v>2027</v>
       </c>
@@ -7617,8 +7706,9 @@
       <c r="W31" s="77"/>
       <c r="X31" s="76"/>
       <c r="Y31" s="77"/>
-    </row>
-    <row r="32" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z31" s="77"/>
+    </row>
+    <row r="32" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31">
         <v>2028</v>
       </c>
@@ -7646,8 +7736,9 @@
       <c r="W32" s="77"/>
       <c r="X32" s="76"/>
       <c r="Y32" s="77"/>
-    </row>
-    <row r="33" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z32" s="77"/>
+    </row>
+    <row r="33" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31">
         <v>2029</v>
       </c>
@@ -7675,8 +7766,9 @@
       <c r="W33" s="77"/>
       <c r="X33" s="76"/>
       <c r="Y33" s="77"/>
-    </row>
-    <row r="34" spans="1:25" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z33" s="77"/>
+    </row>
+    <row r="34" spans="1:26" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="63">
         <v>2030</v>
       </c>
@@ -7708,6 +7800,7 @@
       <c r="W34" s="80"/>
       <c r="X34" s="79"/>
       <c r="Y34" s="80"/>
+      <c r="Z34" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7718,10 +7811,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7729,10 +7822,11 @@
     <col min="1" max="1" width="9" style="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="60" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="60" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="43"/>
+    <col min="4" max="4" width="15.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
@@ -7742,15 +7836,19 @@
       <c r="C1" s="68" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="71"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>85</v>
       </c>
@@ -7760,71 +7858,81 @@
       <c r="C3" s="71" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="44"/>
+    </row>
+    <row r="4" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2000</v>
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="74"/>
-    </row>
-    <row r="5" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="29"/>
+    </row>
+    <row r="5" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2001</v>
       </c>
       <c r="B5" s="75"/>
       <c r="C5" s="77"/>
-    </row>
-    <row r="6" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="44"/>
+    </row>
+    <row r="6" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>2002</v>
       </c>
       <c r="B6" s="75"/>
       <c r="C6" s="77"/>
-    </row>
-    <row r="7" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="44"/>
+    </row>
+    <row r="7" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>2003</v>
       </c>
       <c r="B7" s="75"/>
       <c r="C7" s="77"/>
-    </row>
-    <row r="8" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="190"/>
+    </row>
+    <row r="8" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>2004</v>
       </c>
       <c r="B8" s="75"/>
       <c r="C8" s="77"/>
-    </row>
-    <row r="9" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="190"/>
+    </row>
+    <row r="9" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>2005</v>
       </c>
       <c r="B9" s="75"/>
       <c r="C9" s="77"/>
-    </row>
-    <row r="10" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="190"/>
+    </row>
+    <row r="10" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2006</v>
       </c>
       <c r="B10" s="75"/>
       <c r="C10" s="77"/>
-    </row>
-    <row r="11" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="190"/>
+    </row>
+    <row r="11" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2007</v>
       </c>
       <c r="B11" s="75"/>
       <c r="C11" s="77"/>
-    </row>
-    <row r="12" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="190"/>
+    </row>
+    <row r="12" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2008</v>
       </c>
       <c r="B12" s="75"/>
       <c r="C12" s="77"/>
-    </row>
-    <row r="13" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="190"/>
+    </row>
+    <row r="13" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2009</v>
       </c>
@@ -7834,83 +7942,127 @@
       <c r="C13" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="190"/>
+    </row>
+    <row r="14" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>2010</v>
       </c>
       <c r="B14" s="75"/>
       <c r="C14" s="77"/>
-    </row>
-    <row r="15" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="190"/>
+    </row>
+    <row r="15" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>2011</v>
       </c>
       <c r="B15" s="75"/>
       <c r="C15" s="77"/>
-    </row>
-    <row r="16" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="190"/>
+    </row>
+    <row r="16" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>2012</v>
       </c>
       <c r="B16" s="75"/>
       <c r="C16" s="77"/>
-    </row>
-    <row r="17" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="190"/>
+    </row>
+    <row r="17" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>2013</v>
       </c>
       <c r="B17" s="75"/>
       <c r="C17" s="77"/>
-    </row>
-    <row r="18" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="190"/>
+    </row>
+    <row r="18" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>2014</v>
       </c>
       <c r="B18" s="75"/>
       <c r="C18" s="77"/>
-    </row>
-    <row r="19" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="227">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>2015</v>
       </c>
       <c r="B19" s="75"/>
       <c r="C19" s="77"/>
-    </row>
-    <row r="20" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="227"/>
+    </row>
+    <row r="20" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2016</v>
       </c>
       <c r="B20" s="75"/>
       <c r="C20" s="77"/>
-    </row>
-    <row r="21" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="191"/>
+    </row>
+    <row r="21" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>2017</v>
       </c>
       <c r="B21" s="75"/>
       <c r="C21" s="77"/>
-    </row>
-    <row r="22" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="227"/>
+    </row>
+    <row r="22" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>2018</v>
       </c>
       <c r="B22" s="75"/>
       <c r="C22" s="77"/>
-    </row>
-    <row r="23" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="228"/>
+    </row>
+    <row r="23" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>2019</v>
       </c>
       <c r="B23" s="75"/>
       <c r="C23" s="77"/>
-    </row>
-    <row r="24" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="228"/>
+    </row>
+    <row r="24" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="63">
         <v>2020</v>
       </c>
       <c r="B24" s="78"/>
       <c r="C24" s="80"/>
+      <c r="D24" s="44"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="44"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="44"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="44"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="44"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="44"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="44"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="44"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="44"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="44"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated scripts and fixed bugs
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom.tidhar\Documents\GitHub\STI-HIV-coinfection\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="pars" sheetId="24" r:id="rId1"/>
@@ -14,9 +19,10 @@
     <sheet name="timepars" sheetId="28" r:id="rId5"/>
     <sheet name="scen_1" sheetId="25" r:id="rId6"/>
     <sheet name="scen_2" sheetId="26" r:id="rId7"/>
-    <sheet name="timepars_old" sheetId="20" r:id="rId8"/>
+    <sheet name="scen_3" sheetId="30" r:id="rId8"/>
+    <sheet name="timepars_old" sheetId="20" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -27,7 +33,7 @@
     <author>Michael Traeger</author>
   </authors>
   <commentList>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,10 +57,10 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="1">
+    <comment ref="C8" authorId="1" shapeId="0">
       <text/>
     </comment>
-    <comment ref="C11" authorId="1">
+    <comment ref="C11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0">
+    <comment ref="C18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +221,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1">
+    <comment ref="C1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -273,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1">
+    <comment ref="D1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="2">
+    <comment ref="N1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1">
+    <comment ref="O1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -375,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="2">
+    <comment ref="Q1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -399,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="2">
+    <comment ref="R1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -425,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="2">
+    <comment ref="T1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -449,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="2">
+    <comment ref="U1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -473,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="2">
+    <comment ref="V1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -497,7 +503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="2">
+    <comment ref="X1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="2">
+    <comment ref="Y1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -550,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="2">
+    <comment ref="Z1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -576,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="2">
+    <comment ref="AA1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -605,7 +611,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="2">
+    <comment ref="AB1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -631,7 +637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="2">
+    <comment ref="AC1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -655,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="2">
+    <comment ref="AD1" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -679,7 +685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF2" authorId="1">
+    <comment ref="AF2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -703,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="2">
+    <comment ref="Q8" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -727,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="2">
+    <comment ref="Q9" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -751,7 +757,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q12" authorId="0">
+    <comment ref="Q12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -779,7 +785,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE12" authorId="0">
+    <comment ref="AE12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -803,7 +809,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S13" authorId="2">
+    <comment ref="S13" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -827,7 +833,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="2">
+    <comment ref="A14" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -863,7 +869,7 @@
     <author>Kathleen Ryan</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -887,7 +893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -911,7 +917,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -935,7 +941,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -962,7 +968,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -986,7 +992,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1010,7 +1016,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1034,7 +1040,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1058,7 +1064,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1">
+    <comment ref="X1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1082,7 +1088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1106,7 +1112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1130,7 +1136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1154,7 +1160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1178,7 +1184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="1">
+    <comment ref="B3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1203,7 +1209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1227,7 +1233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0">
+    <comment ref="T3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1251,7 +1257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="1">
+    <comment ref="D18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1287,7 +1293,7 @@
     <author>Kathleen Ryan</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1311,7 +1317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1335,7 +1341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="1">
+    <comment ref="D3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1370,7 +1376,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1394,7 +1400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1428,7 +1434,7 @@
     <author>Tom Tidhar</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1452,7 +1458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1476,7 +1482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1524,7 +1530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1548,7 +1554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1572,7 +1578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1596,7 +1602,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1620,7 +1626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1644,7 +1650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AF1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1668,7 +1674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AG1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1692,7 +1698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1716,7 +1722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1740,7 +1746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1764,7 +1770,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1788,7 +1794,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="0">
+    <comment ref="T4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1812,7 +1818,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W4" authorId="0">
+    <comment ref="W4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1841,7 +1847,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="148">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2283,12 +2289,15 @@
   </si>
   <si>
     <t>annual_pop_growth</t>
+  </si>
+  <si>
+    <t>init_pop_int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -4382,10 +4391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,6 +4527,20 @@
         <v>90000</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="59">
+        <v>0</v>
+      </c>
+      <c r="C10" s="59">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="59">
+        <v>1500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4527,9 +4550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N6" sqref="N6:N13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6242,8 +6265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T1048576"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8023,7 +8046,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8286,6 +8309,345 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="159" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="159" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="161" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="161" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="163"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="74"/>
+    </row>
+    <row r="5" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>2001</v>
+      </c>
+      <c r="B5" s="165"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="77"/>
+    </row>
+    <row r="6" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>2002</v>
+      </c>
+      <c r="B6" s="165"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="77"/>
+    </row>
+    <row r="7" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>2003</v>
+      </c>
+      <c r="B7" s="165"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="77"/>
+    </row>
+    <row r="8" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>2004</v>
+      </c>
+      <c r="B8" s="165"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="77"/>
+    </row>
+    <row r="9" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>2005</v>
+      </c>
+      <c r="B9" s="165"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="77"/>
+    </row>
+    <row r="10" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>2006</v>
+      </c>
+      <c r="B10" s="165"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="77"/>
+    </row>
+    <row r="11" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
+        <v>2007</v>
+      </c>
+      <c r="B11" s="165"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="77"/>
+    </row>
+    <row r="12" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>2008</v>
+      </c>
+      <c r="B12" s="165"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="77"/>
+    </row>
+    <row r="13" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>2009</v>
+      </c>
+      <c r="B13" s="165"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="77"/>
+    </row>
+    <row r="14" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="210"/>
+      <c r="C14" s="211"/>
+      <c r="D14" s="210"/>
+      <c r="E14" s="211"/>
+    </row>
+    <row r="15" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="210"/>
+      <c r="C15" s="211"/>
+      <c r="D15" s="210"/>
+      <c r="E15" s="211"/>
+    </row>
+    <row r="16" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>2012</v>
+      </c>
+      <c r="B16" s="210"/>
+      <c r="C16" s="212"/>
+      <c r="D16" s="210"/>
+      <c r="E16" s="212"/>
+    </row>
+    <row r="17" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>2013</v>
+      </c>
+      <c r="B17" s="210"/>
+      <c r="C17" s="212"/>
+      <c r="D17" s="210"/>
+      <c r="E17" s="212"/>
+    </row>
+    <row r="18" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>2014</v>
+      </c>
+      <c r="B18" s="210"/>
+      <c r="C18" s="212"/>
+      <c r="D18" s="210"/>
+      <c r="E18" s="212"/>
+    </row>
+    <row r="19" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>2015</v>
+      </c>
+      <c r="B19" s="210"/>
+      <c r="C19" s="212"/>
+      <c r="D19" s="210"/>
+      <c r="E19" s="212"/>
+    </row>
+    <row r="20" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>2016</v>
+      </c>
+      <c r="B20" s="210"/>
+      <c r="C20" s="212"/>
+      <c r="D20" s="210"/>
+      <c r="E20" s="212"/>
+    </row>
+    <row r="21" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
+        <v>2017</v>
+      </c>
+      <c r="B21" s="210"/>
+      <c r="C21" s="212"/>
+      <c r="D21" s="210"/>
+      <c r="E21" s="212"/>
+    </row>
+    <row r="22" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
+        <v>2018</v>
+      </c>
+      <c r="B22" s="210"/>
+      <c r="C22" s="212"/>
+      <c r="D22" s="210"/>
+      <c r="E22" s="212"/>
+    </row>
+    <row r="23" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
+        <v>2019</v>
+      </c>
+      <c r="B23" s="163">
+        <v>0.25</v>
+      </c>
+      <c r="C23" s="74">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="163">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="74">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="44">
+        <v>2020</v>
+      </c>
+      <c r="B24" s="210">
+        <v>1</v>
+      </c>
+      <c r="C24" s="211">
+        <v>1</v>
+      </c>
+      <c r="D24" s="210">
+        <v>1</v>
+      </c>
+      <c r="E24" s="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="165"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="77"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="165"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="77"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="165"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="77"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="165"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="165"/>
+      <c r="E28" s="77"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="165"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="165"/>
+      <c r="E29" s="77"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="165"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="165"/>
+      <c r="E30" s="77"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="165"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="165"/>
+      <c r="E31" s="77"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="165"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="165"/>
+      <c r="E32" s="77"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="165"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="77"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="167"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="80"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL34"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added prop_test and manual calibration
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="calibration" sheetId="29" r:id="rId1"/>
@@ -1796,7 +1796,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="149">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2235,6 +2235,15 @@
   </si>
   <si>
     <t>t_test_mult</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Proportion testing</t>
+  </si>
+  <si>
+    <t>prop_test</t>
   </si>
 </sst>
 </file>
@@ -3858,11 +3867,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4022,6 +4029,20 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="59">
+        <v>0.7</v>
+      </c>
+      <c r="C12" s="59">
+        <v>0.999</v>
+      </c>
+      <c r="D12" s="59">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4032,7 +4053,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4506,6 +4527,23 @@
         <v>42714</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="44">
+        <v>1</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="56"/>
     </row>
@@ -4521,8 +4559,8 @@
   <dimension ref="A1:AF25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V7" sqref="J7:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,7 +4642,9 @@
       <c r="O1" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="P1" s="115"/>
+      <c r="P1" s="115" t="s">
+        <v>146</v>
+      </c>
       <c r="Q1" s="116" t="s">
         <v>59</v>
       </c>
@@ -8043,8 +8083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated to Michael's latest data_sti sheet
</commit_message>
<xml_diff>
--- a/data_sti.xlsx
+++ b/data_sti.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9780" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10200"/>
   </bookViews>
   <sheets>
     <sheet name="calibration" sheetId="29" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="scen_2" sheetId="26" r:id="rId7"/>
     <sheet name="timepars_old" sheetId="20" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -352,7 +352,21 @@
 It is assumed that 7.2% of MSM are HIV+ (see excel formula for this column)
 KR:
 Have updated this to the number of men living with HIV in VIC according to DHHS PLHIV dataset. Not restricted to MSM, but can cut 10% to drop non-MSM if needed.
-Will need to request the numbers officially from DHHS for publications? but dont need data request because aggregate needed only</t>
+Will need to request the numbers officially from DHHS for publications? but dont need data request because aggregate needed only
+MT: As Kat suggests above have cut by 10%
+original numbers here: 
+4216
+4491
+4470
+5059
+5306
+5615
+5899
+6205
+6554
+6864
+7224
+7509</t>
         </r>
       </text>
     </comment>
@@ -1071,7 +1085,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Kathleen Ryan:</t>
         </r>
@@ -1080,7 +1094,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 source: https://research.treasury.gov.au/external-paper/shaping-a-nation/</t>
@@ -1256,7 +1270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="1" shapeId="0">
+    <comment ref="D19" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1796,7 +1810,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="148">
   <si>
     <t>Waiting list</t>
   </si>
@@ -2235,9 +2249,6 @@
   </si>
   <si>
     <t>t_test_mult</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Proportion testing</t>
@@ -2256,7 +2267,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2374,19 +2385,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2449,7 +2447,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -2899,36 +2897,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -2959,82 +2927,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
         <color auto="1"/>
       </left>
       <right style="medium">
@@ -3162,7 +3055,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3381,20 +3274,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3417,26 +3299,26 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -3463,15 +3345,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3516,29 +3398,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3869,7 +3754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4031,7 +3918,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" s="59">
         <v>0.7</v>
@@ -4053,7 +3940,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A23" sqref="A23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4529,10 +4416,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="C23" s="44">
         <v>1</v>
@@ -4556,11 +4443,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF25"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V7" sqref="J7:V7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4639,12 +4526,10 @@
       <c r="N1" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="148" t="s">
+      <c r="O1" s="137" t="s">
         <v>105</v>
       </c>
-      <c r="P1" s="115" t="s">
-        <v>146</v>
-      </c>
+      <c r="P1" s="115"/>
       <c r="Q1" s="116" t="s">
         <v>59</v>
       </c>
@@ -4687,66 +4572,66 @@
       <c r="AD1" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="196" t="s">
+      <c r="AE1" s="185" t="s">
         <v>115</v>
       </c>
-      <c r="AF1" s="196" t="s">
+      <c r="AF1" s="185" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="199">
+      <c r="A2" s="188">
         <v>2006</v>
       </c>
-      <c r="B2" s="200"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="202"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="191"/>
       <c r="E2" s="103">
         <v>199</v>
       </c>
       <c r="F2" s="104">
         <v>186</v>
       </c>
-      <c r="G2" s="223">
+      <c r="G2" s="212">
         <v>13</v>
       </c>
-      <c r="H2" s="203">
+      <c r="H2" s="192">
         <v>81</v>
       </c>
-      <c r="I2" s="204">
+      <c r="I2" s="193">
         <v>105</v>
       </c>
-      <c r="J2" s="201">
+      <c r="J2" s="190">
         <v>6</v>
       </c>
-      <c r="K2" s="202">
+      <c r="K2" s="191">
         <v>7</v>
       </c>
-      <c r="L2" s="200">
-        <v>4216</v>
-      </c>
-      <c r="M2" s="201"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="205"/>
-      <c r="P2" s="206"/>
-      <c r="Q2" s="207"/>
-      <c r="R2" s="207"/>
-      <c r="S2" s="207"/>
-      <c r="T2" s="207"/>
-      <c r="U2" s="207"/>
-      <c r="V2" s="207"/>
-      <c r="W2" s="207"/>
-      <c r="X2" s="207"/>
-      <c r="Y2" s="207"/>
-      <c r="Z2" s="207"/>
-      <c r="AA2" s="207"/>
-      <c r="AB2" s="207"/>
-      <c r="AC2" s="207"/>
-      <c r="AD2" s="208"/>
-      <c r="AE2" s="192">
+      <c r="L2" s="219">
+        <v>3415</v>
+      </c>
+      <c r="M2" s="190"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="194"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="196"/>
+      <c r="R2" s="196"/>
+      <c r="S2" s="196"/>
+      <c r="T2" s="196"/>
+      <c r="U2" s="196"/>
+      <c r="V2" s="196"/>
+      <c r="W2" s="196"/>
+      <c r="X2" s="196"/>
+      <c r="Y2" s="196"/>
+      <c r="Z2" s="196"/>
+      <c r="AA2" s="196"/>
+      <c r="AB2" s="196"/>
+      <c r="AC2" s="196"/>
+      <c r="AD2" s="197"/>
+      <c r="AE2" s="181">
         <v>30713</v>
       </c>
-      <c r="AF2" s="192">
+      <c r="AF2" s="181">
         <v>30713</v>
       </c>
     </row>
@@ -4754,16 +4639,16 @@
       <c r="A3" s="10">
         <v>2007</v>
       </c>
-      <c r="B3" s="188"/>
-      <c r="C3" s="210"/>
-      <c r="D3" s="182"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="199"/>
+      <c r="D3" s="171"/>
       <c r="E3" s="103">
         <v>184</v>
       </c>
       <c r="F3" s="104">
         <v>167</v>
       </c>
-      <c r="G3" s="224">
+      <c r="G3" s="213">
         <v>17</v>
       </c>
       <c r="H3" s="103">
@@ -4772,18 +4657,18 @@
       <c r="I3" s="104">
         <v>98</v>
       </c>
-      <c r="J3" s="211">
+      <c r="J3" s="200">
         <v>7</v>
       </c>
       <c r="K3" s="105">
         <v>10</v>
       </c>
       <c r="L3" s="106">
-        <v>4491</v>
+        <v>3638</v>
       </c>
       <c r="M3" s="107"/>
       <c r="N3" s="108"/>
-      <c r="O3" s="149">
+      <c r="O3" s="138">
         <v>0.7</v>
       </c>
       <c r="P3" s="96"/>
@@ -4795,19 +4680,19 @@
       </c>
       <c r="S3" s="28">
         <f t="shared" ref="S3:S13" si="0">B3-T3</f>
-        <v>-4491</v>
+        <v>-3638</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ref="T3:T14" si="1">L3</f>
-        <v>4491</v>
+        <v>3638</v>
       </c>
       <c r="U3" s="33">
         <f>ROUND(Q3*S3,0)</f>
-        <v>-105</v>
+        <v>-85</v>
       </c>
       <c r="V3" s="33">
         <f t="shared" ref="V3" si="2">ROUND(R3*T3,0)</f>
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="W3" s="11">
         <v>1007</v>
@@ -4834,8 +4719,8 @@
         <v>113.70439800000001</v>
       </c>
       <c r="AD3" s="13"/>
-      <c r="AE3" s="198"/>
-      <c r="AF3" s="209">
+      <c r="AE3" s="187"/>
+      <c r="AF3" s="198">
         <f>AF2+532.4</f>
         <v>31245.4</v>
       </c>
@@ -4844,22 +4729,22 @@
       <c r="A4" s="10">
         <v>2008</v>
       </c>
-      <c r="B4" s="188">
+      <c r="B4" s="177">
         <f>SUM(C4:D4)</f>
-        <v>27007.800000000003</v>
-      </c>
-      <c r="C4" s="210">
+        <v>27913.800000000003</v>
+      </c>
+      <c r="C4" s="199">
         <f t="shared" ref="C4:C15" si="3">AF4-(D4+L4)</f>
-        <v>27007.800000000003</v>
-      </c>
-      <c r="D4" s="182"/>
-      <c r="E4" s="226">
+        <v>27913.800000000003</v>
+      </c>
+      <c r="D4" s="171"/>
+      <c r="E4" s="215">
         <v>181</v>
       </c>
       <c r="F4" s="104">
         <v>165</v>
       </c>
-      <c r="G4" s="224">
+      <c r="G4" s="213">
         <v>16</v>
       </c>
       <c r="H4" s="103">
@@ -4868,28 +4753,28 @@
       <c r="I4" s="104">
         <v>94</v>
       </c>
-      <c r="J4" s="211">
+      <c r="J4" s="200">
         <v>8</v>
       </c>
       <c r="K4" s="105">
         <v>8</v>
       </c>
-      <c r="L4" s="188">
-        <v>4770</v>
-      </c>
-      <c r="M4" s="192"/>
-      <c r="N4" s="182"/>
-      <c r="O4" s="150"/>
+      <c r="L4" s="177">
+        <v>3864</v>
+      </c>
+      <c r="M4" s="181"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="139"/>
       <c r="P4" s="97"/>
       <c r="Q4" s="40"/>
       <c r="R4" s="40"/>
       <c r="S4" s="28">
         <f t="shared" si="0"/>
-        <v>22237.800000000003</v>
+        <v>24049.800000000003</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" si="1"/>
-        <v>4770</v>
+        <v>3864</v>
       </c>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
@@ -4918,8 +4803,8 @@
         <v>104.106708</v>
       </c>
       <c r="AD4" s="13"/>
-      <c r="AE4" s="198"/>
-      <c r="AF4" s="209">
+      <c r="AE4" s="187"/>
+      <c r="AF4" s="198">
         <f t="shared" ref="AF4:AF7" si="7">AF3+532.4</f>
         <v>31777.800000000003</v>
       </c>
@@ -4928,22 +4813,22 @@
       <c r="A5" s="10">
         <v>2009</v>
       </c>
-      <c r="B5" s="188">
+      <c r="B5" s="177">
         <f t="shared" ref="B5:B15" si="8">SUM(C5:D5)</f>
-        <v>27251.200000000004</v>
-      </c>
-      <c r="C5" s="210">
+        <v>28212.200000000004</v>
+      </c>
+      <c r="C5" s="199">
         <f t="shared" si="3"/>
-        <v>27251.200000000004</v>
-      </c>
-      <c r="D5" s="182"/>
-      <c r="E5" s="225">
+        <v>28212.200000000004</v>
+      </c>
+      <c r="D5" s="171"/>
+      <c r="E5" s="214">
         <v>197</v>
       </c>
       <c r="F5" s="104">
         <v>183</v>
       </c>
-      <c r="G5" s="224">
+      <c r="G5" s="213">
         <v>14</v>
       </c>
       <c r="H5" s="103">
@@ -4952,28 +4837,28 @@
       <c r="I5" s="104">
         <v>98</v>
       </c>
-      <c r="J5" s="211">
+      <c r="J5" s="200">
         <v>7</v>
       </c>
       <c r="K5" s="105">
         <v>7</v>
       </c>
-      <c r="L5" s="188">
-        <v>5059</v>
-      </c>
-      <c r="M5" s="192"/>
-      <c r="N5" s="182"/>
-      <c r="O5" s="150"/>
+      <c r="L5" s="177">
+        <v>4098</v>
+      </c>
+      <c r="M5" s="181"/>
+      <c r="N5" s="171"/>
+      <c r="O5" s="139"/>
       <c r="P5" s="97"/>
       <c r="Q5" s="40"/>
       <c r="R5" s="40"/>
       <c r="S5" s="28">
         <f t="shared" si="0"/>
-        <v>22192.200000000004</v>
+        <v>24114.200000000004</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" si="1"/>
-        <v>5059</v>
+        <v>4098</v>
       </c>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
@@ -5002,8 +4887,8 @@
         <v>167.11272000000002</v>
       </c>
       <c r="AD5" s="14"/>
-      <c r="AE5" s="198"/>
-      <c r="AF5" s="209">
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="198">
         <f t="shared" si="7"/>
         <v>32310.200000000004</v>
       </c>
@@ -5012,15 +4897,15 @@
       <c r="A6" s="10">
         <v>2010</v>
       </c>
-      <c r="B6" s="188">
+      <c r="B6" s="177">
         <f t="shared" si="8"/>
-        <v>27536.600000000006</v>
-      </c>
-      <c r="C6" s="210">
+        <v>28544.600000000006</v>
+      </c>
+      <c r="C6" s="199">
         <f t="shared" si="3"/>
-        <v>26220.496600000006</v>
-      </c>
-      <c r="D6" s="183">
+        <v>27228.496600000006</v>
+      </c>
+      <c r="D6" s="172">
         <v>1316.1034</v>
       </c>
       <c r="E6" s="119">
@@ -5029,7 +4914,7 @@
       <c r="F6" s="104">
         <v>153</v>
       </c>
-      <c r="G6" s="224">
+      <c r="G6" s="213">
         <v>21</v>
       </c>
       <c r="H6" s="103">
@@ -5038,18 +4923,18 @@
       <c r="I6" s="104">
         <v>68</v>
       </c>
-      <c r="J6" s="211">
+      <c r="J6" s="200">
         <v>7</v>
       </c>
       <c r="K6" s="105">
         <v>14</v>
       </c>
-      <c r="L6" s="188">
-        <v>5306</v>
-      </c>
-      <c r="M6" s="192"/>
-      <c r="N6" s="182"/>
-      <c r="O6" s="149"/>
+      <c r="L6" s="177">
+        <v>4298</v>
+      </c>
+      <c r="M6" s="181"/>
+      <c r="N6" s="171"/>
+      <c r="O6" s="138"/>
       <c r="P6" s="97"/>
       <c r="Q6" s="40">
         <v>4.0273972602739724E-2</v>
@@ -5059,19 +4944,19 @@
       </c>
       <c r="S6" s="28">
         <f t="shared" si="0"/>
-        <v>22230.600000000006</v>
+        <v>24246.600000000006</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>5306</v>
+        <v>4298</v>
       </c>
       <c r="U6" s="32">
         <f t="shared" ref="U6:U12" si="9">ROUND(Q6*S6,0)</f>
-        <v>895</v>
+        <v>977</v>
       </c>
       <c r="V6" s="32">
         <f t="shared" ref="V6:V13" si="10">ROUND(R6*T6,0)</f>
-        <v>229</v>
+        <v>185</v>
       </c>
       <c r="W6" s="11">
         <v>1758</v>
@@ -5098,8 +4983,8 @@
         <v>198.50281199999998</v>
       </c>
       <c r="AD6" s="14"/>
-      <c r="AE6" s="198"/>
-      <c r="AF6" s="209">
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="198">
         <f t="shared" si="7"/>
         <v>32842.600000000006</v>
       </c>
@@ -5108,15 +4993,15 @@
       <c r="A7" s="10">
         <v>2011</v>
       </c>
-      <c r="B7" s="188">
+      <c r="B7" s="177">
         <f>SUM(C7:D7)</f>
-        <v>27760.000000000007</v>
-      </c>
-      <c r="C7" s="210">
+        <v>28827.000000000007</v>
+      </c>
+      <c r="C7" s="199">
         <f t="shared" si="3"/>
-        <v>26586.372400000007</v>
-      </c>
-      <c r="D7" s="183">
+        <v>27653.372400000007</v>
+      </c>
+      <c r="D7" s="172">
         <v>1173.6276</v>
       </c>
       <c r="E7" s="119">
@@ -5125,7 +5010,7 @@
       <c r="F7" s="104">
         <v>190</v>
       </c>
-      <c r="G7" s="224">
+      <c r="G7" s="213">
         <v>20</v>
       </c>
       <c r="H7" s="119">
@@ -5134,18 +5019,18 @@
       <c r="I7" s="121">
         <v>91</v>
       </c>
-      <c r="J7" s="212">
+      <c r="J7" s="201">
         <v>7</v>
       </c>
-      <c r="K7" s="213">
+      <c r="K7" s="202">
         <v>13</v>
       </c>
-      <c r="L7" s="188">
-        <v>5615</v>
-      </c>
-      <c r="M7" s="192"/>
-      <c r="N7" s="182"/>
-      <c r="O7" s="150"/>
+      <c r="L7" s="177">
+        <v>4548</v>
+      </c>
+      <c r="M7" s="181"/>
+      <c r="N7" s="171"/>
+      <c r="O7" s="139"/>
       <c r="P7" s="97"/>
       <c r="Q7" s="40">
         <v>3.7534246575342468E-2</v>
@@ -5155,19 +5040,19 @@
       </c>
       <c r="S7" s="28">
         <f t="shared" si="0"/>
-        <v>22145.000000000007</v>
+        <v>24279.000000000007</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" si="1"/>
-        <v>5615</v>
+        <v>4548</v>
       </c>
       <c r="U7" s="32">
         <f t="shared" si="9"/>
-        <v>831</v>
+        <v>911</v>
       </c>
       <c r="V7" s="32">
         <f t="shared" si="10"/>
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="W7" s="11">
         <v>1863</v>
@@ -5194,10 +5079,10 @@
         <v>210.35878200000002</v>
       </c>
       <c r="AD7" s="14"/>
-      <c r="AE7" s="192">
+      <c r="AE7" s="181">
         <v>33375</v>
       </c>
-      <c r="AF7" s="209">
+      <c r="AF7" s="198">
         <f t="shared" si="7"/>
         <v>33375.000000000007</v>
       </c>
@@ -5206,44 +5091,44 @@
       <c r="A8" s="10">
         <v>2012</v>
       </c>
-      <c r="B8" s="188">
+      <c r="B8" s="177">
         <f t="shared" si="8"/>
-        <v>28064.000000000007</v>
-      </c>
-      <c r="C8" s="210">
+        <v>29185.000000000007</v>
+      </c>
+      <c r="C8" s="199">
         <f t="shared" si="3"/>
-        <v>26959.744400000007</v>
-      </c>
-      <c r="D8" s="183">
+        <v>28080.744400000007</v>
+      </c>
+      <c r="D8" s="172">
         <v>1104.2556</v>
       </c>
-      <c r="E8" s="184">
+      <c r="E8" s="173">
         <v>206</v>
       </c>
-      <c r="F8" s="185">
+      <c r="F8" s="174">
         <v>172</v>
       </c>
-      <c r="G8" s="186">
+      <c r="G8" s="175">
         <v>34</v>
       </c>
-      <c r="H8" s="185">
+      <c r="H8" s="174">
         <v>101</v>
       </c>
-      <c r="I8" s="184">
+      <c r="I8" s="173">
         <v>71</v>
       </c>
-      <c r="J8" s="186">
+      <c r="J8" s="175">
         <v>10</v>
       </c>
-      <c r="K8" s="222">
+      <c r="K8" s="211">
         <v>24</v>
       </c>
-      <c r="L8" s="188">
-        <v>5899</v>
-      </c>
-      <c r="M8" s="192"/>
-      <c r="N8" s="182"/>
-      <c r="O8" s="149">
+      <c r="L8" s="177">
+        <v>4778</v>
+      </c>
+      <c r="M8" s="181"/>
+      <c r="N8" s="171"/>
+      <c r="O8" s="138">
         <v>0.91200000000000003</v>
       </c>
       <c r="P8" s="97"/>
@@ -5255,19 +5140,19 @@
       </c>
       <c r="S8" s="28">
         <f t="shared" si="0"/>
-        <v>22165.000000000007</v>
+        <v>24407.000000000007</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>5899</v>
+        <v>4778</v>
       </c>
       <c r="U8" s="32">
         <f t="shared" si="9"/>
-        <v>1081</v>
+        <v>1190</v>
       </c>
       <c r="V8" s="32">
         <f t="shared" si="10"/>
-        <v>318</v>
+        <v>257</v>
       </c>
       <c r="W8" s="11">
         <v>2436</v>
@@ -5294,8 +5179,8 @@
         <v>275.05850400000003</v>
       </c>
       <c r="AD8" s="14"/>
-      <c r="AE8" s="198"/>
-      <c r="AF8" s="198">
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="187">
         <f>AF7+588</f>
         <v>33963.000000000007</v>
       </c>
@@ -5304,44 +5189,44 @@
       <c r="A9" s="10">
         <v>2013</v>
       </c>
-      <c r="B9" s="188">
+      <c r="B9" s="177">
         <f t="shared" si="8"/>
-        <v>28346.000000000007</v>
-      </c>
-      <c r="C9" s="210">
+        <v>29525.000000000007</v>
+      </c>
+      <c r="C9" s="199">
         <f t="shared" si="3"/>
-        <v>27200.205800000007</v>
-      </c>
-      <c r="D9" s="183">
+        <v>28379.205800000007</v>
+      </c>
+      <c r="D9" s="172">
         <v>1145.7942</v>
       </c>
-      <c r="E9" s="184">
+      <c r="E9" s="173">
         <v>233</v>
       </c>
-      <c r="F9" s="185">
+      <c r="F9" s="174">
         <v>184</v>
       </c>
-      <c r="G9" s="186">
+      <c r="G9" s="175">
         <v>49</v>
       </c>
-      <c r="H9" s="185">
+      <c r="H9" s="174">
         <v>106</v>
       </c>
-      <c r="I9" s="184">
+      <c r="I9" s="173">
         <v>78</v>
       </c>
-      <c r="J9" s="186">
+      <c r="J9" s="175">
         <v>14</v>
       </c>
-      <c r="K9" s="222">
+      <c r="K9" s="211">
         <v>35</v>
       </c>
-      <c r="L9" s="188">
-        <v>6205</v>
-      </c>
-      <c r="M9" s="192"/>
-      <c r="N9" s="182"/>
-      <c r="O9" s="149"/>
+      <c r="L9" s="177">
+        <v>5026</v>
+      </c>
+      <c r="M9" s="181"/>
+      <c r="N9" s="171"/>
+      <c r="O9" s="138"/>
       <c r="P9" s="97"/>
       <c r="Q9" s="40">
         <v>5.2876712328767124E-2</v>
@@ -5351,19 +5236,19 @@
       </c>
       <c r="S9" s="28">
         <f t="shared" si="0"/>
-        <v>22141.000000000007</v>
+        <v>24499.000000000007</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" si="1"/>
-        <v>6205</v>
+        <v>5026</v>
       </c>
       <c r="U9" s="32">
         <f t="shared" si="9"/>
-        <v>1171</v>
+        <v>1295</v>
       </c>
       <c r="V9" s="32">
         <f t="shared" si="10"/>
-        <v>389</v>
+        <v>315</v>
       </c>
       <c r="W9" s="11">
         <v>2978</v>
@@ -5390,8 +5275,8 @@
         <v>336.25789200000003</v>
       </c>
       <c r="AD9" s="14"/>
-      <c r="AE9" s="198"/>
-      <c r="AF9" s="198">
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="187">
         <f t="shared" ref="AF9:AF15" si="11">AF8+588</f>
         <v>34551.000000000007</v>
       </c>
@@ -5400,44 +5285,44 @@
       <c r="A10" s="10">
         <v>2014</v>
       </c>
-      <c r="B10" s="188">
+      <c r="B10" s="177">
         <f t="shared" si="8"/>
-        <v>28585.000000000007</v>
-      </c>
-      <c r="C10" s="210">
+        <v>29830.000000000007</v>
+      </c>
+      <c r="C10" s="199">
         <f t="shared" si="3"/>
-        <v>27281.934400000006</v>
-      </c>
-      <c r="D10" s="183">
+        <v>28526.934400000006</v>
+      </c>
+      <c r="D10" s="172">
         <v>1303.0656000000001</v>
       </c>
-      <c r="E10" s="184">
+      <c r="E10" s="173">
         <v>235</v>
       </c>
-      <c r="F10" s="185">
+      <c r="F10" s="174">
         <v>200</v>
       </c>
-      <c r="G10" s="186">
+      <c r="G10" s="175">
         <v>35</v>
       </c>
-      <c r="H10" s="185">
+      <c r="H10" s="174">
         <v>133</v>
       </c>
-      <c r="I10" s="184">
+      <c r="I10" s="173">
         <v>67</v>
       </c>
-      <c r="J10" s="186">
+      <c r="J10" s="175">
         <v>25</v>
       </c>
-      <c r="K10" s="222">
+      <c r="K10" s="211">
         <v>10</v>
       </c>
-      <c r="L10" s="188">
-        <v>6554</v>
-      </c>
-      <c r="M10" s="192"/>
-      <c r="N10" s="182"/>
-      <c r="O10" s="149">
+      <c r="L10" s="177">
+        <v>5309</v>
+      </c>
+      <c r="M10" s="181"/>
+      <c r="N10" s="171"/>
+      <c r="O10" s="138">
         <v>0.88</v>
       </c>
       <c r="P10" s="97"/>
@@ -5449,19 +5334,19 @@
       </c>
       <c r="S10" s="28">
         <f t="shared" si="0"/>
-        <v>22031.000000000007</v>
+        <v>24521.000000000007</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>6554</v>
+        <v>5309</v>
       </c>
       <c r="U10" s="32">
         <f t="shared" si="9"/>
-        <v>1135</v>
+        <v>1263</v>
       </c>
       <c r="V10" s="32">
         <f t="shared" si="10"/>
-        <v>349</v>
+        <v>283</v>
       </c>
       <c r="W10" s="11">
         <v>3269</v>
@@ -5488,8 +5373,8 @@
         <v>369.11586600000004</v>
       </c>
       <c r="AD10" s="14"/>
-      <c r="AE10" s="198"/>
-      <c r="AF10" s="198">
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="187">
         <f t="shared" si="11"/>
         <v>35139.000000000007</v>
       </c>
@@ -5498,44 +5383,44 @@
       <c r="A11" s="10">
         <v>2015</v>
       </c>
-      <c r="B11" s="188">
+      <c r="B11" s="177">
         <f t="shared" si="8"/>
-        <v>28863.000000000007</v>
-      </c>
-      <c r="C11" s="210">
+        <v>30167.000000000007</v>
+      </c>
+      <c r="C11" s="199">
         <f t="shared" si="3"/>
-        <v>27407.579200000007</v>
-      </c>
-      <c r="D11" s="183">
+        <v>28711.579200000007</v>
+      </c>
+      <c r="D11" s="172">
         <v>1455.4208000000001</v>
       </c>
-      <c r="E11" s="184">
+      <c r="E11" s="173">
         <v>218</v>
       </c>
-      <c r="F11" s="185">
+      <c r="F11" s="174">
         <v>177</v>
       </c>
-      <c r="G11" s="186">
+      <c r="G11" s="175">
         <v>41</v>
       </c>
-      <c r="H11" s="185">
+      <c r="H11" s="174">
         <v>115</v>
       </c>
-      <c r="I11" s="184">
+      <c r="I11" s="173">
         <v>62</v>
       </c>
-      <c r="J11" s="186">
+      <c r="J11" s="175">
         <v>23</v>
       </c>
-      <c r="K11" s="222">
+      <c r="K11" s="211">
         <v>18</v>
       </c>
-      <c r="L11" s="188">
-        <v>6864</v>
-      </c>
-      <c r="M11" s="192"/>
-      <c r="N11" s="182"/>
-      <c r="O11" s="149">
+      <c r="L11" s="177">
+        <v>5560</v>
+      </c>
+      <c r="M11" s="181"/>
+      <c r="N11" s="171"/>
+      <c r="O11" s="138">
         <v>0.88</v>
       </c>
       <c r="P11" s="97"/>
@@ -5547,19 +5432,19 @@
       </c>
       <c r="S11" s="28">
         <f t="shared" si="0"/>
-        <v>21999.000000000007</v>
+        <v>24607.000000000007</v>
       </c>
       <c r="T11" s="28">
         <f t="shared" si="1"/>
-        <v>6864</v>
+        <v>5560</v>
       </c>
       <c r="U11" s="32">
         <f t="shared" si="9"/>
-        <v>1465</v>
+        <v>1638</v>
       </c>
       <c r="V11" s="32">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>374</v>
       </c>
       <c r="W11" s="11">
         <v>4865</v>
@@ -5586,8 +5471,8 @@
         <v>549.32661000000007</v>
       </c>
       <c r="AD11" s="14"/>
-      <c r="AE11" s="198"/>
-      <c r="AF11" s="198">
+      <c r="AE11" s="187"/>
+      <c r="AF11" s="187">
         <f t="shared" si="11"/>
         <v>35727.000000000007</v>
       </c>
@@ -5596,44 +5481,44 @@
       <c r="A12" s="10">
         <v>2016</v>
       </c>
-      <c r="B12" s="188">
+      <c r="B12" s="177">
         <f>SUM(C12:D12)</f>
-        <v>29091.000000000007</v>
-      </c>
-      <c r="C12" s="210">
+        <v>30464.000000000007</v>
+      </c>
+      <c r="C12" s="199">
         <f t="shared" si="3"/>
-        <v>27444.524200000007</v>
-      </c>
-      <c r="D12" s="183">
+        <v>28817.524200000007</v>
+      </c>
+      <c r="D12" s="172">
         <v>1646.4758000000002</v>
       </c>
-      <c r="E12" s="184">
+      <c r="E12" s="173">
         <v>244</v>
       </c>
-      <c r="F12" s="185">
+      <c r="F12" s="174">
         <v>180</v>
       </c>
-      <c r="G12" s="186">
+      <c r="G12" s="175">
         <v>64</v>
       </c>
-      <c r="H12" s="185">
+      <c r="H12" s="174">
         <v>102</v>
       </c>
-      <c r="I12" s="184">
+      <c r="I12" s="173">
         <v>78</v>
       </c>
-      <c r="J12" s="186">
+      <c r="J12" s="175">
         <v>32</v>
       </c>
-      <c r="K12" s="222">
+      <c r="K12" s="211">
         <v>32</v>
       </c>
-      <c r="L12" s="188">
-        <v>7224</v>
-      </c>
-      <c r="M12" s="192"/>
-      <c r="N12" s="182"/>
-      <c r="O12" s="149">
+      <c r="L12" s="177">
+        <v>5851</v>
+      </c>
+      <c r="M12" s="181"/>
+      <c r="N12" s="171"/>
+      <c r="O12" s="138">
         <v>0.89</v>
       </c>
       <c r="P12" s="97"/>
@@ -5645,19 +5530,19 @@
       </c>
       <c r="S12" s="28">
         <f t="shared" si="0"/>
-        <v>21867.000000000007</v>
+        <v>24613.000000000007</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>7224</v>
+        <v>5851</v>
       </c>
       <c r="U12" s="32">
         <f t="shared" si="9"/>
-        <v>1384</v>
+        <v>1558</v>
       </c>
       <c r="V12" s="32">
         <f t="shared" si="10"/>
-        <v>500</v>
+        <v>405</v>
       </c>
       <c r="W12" s="11">
         <v>6265</v>
@@ -5686,10 +5571,10 @@
       <c r="AD12" s="42">
         <v>0.18</v>
       </c>
-      <c r="AE12" s="192">
+      <c r="AE12" s="181">
         <v>36315</v>
       </c>
-      <c r="AF12" s="198">
+      <c r="AF12" s="187">
         <f t="shared" si="11"/>
         <v>36315.000000000007</v>
       </c>
@@ -5698,44 +5583,44 @@
       <c r="A13" s="10">
         <v>2017</v>
       </c>
-      <c r="B13" s="188">
+      <c r="B13" s="177">
         <f t="shared" si="8"/>
-        <v>29394.000000000011</v>
-      </c>
-      <c r="C13" s="210">
+        <v>30821.000000000011</v>
+      </c>
+      <c r="C13" s="199">
         <f t="shared" si="3"/>
-        <v>27511.781600000009</v>
-      </c>
-      <c r="D13" s="183">
+        <v>28938.781600000009</v>
+      </c>
+      <c r="D13" s="172">
         <v>1882.2184</v>
       </c>
-      <c r="E13" s="184">
+      <c r="E13" s="173">
         <v>207</v>
       </c>
-      <c r="F13" s="185">
+      <c r="F13" s="174">
         <v>147</v>
       </c>
-      <c r="G13" s="186">
+      <c r="G13" s="175">
         <v>60</v>
       </c>
-      <c r="H13" s="185">
+      <c r="H13" s="174">
         <v>74</v>
       </c>
-      <c r="I13" s="184">
+      <c r="I13" s="173">
         <v>73</v>
       </c>
-      <c r="J13" s="186">
+      <c r="J13" s="175">
         <v>27</v>
       </c>
-      <c r="K13" s="222">
+      <c r="K13" s="211">
         <v>33</v>
       </c>
-      <c r="L13" s="188">
-        <v>7509</v>
-      </c>
-      <c r="M13" s="192"/>
-      <c r="N13" s="182"/>
-      <c r="O13" s="150">
+      <c r="L13" s="177">
+        <v>6082</v>
+      </c>
+      <c r="M13" s="181"/>
+      <c r="N13" s="171"/>
+      <c r="O13" s="139">
         <v>0.9</v>
       </c>
       <c r="P13" s="97"/>
@@ -5748,16 +5633,16 @@
       </c>
       <c r="S13" s="28">
         <f t="shared" si="0"/>
-        <v>21885.000000000011</v>
+        <v>24739.000000000011</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>7509</v>
+        <v>6082</v>
       </c>
       <c r="U13" s="12"/>
       <c r="V13" s="32">
         <f t="shared" si="10"/>
-        <v>351</v>
+        <v>284</v>
       </c>
       <c r="W13" s="11">
         <v>7289</v>
@@ -5783,8 +5668,8 @@
         <f t="shared" si="6"/>
         <v>413.28630000000004</v>
       </c>
-      <c r="AE13" s="198"/>
-      <c r="AF13" s="198">
+      <c r="AE13" s="187"/>
+      <c r="AF13" s="187">
         <f>AF12+588</f>
         <v>36903.000000000007</v>
       </c>
@@ -5793,42 +5678,42 @@
       <c r="A14" s="10">
         <v>2018</v>
       </c>
-      <c r="B14" s="188">
+      <c r="B14" s="177">
         <f t="shared" si="8"/>
         <v>37491.000000000007</v>
       </c>
-      <c r="C14" s="210">
+      <c r="C14" s="199">
         <f t="shared" si="3"/>
         <v>35358.027200000004</v>
       </c>
-      <c r="D14" s="183">
+      <c r="D14" s="172">
         <v>2132.9728</v>
       </c>
-      <c r="E14" s="184">
+      <c r="E14" s="173">
         <v>174</v>
       </c>
-      <c r="F14" s="185">
+      <c r="F14" s="174">
         <v>120</v>
       </c>
-      <c r="G14" s="187">
+      <c r="G14" s="176">
         <v>54</v>
       </c>
-      <c r="H14" s="185">
+      <c r="H14" s="174">
         <v>60</v>
       </c>
-      <c r="I14" s="184">
+      <c r="I14" s="173">
         <v>60</v>
       </c>
-      <c r="J14" s="187">
+      <c r="J14" s="176">
         <v>19</v>
       </c>
-      <c r="K14" s="185">
+      <c r="K14" s="174">
         <v>35</v>
       </c>
-      <c r="L14" s="188"/>
-      <c r="M14" s="192"/>
-      <c r="N14" s="182"/>
-      <c r="O14" s="149">
+      <c r="L14" s="177"/>
+      <c r="M14" s="181"/>
+      <c r="N14" s="171"/>
+      <c r="O14" s="138">
         <v>0.9</v>
       </c>
       <c r="P14" s="123"/>
@@ -5836,8 +5721,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE14" s="197"/>
-      <c r="AF14" s="198">
+      <c r="AE14" s="186"/>
+      <c r="AF14" s="187">
         <f t="shared" si="11"/>
         <v>37491.000000000007</v>
       </c>
@@ -5846,20 +5731,26 @@
       <c r="A15" s="120">
         <v>2019</v>
       </c>
-      <c r="B15" s="188">
+      <c r="B15" s="177">
         <f t="shared" si="8"/>
         <v>38079.000000000007</v>
       </c>
-      <c r="C15" s="210">
+      <c r="C15" s="199">
         <f t="shared" si="3"/>
         <v>35727.806200000006</v>
       </c>
-      <c r="D15" s="183">
+      <c r="D15" s="172">
         <v>2351.1938</v>
       </c>
-      <c r="E15" s="119"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="122"/>
+      <c r="E15" s="119">
+        <v>196</v>
+      </c>
+      <c r="F15" s="121">
+        <v>101</v>
+      </c>
+      <c r="G15" s="122">
+        <v>95</v>
+      </c>
       <c r="H15" s="119"/>
       <c r="I15" s="121"/>
       <c r="J15" s="121"/>
@@ -5867,18 +5758,18 @@
       <c r="L15" s="106"/>
       <c r="M15" s="107"/>
       <c r="N15" s="108"/>
-      <c r="O15" s="151"/>
+      <c r="O15" s="140"/>
       <c r="P15" s="123"/>
-      <c r="AE15" s="198"/>
-      <c r="AF15" s="198">
+      <c r="AE15" s="187"/>
+      <c r="AF15" s="187">
         <f t="shared" si="11"/>
         <v>38079.000000000007</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G16" s="10"/>
-      <c r="H16" s="214"/>
-      <c r="I16" s="214"/>
+      <c r="H16" s="203"/>
+      <c r="I16" s="203"/>
       <c r="J16" s="120"/>
       <c r="K16" s="120"/>
       <c r="S16" s="124"/>
@@ -5956,6 +5847,21 @@
       <c r="D25" s="10"/>
       <c r="L25" s="43"/>
       <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L26" s="43"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L27" s="43"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L28" s="43"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L29" s="43"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L30" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5968,8 +5874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5985,7 +5891,7 @@
       <c r="D1" s="127" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="141" t="s">
+      <c r="E1" s="134" t="s">
         <v>110</v>
       </c>
       <c r="F1" s="127" t="s">
@@ -5995,176 +5901,176 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="129" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="130">
-        <v>1</v>
-      </c>
-      <c r="C2" s="131">
-        <v>1</v>
-      </c>
-      <c r="D2" s="131">
-        <v>1</v>
-      </c>
-      <c r="E2" s="146">
-        <v>1</v>
-      </c>
-      <c r="F2" s="131">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="130">
+        <v>2</v>
+      </c>
+      <c r="D2" s="130">
+        <v>2</v>
+      </c>
+      <c r="E2" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="132">
+        <v>0.5</v>
       </c>
       <c r="G2" s="132">
-        <v>1</v>
-      </c>
-      <c r="I2" s="230" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="220" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="230"/>
-      <c r="K2" s="230"/>
-      <c r="L2" s="230"/>
-      <c r="M2" s="230"/>
-      <c r="N2" s="230"/>
-      <c r="O2" s="230"/>
-      <c r="P2" s="230"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="133" t="s">
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
+      <c r="M2" s="220"/>
+      <c r="N2" s="220"/>
+      <c r="O2" s="220"/>
+      <c r="P2" s="220"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="131" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="134">
-        <v>1</v>
-      </c>
-      <c r="C3" s="135">
-        <v>1</v>
-      </c>
-      <c r="D3" s="135">
-        <v>1</v>
-      </c>
-      <c r="E3" s="144">
-        <v>1</v>
-      </c>
-      <c r="F3" s="135">
-        <v>1</v>
-      </c>
-      <c r="G3" s="136">
-        <v>1</v>
-      </c>
-      <c r="I3" s="230"/>
-      <c r="J3" s="230"/>
-      <c r="K3" s="230"/>
-      <c r="L3" s="230"/>
-      <c r="M3" s="230"/>
-      <c r="N3" s="230"/>
-      <c r="O3" s="230"/>
-      <c r="P3" s="230"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="133" t="s">
+      <c r="B3" s="130">
+        <v>2</v>
+      </c>
+      <c r="C3" s="130">
+        <v>2</v>
+      </c>
+      <c r="D3" s="130">
+        <v>2</v>
+      </c>
+      <c r="E3" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="220"/>
+      <c r="J3" s="220"/>
+      <c r="K3" s="220"/>
+      <c r="L3" s="220"/>
+      <c r="M3" s="220"/>
+      <c r="N3" s="220"/>
+      <c r="O3" s="220"/>
+      <c r="P3" s="220"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="134">
-        <v>1</v>
-      </c>
-      <c r="C4" s="135">
-        <v>1</v>
-      </c>
-      <c r="D4" s="135">
-        <v>1</v>
-      </c>
-      <c r="E4" s="144">
-        <v>1</v>
-      </c>
-      <c r="F4" s="135">
-        <v>1</v>
-      </c>
-      <c r="G4" s="136">
-        <v>1</v>
-      </c>
-      <c r="I4" s="230"/>
-      <c r="J4" s="230"/>
-      <c r="K4" s="230"/>
-      <c r="L4" s="230"/>
-      <c r="M4" s="230"/>
-      <c r="N4" s="230"/>
-      <c r="O4" s="230"/>
-      <c r="P4" s="230"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="142" t="s">
+      <c r="B4" s="130">
+        <v>2</v>
+      </c>
+      <c r="C4" s="130">
+        <v>2</v>
+      </c>
+      <c r="D4" s="130">
+        <v>2</v>
+      </c>
+      <c r="E4" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="220"/>
+      <c r="J4" s="220"/>
+      <c r="K4" s="220"/>
+      <c r="L4" s="220"/>
+      <c r="M4" s="220"/>
+      <c r="N4" s="220"/>
+      <c r="O4" s="220"/>
+      <c r="P4" s="220"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="135" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="143">
-        <v>1</v>
-      </c>
-      <c r="C5" s="144">
-        <v>1</v>
-      </c>
-      <c r="D5" s="144">
-        <v>1</v>
-      </c>
-      <c r="E5" s="144">
-        <v>1</v>
-      </c>
-      <c r="F5" s="144">
-        <v>1</v>
-      </c>
-      <c r="G5" s="145">
-        <v>1</v>
-      </c>
-      <c r="I5" s="230"/>
-      <c r="J5" s="230"/>
-      <c r="K5" s="230"/>
-      <c r="L5" s="230"/>
-      <c r="M5" s="230"/>
-      <c r="N5" s="230"/>
-      <c r="O5" s="230"/>
-      <c r="P5" s="230"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="133" t="s">
+      <c r="B5" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="136">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="130">
+        <v>2</v>
+      </c>
+      <c r="F5" s="130">
+        <v>2</v>
+      </c>
+      <c r="G5" s="130">
+        <v>2</v>
+      </c>
+      <c r="I5" s="220"/>
+      <c r="J5" s="220"/>
+      <c r="K5" s="220"/>
+      <c r="L5" s="220"/>
+      <c r="M5" s="220"/>
+      <c r="N5" s="220"/>
+      <c r="O5" s="220"/>
+      <c r="P5" s="220"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="134">
-        <v>1</v>
-      </c>
-      <c r="C6" s="135">
-        <v>1</v>
-      </c>
-      <c r="D6" s="135">
-        <v>1</v>
-      </c>
-      <c r="E6" s="144">
-        <v>1</v>
-      </c>
-      <c r="F6" s="135">
-        <v>1</v>
-      </c>
-      <c r="G6" s="136">
-        <v>1</v>
+      <c r="B6" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="130">
+        <v>2</v>
+      </c>
+      <c r="F6" s="130">
+        <v>2</v>
+      </c>
+      <c r="G6" s="130">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="133" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="138">
-        <v>1</v>
-      </c>
-      <c r="C7" s="139">
-        <v>1</v>
-      </c>
-      <c r="D7" s="139">
-        <v>1</v>
-      </c>
-      <c r="E7" s="147">
-        <v>1</v>
-      </c>
-      <c r="F7" s="139">
-        <v>1</v>
-      </c>
-      <c r="G7" s="140">
-        <v>1</v>
+      <c r="B7" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="130">
+        <v>2</v>
+      </c>
+      <c r="F7" s="130">
+        <v>2</v>
+      </c>
+      <c r="G7" s="130">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6180,8 +6086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6236,16 +6142,16 @@
       <c r="G1" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="162" t="s">
+      <c r="H1" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="163" t="s">
+      <c r="I1" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="162" t="s">
+      <c r="J1" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="152" t="s">
         <v>69</v>
       </c>
       <c r="L1" s="68" t="s">
@@ -6254,16 +6160,16 @@
       <c r="M1" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="162" t="s">
+      <c r="N1" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="163" t="s">
+      <c r="O1" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="162" t="s">
+      <c r="P1" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="163" t="s">
+      <c r="Q1" s="152" t="s">
         <v>69</v>
       </c>
       <c r="R1" s="68" t="s">
@@ -6290,7 +6196,7 @@
       <c r="Y1" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="Z1" s="229" t="s">
+      <c r="Z1" s="218" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6306,16 +6212,16 @@
       <c r="G2" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="164" t="s">
+      <c r="H2" s="153" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="165" t="s">
+      <c r="I2" s="154" t="s">
         <v>126</v>
       </c>
-      <c r="J2" s="164" t="s">
+      <c r="J2" s="153" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="165" t="s">
+      <c r="K2" s="154" t="s">
         <v>128</v>
       </c>
       <c r="L2" s="71" t="s">
@@ -6324,16 +6230,16 @@
       <c r="M2" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="164" t="s">
+      <c r="N2" s="153" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="165" t="s">
+      <c r="O2" s="154" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="164" t="s">
+      <c r="P2" s="153" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" s="165" t="s">
+      <c r="Q2" s="154" t="s">
         <v>128</v>
       </c>
       <c r="R2" s="71" t="s">
@@ -6378,22 +6284,22 @@
       <c r="L3" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="218" t="s">
+      <c r="M3" s="207" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="219" t="s">
+      <c r="N3" s="208" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="220" t="s">
+      <c r="O3" s="209" t="s">
         <v>98</v>
       </c>
-      <c r="P3" s="219" t="s">
+      <c r="P3" s="208" t="s">
         <v>98</v>
       </c>
-      <c r="Q3" s="220" t="s">
+      <c r="Q3" s="209" t="s">
         <v>98</v>
       </c>
-      <c r="R3" s="221" t="s">
+      <c r="R3" s="210" t="s">
         <v>98</v>
       </c>
       <c r="S3" s="70" t="s">
@@ -6436,20 +6342,20 @@
         <v>0.7</v>
       </c>
       <c r="G4" s="72"/>
-      <c r="H4" s="166"/>
-      <c r="I4" s="167"/>
-      <c r="J4" s="166"/>
-      <c r="K4" s="167">
+      <c r="H4" s="155"/>
+      <c r="I4" s="156"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="156">
         <v>0.25</v>
       </c>
       <c r="L4" s="74">
         <v>0.25</v>
       </c>
       <c r="M4" s="72"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="167"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167">
+      <c r="N4" s="155"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="155"/>
+      <c r="Q4" s="156">
         <v>0.25</v>
       </c>
       <c r="R4" s="74">
@@ -6483,16 +6389,16 @@
       <c r="E5" s="77"/>
       <c r="F5" s="62"/>
       <c r="G5" s="75"/>
-      <c r="H5" s="168"/>
-      <c r="I5" s="169"/>
-      <c r="J5" s="168"/>
-      <c r="K5" s="169"/>
+      <c r="H5" s="157"/>
+      <c r="I5" s="158"/>
+      <c r="J5" s="157"/>
+      <c r="K5" s="158"/>
       <c r="L5" s="77"/>
       <c r="M5" s="75"/>
-      <c r="N5" s="168"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="168"/>
-      <c r="Q5" s="169"/>
+      <c r="N5" s="157"/>
+      <c r="O5" s="158"/>
+      <c r="P5" s="157"/>
+      <c r="Q5" s="158"/>
       <c r="R5" s="77"/>
       <c r="S5" s="76"/>
       <c r="T5" s="77"/>
@@ -6512,16 +6418,16 @@
       <c r="E6" s="77"/>
       <c r="F6" s="62"/>
       <c r="G6" s="75"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="169"/>
-      <c r="J6" s="168"/>
-      <c r="K6" s="169"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="157"/>
+      <c r="K6" s="158"/>
       <c r="L6" s="77"/>
       <c r="M6" s="75"/>
-      <c r="N6" s="168"/>
-      <c r="O6" s="169"/>
-      <c r="P6" s="168"/>
-      <c r="Q6" s="169"/>
+      <c r="N6" s="157"/>
+      <c r="O6" s="158"/>
+      <c r="P6" s="157"/>
+      <c r="Q6" s="158"/>
       <c r="R6" s="77"/>
       <c r="S6" s="76"/>
       <c r="T6" s="77"/>
@@ -6535,7 +6441,7 @@
       <c r="A7" s="31">
         <v>2003</v>
       </c>
-      <c r="B7" s="190">
+      <c r="B7" s="179">
         <v>0.26</v>
       </c>
       <c r="C7" s="44"/>
@@ -6543,16 +6449,16 @@
       <c r="E7" s="77"/>
       <c r="F7" s="62"/>
       <c r="G7" s="75"/>
-      <c r="H7" s="168"/>
-      <c r="I7" s="169"/>
-      <c r="J7" s="168"/>
-      <c r="K7" s="169"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="157"/>
+      <c r="K7" s="158"/>
       <c r="L7" s="77"/>
       <c r="M7" s="75"/>
-      <c r="N7" s="168"/>
-      <c r="O7" s="169"/>
-      <c r="P7" s="168"/>
-      <c r="Q7" s="169"/>
+      <c r="N7" s="157"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="157"/>
+      <c r="Q7" s="158"/>
       <c r="R7" s="77"/>
       <c r="S7" s="76"/>
       <c r="T7" s="77"/>
@@ -6566,7 +6472,7 @@
       <c r="A8" s="31">
         <v>2004</v>
       </c>
-      <c r="B8" s="190">
+      <c r="B8" s="179">
         <v>0.24</v>
       </c>
       <c r="C8" s="44"/>
@@ -6574,16 +6480,16 @@
       <c r="E8" s="77"/>
       <c r="F8" s="62"/>
       <c r="G8" s="75"/>
-      <c r="H8" s="168"/>
-      <c r="I8" s="169"/>
-      <c r="J8" s="168"/>
-      <c r="K8" s="169"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="158"/>
+      <c r="J8" s="157"/>
+      <c r="K8" s="158"/>
       <c r="L8" s="77"/>
       <c r="M8" s="75"/>
-      <c r="N8" s="168"/>
-      <c r="O8" s="169"/>
-      <c r="P8" s="168"/>
-      <c r="Q8" s="169"/>
+      <c r="N8" s="157"/>
+      <c r="O8" s="158"/>
+      <c r="P8" s="157"/>
+      <c r="Q8" s="158"/>
       <c r="R8" s="77"/>
       <c r="S8" s="76"/>
       <c r="T8" s="77"/>
@@ -6597,7 +6503,7 @@
       <c r="A9" s="31">
         <v>2005</v>
       </c>
-      <c r="B9" s="190">
+      <c r="B9" s="179">
         <v>0.28000000000000003</v>
       </c>
       <c r="C9" s="44"/>
@@ -6605,16 +6511,16 @@
       <c r="E9" s="77"/>
       <c r="F9" s="62"/>
       <c r="G9" s="75"/>
-      <c r="H9" s="168"/>
-      <c r="I9" s="169"/>
-      <c r="J9" s="168"/>
-      <c r="K9" s="169"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="158"/>
+      <c r="J9" s="157"/>
+      <c r="K9" s="158"/>
       <c r="L9" s="77"/>
       <c r="M9" s="75"/>
-      <c r="N9" s="168"/>
-      <c r="O9" s="169"/>
-      <c r="P9" s="168"/>
-      <c r="Q9" s="169"/>
+      <c r="N9" s="157"/>
+      <c r="O9" s="158"/>
+      <c r="P9" s="157"/>
+      <c r="Q9" s="158"/>
       <c r="R9" s="77"/>
       <c r="S9" s="76"/>
       <c r="T9" s="77"/>
@@ -6628,7 +6534,7 @@
       <c r="A10" s="31">
         <v>2006</v>
       </c>
-      <c r="B10" s="190">
+      <c r="B10" s="179">
         <v>0.26</v>
       </c>
       <c r="C10" s="44"/>
@@ -6647,7 +6553,7 @@
       <c r="J10" s="75">
         <v>2.82</v>
       </c>
-      <c r="K10" s="169"/>
+      <c r="K10" s="158"/>
       <c r="L10" s="77"/>
       <c r="M10" s="75">
         <v>2.46</v>
@@ -6661,7 +6567,7 @@
       <c r="P10" s="75">
         <v>2.46</v>
       </c>
-      <c r="Q10" s="169"/>
+      <c r="Q10" s="158"/>
       <c r="R10" s="77"/>
       <c r="S10" s="76"/>
       <c r="T10" s="77"/>
@@ -6675,7 +6581,7 @@
       <c r="A11" s="31">
         <v>2007</v>
       </c>
-      <c r="B11" s="190">
+      <c r="B11" s="179">
         <v>0.26</v>
       </c>
       <c r="C11" s="44"/>
@@ -6694,7 +6600,7 @@
       <c r="J11" s="75">
         <v>3.06</v>
       </c>
-      <c r="K11" s="169"/>
+      <c r="K11" s="158"/>
       <c r="L11" s="77"/>
       <c r="M11" s="75">
         <v>2.77</v>
@@ -6708,7 +6614,7 @@
       <c r="P11" s="75">
         <v>2.77</v>
       </c>
-      <c r="Q11" s="169"/>
+      <c r="Q11" s="158"/>
       <c r="R11" s="77"/>
       <c r="S11" s="76">
         <v>0.75</v>
@@ -6726,7 +6632,7 @@
       <c r="A12" s="31">
         <v>2008</v>
       </c>
-      <c r="B12" s="190">
+      <c r="B12" s="179">
         <v>0.27</v>
       </c>
       <c r="C12" s="44"/>
@@ -6745,7 +6651,7 @@
       <c r="J12" s="75">
         <v>2.4300000000000002</v>
       </c>
-      <c r="K12" s="169"/>
+      <c r="K12" s="158"/>
       <c r="L12" s="77"/>
       <c r="M12" s="75">
         <v>2.91</v>
@@ -6759,7 +6665,7 @@
       <c r="P12" s="75">
         <v>2.91</v>
       </c>
-      <c r="Q12" s="169"/>
+      <c r="Q12" s="158"/>
       <c r="R12" s="77"/>
       <c r="S12" s="76"/>
       <c r="T12" s="77"/>
@@ -6773,11 +6679,11 @@
       <c r="A13" s="31">
         <v>2009</v>
       </c>
-      <c r="B13" s="190">
+      <c r="B13" s="179">
         <v>0.28999999999999998</v>
       </c>
       <c r="C13" s="44"/>
-      <c r="D13" s="189">
+      <c r="D13" s="178">
         <v>0</v>
       </c>
       <c r="F13" s="62"/>
@@ -6793,7 +6699,7 @@
       <c r="J13" s="75">
         <v>2.65</v>
       </c>
-      <c r="K13" s="169"/>
+      <c r="K13" s="158"/>
       <c r="L13" s="77"/>
       <c r="M13" s="75">
         <v>1.07</v>
@@ -6807,8 +6713,8 @@
       <c r="P13" s="75">
         <v>1.07</v>
       </c>
-      <c r="Q13" s="215"/>
-      <c r="R13" s="216"/>
+      <c r="Q13" s="204"/>
+      <c r="R13" s="205"/>
       <c r="S13" s="76"/>
       <c r="T13" s="77"/>
       <c r="U13" s="75"/>
@@ -6821,11 +6727,11 @@
       <c r="A14" s="31">
         <v>2010</v>
       </c>
-      <c r="B14" s="190">
+      <c r="B14" s="179">
         <v>0.32</v>
       </c>
       <c r="C14" s="44"/>
-      <c r="D14" s="189">
+      <c r="D14" s="178">
         <v>0</v>
       </c>
       <c r="F14" s="62"/>
@@ -6841,8 +6747,8 @@
       <c r="J14" s="75">
         <v>2.23</v>
       </c>
-      <c r="K14" s="215"/>
-      <c r="L14" s="216"/>
+      <c r="K14" s="204"/>
+      <c r="L14" s="205"/>
       <c r="M14" s="75">
         <v>2.71</v>
       </c>
@@ -6855,8 +6761,8 @@
       <c r="P14" s="75">
         <v>2.71</v>
       </c>
-      <c r="Q14" s="215"/>
-      <c r="R14" s="216"/>
+      <c r="Q14" s="204"/>
+      <c r="R14" s="205"/>
       <c r="S14" s="76">
         <v>0.75</v>
       </c>
@@ -6873,11 +6779,11 @@
       <c r="A15" s="31">
         <v>2011</v>
       </c>
-      <c r="B15" s="190">
+      <c r="B15" s="179">
         <v>0.31</v>
       </c>
       <c r="C15" s="44"/>
-      <c r="D15" s="189">
+      <c r="D15" s="178">
         <v>0</v>
       </c>
       <c r="F15" s="62"/>
@@ -6893,8 +6799,8 @@
       <c r="J15" s="75">
         <v>1.92</v>
       </c>
-      <c r="K15" s="215"/>
-      <c r="L15" s="216"/>
+      <c r="K15" s="204"/>
+      <c r="L15" s="205"/>
       <c r="M15" s="75">
         <v>1.92</v>
       </c>
@@ -6907,8 +6813,8 @@
       <c r="P15" s="75">
         <v>1.92</v>
       </c>
-      <c r="Q15" s="215"/>
-      <c r="R15" s="216"/>
+      <c r="Q15" s="204"/>
+      <c r="R15" s="205"/>
       <c r="S15" s="76"/>
       <c r="T15" s="77"/>
       <c r="U15" s="75"/>
@@ -6921,11 +6827,11 @@
       <c r="A16" s="31">
         <v>2012</v>
       </c>
-      <c r="B16" s="190">
+      <c r="B16" s="179">
         <v>0.28000000000000003</v>
       </c>
       <c r="C16" s="44"/>
-      <c r="D16" s="189">
+      <c r="D16" s="178">
         <v>0</v>
       </c>
       <c r="F16" s="62"/>
@@ -6941,8 +6847,8 @@
       <c r="J16" s="43">
         <v>1.91</v>
       </c>
-      <c r="K16" s="215"/>
-      <c r="L16" s="217"/>
+      <c r="K16" s="204"/>
+      <c r="L16" s="206"/>
       <c r="M16" s="43">
         <v>2.37</v>
       </c>
@@ -6955,7 +6861,7 @@
       <c r="P16" s="43">
         <v>2.37</v>
       </c>
-      <c r="Q16" s="215"/>
+      <c r="Q16" s="204"/>
       <c r="R16" s="77"/>
       <c r="S16" s="76">
         <v>0.82</v>
@@ -6973,11 +6879,11 @@
       <c r="A17" s="31">
         <v>2013</v>
       </c>
-      <c r="B17" s="190">
+      <c r="B17" s="179">
         <v>0.3</v>
       </c>
       <c r="C17" s="44"/>
-      <c r="D17" s="189">
+      <c r="D17" s="178">
         <v>0</v>
       </c>
       <c r="F17" s="62"/>
@@ -6993,8 +6899,8 @@
       <c r="J17" s="43">
         <v>2.34</v>
       </c>
-      <c r="K17" s="215"/>
-      <c r="L17" s="217"/>
+      <c r="K17" s="204"/>
+      <c r="L17" s="206"/>
       <c r="M17" s="43">
         <v>2.84</v>
       </c>
@@ -7007,7 +6913,7 @@
       <c r="P17" s="43">
         <v>2.84</v>
       </c>
-      <c r="Q17" s="215"/>
+      <c r="Q17" s="204"/>
       <c r="R17" s="77"/>
       <c r="S17" s="76">
         <v>0.86</v>
@@ -7025,14 +6931,14 @@
       <c r="A18" s="31">
         <v>2014</v>
       </c>
-      <c r="B18" s="227">
+      <c r="B18" s="216">
         <v>0.32297447280799113</v>
       </c>
       <c r="C18" s="44"/>
-      <c r="D18" s="189">
-        <v>143</v>
-      </c>
-      <c r="E18" s="191">
+      <c r="D18" s="178">
+        <v>0</v>
+      </c>
+      <c r="E18" s="180">
         <v>0</v>
       </c>
       <c r="F18" s="62"/>
@@ -7048,8 +6954,8 @@
       <c r="J18" s="43">
         <v>1.5</v>
       </c>
-      <c r="K18" s="215"/>
-      <c r="L18" s="217"/>
+      <c r="K18" s="204"/>
+      <c r="L18" s="206"/>
       <c r="M18" s="43">
         <v>0.96</v>
       </c>
@@ -7062,7 +6968,7 @@
       <c r="P18" s="43">
         <v>0.96</v>
       </c>
-      <c r="Q18" s="215"/>
+      <c r="Q18" s="204"/>
       <c r="R18" s="77"/>
       <c r="S18" s="76">
         <v>0.89</v>
@@ -7080,14 +6986,14 @@
       <c r="A19" s="31">
         <v>2015</v>
       </c>
-      <c r="B19" s="227">
+      <c r="B19" s="216">
         <v>0.35719557195571955</v>
       </c>
       <c r="C19" s="44"/>
-      <c r="D19" s="189">
+      <c r="D19" s="178">
         <v>143</v>
       </c>
-      <c r="E19" s="191">
+      <c r="E19" s="180">
         <v>0</v>
       </c>
       <c r="F19" s="62"/>
@@ -7103,8 +7009,8 @@
       <c r="J19" s="43">
         <v>2.08</v>
       </c>
-      <c r="K19" s="215"/>
-      <c r="L19" s="217"/>
+      <c r="K19" s="204"/>
+      <c r="L19" s="206"/>
       <c r="M19" s="43">
         <v>1.45</v>
       </c>
@@ -7117,7 +7023,7 @@
       <c r="P19" s="43">
         <v>1.45</v>
       </c>
-      <c r="Q19" s="215"/>
+      <c r="Q19" s="204"/>
       <c r="R19" s="77"/>
       <c r="S19" s="76">
         <v>0.92</v>
@@ -7135,14 +7041,14 @@
       <c r="A20" s="31">
         <v>2016</v>
       </c>
-      <c r="B20" s="191">
+      <c r="B20" s="180">
         <v>0.3888888888888889</v>
       </c>
       <c r="C20" s="44"/>
-      <c r="D20" s="189">
-        <v>2841</v>
-      </c>
-      <c r="E20" s="191">
+      <c r="D20" s="178">
+        <v>143</v>
+      </c>
+      <c r="E20" s="180">
         <f>data!D12*0.03</f>
         <v>49.394274000000003</v>
       </c>
@@ -7159,8 +7065,8 @@
       <c r="J20" s="43">
         <v>2.73</v>
       </c>
-      <c r="K20" s="215"/>
-      <c r="L20" s="217"/>
+      <c r="K20" s="204"/>
+      <c r="L20" s="206"/>
       <c r="M20" s="43">
         <v>2.5499999999999998</v>
       </c>
@@ -7173,7 +7079,7 @@
       <c r="P20" s="43">
         <v>2.5499999999999998</v>
       </c>
-      <c r="Q20" s="215"/>
+      <c r="Q20" s="204"/>
       <c r="R20" s="77"/>
       <c r="S20" s="76">
         <v>0.95</v>
@@ -7191,14 +7097,14 @@
       <c r="A21" s="31">
         <v>2017</v>
       </c>
-      <c r="B21" s="227">
+      <c r="B21" s="216">
         <v>0.49761417859577367</v>
       </c>
       <c r="C21" s="44"/>
-      <c r="D21" s="189">
-        <v>3727</v>
-      </c>
-      <c r="E21" s="191">
+      <c r="D21" s="178">
+        <v>2841</v>
+      </c>
+      <c r="E21" s="180">
         <f>data!D13*0.07</f>
         <v>131.75528800000001</v>
       </c>
@@ -7215,8 +7121,8 @@
       <c r="J21" s="43">
         <v>2.71</v>
       </c>
-      <c r="K21" s="215"/>
-      <c r="L21" s="217"/>
+      <c r="K21" s="204"/>
+      <c r="L21" s="206"/>
       <c r="M21" s="43">
         <v>2.23</v>
       </c>
@@ -7229,8 +7135,8 @@
       <c r="P21" s="43">
         <v>2.23</v>
       </c>
-      <c r="Q21" s="215"/>
-      <c r="R21" s="216"/>
+      <c r="Q21" s="204"/>
+      <c r="R21" s="205"/>
       <c r="S21" s="76"/>
       <c r="T21" s="77"/>
       <c r="U21" s="75"/>
@@ -7243,14 +7149,14 @@
       <c r="A22" s="31">
         <v>2018</v>
       </c>
-      <c r="B22" s="228">
+      <c r="B22" s="217">
         <v>0.53368660105980315</v>
       </c>
       <c r="C22" s="44"/>
-      <c r="D22" s="189">
-        <v>3995</v>
-      </c>
-      <c r="E22" s="191">
+      <c r="D22" s="178">
+        <v>3727</v>
+      </c>
+      <c r="E22" s="180">
         <f>data!D14*0.07</f>
         <v>149.30809600000001</v>
       </c>
@@ -7267,8 +7173,8 @@
       <c r="J22" s="43">
         <v>2.75</v>
       </c>
-      <c r="K22" s="215"/>
-      <c r="L22" s="217"/>
+      <c r="K22" s="204"/>
+      <c r="L22" s="206"/>
       <c r="M22" s="43">
         <v>2.2599999999999998</v>
       </c>
@@ -7281,7 +7187,7 @@
       <c r="P22" s="43">
         <v>2.2599999999999998</v>
       </c>
-      <c r="Q22" s="215"/>
+      <c r="Q22" s="204"/>
       <c r="R22" s="77"/>
       <c r="S22" s="76"/>
       <c r="T22" s="77"/>
@@ -7295,29 +7201,29 @@
       <c r="A23" s="31">
         <v>2019</v>
       </c>
-      <c r="B23" s="228">
+      <c r="B23" s="217">
         <v>0.59571788413098237</v>
       </c>
       <c r="C23" s="44"/>
-      <c r="D23" s="189">
-        <v>4525</v>
-      </c>
-      <c r="E23" s="191">
+      <c r="D23" s="178">
+        <v>3995</v>
+      </c>
+      <c r="E23" s="180">
         <f>data!D15*0.07</f>
         <v>164.58356600000002</v>
       </c>
       <c r="F23" s="62"/>
-      <c r="G23" s="193"/>
-      <c r="H23" s="194"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="194"/>
-      <c r="K23" s="215"/>
-      <c r="L23" s="217"/>
-      <c r="M23" s="193"/>
-      <c r="N23" s="194"/>
-      <c r="O23" s="195"/>
-      <c r="P23" s="194"/>
-      <c r="Q23" s="215"/>
+      <c r="G23" s="182"/>
+      <c r="H23" s="183"/>
+      <c r="I23" s="184"/>
+      <c r="J23" s="183"/>
+      <c r="K23" s="204"/>
+      <c r="L23" s="206"/>
+      <c r="M23" s="182"/>
+      <c r="N23" s="183"/>
+      <c r="O23" s="184"/>
+      <c r="P23" s="183"/>
+      <c r="Q23" s="204"/>
       <c r="R23" s="77"/>
       <c r="S23" s="76"/>
       <c r="T23" s="77"/>
@@ -7333,20 +7239,22 @@
       </c>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
-      <c r="D24" s="75"/>
+      <c r="D24" s="178">
+        <v>4525</v>
+      </c>
       <c r="E24" s="77"/>
       <c r="F24" s="62"/>
       <c r="G24" s="75"/>
-      <c r="H24" s="168"/>
-      <c r="I24" s="169"/>
-      <c r="J24" s="168"/>
-      <c r="K24" s="215"/>
-      <c r="L24" s="216"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="204"/>
+      <c r="L24" s="205"/>
       <c r="M24" s="75"/>
-      <c r="N24" s="168"/>
-      <c r="O24" s="169"/>
-      <c r="P24" s="168"/>
-      <c r="Q24" s="215"/>
+      <c r="N24" s="157"/>
+      <c r="O24" s="158"/>
+      <c r="P24" s="157"/>
+      <c r="Q24" s="204"/>
       <c r="R24" s="77"/>
       <c r="S24" s="76"/>
       <c r="T24" s="77"/>
@@ -7366,16 +7274,16 @@
       <c r="E25" s="77"/>
       <c r="F25" s="62"/>
       <c r="G25" s="75"/>
-      <c r="H25" s="168"/>
-      <c r="I25" s="169"/>
-      <c r="J25" s="168"/>
-      <c r="K25" s="169"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="157"/>
+      <c r="K25" s="158"/>
       <c r="L25" s="77"/>
       <c r="M25" s="75"/>
-      <c r="N25" s="168"/>
-      <c r="O25" s="169"/>
-      <c r="P25" s="168"/>
-      <c r="Q25" s="169"/>
+      <c r="N25" s="157"/>
+      <c r="O25" s="158"/>
+      <c r="P25" s="157"/>
+      <c r="Q25" s="158"/>
       <c r="R25" s="77"/>
       <c r="S25" s="76"/>
       <c r="T25" s="77"/>
@@ -7395,16 +7303,16 @@
       <c r="E26" s="77"/>
       <c r="F26" s="62"/>
       <c r="G26" s="75"/>
-      <c r="H26" s="168"/>
-      <c r="I26" s="169"/>
-      <c r="J26" s="168"/>
-      <c r="K26" s="169"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="158"/>
       <c r="L26" s="77"/>
       <c r="M26" s="75"/>
-      <c r="N26" s="168"/>
-      <c r="O26" s="169"/>
-      <c r="P26" s="168"/>
-      <c r="Q26" s="169"/>
+      <c r="N26" s="157"/>
+      <c r="O26" s="158"/>
+      <c r="P26" s="157"/>
+      <c r="Q26" s="158"/>
       <c r="R26" s="77"/>
       <c r="S26" s="76"/>
       <c r="T26" s="77"/>
@@ -7424,16 +7332,16 @@
       <c r="E27" s="77"/>
       <c r="F27" s="62"/>
       <c r="G27" s="75"/>
-      <c r="H27" s="168"/>
-      <c r="I27" s="169"/>
-      <c r="J27" s="168"/>
-      <c r="K27" s="169"/>
+      <c r="H27" s="157"/>
+      <c r="I27" s="158"/>
+      <c r="J27" s="157"/>
+      <c r="K27" s="158"/>
       <c r="L27" s="77"/>
       <c r="M27" s="75"/>
-      <c r="N27" s="168"/>
-      <c r="O27" s="169"/>
-      <c r="P27" s="168"/>
-      <c r="Q27" s="169"/>
+      <c r="N27" s="157"/>
+      <c r="O27" s="158"/>
+      <c r="P27" s="157"/>
+      <c r="Q27" s="158"/>
       <c r="R27" s="77"/>
       <c r="S27" s="76"/>
       <c r="T27" s="77"/>
@@ -7453,16 +7361,16 @@
       <c r="E28" s="77"/>
       <c r="F28" s="62"/>
       <c r="G28" s="75"/>
-      <c r="H28" s="168"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="168"/>
-      <c r="K28" s="169"/>
+      <c r="H28" s="157"/>
+      <c r="I28" s="158"/>
+      <c r="J28" s="157"/>
+      <c r="K28" s="158"/>
       <c r="L28" s="77"/>
       <c r="M28" s="75"/>
-      <c r="N28" s="168"/>
-      <c r="O28" s="169"/>
-      <c r="P28" s="168"/>
-      <c r="Q28" s="169"/>
+      <c r="N28" s="157"/>
+      <c r="O28" s="158"/>
+      <c r="P28" s="157"/>
+      <c r="Q28" s="158"/>
       <c r="R28" s="77"/>
       <c r="S28" s="76"/>
       <c r="T28" s="77"/>
@@ -7482,16 +7390,16 @@
       <c r="E29" s="77"/>
       <c r="F29" s="62"/>
       <c r="G29" s="75"/>
-      <c r="H29" s="168"/>
-      <c r="I29" s="169"/>
-      <c r="J29" s="168"/>
-      <c r="K29" s="169"/>
+      <c r="H29" s="157"/>
+      <c r="I29" s="158"/>
+      <c r="J29" s="157"/>
+      <c r="K29" s="158"/>
       <c r="L29" s="77"/>
       <c r="M29" s="75"/>
-      <c r="N29" s="168"/>
-      <c r="O29" s="169"/>
-      <c r="P29" s="168"/>
-      <c r="Q29" s="169"/>
+      <c r="N29" s="157"/>
+      <c r="O29" s="158"/>
+      <c r="P29" s="157"/>
+      <c r="Q29" s="158"/>
       <c r="R29" s="77"/>
       <c r="S29" s="76"/>
       <c r="T29" s="77"/>
@@ -7511,16 +7419,16 @@
       <c r="E30" s="77"/>
       <c r="F30" s="62"/>
       <c r="G30" s="75"/>
-      <c r="H30" s="168"/>
-      <c r="I30" s="169"/>
-      <c r="J30" s="168"/>
-      <c r="K30" s="169"/>
+      <c r="H30" s="157"/>
+      <c r="I30" s="158"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="158"/>
       <c r="L30" s="77"/>
       <c r="M30" s="75"/>
-      <c r="N30" s="168"/>
-      <c r="O30" s="169"/>
-      <c r="P30" s="168"/>
-      <c r="Q30" s="169"/>
+      <c r="N30" s="157"/>
+      <c r="O30" s="158"/>
+      <c r="P30" s="157"/>
+      <c r="Q30" s="158"/>
       <c r="R30" s="77"/>
       <c r="S30" s="76"/>
       <c r="T30" s="77"/>
@@ -7540,16 +7448,16 @@
       <c r="E31" s="77"/>
       <c r="F31" s="62"/>
       <c r="G31" s="75"/>
-      <c r="H31" s="168"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="168"/>
-      <c r="K31" s="169"/>
+      <c r="H31" s="157"/>
+      <c r="I31" s="158"/>
+      <c r="J31" s="157"/>
+      <c r="K31" s="158"/>
       <c r="L31" s="77"/>
       <c r="M31" s="75"/>
-      <c r="N31" s="168"/>
-      <c r="O31" s="169"/>
-      <c r="P31" s="168"/>
-      <c r="Q31" s="169"/>
+      <c r="N31" s="157"/>
+      <c r="O31" s="158"/>
+      <c r="P31" s="157"/>
+      <c r="Q31" s="158"/>
       <c r="R31" s="77"/>
       <c r="S31" s="76"/>
       <c r="T31" s="77"/>
@@ -7569,16 +7477,16 @@
       <c r="E32" s="77"/>
       <c r="F32" s="62"/>
       <c r="G32" s="75"/>
-      <c r="H32" s="168"/>
-      <c r="I32" s="169"/>
-      <c r="J32" s="168"/>
-      <c r="K32" s="169"/>
+      <c r="H32" s="157"/>
+      <c r="I32" s="158"/>
+      <c r="J32" s="157"/>
+      <c r="K32" s="158"/>
       <c r="L32" s="77"/>
       <c r="M32" s="75"/>
-      <c r="N32" s="168"/>
-      <c r="O32" s="169"/>
-      <c r="P32" s="168"/>
-      <c r="Q32" s="169"/>
+      <c r="N32" s="157"/>
+      <c r="O32" s="158"/>
+      <c r="P32" s="157"/>
+      <c r="Q32" s="158"/>
       <c r="R32" s="77"/>
       <c r="S32" s="76"/>
       <c r="T32" s="77"/>
@@ -7598,16 +7506,16 @@
       <c r="E33" s="77"/>
       <c r="F33" s="62"/>
       <c r="G33" s="75"/>
-      <c r="H33" s="168"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="168"/>
-      <c r="K33" s="169"/>
+      <c r="H33" s="157"/>
+      <c r="I33" s="158"/>
+      <c r="J33" s="157"/>
+      <c r="K33" s="158"/>
       <c r="L33" s="77"/>
       <c r="M33" s="75"/>
-      <c r="N33" s="168"/>
-      <c r="O33" s="169"/>
-      <c r="P33" s="168"/>
-      <c r="Q33" s="169"/>
+      <c r="N33" s="157"/>
+      <c r="O33" s="158"/>
+      <c r="P33" s="157"/>
+      <c r="Q33" s="158"/>
       <c r="R33" s="77"/>
       <c r="S33" s="76"/>
       <c r="T33" s="77"/>
@@ -7627,16 +7535,16 @@
       <c r="E34" s="80"/>
       <c r="F34" s="64"/>
       <c r="G34" s="78"/>
-      <c r="H34" s="170"/>
-      <c r="I34" s="171"/>
-      <c r="J34" s="170"/>
-      <c r="K34" s="171"/>
+      <c r="H34" s="159"/>
+      <c r="I34" s="160"/>
+      <c r="J34" s="159"/>
+      <c r="K34" s="160"/>
       <c r="L34" s="80"/>
       <c r="M34" s="78"/>
-      <c r="N34" s="170"/>
-      <c r="O34" s="171"/>
-      <c r="P34" s="170"/>
-      <c r="Q34" s="171"/>
+      <c r="N34" s="159"/>
+      <c r="O34" s="160"/>
+      <c r="P34" s="159"/>
+      <c r="Q34" s="160"/>
       <c r="R34" s="80"/>
       <c r="S34" s="79">
         <v>0.99</v>
@@ -7661,8 +7569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7864,8 +7772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8083,8 +7991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8144,16 +8052,16 @@
       <c r="G1" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="162" t="s">
+      <c r="H1" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="163" t="s">
+      <c r="I1" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="162" t="s">
+      <c r="J1" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="152" t="s">
         <v>69</v>
       </c>
       <c r="L1" s="68" t="s">
@@ -8180,10 +8088,10 @@
       <c r="S1" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="172" t="s">
+      <c r="T1" s="161" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="173" t="s">
+      <c r="U1" s="162" t="s">
         <v>92</v>
       </c>
       <c r="V1" s="82" t="s">
@@ -8198,10 +8106,10 @@
       <c r="Y1" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="152" t="s">
+      <c r="Z1" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="153" t="s">
+      <c r="AA1" s="142" t="s">
         <v>75</v>
       </c>
       <c r="AB1" s="82" t="s">
@@ -8250,16 +8158,16 @@
       <c r="G2" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="164" t="s">
+      <c r="H2" s="153" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="165" t="s">
+      <c r="I2" s="154" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="164" t="s">
+      <c r="J2" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="165" t="s">
+      <c r="K2" s="154" t="s">
         <v>72</v>
       </c>
       <c r="L2" s="71" t="s">
@@ -8276,10 +8184,10 @@
       <c r="S2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="174" t="s">
+      <c r="T2" s="163" t="s">
         <v>72</v>
       </c>
-      <c r="U2" s="175" t="s">
+      <c r="U2" s="164" t="s">
         <v>70</v>
       </c>
       <c r="V2" s="85" t="s">
@@ -8294,10 +8202,10 @@
       <c r="Y2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="Z2" s="154" t="s">
+      <c r="Z2" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="AA2" s="155" t="s">
+      <c r="AA2" s="144" t="s">
         <v>70</v>
       </c>
       <c r="AB2" s="85" t="s">
@@ -8344,16 +8252,16 @@
       <c r="G3" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="164" t="s">
+      <c r="H3" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="165" t="s">
+      <c r="I3" s="154" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="164" t="s">
+      <c r="J3" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="165" t="s">
+      <c r="K3" s="154" t="s">
         <v>73</v>
       </c>
       <c r="L3" s="71" t="s">
@@ -8380,10 +8288,10 @@
       <c r="S3" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="T3" s="174" t="s">
+      <c r="T3" s="163" t="s">
         <v>97</v>
       </c>
-      <c r="U3" s="175" t="s">
+      <c r="U3" s="164" t="s">
         <v>98</v>
       </c>
       <c r="V3" s="85" t="s">
@@ -8398,10 +8306,10 @@
       <c r="Y3" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="Z3" s="154" t="s">
+      <c r="Z3" s="143" t="s">
         <v>97</v>
       </c>
-      <c r="AA3" s="155" t="s">
+      <c r="AA3" s="144" t="s">
         <v>98</v>
       </c>
       <c r="AB3" s="85" t="s">
@@ -8442,16 +8350,16 @@
       <c r="G4" s="72">
         <v>1</v>
       </c>
-      <c r="H4" s="166">
+      <c r="H4" s="155">
         <v>10</v>
       </c>
-      <c r="I4" s="167">
+      <c r="I4" s="156">
         <v>0.5</v>
       </c>
-      <c r="J4" s="166">
+      <c r="J4" s="155">
         <v>4</v>
       </c>
-      <c r="K4" s="167">
+      <c r="K4" s="156">
         <f>3/12</f>
         <v>0.25</v>
       </c>
@@ -8476,10 +8384,10 @@
       <c r="S4" s="88">
         <v>1</v>
       </c>
-      <c r="T4" s="176">
+      <c r="T4" s="165">
         <v>0.03</v>
       </c>
-      <c r="U4" s="177">
+      <c r="U4" s="166">
         <v>1</v>
       </c>
       <c r="V4" s="88">
@@ -8494,10 +8402,10 @@
       <c r="Y4" s="88">
         <v>0</v>
       </c>
-      <c r="Z4" s="156">
+      <c r="Z4" s="145">
         <v>0</v>
       </c>
-      <c r="AA4" s="157">
+      <c r="AA4" s="146">
         <v>1</v>
       </c>
       <c r="AB4" s="88">
@@ -8544,10 +8452,10 @@
       <c r="E5" s="77"/>
       <c r="F5" s="62"/>
       <c r="G5" s="75"/>
-      <c r="H5" s="168"/>
-      <c r="I5" s="169"/>
-      <c r="J5" s="168"/>
-      <c r="K5" s="169"/>
+      <c r="H5" s="157"/>
+      <c r="I5" s="158"/>
+      <c r="J5" s="157"/>
+      <c r="K5" s="158"/>
       <c r="L5" s="77"/>
       <c r="M5" s="76"/>
       <c r="N5" s="77"/>
@@ -8556,14 +8464,14 @@
       <c r="Q5" s="77"/>
       <c r="R5" s="90"/>
       <c r="S5" s="91"/>
-      <c r="T5" s="178"/>
-      <c r="U5" s="179"/>
+      <c r="T5" s="167"/>
+      <c r="U5" s="168"/>
       <c r="V5" s="91"/>
       <c r="W5" s="92"/>
       <c r="X5" s="90"/>
       <c r="Y5" s="91"/>
-      <c r="Z5" s="158"/>
-      <c r="AA5" s="159"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="148"/>
       <c r="AB5" s="91"/>
       <c r="AC5" s="92"/>
       <c r="AD5" s="101"/>
@@ -8586,10 +8494,10 @@
       <c r="E6" s="77"/>
       <c r="F6" s="62"/>
       <c r="G6" s="75"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="169"/>
-      <c r="J6" s="168"/>
-      <c r="K6" s="169"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="157"/>
+      <c r="K6" s="158"/>
       <c r="L6" s="77"/>
       <c r="M6" s="76"/>
       <c r="N6" s="77"/>
@@ -8598,14 +8506,14 @@
       <c r="Q6" s="77"/>
       <c r="R6" s="90"/>
       <c r="S6" s="91"/>
-      <c r="T6" s="178"/>
-      <c r="U6" s="179"/>
+      <c r="T6" s="167"/>
+      <c r="U6" s="168"/>
       <c r="V6" s="91"/>
       <c r="W6" s="92"/>
       <c r="X6" s="90"/>
       <c r="Y6" s="91"/>
-      <c r="Z6" s="158"/>
-      <c r="AA6" s="159"/>
+      <c r="Z6" s="147"/>
+      <c r="AA6" s="148"/>
       <c r="AB6" s="91"/>
       <c r="AC6" s="92"/>
       <c r="AD6" s="101"/>
@@ -8628,10 +8536,10 @@
       <c r="E7" s="77"/>
       <c r="F7" s="62"/>
       <c r="G7" s="75"/>
-      <c r="H7" s="168"/>
-      <c r="I7" s="169"/>
-      <c r="J7" s="168"/>
-      <c r="K7" s="169"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="157"/>
+      <c r="K7" s="158"/>
       <c r="L7" s="77"/>
       <c r="M7" s="76"/>
       <c r="N7" s="77"/>
@@ -8640,14 +8548,14 @@
       <c r="Q7" s="77"/>
       <c r="R7" s="90"/>
       <c r="S7" s="91"/>
-      <c r="T7" s="178"/>
-      <c r="U7" s="179"/>
+      <c r="T7" s="167"/>
+      <c r="U7" s="168"/>
       <c r="V7" s="91"/>
       <c r="W7" s="92"/>
       <c r="X7" s="90"/>
       <c r="Y7" s="91"/>
-      <c r="Z7" s="158"/>
-      <c r="AA7" s="159"/>
+      <c r="Z7" s="147"/>
+      <c r="AA7" s="148"/>
       <c r="AB7" s="91"/>
       <c r="AC7" s="92"/>
       <c r="AD7" s="101"/>
@@ -8670,10 +8578,10 @@
       <c r="E8" s="77"/>
       <c r="F8" s="62"/>
       <c r="G8" s="75"/>
-      <c r="H8" s="168"/>
-      <c r="I8" s="169"/>
-      <c r="J8" s="168"/>
-      <c r="K8" s="169"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="158"/>
+      <c r="J8" s="157"/>
+      <c r="K8" s="158"/>
       <c r="L8" s="77"/>
       <c r="M8" s="76"/>
       <c r="N8" s="77"/>
@@ -8682,14 +8590,14 @@
       <c r="Q8" s="77"/>
       <c r="R8" s="90"/>
       <c r="S8" s="91"/>
-      <c r="T8" s="178"/>
-      <c r="U8" s="179"/>
+      <c r="T8" s="167"/>
+      <c r="U8" s="168"/>
       <c r="V8" s="91"/>
       <c r="W8" s="92"/>
       <c r="X8" s="90"/>
       <c r="Y8" s="91"/>
-      <c r="Z8" s="158"/>
-      <c r="AA8" s="159"/>
+      <c r="Z8" s="147"/>
+      <c r="AA8" s="148"/>
       <c r="AB8" s="91"/>
       <c r="AC8" s="92"/>
       <c r="AD8" s="101"/>
@@ -8712,10 +8620,10 @@
       <c r="E9" s="77"/>
       <c r="F9" s="62"/>
       <c r="G9" s="75"/>
-      <c r="H9" s="168"/>
-      <c r="I9" s="169"/>
-      <c r="J9" s="168"/>
-      <c r="K9" s="169"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="158"/>
+      <c r="J9" s="157"/>
+      <c r="K9" s="158"/>
       <c r="L9" s="77"/>
       <c r="M9" s="76"/>
       <c r="N9" s="77"/>
@@ -8724,14 +8632,14 @@
       <c r="Q9" s="77"/>
       <c r="R9" s="90"/>
       <c r="S9" s="91"/>
-      <c r="T9" s="178"/>
-      <c r="U9" s="179"/>
+      <c r="T9" s="167"/>
+      <c r="U9" s="168"/>
       <c r="V9" s="91"/>
       <c r="W9" s="92"/>
       <c r="X9" s="90"/>
       <c r="Y9" s="91"/>
-      <c r="Z9" s="158"/>
-      <c r="AA9" s="159"/>
+      <c r="Z9" s="147"/>
+      <c r="AA9" s="148"/>
       <c r="AB9" s="91"/>
       <c r="AC9" s="92"/>
       <c r="AD9" s="101"/>
@@ -8754,10 +8662,10 @@
       <c r="E10" s="77"/>
       <c r="F10" s="62"/>
       <c r="G10" s="75"/>
-      <c r="H10" s="168"/>
-      <c r="I10" s="169"/>
-      <c r="J10" s="168"/>
-      <c r="K10" s="169"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="157"/>
+      <c r="K10" s="158"/>
       <c r="L10" s="77"/>
       <c r="M10" s="76"/>
       <c r="N10" s="77"/>
@@ -8766,14 +8674,14 @@
       <c r="Q10" s="77"/>
       <c r="R10" s="90"/>
       <c r="S10" s="91"/>
-      <c r="T10" s="178"/>
-      <c r="U10" s="179"/>
+      <c r="T10" s="167"/>
+      <c r="U10" s="168"/>
       <c r="V10" s="91"/>
       <c r="W10" s="92"/>
       <c r="X10" s="90"/>
       <c r="Y10" s="91"/>
-      <c r="Z10" s="158"/>
-      <c r="AA10" s="159"/>
+      <c r="Z10" s="147"/>
+      <c r="AA10" s="148"/>
       <c r="AB10" s="91"/>
       <c r="AC10" s="92"/>
       <c r="AD10" s="101"/>
@@ -8796,10 +8704,10 @@
       <c r="E11" s="77"/>
       <c r="F11" s="62"/>
       <c r="G11" s="75"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="169"/>
-      <c r="J11" s="168"/>
-      <c r="K11" s="169"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="158"/>
+      <c r="J11" s="157"/>
+      <c r="K11" s="158"/>
       <c r="L11" s="77"/>
       <c r="M11" s="76">
         <v>0.75</v>
@@ -8812,14 +8720,14 @@
       <c r="Q11" s="77"/>
       <c r="R11" s="90"/>
       <c r="S11" s="91"/>
-      <c r="T11" s="178"/>
-      <c r="U11" s="179"/>
+      <c r="T11" s="167"/>
+      <c r="U11" s="168"/>
       <c r="V11" s="91"/>
       <c r="W11" s="92"/>
       <c r="X11" s="90"/>
       <c r="Y11" s="91"/>
-      <c r="Z11" s="158"/>
-      <c r="AA11" s="159"/>
+      <c r="Z11" s="147"/>
+      <c r="AA11" s="148"/>
       <c r="AB11" s="91"/>
       <c r="AC11" s="92"/>
       <c r="AD11" s="101"/>
@@ -8842,10 +8750,10 @@
       <c r="E12" s="77"/>
       <c r="F12" s="62"/>
       <c r="G12" s="75"/>
-      <c r="H12" s="168"/>
-      <c r="I12" s="169"/>
-      <c r="J12" s="168"/>
-      <c r="K12" s="169"/>
+      <c r="H12" s="157"/>
+      <c r="I12" s="158"/>
+      <c r="J12" s="157"/>
+      <c r="K12" s="158"/>
       <c r="L12" s="77"/>
       <c r="M12" s="76"/>
       <c r="N12" s="77"/>
@@ -8854,14 +8762,14 @@
       <c r="Q12" s="77"/>
       <c r="R12" s="90"/>
       <c r="S12" s="91"/>
-      <c r="T12" s="178"/>
-      <c r="U12" s="179"/>
+      <c r="T12" s="167"/>
+      <c r="U12" s="168"/>
       <c r="V12" s="91"/>
       <c r="W12" s="92"/>
       <c r="X12" s="90"/>
       <c r="Y12" s="91"/>
-      <c r="Z12" s="158"/>
-      <c r="AA12" s="159"/>
+      <c r="Z12" s="147"/>
+      <c r="AA12" s="148"/>
       <c r="AB12" s="91"/>
       <c r="AC12" s="92"/>
       <c r="AD12" s="101"/>
@@ -8886,10 +8794,10 @@
       <c r="E13" s="77"/>
       <c r="F13" s="62"/>
       <c r="G13" s="75"/>
-      <c r="H13" s="168"/>
-      <c r="I13" s="169"/>
-      <c r="J13" s="168"/>
-      <c r="K13" s="169"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="158"/>
+      <c r="J13" s="157"/>
+      <c r="K13" s="158"/>
       <c r="L13" s="77"/>
       <c r="M13" s="76"/>
       <c r="N13" s="77"/>
@@ -8898,14 +8806,14 @@
       <c r="Q13" s="77"/>
       <c r="R13" s="90"/>
       <c r="S13" s="91"/>
-      <c r="T13" s="178"/>
-      <c r="U13" s="179"/>
+      <c r="T13" s="167"/>
+      <c r="U13" s="168"/>
       <c r="V13" s="91"/>
       <c r="W13" s="92"/>
       <c r="X13" s="90"/>
       <c r="Y13" s="91"/>
-      <c r="Z13" s="158"/>
-      <c r="AA13" s="159"/>
+      <c r="Z13" s="147"/>
+      <c r="AA13" s="148"/>
       <c r="AB13" s="91"/>
       <c r="AC13" s="92"/>
       <c r="AD13" s="101"/>
@@ -8932,10 +8840,10 @@
       </c>
       <c r="F14" s="62"/>
       <c r="G14" s="75"/>
-      <c r="H14" s="168"/>
-      <c r="I14" s="169"/>
-      <c r="J14" s="168"/>
-      <c r="K14" s="169"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="158"/>
+      <c r="J14" s="157"/>
+      <c r="K14" s="158"/>
       <c r="L14" s="77"/>
       <c r="M14" s="76">
         <v>0.75</v>
@@ -8948,14 +8856,14 @@
       <c r="Q14" s="77"/>
       <c r="R14" s="90"/>
       <c r="S14" s="91"/>
-      <c r="T14" s="178"/>
-      <c r="U14" s="179"/>
+      <c r="T14" s="167"/>
+      <c r="U14" s="168"/>
       <c r="V14" s="91"/>
       <c r="W14" s="92"/>
       <c r="X14" s="90"/>
       <c r="Y14" s="91"/>
-      <c r="Z14" s="158"/>
-      <c r="AA14" s="159"/>
+      <c r="Z14" s="147"/>
+      <c r="AA14" s="148"/>
       <c r="AB14" s="91"/>
       <c r="AC14" s="92"/>
       <c r="AD14" s="101"/>
@@ -8980,10 +8888,10 @@
       </c>
       <c r="F15" s="62"/>
       <c r="G15" s="75"/>
-      <c r="H15" s="168"/>
-      <c r="I15" s="169"/>
-      <c r="J15" s="168"/>
-      <c r="K15" s="169"/>
+      <c r="H15" s="157"/>
+      <c r="I15" s="158"/>
+      <c r="J15" s="157"/>
+      <c r="K15" s="158"/>
       <c r="L15" s="77"/>
       <c r="M15" s="76"/>
       <c r="N15" s="77"/>
@@ -8992,14 +8900,14 @@
       <c r="Q15" s="77"/>
       <c r="R15" s="90"/>
       <c r="S15" s="91"/>
-      <c r="T15" s="178"/>
-      <c r="U15" s="179"/>
+      <c r="T15" s="167"/>
+      <c r="U15" s="168"/>
       <c r="V15" s="91"/>
       <c r="W15" s="92"/>
       <c r="X15" s="90"/>
       <c r="Y15" s="91"/>
-      <c r="Z15" s="158"/>
-      <c r="AA15" s="159"/>
+      <c r="Z15" s="147"/>
+      <c r="AA15" s="148"/>
       <c r="AB15" s="91"/>
       <c r="AC15" s="92"/>
       <c r="AD15" s="101"/>
@@ -9022,10 +8930,10 @@
       <c r="E16" s="77"/>
       <c r="F16" s="62"/>
       <c r="G16" s="75"/>
-      <c r="H16" s="168"/>
-      <c r="I16" s="169"/>
-      <c r="J16" s="168"/>
-      <c r="K16" s="169"/>
+      <c r="H16" s="157"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="157"/>
+      <c r="K16" s="158"/>
       <c r="L16" s="77"/>
       <c r="M16" s="76">
         <v>0.82</v>
@@ -9038,14 +8946,14 @@
       <c r="Q16" s="77"/>
       <c r="R16" s="90"/>
       <c r="S16" s="91"/>
-      <c r="T16" s="178"/>
-      <c r="U16" s="179"/>
+      <c r="T16" s="167"/>
+      <c r="U16" s="168"/>
       <c r="V16" s="91"/>
       <c r="W16" s="92"/>
       <c r="X16" s="90"/>
       <c r="Y16" s="91"/>
-      <c r="Z16" s="158"/>
-      <c r="AA16" s="159"/>
+      <c r="Z16" s="147"/>
+      <c r="AA16" s="148"/>
       <c r="AB16" s="91"/>
       <c r="AC16" s="92"/>
       <c r="AD16" s="101"/>
@@ -9068,10 +8976,10 @@
       <c r="E17" s="77"/>
       <c r="F17" s="62"/>
       <c r="G17" s="75"/>
-      <c r="H17" s="168"/>
-      <c r="I17" s="169"/>
-      <c r="J17" s="168"/>
-      <c r="K17" s="169"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="158"/>
+      <c r="J17" s="157"/>
+      <c r="K17" s="158"/>
       <c r="L17" s="77"/>
       <c r="M17" s="76">
         <v>0.86</v>
@@ -9084,14 +8992,14 @@
       <c r="Q17" s="77"/>
       <c r="R17" s="90"/>
       <c r="S17" s="91"/>
-      <c r="T17" s="178"/>
-      <c r="U17" s="179"/>
+      <c r="T17" s="167"/>
+      <c r="U17" s="168"/>
       <c r="V17" s="91"/>
       <c r="W17" s="92"/>
       <c r="X17" s="90"/>
       <c r="Y17" s="91"/>
-      <c r="Z17" s="158"/>
-      <c r="AA17" s="159"/>
+      <c r="Z17" s="147"/>
+      <c r="AA17" s="148"/>
       <c r="AB17" s="91"/>
       <c r="AC17" s="92"/>
       <c r="AD17" s="101"/>
@@ -9114,10 +9022,10 @@
       <c r="E18" s="77"/>
       <c r="F18" s="62"/>
       <c r="G18" s="75"/>
-      <c r="H18" s="168"/>
-      <c r="I18" s="169"/>
-      <c r="J18" s="168"/>
-      <c r="K18" s="169"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="158"/>
+      <c r="J18" s="157"/>
+      <c r="K18" s="158"/>
       <c r="L18" s="77"/>
       <c r="M18" s="76">
         <v>0.89</v>
@@ -9130,14 +9038,14 @@
       <c r="Q18" s="77"/>
       <c r="R18" s="90"/>
       <c r="S18" s="91"/>
-      <c r="T18" s="178"/>
-      <c r="U18" s="179"/>
+      <c r="T18" s="167"/>
+      <c r="U18" s="168"/>
       <c r="V18" s="91"/>
       <c r="W18" s="92"/>
       <c r="X18" s="90"/>
       <c r="Y18" s="91"/>
-      <c r="Z18" s="158"/>
-      <c r="AA18" s="159"/>
+      <c r="Z18" s="147"/>
+      <c r="AA18" s="148"/>
       <c r="AB18" s="91"/>
       <c r="AC18" s="92"/>
       <c r="AD18" s="101"/>
@@ -9160,10 +9068,10 @@
       <c r="E19" s="77"/>
       <c r="F19" s="62"/>
       <c r="G19" s="75"/>
-      <c r="H19" s="168"/>
-      <c r="I19" s="169"/>
-      <c r="J19" s="168"/>
-      <c r="K19" s="169"/>
+      <c r="H19" s="157"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="157"/>
+      <c r="K19" s="158"/>
       <c r="L19" s="77"/>
       <c r="M19" s="76">
         <v>0.92</v>
@@ -9176,14 +9084,14 @@
       <c r="Q19" s="77"/>
       <c r="R19" s="90"/>
       <c r="S19" s="91"/>
-      <c r="T19" s="178"/>
-      <c r="U19" s="179"/>
+      <c r="T19" s="167"/>
+      <c r="U19" s="168"/>
       <c r="V19" s="91"/>
       <c r="W19" s="92"/>
       <c r="X19" s="90"/>
       <c r="Y19" s="91"/>
-      <c r="Z19" s="158"/>
-      <c r="AA19" s="159"/>
+      <c r="Z19" s="147"/>
+      <c r="AA19" s="148"/>
       <c r="AB19" s="91"/>
       <c r="AC19" s="92"/>
       <c r="AD19" s="101"/>
@@ -9210,10 +9118,10 @@
       </c>
       <c r="F20" s="62"/>
       <c r="G20" s="75"/>
-      <c r="H20" s="168"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="168"/>
-      <c r="K20" s="169"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="158"/>
+      <c r="J20" s="157"/>
+      <c r="K20" s="158"/>
       <c r="L20" s="77"/>
       <c r="M20" s="76">
         <v>0.95</v>
@@ -9226,14 +9134,14 @@
       <c r="Q20" s="77"/>
       <c r="R20" s="90"/>
       <c r="S20" s="91"/>
-      <c r="T20" s="178"/>
-      <c r="U20" s="179"/>
+      <c r="T20" s="167"/>
+      <c r="U20" s="168"/>
       <c r="V20" s="91"/>
       <c r="W20" s="92"/>
       <c r="X20" s="90"/>
       <c r="Y20" s="91"/>
-      <c r="Z20" s="158"/>
-      <c r="AA20" s="159"/>
+      <c r="Z20" s="147"/>
+      <c r="AA20" s="148"/>
       <c r="AB20" s="91"/>
       <c r="AC20" s="92"/>
       <c r="AD20" s="101"/>
@@ -9256,10 +9164,10 @@
       <c r="E21" s="77"/>
       <c r="F21" s="62"/>
       <c r="G21" s="75"/>
-      <c r="H21" s="168"/>
-      <c r="I21" s="169"/>
-      <c r="J21" s="168"/>
-      <c r="K21" s="169"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="158"/>
+      <c r="J21" s="157"/>
+      <c r="K21" s="158"/>
       <c r="L21" s="77"/>
       <c r="M21" s="76"/>
       <c r="N21" s="77"/>
@@ -9268,14 +9176,14 @@
       <c r="Q21" s="77"/>
       <c r="R21" s="90"/>
       <c r="S21" s="91"/>
-      <c r="T21" s="178"/>
-      <c r="U21" s="179"/>
+      <c r="T21" s="167"/>
+      <c r="U21" s="168"/>
       <c r="V21" s="91"/>
       <c r="W21" s="92"/>
       <c r="X21" s="90"/>
       <c r="Y21" s="91"/>
-      <c r="Z21" s="158"/>
-      <c r="AA21" s="159"/>
+      <c r="Z21" s="147"/>
+      <c r="AA21" s="148"/>
       <c r="AB21" s="91"/>
       <c r="AC21" s="92"/>
       <c r="AD21" s="101"/>
@@ -9298,10 +9206,10 @@
       <c r="E22" s="77"/>
       <c r="F22" s="62"/>
       <c r="G22" s="75"/>
-      <c r="H22" s="168"/>
-      <c r="I22" s="169"/>
-      <c r="J22" s="168"/>
-      <c r="K22" s="169"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="158"/>
+      <c r="J22" s="157"/>
+      <c r="K22" s="158"/>
       <c r="L22" s="77"/>
       <c r="M22" s="76"/>
       <c r="N22" s="77"/>
@@ -9310,14 +9218,14 @@
       <c r="Q22" s="77"/>
       <c r="R22" s="90"/>
       <c r="S22" s="91"/>
-      <c r="T22" s="178"/>
-      <c r="U22" s="179"/>
+      <c r="T22" s="167"/>
+      <c r="U22" s="168"/>
       <c r="V22" s="91"/>
       <c r="W22" s="92"/>
       <c r="X22" s="90"/>
       <c r="Y22" s="91"/>
-      <c r="Z22" s="158"/>
-      <c r="AA22" s="159"/>
+      <c r="Z22" s="147"/>
+      <c r="AA22" s="148"/>
       <c r="AB22" s="91"/>
       <c r="AC22" s="92"/>
       <c r="AD22" s="101"/>
@@ -9340,10 +9248,10 @@
       <c r="E23" s="77"/>
       <c r="F23" s="62"/>
       <c r="G23" s="75"/>
-      <c r="H23" s="168"/>
-      <c r="I23" s="169"/>
-      <c r="J23" s="168"/>
-      <c r="K23" s="169"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="158"/>
+      <c r="J23" s="157"/>
+      <c r="K23" s="158"/>
       <c r="L23" s="77"/>
       <c r="M23" s="76"/>
       <c r="N23" s="77"/>
@@ -9352,14 +9260,14 @@
       <c r="Q23" s="77"/>
       <c r="R23" s="90"/>
       <c r="S23" s="91"/>
-      <c r="T23" s="178"/>
-      <c r="U23" s="179"/>
+      <c r="T23" s="167"/>
+      <c r="U23" s="168"/>
       <c r="V23" s="91"/>
       <c r="W23" s="92"/>
       <c r="X23" s="90"/>
       <c r="Y23" s="91"/>
-      <c r="Z23" s="158"/>
-      <c r="AA23" s="159"/>
+      <c r="Z23" s="147"/>
+      <c r="AA23" s="148"/>
       <c r="AB23" s="91"/>
       <c r="AC23" s="92"/>
       <c r="AD23" s="101"/>
@@ -9382,10 +9290,10 @@
       <c r="E24" s="77"/>
       <c r="F24" s="62"/>
       <c r="G24" s="75"/>
-      <c r="H24" s="168"/>
-      <c r="I24" s="169"/>
-      <c r="J24" s="168"/>
-      <c r="K24" s="169"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="158"/>
       <c r="L24" s="77"/>
       <c r="M24" s="76"/>
       <c r="N24" s="77"/>
@@ -9394,14 +9302,14 @@
       <c r="Q24" s="77"/>
       <c r="R24" s="90"/>
       <c r="S24" s="91"/>
-      <c r="T24" s="178"/>
-      <c r="U24" s="179"/>
+      <c r="T24" s="167"/>
+      <c r="U24" s="168"/>
       <c r="V24" s="91"/>
       <c r="W24" s="92"/>
       <c r="X24" s="90"/>
       <c r="Y24" s="91"/>
-      <c r="Z24" s="158"/>
-      <c r="AA24" s="159"/>
+      <c r="Z24" s="147"/>
+      <c r="AA24" s="148"/>
       <c r="AB24" s="91"/>
       <c r="AC24" s="92"/>
       <c r="AD24" s="101"/>
@@ -9424,10 +9332,10 @@
       <c r="E25" s="77"/>
       <c r="F25" s="62"/>
       <c r="G25" s="75"/>
-      <c r="H25" s="168"/>
-      <c r="I25" s="169"/>
-      <c r="J25" s="168"/>
-      <c r="K25" s="169"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="157"/>
+      <c r="K25" s="158"/>
       <c r="L25" s="77"/>
       <c r="M25" s="76"/>
       <c r="N25" s="77"/>
@@ -9436,14 +9344,14 @@
       <c r="Q25" s="77"/>
       <c r="R25" s="90"/>
       <c r="S25" s="91"/>
-      <c r="T25" s="178"/>
-      <c r="U25" s="179"/>
+      <c r="T25" s="167"/>
+      <c r="U25" s="168"/>
       <c r="V25" s="91"/>
       <c r="W25" s="92"/>
       <c r="X25" s="90"/>
       <c r="Y25" s="91"/>
-      <c r="Z25" s="158"/>
-      <c r="AA25" s="159"/>
+      <c r="Z25" s="147"/>
+      <c r="AA25" s="148"/>
       <c r="AB25" s="91"/>
       <c r="AC25" s="92"/>
       <c r="AD25" s="101"/>
@@ -9466,10 +9374,10 @@
       <c r="E26" s="77"/>
       <c r="F26" s="62"/>
       <c r="G26" s="75"/>
-      <c r="H26" s="168"/>
-      <c r="I26" s="169"/>
-      <c r="J26" s="168"/>
-      <c r="K26" s="169"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="158"/>
       <c r="L26" s="77"/>
       <c r="M26" s="76"/>
       <c r="N26" s="77"/>
@@ -9478,14 +9386,14 @@
       <c r="Q26" s="77"/>
       <c r="R26" s="90"/>
       <c r="S26" s="91"/>
-      <c r="T26" s="178"/>
-      <c r="U26" s="179"/>
+      <c r="T26" s="167"/>
+      <c r="U26" s="168"/>
       <c r="V26" s="91"/>
       <c r="W26" s="92"/>
       <c r="X26" s="90"/>
       <c r="Y26" s="91"/>
-      <c r="Z26" s="158"/>
-      <c r="AA26" s="159"/>
+      <c r="Z26" s="147"/>
+      <c r="AA26" s="148"/>
       <c r="AB26" s="91"/>
       <c r="AC26" s="92"/>
       <c r="AD26" s="101"/>
@@ -9508,10 +9416,10 @@
       <c r="E27" s="77"/>
       <c r="F27" s="62"/>
       <c r="G27" s="75"/>
-      <c r="H27" s="168"/>
-      <c r="I27" s="169"/>
-      <c r="J27" s="168"/>
-      <c r="K27" s="169"/>
+      <c r="H27" s="157"/>
+      <c r="I27" s="158"/>
+      <c r="J27" s="157"/>
+      <c r="K27" s="158"/>
       <c r="L27" s="77"/>
       <c r="M27" s="76"/>
       <c r="N27" s="77"/>
@@ -9520,14 +9428,14 @@
       <c r="Q27" s="77"/>
       <c r="R27" s="90"/>
       <c r="S27" s="91"/>
-      <c r="T27" s="178"/>
-      <c r="U27" s="179"/>
+      <c r="T27" s="167"/>
+      <c r="U27" s="168"/>
       <c r="V27" s="91"/>
       <c r="W27" s="92"/>
       <c r="X27" s="90"/>
       <c r="Y27" s="91"/>
-      <c r="Z27" s="158"/>
-      <c r="AA27" s="159"/>
+      <c r="Z27" s="147"/>
+      <c r="AA27" s="148"/>
       <c r="AB27" s="91"/>
       <c r="AC27" s="92"/>
       <c r="AD27" s="101"/>
@@ -9550,10 +9458,10 @@
       <c r="E28" s="77"/>
       <c r="F28" s="62"/>
       <c r="G28" s="75"/>
-      <c r="H28" s="168"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="168"/>
-      <c r="K28" s="169"/>
+      <c r="H28" s="157"/>
+      <c r="I28" s="158"/>
+      <c r="J28" s="157"/>
+      <c r="K28" s="158"/>
       <c r="L28" s="77"/>
       <c r="M28" s="76"/>
       <c r="N28" s="77"/>
@@ -9562,14 +9470,14 @@
       <c r="Q28" s="77"/>
       <c r="R28" s="90"/>
       <c r="S28" s="91"/>
-      <c r="T28" s="178"/>
-      <c r="U28" s="179"/>
+      <c r="T28" s="167"/>
+      <c r="U28" s="168"/>
       <c r="V28" s="91"/>
       <c r="W28" s="92"/>
       <c r="X28" s="90"/>
       <c r="Y28" s="91"/>
-      <c r="Z28" s="158"/>
-      <c r="AA28" s="159"/>
+      <c r="Z28" s="147"/>
+      <c r="AA28" s="148"/>
       <c r="AB28" s="91"/>
       <c r="AC28" s="92"/>
       <c r="AD28" s="101"/>
@@ -9592,10 +9500,10 @@
       <c r="E29" s="77"/>
       <c r="F29" s="62"/>
       <c r="G29" s="75"/>
-      <c r="H29" s="168"/>
-      <c r="I29" s="169"/>
-      <c r="J29" s="168"/>
-      <c r="K29" s="169"/>
+      <c r="H29" s="157"/>
+      <c r="I29" s="158"/>
+      <c r="J29" s="157"/>
+      <c r="K29" s="158"/>
       <c r="L29" s="77"/>
       <c r="M29" s="76">
         <v>0.95</v>
@@ -9608,14 +9516,14 @@
       <c r="Q29" s="77"/>
       <c r="R29" s="90"/>
       <c r="S29" s="91"/>
-      <c r="T29" s="178"/>
-      <c r="U29" s="179"/>
+      <c r="T29" s="167"/>
+      <c r="U29" s="168"/>
       <c r="V29" s="91"/>
       <c r="W29" s="92"/>
       <c r="X29" s="90"/>
       <c r="Y29" s="91"/>
-      <c r="Z29" s="158"/>
-      <c r="AA29" s="159"/>
+      <c r="Z29" s="147"/>
+      <c r="AA29" s="148"/>
       <c r="AB29" s="91"/>
       <c r="AC29" s="92"/>
       <c r="AD29" s="101"/>
@@ -9638,10 +9546,10 @@
       <c r="E30" s="77"/>
       <c r="F30" s="62"/>
       <c r="G30" s="75"/>
-      <c r="H30" s="168"/>
-      <c r="I30" s="169"/>
-      <c r="J30" s="168"/>
-      <c r="K30" s="169"/>
+      <c r="H30" s="157"/>
+      <c r="I30" s="158"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="158"/>
       <c r="L30" s="77"/>
       <c r="M30" s="76"/>
       <c r="N30" s="77"/>
@@ -9650,14 +9558,14 @@
       <c r="Q30" s="77"/>
       <c r="R30" s="90"/>
       <c r="S30" s="91"/>
-      <c r="T30" s="178"/>
-      <c r="U30" s="179"/>
+      <c r="T30" s="167"/>
+      <c r="U30" s="168"/>
       <c r="V30" s="91"/>
       <c r="W30" s="92"/>
       <c r="X30" s="90"/>
       <c r="Y30" s="91"/>
-      <c r="Z30" s="158"/>
-      <c r="AA30" s="159"/>
+      <c r="Z30" s="147"/>
+      <c r="AA30" s="148"/>
       <c r="AB30" s="91"/>
       <c r="AC30" s="92"/>
       <c r="AD30" s="101"/>
@@ -9680,10 +9588,10 @@
       <c r="E31" s="77"/>
       <c r="F31" s="62"/>
       <c r="G31" s="75"/>
-      <c r="H31" s="168"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="168"/>
-      <c r="K31" s="169"/>
+      <c r="H31" s="157"/>
+      <c r="I31" s="158"/>
+      <c r="J31" s="157"/>
+      <c r="K31" s="158"/>
       <c r="L31" s="77"/>
       <c r="M31" s="76"/>
       <c r="N31" s="77"/>
@@ -9692,14 +9600,14 @@
       <c r="Q31" s="77"/>
       <c r="R31" s="90"/>
       <c r="S31" s="91"/>
-      <c r="T31" s="178"/>
-      <c r="U31" s="179"/>
+      <c r="T31" s="167"/>
+      <c r="U31" s="168"/>
       <c r="V31" s="91"/>
       <c r="W31" s="92"/>
       <c r="X31" s="90"/>
       <c r="Y31" s="91"/>
-      <c r="Z31" s="158"/>
-      <c r="AA31" s="159"/>
+      <c r="Z31" s="147"/>
+      <c r="AA31" s="148"/>
       <c r="AB31" s="91"/>
       <c r="AC31" s="92"/>
       <c r="AD31" s="101"/>
@@ -9722,10 +9630,10 @@
       <c r="E32" s="77"/>
       <c r="F32" s="62"/>
       <c r="G32" s="75"/>
-      <c r="H32" s="168"/>
-      <c r="I32" s="169"/>
-      <c r="J32" s="168"/>
-      <c r="K32" s="169"/>
+      <c r="H32" s="157"/>
+      <c r="I32" s="158"/>
+      <c r="J32" s="157"/>
+      <c r="K32" s="158"/>
       <c r="L32" s="77"/>
       <c r="M32" s="76"/>
       <c r="N32" s="77"/>
@@ -9734,14 +9642,14 @@
       <c r="Q32" s="77"/>
       <c r="R32" s="90"/>
       <c r="S32" s="91"/>
-      <c r="T32" s="178"/>
-      <c r="U32" s="179"/>
+      <c r="T32" s="167"/>
+      <c r="U32" s="168"/>
       <c r="V32" s="91"/>
       <c r="W32" s="92"/>
       <c r="X32" s="90"/>
       <c r="Y32" s="91"/>
-      <c r="Z32" s="158"/>
-      <c r="AA32" s="159"/>
+      <c r="Z32" s="147"/>
+      <c r="AA32" s="148"/>
       <c r="AB32" s="91"/>
       <c r="AC32" s="92"/>
       <c r="AD32" s="101"/>
@@ -9764,10 +9672,10 @@
       <c r="E33" s="77"/>
       <c r="F33" s="62"/>
       <c r="G33" s="75"/>
-      <c r="H33" s="168"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="168"/>
-      <c r="K33" s="169"/>
+      <c r="H33" s="157"/>
+      <c r="I33" s="158"/>
+      <c r="J33" s="157"/>
+      <c r="K33" s="158"/>
       <c r="L33" s="77"/>
       <c r="M33" s="76"/>
       <c r="N33" s="77"/>
@@ -9776,14 +9684,14 @@
       <c r="Q33" s="77"/>
       <c r="R33" s="90"/>
       <c r="S33" s="91"/>
-      <c r="T33" s="178"/>
-      <c r="U33" s="179"/>
+      <c r="T33" s="167"/>
+      <c r="U33" s="168"/>
       <c r="V33" s="91"/>
       <c r="W33" s="92"/>
       <c r="X33" s="90"/>
       <c r="Y33" s="91"/>
-      <c r="Z33" s="158"/>
-      <c r="AA33" s="159"/>
+      <c r="Z33" s="147"/>
+      <c r="AA33" s="148"/>
       <c r="AB33" s="91"/>
       <c r="AC33" s="92"/>
       <c r="AD33" s="101"/>
@@ -9806,10 +9714,10 @@
       <c r="E34" s="80"/>
       <c r="F34" s="64"/>
       <c r="G34" s="78"/>
-      <c r="H34" s="170"/>
-      <c r="I34" s="171"/>
-      <c r="J34" s="170"/>
-      <c r="K34" s="171"/>
+      <c r="H34" s="159"/>
+      <c r="I34" s="160"/>
+      <c r="J34" s="159"/>
+      <c r="K34" s="160"/>
       <c r="L34" s="80"/>
       <c r="M34" s="79">
         <v>0.99</v>
@@ -9822,14 +9730,14 @@
       <c r="Q34" s="80"/>
       <c r="R34" s="93"/>
       <c r="S34" s="94"/>
-      <c r="T34" s="180"/>
-      <c r="U34" s="181"/>
+      <c r="T34" s="169"/>
+      <c r="U34" s="170"/>
       <c r="V34" s="94"/>
       <c r="W34" s="95"/>
       <c r="X34" s="93"/>
       <c r="Y34" s="94"/>
-      <c r="Z34" s="160"/>
-      <c r="AA34" s="161"/>
+      <c r="Z34" s="149"/>
+      <c r="AA34" s="150"/>
       <c r="AB34" s="94"/>
       <c r="AC34" s="95"/>
       <c r="AD34" s="102"/>

</xml_diff>